<commit_message>
V. 54 Cómo vender drogas online (a toda pastilla)
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5CA73C-1E99-46CE-A0AB-0203D3376DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F80F1D-76CE-4CBE-8161-A230D48DE3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,6 +63,7 @@
     <author>tc={9C26C127-20FF-4258-B62D-B6B902EB0E98}</author>
     <author>tc={162EA199-65BB-48FF-A9B1-580BDA0F2A25}</author>
     <author>tc={BC097833-5E05-4B57-A72A-B55B23EF385A}</author>
+    <author>tc={D69ACFED-A245-418D-8836-7787A10A08B4}</author>
     <author>tc={E34E6F01-0047-4D5E-A9F0-76B7D80CE842}</author>
     <author>tc={64FF07EB-F3D4-47C4-B23E-4905CF85CACC}</author>
     <author>tc={ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}</author>
@@ -275,7 +276,15 @@
     10 temporadas</t>
       </text>
     </comment>
-    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    4 temporadas</t>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -283,7 +292,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -291,7 +300,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+    <comment ref="B34" authorId="27" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -299,7 +308,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B36" authorId="27" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+    <comment ref="B37" authorId="28" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -307,7 +316,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="28" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+    <comment ref="B38" authorId="29" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -315,7 +324,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B39" authorId="29" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+    <comment ref="B40" authorId="30" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -323,7 +332,7 @@
     5 temporadas</t>
       </text>
     </comment>
-    <comment ref="B40" authorId="30" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+    <comment ref="B41" authorId="31" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -331,7 +340,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B41" authorId="31" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+    <comment ref="B42" authorId="32" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -339,7 +348,7 @@
     14 temporadas</t>
       </text>
     </comment>
-    <comment ref="B43" authorId="32" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+    <comment ref="B44" authorId="33" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -347,7 +356,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="33" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+    <comment ref="B45" authorId="34" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -355,7 +364,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B45" authorId="34" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+    <comment ref="B46" authorId="35" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -363,7 +372,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B47" authorId="35" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+    <comment ref="B48" authorId="36" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -371,7 +380,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B50" authorId="36" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+    <comment ref="B51" authorId="37" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -379,7 +388,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B54" authorId="37" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+    <comment ref="B55" authorId="38" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -387,7 +396,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B55" authorId="38" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+    <comment ref="B56" authorId="39" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -395,7 +404,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B56" authorId="39" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+    <comment ref="B57" authorId="40" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -403,7 +412,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B57" authorId="40" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <comment ref="B58" authorId="41" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -411,7 +420,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B58" authorId="41" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+    <comment ref="B59" authorId="42" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -486,7 +495,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="143">
   <si>
     <t>Película</t>
   </si>
@@ -912,6 +921,9 @@
   </si>
   <si>
     <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Cómo vender drogas online (a toda pastilla)</t>
   </si>
 </sst>
 </file>
@@ -962,7 +974,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1243,10 +1255,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:N58" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="B2:N58" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N58">
-    <sortCondition descending="1" ref="C2:C58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:N59" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B2:N59" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N59">
+    <sortCondition descending="1" ref="C2:C59"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="22"/>
@@ -1626,58 +1638,61 @@
   <threadedComment ref="B30" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
     <text>10 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B31" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+  <threadedComment ref="B31" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+    <text>4 temporadas</text>
+  </threadedComment>
+  <threadedComment ref="B32" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B32" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+  <threadedComment ref="B33" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B33" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+  <threadedComment ref="B34" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B36" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+  <threadedComment ref="B37" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B37" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+  <threadedComment ref="B38" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B39" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+  <threadedComment ref="B40" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
     <text>5 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B40" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+  <threadedComment ref="B41" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B41" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+  <threadedComment ref="B42" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
     <text>14 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+  <threadedComment ref="B44" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B44" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+  <threadedComment ref="B45" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+  <threadedComment ref="B46" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B47" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+  <threadedComment ref="B48" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B50" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+  <threadedComment ref="B51" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B54" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+  <threadedComment ref="B55" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B55" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+  <threadedComment ref="B56" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B56" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+  <threadedComment ref="B57" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B57" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+  <threadedComment ref="B58" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B58" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+  <threadedComment ref="B59" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
     <text>4 temporadas</text>
   </threadedComment>
 </ThreadedComments>
@@ -1689,10 +1704,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:P58"/>
+  <dimension ref="B2:P59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,50 +2797,50 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C31" s="5">
         <f>AVERAGE(D31,E31,F31,G31,H31,I31,I31,J31)</f>
-        <v>7.6000000000000005</v>
+        <v>7.6499999999999995</v>
       </c>
       <c r="D31" s="1">
         <v>8</v>
       </c>
       <c r="E31" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F31" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G31" s="1">
         <v>8</v>
       </c>
       <c r="H31" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I31" s="3">
-        <v>8.6</v>
+        <v>7.8</v>
       </c>
       <c r="J31" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="K31" s="1"/>
-      <c r="L31" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.6</v>
+      </c>
+      <c r="K31" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L31" s="1"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C32" s="5">
         <f>AVERAGE(D32,E32,F32,G32,H32,I32,I32,J32)</f>
-        <v>7.3750000000000009</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="D32" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E32" s="1">
         <v>8</v>
@@ -2834,52 +2849,52 @@
         <v>8</v>
       </c>
       <c r="G32" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H32" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I32" s="3">
-        <v>6.7</v>
+        <v>8.6</v>
       </c>
       <c r="J32" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K32" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L32" s="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="K32" s="1"/>
+      <c r="L32" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C33" s="5">
         <f>AVERAGE(D33,E33,F33,G33,H33,I33,I33,J33)</f>
-        <v>7.375</v>
+        <v>7.3750000000000009</v>
       </c>
       <c r="D33" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E33" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G33" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H33" s="1">
         <v>7</v>
       </c>
       <c r="I33" s="3">
-        <v>8.4</v>
+        <v>6.7</v>
       </c>
       <c r="J33" s="3">
-        <v>7.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K33" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2890,141 +2905,141 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="C34" s="5">
         <f>AVERAGE(D34,E34,F34,G34,H34,I34,I34,J34)</f>
-        <v>7.35</v>
+        <v>7.375</v>
       </c>
       <c r="D34" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F34" s="1">
         <v>7</v>
       </c>
       <c r="G34" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H34" s="1">
         <v>7</v>
       </c>
       <c r="I34" s="3">
-        <v>8.5</v>
+        <v>8.4</v>
       </c>
       <c r="J34" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="K34" s="1"/>
+        <v>7.2</v>
+      </c>
+      <c r="K34" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L34" s="1"/>
-      <c r="M34" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C35" s="5">
         <f>AVERAGE(D35,E35,F35,G35,H35,I35,I35,J35)</f>
-        <v>7.3250000000000002</v>
+        <v>7.35</v>
       </c>
       <c r="D35" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="1">
         <v>7</v>
       </c>
       <c r="G35" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I35" s="3">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="J35" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="K35" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L35" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+        <v>7.8</v>
+      </c>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="C36" s="5">
         <f>AVERAGE(D36,E36,F36,G36,H36,I36,I36,J36)</f>
-        <v>7.3125000000000009</v>
+        <v>7.3250000000000002</v>
       </c>
       <c r="D36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H36" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I36" s="3">
-        <v>6.7</v>
+        <v>8</v>
       </c>
       <c r="J36" s="3">
-        <v>6.1</v>
+        <v>6.6</v>
       </c>
       <c r="K36" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L36" s="1"/>
+      <c r="L36" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="C37" s="5">
         <f>AVERAGE(D37,E37,F37,G37,H37,I37,I37,J37)</f>
-        <v>7.3125</v>
+        <v>7.3125000000000009</v>
       </c>
       <c r="D37" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G37" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H37" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I37" s="3">
-        <v>9.1</v>
+        <v>6.7</v>
       </c>
       <c r="J37" s="3">
-        <v>8.3000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="K37" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3035,17 +3050,17 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C38" s="5">
         <f>AVERAGE(D38,E38,F38,G38,H38,I38,I38,J38)</f>
-        <v>7.3</v>
+        <v>7.3125</v>
       </c>
       <c r="D38" s="1">
         <v>6</v>
       </c>
       <c r="E38" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F38" s="1">
         <v>6</v>
@@ -3057,69 +3072,70 @@
         <v>7</v>
       </c>
       <c r="I38" s="3">
-        <v>8.5</v>
+        <v>9.1</v>
       </c>
       <c r="J38" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="K38" s="1"/>
-      <c r="L38" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K38" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L38" s="1"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C39" s="5">
         <f>AVERAGE(D39,E39,F39,G39,H39,I39,I39,J39)</f>
-        <v>7.2374999999999989</v>
+        <v>7.3</v>
       </c>
       <c r="D39" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F39" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G39" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H39" s="1">
         <v>7</v>
       </c>
       <c r="I39" s="3">
-        <v>8.3000000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="J39" s="3">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L39" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C40" s="5">
         <f>AVERAGE(D40,E40,F40,G40,H40,I40,I40,J40)</f>
-        <v>7.2</v>
+        <v>7.2374999999999989</v>
       </c>
       <c r="D40" s="1">
         <v>7</v>
       </c>
       <c r="E40" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F40" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G40" s="1">
         <v>6</v>
@@ -3128,10 +3144,10 @@
         <v>7</v>
       </c>
       <c r="I40" s="3">
-        <v>8.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J40" s="3">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -3141,210 +3157,210 @@
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C41" s="5">
         <f>AVERAGE(D41,E41,F41,G41,H41,I41,I41,J41)</f>
-        <v>7.1749999999999998</v>
+        <v>7.2</v>
       </c>
       <c r="D41" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G41" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H41" s="1">
         <v>7</v>
       </c>
       <c r="I41" s="3">
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="J41" s="3">
-        <v>5.4</v>
+        <v>7.4</v>
       </c>
       <c r="K41" s="1"/>
-      <c r="L41" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L41" s="1"/>
       <c r="M41" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C42" s="5">
         <f>AVERAGE(D42,E42,F42,G42,H42,I42,I42,J42)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1749999999999998</v>
       </c>
       <c r="D42" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E42" s="1">
         <v>6</v>
       </c>
       <c r="F42" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G42" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H42" s="1">
         <v>7</v>
       </c>
       <c r="I42" s="3">
-        <v>8.6999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="J42" s="3">
-        <v>8.6</v>
+        <v>5.4</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" s="1"/>
+      <c r="L42" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M42" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C43" s="5">
         <f>AVERAGE(D43,E43,F43,G43,H43,I43,I43,J43)</f>
-        <v>7.0250000000000004</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D43" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
       </c>
       <c r="F43" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G43" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H43" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I43" s="3">
-        <v>8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J43" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="K43" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>8.6</v>
+      </c>
+      <c r="K43" s="1"/>
       <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="M43" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,F44,G44,H44,I44,I44,J44)</f>
-        <v>6.8500000000000005</v>
+        <v>7.0250000000000004</v>
       </c>
       <c r="D44" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F44" s="1">
         <v>7</v>
       </c>
       <c r="G44" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H44" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I44" s="3">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="J44" s="3">
-        <v>6.4</v>
+        <v>7.2</v>
       </c>
       <c r="K44" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L44" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L44" s="1"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,F45,G45,H45,I45,I45,J45)</f>
-        <v>6.8250000000000002</v>
+        <v>6.8500000000000005</v>
       </c>
       <c r="D45" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G45" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I45" s="3">
-        <v>8.6</v>
+        <v>7.7</v>
       </c>
       <c r="J45" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="K45" s="1"/>
-      <c r="L45" s="1"/>
-      <c r="M45" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.4</v>
+      </c>
+      <c r="K45" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L45" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,F46,G46,H46,I46,I46,J46)</f>
-        <v>6.8</v>
+        <v>6.8250000000000002</v>
       </c>
       <c r="D46" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F46" s="1">
         <v>6</v>
       </c>
       <c r="G46" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H46" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I46" s="3">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="J46" s="3">
         <v>7.4</v>
@@ -3357,53 +3373,52 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,F47,G47,H47,I47,I47,J47)</f>
-        <v>6.6749999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="D47" s="1">
+        <v>6</v>
+      </c>
+      <c r="E47" s="1">
         <v>5</v>
       </c>
-      <c r="E47" s="1">
-        <v>8</v>
-      </c>
       <c r="F47" s="1">
         <v>6</v>
       </c>
       <c r="G47" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I47" s="3">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="J47" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="K47" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
+      <c r="M47" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,F48,G48,H48,I48,I48,J48)</f>
-        <v>6.6125000000000007</v>
+        <v>6.6749999999999998</v>
       </c>
       <c r="D48" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1">
         <v>6</v>
@@ -3412,36 +3427,34 @@
         <v>7</v>
       </c>
       <c r="H48" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I48" s="3">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="J48" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="K48" s="1"/>
-      <c r="L48" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>5.4</v>
+      </c>
+      <c r="K48" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L48" s="1"/>
       <c r="M48" s="1"/>
-      <c r="N48" s="1" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
+      <c r="N48" s="1"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,F49,G49,H49,I49,I49,J49)</f>
-        <v>6.5249999999999995</v>
+        <v>6.6125000000000007</v>
       </c>
       <c r="D49" s="1">
         <v>6</v>
       </c>
       <c r="E49" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F49" s="1">
         <v>6</v>
@@ -3450,230 +3463,232 @@
         <v>7</v>
       </c>
       <c r="H49" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I49" s="3">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="J49" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="K49" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L49" s="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="K49" s="1"/>
+      <c r="L49" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="N49" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,F50,G50,H50,I50,I50,J50)</f>
-        <v>6.4750000000000005</v>
+        <v>6.5249999999999995</v>
       </c>
       <c r="D50" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E50" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F50" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G50" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H50" s="1">
         <v>6</v>
       </c>
       <c r="I50" s="3">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="J50" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="K50" s="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="K50" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L50" s="1"/>
-      <c r="M50" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,F51,G51,H51,I51,I51,J51)</f>
-        <v>6.3500000000000005</v>
+        <v>6.4750000000000005</v>
       </c>
       <c r="D51" s="1">
+        <v>8</v>
+      </c>
+      <c r="E51" s="1">
+        <v>4</v>
+      </c>
+      <c r="F51" s="1">
+        <v>7</v>
+      </c>
+      <c r="G51" s="1">
         <v>5</v>
       </c>
-      <c r="E51" s="1">
-        <v>5</v>
-      </c>
-      <c r="F51" s="1">
-        <v>5</v>
-      </c>
-      <c r="G51" s="1">
-        <v>6</v>
-      </c>
       <c r="H51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I51" s="3">
-        <v>8.1999999999999993</v>
+        <v>7.7</v>
       </c>
       <c r="J51" s="3">
         <v>6.4</v>
       </c>
-      <c r="K51" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L51" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,F52,G52,H52,I52,I52,J52)</f>
-        <v>6.2750000000000004</v>
+        <v>6.3500000000000005</v>
       </c>
       <c r="D52" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F52" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G52" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H52" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I52" s="3">
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="J52" s="3">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="K52" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L52" s="1"/>
+      <c r="L52" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,F53,G53,H53,I53,I53,J53)</f>
-        <v>6.1750000000000007</v>
+        <v>6.2750000000000004</v>
       </c>
       <c r="D53" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
+        <v>6</v>
+      </c>
+      <c r="F53" s="1">
+        <v>6</v>
+      </c>
+      <c r="G53" s="1">
         <v>5</v>
       </c>
-      <c r="F53" s="1">
-        <v>6</v>
-      </c>
-      <c r="G53" s="1">
-        <v>6</v>
-      </c>
       <c r="H53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I53" s="3">
-        <v>6.6</v>
+        <v>8.1</v>
       </c>
       <c r="J53" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="K53" s="1"/>
-      <c r="L53" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K53" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L53" s="1"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,F54,G54,H54,I54,I54,J54)</f>
-        <v>6.1</v>
+        <v>6.1750000000000007</v>
       </c>
       <c r="D54" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E54" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F54" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H54" s="1">
         <v>6</v>
       </c>
       <c r="I54" s="3">
-        <v>7.3</v>
+        <v>6.6</v>
       </c>
       <c r="J54" s="3">
         <v>6.2</v>
       </c>
-      <c r="K54" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,F55,G55,H55,I55,I55,J55)</f>
-        <v>5.9124999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D55" s="1">
+        <v>6</v>
+      </c>
+      <c r="E55" s="1">
+        <v>7</v>
+      </c>
+      <c r="F55" s="1">
         <v>4</v>
       </c>
-      <c r="E55" s="1">
-        <v>7</v>
-      </c>
-      <c r="F55" s="1">
+      <c r="G55" s="1">
         <v>5</v>
       </c>
-      <c r="G55" s="1">
-        <v>3</v>
-      </c>
       <c r="H55" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I55" s="3">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="J55" s="3">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="K55" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3684,32 +3699,32 @@
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,F56,G56,H56,I56,I56,J56)</f>
-        <v>5.9</v>
+        <v>5.9124999999999996</v>
       </c>
       <c r="D56" s="1">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
         <v>5</v>
       </c>
-      <c r="E56" s="1">
-        <v>7</v>
-      </c>
-      <c r="F56" s="1">
-        <v>7</v>
-      </c>
       <c r="G56" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H56" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I56" s="3">
-        <v>6.1</v>
+        <v>7.5</v>
       </c>
       <c r="J56" s="3">
-        <v>5</v>
+        <v>6.3</v>
       </c>
       <c r="K56" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3720,11 +3735,11 @@
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,F57,G57,H57,I57,I57,J57)</f>
-        <v>5.3375000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="D57" s="1">
         <v>5</v>
@@ -3733,61 +3748,97 @@
         <v>7</v>
       </c>
       <c r="F57" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1">
+        <v>8</v>
+      </c>
+      <c r="H57" s="1">
+        <v>3</v>
+      </c>
+      <c r="I57" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="J57" s="3">
         <v>5</v>
       </c>
-      <c r="H57" s="1">
-        <v>7</v>
-      </c>
-      <c r="I57" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J57" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="K57" s="1"/>
+      <c r="K57" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L57" s="1"/>
-      <c r="M57" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,F58,G58,H58,I58,I58,J58)</f>
+        <v>5.3375000000000004</v>
+      </c>
+      <c r="D58" s="1">
+        <v>5</v>
+      </c>
+      <c r="E58" s="1">
+        <v>7</v>
+      </c>
+      <c r="F58" s="1">
+        <v>6</v>
+      </c>
+      <c r="G58" s="1">
+        <v>5</v>
+      </c>
+      <c r="H58" s="1">
+        <v>7</v>
+      </c>
+      <c r="I58" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J58" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C59" s="5">
+        <f>AVERAGE(D59,E59,F59,G59,H59,I59,I59,J59)</f>
         <v>4.7124999999999995</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D59" s="1">
         <v>2</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="1">
         <v>4</v>
       </c>
-      <c r="F58" s="1">
+      <c r="F59" s="1">
         <v>2</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G59" s="1">
         <v>3</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H59" s="1">
         <v>5</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I59" s="3">
         <v>7.7</v>
       </c>
-      <c r="J58" s="3">
+      <c r="J59" s="3">
         <v>6.3</v>
       </c>
-      <c r="K58" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
+      <c r="K59" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
V. 55 Mindfulness para asesinos
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F80F1D-76CE-4CBE-8161-A230D48DE3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB34516-4E52-4703-A600-91B94E3D5D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,6 +60,7 @@
     <author>tc={E767B4D9-B138-43E0-903B-85823960EFBB}</author>
     <author>tc={97D38487-0228-4117-9D87-BCCFD4EC6983}</author>
     <author>tc={B1E35BAB-7C71-4B4F-9EE2-76495541B293}</author>
+    <author>tc={C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}</author>
     <author>tc={9C26C127-20FF-4258-B62D-B6B902EB0E98}</author>
     <author>tc={162EA199-65BB-48FF-A9B1-580BDA0F2A25}</author>
     <author>tc={BC097833-5E05-4B57-A72A-B55B23EF385A}</author>
@@ -252,7 +253,15 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B28" authorId="21" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+    <comment ref="B28" authorId="21" shapeId="0" xr:uid="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    1 temporada</t>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="22" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -260,7 +269,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B29" authorId="22" shapeId="0" xr:uid="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
+    <comment ref="B30" authorId="23" shapeId="0" xr:uid="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -268,7 +277,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B30" authorId="23" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -276,7 +285,7 @@
     10 temporadas</t>
       </text>
     </comment>
-    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -284,7 +293,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -292,7 +301,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+    <comment ref="B34" authorId="27" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -300,7 +309,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B34" authorId="27" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+    <comment ref="B35" authorId="28" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -308,7 +317,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="28" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+    <comment ref="B38" authorId="29" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -316,7 +325,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B38" authorId="29" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+    <comment ref="B39" authorId="30" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -324,7 +333,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B40" authorId="30" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+    <comment ref="B41" authorId="31" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -332,7 +341,7 @@
     5 temporadas</t>
       </text>
     </comment>
-    <comment ref="B41" authorId="31" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+    <comment ref="B42" authorId="32" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -340,7 +349,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="32" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+    <comment ref="B43" authorId="33" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -348,7 +357,7 @@
     14 temporadas</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="33" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+    <comment ref="B45" authorId="34" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -356,7 +365,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B45" authorId="34" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+    <comment ref="B46" authorId="35" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -364,7 +373,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B46" authorId="35" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+    <comment ref="B47" authorId="36" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -372,7 +381,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B48" authorId="36" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+    <comment ref="B49" authorId="37" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -380,7 +389,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B51" authorId="37" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+    <comment ref="B52" authorId="38" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -388,7 +397,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B55" authorId="38" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+    <comment ref="B56" authorId="39" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -396,7 +405,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B56" authorId="39" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+    <comment ref="B57" authorId="40" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -404,7 +413,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B57" authorId="40" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+    <comment ref="B58" authorId="41" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -412,7 +421,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B58" authorId="41" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <comment ref="B59" authorId="42" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -420,7 +429,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B59" authorId="42" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+    <comment ref="B60" authorId="43" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -495,7 +504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="144">
   <si>
     <t>Película</t>
   </si>
@@ -924,6 +933,9 @@
   </si>
   <si>
     <t>Cómo vender drogas online (a toda pastilla)</t>
+  </si>
+  <si>
+    <t>Mindfulness para asesinos</t>
   </si>
 </sst>
 </file>
@@ -974,7 +986,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1255,10 +1267,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:N59" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="B2:N59" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N59">
-    <sortCondition descending="1" ref="C2:C59"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:N60" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+  <autoFilter ref="B2:N60" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:N60">
+    <sortCondition descending="1" ref="C2:C60"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="22"/>
@@ -1629,70 +1641,73 @@
   <threadedComment ref="B27" dT="2024-07-08T19:01:48.87" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B28" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+  <threadedComment ref="B28" dT="2025-04-19T09:54:12.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
+    <text>1 temporada</text>
+  </threadedComment>
+  <threadedComment ref="B29" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B29" dT="2024-07-08T19:06:42.39" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
+  <threadedComment ref="B30" dT="2024-07-08T19:06:42.39" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B30" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+  <threadedComment ref="B31" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
     <text>10 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B31" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+  <threadedComment ref="B32" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B32" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+  <threadedComment ref="B33" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B33" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+  <threadedComment ref="B34" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B34" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+  <threadedComment ref="B35" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B37" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+  <threadedComment ref="B38" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B38" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+  <threadedComment ref="B39" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B40" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+  <threadedComment ref="B41" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
     <text>5 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B41" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+  <threadedComment ref="B42" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B42" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+  <threadedComment ref="B43" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
     <text>14 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B44" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+  <threadedComment ref="B45" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+  <threadedComment ref="B46" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B46" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+  <threadedComment ref="B47" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B48" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+  <threadedComment ref="B49" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B51" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+  <threadedComment ref="B52" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B55" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+  <threadedComment ref="B56" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B56" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+  <threadedComment ref="B57" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B57" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+  <threadedComment ref="B58" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B58" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+  <threadedComment ref="B59" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B59" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+  <threadedComment ref="B60" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
     <text>4 temporadas</text>
   </threadedComment>
 </ThreadedComments>
@@ -1704,10 +1719,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:P59"/>
+  <dimension ref="B2:P60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2684,107 +2699,104 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>43</v>
+        <v>143</v>
       </c>
       <c r="C28" s="5">
         <f>AVERAGE(D28,E28,F28,G28,H28,I28,I28,J28)</f>
-        <v>7.6875000000000009</v>
+        <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E28" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F28" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H28" s="1">
         <v>8</v>
       </c>
       <c r="I28" s="3">
-        <v>7.2</v>
+        <v>7.4</v>
       </c>
       <c r="J28" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="K28" s="1"/>
-      <c r="L28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.5</v>
+      </c>
+      <c r="K28" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L28" s="1"/>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="C29" s="5">
         <f>AVERAGE(D29,E29,F29,G29,H29,I29,I29,J29)</f>
-        <v>7.65</v>
+        <v>7.6875000000000009</v>
       </c>
       <c r="D29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G29" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H29" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I29" s="3">
-        <v>8.1</v>
+        <v>7.2</v>
       </c>
       <c r="J29" s="3">
-        <v>7</v>
-      </c>
-      <c r="K29" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.1</v>
+      </c>
+      <c r="K29" s="1"/>
       <c r="L29" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="M29" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="C30" s="5">
         <f>AVERAGE(D30,E30,F30,G30,H30,I30,I30,J30)</f>
-        <v>7.6499999999999995</v>
+        <v>7.65</v>
       </c>
       <c r="D30" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G30" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H30" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I30" s="3">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="J30" s="3">
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="K30" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2792,12 +2804,13 @@
       <c r="L30" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
+      <c r="M30" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="C31" s="5">
         <f>AVERAGE(D31,E31,F31,G31,H31,I31,I31,J31)</f>
@@ -2807,7 +2820,7 @@
         <v>8</v>
       </c>
       <c r="E31" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1">
         <v>7</v>
@@ -2816,67 +2829,69 @@
         <v>8</v>
       </c>
       <c r="H31" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I31" s="3">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="J31" s="3">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="K31" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L31" s="1"/>
+      <c r="L31" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C32" s="5">
         <f>AVERAGE(D32,E32,F32,G32,H32,I32,I32,J32)</f>
-        <v>7.6000000000000005</v>
+        <v>7.6499999999999995</v>
       </c>
       <c r="D32" s="1">
         <v>8</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F32" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1">
         <v>8</v>
       </c>
       <c r="H32" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I32" s="3">
-        <v>8.6</v>
+        <v>7.8</v>
       </c>
       <c r="J32" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="K32" s="1"/>
-      <c r="L32" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.6</v>
+      </c>
+      <c r="K32" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L32" s="1"/>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>80</v>
+        <v>47</v>
       </c>
       <c r="C33" s="5">
         <f>AVERAGE(D33,E33,F33,G33,H33,I33,I33,J33)</f>
-        <v>7.3750000000000009</v>
+        <v>7.6000000000000005</v>
       </c>
       <c r="D33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1">
         <v>8</v>
@@ -2885,52 +2900,52 @@
         <v>8</v>
       </c>
       <c r="G33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H33" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I33" s="3">
-        <v>6.7</v>
+        <v>8.6</v>
       </c>
       <c r="J33" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="K33" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L33" s="1"/>
+        <v>7.6</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C34" s="5">
         <f>AVERAGE(D34,E34,F34,G34,H34,I34,I34,J34)</f>
-        <v>7.375</v>
+        <v>7.3750000000000009</v>
       </c>
       <c r="D34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H34" s="1">
         <v>7</v>
       </c>
       <c r="I34" s="3">
-        <v>8.4</v>
+        <v>6.7</v>
       </c>
       <c r="J34" s="3">
-        <v>7.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K34" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2941,141 +2956,141 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="C35" s="5">
         <f>AVERAGE(D35,E35,F35,G35,H35,I35,I35,J35)</f>
-        <v>7.35</v>
+        <v>7.375</v>
       </c>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F35" s="1">
         <v>7</v>
       </c>
       <c r="G35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H35" s="1">
         <v>7</v>
       </c>
       <c r="I35" s="3">
-        <v>8.5</v>
+        <v>8.4</v>
       </c>
       <c r="J35" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="K35" s="1"/>
+        <v>7.2</v>
+      </c>
+      <c r="K35" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L35" s="1"/>
-      <c r="M35" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
         <f>AVERAGE(D36,E36,F36,G36,H36,I36,I36,J36)</f>
-        <v>7.3250000000000002</v>
+        <v>7.35</v>
       </c>
       <c r="D36" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" s="1">
         <v>7</v>
       </c>
       <c r="G36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H36" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I36" s="3">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="J36" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="K36" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L36" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M36" s="1"/>
-      <c r="N36" s="1"/>
+        <v>7.8</v>
+      </c>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>141</v>
+        <v>29</v>
       </c>
       <c r="C37" s="5">
         <f>AVERAGE(D37,E37,F37,G37,H37,I37,I37,J37)</f>
-        <v>7.3125000000000009</v>
+        <v>7.3250000000000002</v>
       </c>
       <c r="D37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H37" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I37" s="3">
-        <v>6.7</v>
+        <v>8</v>
       </c>
       <c r="J37" s="3">
-        <v>6.1</v>
+        <v>6.6</v>
       </c>
       <c r="K37" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L37" s="1"/>
+      <c r="L37" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="C38" s="5">
         <f>AVERAGE(D38,E38,F38,G38,H38,I38,I38,J38)</f>
-        <v>7.3125</v>
+        <v>7.3125000000000009</v>
       </c>
       <c r="D38" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F38" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G38" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H38" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I38" s="3">
-        <v>9.1</v>
+        <v>6.7</v>
       </c>
       <c r="J38" s="3">
-        <v>8.3000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="K38" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3086,17 +3101,17 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C39" s="5">
         <f>AVERAGE(D39,E39,F39,G39,H39,I39,I39,J39)</f>
-        <v>7.3</v>
+        <v>7.3125</v>
       </c>
       <c r="D39" s="1">
         <v>6</v>
       </c>
       <c r="E39" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F39" s="1">
         <v>6</v>
@@ -3108,69 +3123,70 @@
         <v>7</v>
       </c>
       <c r="I39" s="3">
-        <v>8.5</v>
+        <v>9.1</v>
       </c>
       <c r="J39" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="K39" s="1"/>
-      <c r="L39" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K39" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L39" s="1"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="C40" s="5">
         <f>AVERAGE(D40,E40,F40,G40,H40,I40,I40,J40)</f>
-        <v>7.2374999999999989</v>
+        <v>7.3</v>
       </c>
       <c r="D40" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F40" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G40" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H40" s="1">
         <v>7</v>
       </c>
       <c r="I40" s="3">
-        <v>8.3000000000000007</v>
+        <v>8.5</v>
       </c>
       <c r="J40" s="3">
-        <v>7.3</v>
+        <v>7.4</v>
       </c>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L40" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C41" s="5">
         <f>AVERAGE(D41,E41,F41,G41,H41,I41,I41,J41)</f>
-        <v>7.2</v>
+        <v>7.2374999999999989</v>
       </c>
       <c r="D41" s="1">
         <v>7</v>
       </c>
       <c r="E41" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F41" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
         <v>6</v>
@@ -3179,10 +3195,10 @@
         <v>7</v>
       </c>
       <c r="I41" s="3">
-        <v>8.6</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J41" s="3">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -3192,210 +3208,210 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C42" s="5">
         <f>AVERAGE(D42,E42,F42,G42,H42,I42,I42,J42)</f>
-        <v>7.1749999999999998</v>
+        <v>7.2</v>
       </c>
       <c r="D42" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E42" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H42" s="1">
         <v>7</v>
       </c>
       <c r="I42" s="3">
-        <v>7.5</v>
+        <v>8.6</v>
       </c>
       <c r="J42" s="3">
-        <v>5.4</v>
+        <v>7.4</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L42" s="1"/>
       <c r="M42" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="C43" s="5">
         <f>AVERAGE(D43,E43,F43,G43,H43,I43,I43,J43)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1">
         <v>6</v>
       </c>
       <c r="F43" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H43" s="1">
         <v>7</v>
       </c>
       <c r="I43" s="3">
-        <v>8.6999999999999993</v>
+        <v>7.5</v>
       </c>
       <c r="J43" s="3">
-        <v>8.6</v>
+        <v>5.4</v>
       </c>
       <c r="K43" s="1"/>
-      <c r="L43" s="1"/>
+      <c r="L43" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M43" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>76</v>
+        <v>44</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,F44,G44,H44,I44,I44,J44)</f>
-        <v>7.0250000000000004</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D44" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" s="1">
         <v>6</v>
       </c>
       <c r="F44" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G44" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H44" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I44" s="3">
-        <v>8</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="J44" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="K44" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>8.6</v>
+      </c>
+      <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="M44" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,F45,G45,H45,I45,I45,J45)</f>
-        <v>6.8500000000000005</v>
+        <v>7.0250000000000004</v>
       </c>
       <c r="D45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E45" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F45" s="1">
         <v>7</v>
       </c>
       <c r="G45" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H45" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I45" s="3">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="J45" s="3">
-        <v>6.4</v>
+        <v>7.2</v>
       </c>
       <c r="K45" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L45" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L45" s="1"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,F46,G46,H46,I46,I46,J46)</f>
-        <v>6.8250000000000002</v>
+        <v>6.8500000000000005</v>
       </c>
       <c r="D46" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F46" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G46" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H46" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I46" s="3">
-        <v>8.6</v>
+        <v>7.7</v>
       </c>
       <c r="J46" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="K46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="M46" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.4</v>
+      </c>
+      <c r="K46" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L46" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,F47,G47,H47,I47,I47,J47)</f>
-        <v>6.8</v>
+        <v>6.8250000000000002</v>
       </c>
       <c r="D47" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E47" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F47" s="1">
         <v>6</v>
       </c>
       <c r="G47" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H47" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I47" s="3">
-        <v>8.5</v>
+        <v>8.6</v>
       </c>
       <c r="J47" s="3">
         <v>7.4</v>
@@ -3408,53 +3424,52 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,F48,G48,H48,I48,I48,J48)</f>
-        <v>6.6749999999999998</v>
+        <v>6.8</v>
       </c>
       <c r="D48" s="1">
+        <v>6</v>
+      </c>
+      <c r="E48" s="1">
         <v>5</v>
       </c>
-      <c r="E48" s="1">
-        <v>8</v>
-      </c>
       <c r="F48" s="1">
         <v>6</v>
       </c>
       <c r="G48" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H48" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I48" s="3">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="J48" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="K48" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
+      <c r="M48" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,F49,G49,H49,I49,I49,J49)</f>
-        <v>6.6125000000000007</v>
+        <v>6.6749999999999998</v>
       </c>
       <c r="D49" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E49" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1">
         <v>6</v>
@@ -3463,36 +3478,34 @@
         <v>7</v>
       </c>
       <c r="H49" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I49" s="3">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="J49" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="K49" s="1"/>
-      <c r="L49" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>5.4</v>
+      </c>
+      <c r="K49" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L49" s="1"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="1" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
+      <c r="N49" s="1"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>13</v>
+        <v>106</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,F50,G50,H50,I50,I50,J50)</f>
-        <v>6.5249999999999995</v>
+        <v>6.6125000000000007</v>
       </c>
       <c r="D50" s="1">
         <v>6</v>
       </c>
       <c r="E50" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F50" s="1">
         <v>6</v>
@@ -3501,230 +3514,232 @@
         <v>7</v>
       </c>
       <c r="H50" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I50" s="3">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="J50" s="3">
-        <v>6.6</v>
-      </c>
-      <c r="K50" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L50" s="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="K50" s="1"/>
+      <c r="L50" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
+      <c r="N50" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,F51,G51,H51,I51,I51,J51)</f>
-        <v>6.4750000000000005</v>
+        <v>6.5249999999999995</v>
       </c>
       <c r="D51" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E51" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G51" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H51" s="1">
         <v>6</v>
       </c>
       <c r="I51" s="3">
-        <v>7.7</v>
+        <v>7.8</v>
       </c>
       <c r="J51" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="K51" s="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="K51" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L51" s="1"/>
-      <c r="M51" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,F52,G52,H52,I52,I52,J52)</f>
-        <v>6.3500000000000005</v>
+        <v>6.4750000000000005</v>
       </c>
       <c r="D52" s="1">
+        <v>8</v>
+      </c>
+      <c r="E52" s="1">
+        <v>4</v>
+      </c>
+      <c r="F52" s="1">
+        <v>7</v>
+      </c>
+      <c r="G52" s="1">
         <v>5</v>
       </c>
-      <c r="E52" s="1">
-        <v>5</v>
-      </c>
-      <c r="F52" s="1">
-        <v>5</v>
-      </c>
-      <c r="G52" s="1">
-        <v>6</v>
-      </c>
       <c r="H52" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I52" s="3">
-        <v>8.1999999999999993</v>
+        <v>7.7</v>
       </c>
       <c r="J52" s="3">
         <v>6.4</v>
       </c>
-      <c r="K52" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L52" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,F53,G53,H53,I53,I53,J53)</f>
-        <v>6.2750000000000004</v>
+        <v>6.3500000000000005</v>
       </c>
       <c r="D53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G53" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H53" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I53" s="3">
-        <v>8.1</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="J53" s="3">
-        <v>6</v>
+        <v>6.4</v>
       </c>
       <c r="K53" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L53" s="1"/>
+      <c r="L53" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,F54,G54,H54,I54,I54,J54)</f>
-        <v>6.1750000000000007</v>
+        <v>6.2750000000000004</v>
       </c>
       <c r="D54" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1">
+        <v>6</v>
+      </c>
+      <c r="F54" s="1">
+        <v>6</v>
+      </c>
+      <c r="G54" s="1">
         <v>5</v>
       </c>
-      <c r="F54" s="1">
-        <v>6</v>
-      </c>
-      <c r="G54" s="1">
-        <v>6</v>
-      </c>
       <c r="H54" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I54" s="3">
-        <v>6.6</v>
+        <v>8.1</v>
       </c>
       <c r="J54" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="K54" s="1"/>
-      <c r="L54" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K54" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,F55,G55,H55,I55,I55,J55)</f>
-        <v>6.1</v>
+        <v>6.1750000000000007</v>
       </c>
       <c r="D55" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F55" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G55" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H55" s="1">
         <v>6</v>
       </c>
       <c r="I55" s="3">
-        <v>7.3</v>
+        <v>6.6</v>
       </c>
       <c r="J55" s="3">
         <v>6.2</v>
       </c>
-      <c r="K55" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,F56,G56,H56,I56,I56,J56)</f>
-        <v>5.9124999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="D56" s="1">
+        <v>6</v>
+      </c>
+      <c r="E56" s="1">
+        <v>7</v>
+      </c>
+      <c r="F56" s="1">
         <v>4</v>
       </c>
-      <c r="E56" s="1">
-        <v>7</v>
-      </c>
-      <c r="F56" s="1">
+      <c r="G56" s="1">
         <v>5</v>
       </c>
-      <c r="G56" s="1">
-        <v>3</v>
-      </c>
       <c r="H56" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I56" s="3">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="J56" s="3">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
       <c r="K56" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3735,32 +3750,32 @@
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,F57,G57,H57,I57,I57,J57)</f>
-        <v>5.9</v>
+        <v>5.9124999999999996</v>
       </c>
       <c r="D57" s="1">
+        <v>4</v>
+      </c>
+      <c r="E57" s="1">
+        <v>7</v>
+      </c>
+      <c r="F57" s="1">
         <v>5</v>
       </c>
-      <c r="E57" s="1">
-        <v>7</v>
-      </c>
-      <c r="F57" s="1">
-        <v>7</v>
-      </c>
       <c r="G57" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="H57" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I57" s="3">
-        <v>6.1</v>
+        <v>7.5</v>
       </c>
       <c r="J57" s="3">
-        <v>5</v>
+        <v>6.3</v>
       </c>
       <c r="K57" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3771,11 +3786,11 @@
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,F58,G58,H58,I58,I58,J58)</f>
-        <v>5.3375000000000004</v>
+        <v>5.9</v>
       </c>
       <c r="D58" s="1">
         <v>5</v>
@@ -3784,61 +3799,97 @@
         <v>7</v>
       </c>
       <c r="F58" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G58" s="1">
+        <v>8</v>
+      </c>
+      <c r="H58" s="1">
+        <v>3</v>
+      </c>
+      <c r="I58" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="J58" s="3">
         <v>5</v>
       </c>
-      <c r="H58" s="1">
-        <v>7</v>
-      </c>
-      <c r="I58" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="J58" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="K58" s="1"/>
+      <c r="K58" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="L58" s="1"/>
-      <c r="M58" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,F59,G59,H59,I59,I59,J59)</f>
+        <v>5.3375000000000004</v>
+      </c>
+      <c r="D59" s="1">
+        <v>5</v>
+      </c>
+      <c r="E59" s="1">
+        <v>7</v>
+      </c>
+      <c r="F59" s="1">
+        <v>6</v>
+      </c>
+      <c r="G59" s="1">
+        <v>5</v>
+      </c>
+      <c r="H59" s="1">
+        <v>7</v>
+      </c>
+      <c r="I59" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J59" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C60" s="5">
+        <f>AVERAGE(D60,E60,F60,G60,H60,I60,I60,J60)</f>
         <v>4.7124999999999995</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D60" s="1">
         <v>2</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E60" s="1">
         <v>4</v>
       </c>
-      <c r="F59" s="1">
+      <c r="F60" s="1">
         <v>2</v>
       </c>
-      <c r="G59" s="1">
+      <c r="G60" s="1">
         <v>3</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H60" s="1">
         <v>5</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I60" s="3">
         <v>7.7</v>
       </c>
-      <c r="J59" s="3">
+      <c r="J60" s="3">
         <v>6.3</v>
       </c>
-      <c r="K59" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
+      <c r="K60" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
V. 56 Equipaje de mano
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB34516-4E52-4703-A600-91B94E3D5D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C9DBD5-D96B-49B3-B999-0E78E70F2057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -504,7 +504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="145">
   <si>
     <t>Película</t>
   </si>
@@ -936,6 +936,9 @@
   </si>
   <si>
     <t>Mindfulness para asesinos</t>
+  </si>
+  <si>
+    <t>Equipaje de mano</t>
   </si>
 </sst>
 </file>
@@ -945,7 +948,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,12 +984,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1030,7 +1027,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1053,6 +1050,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1294,10 +1294,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I72" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I72" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I72">
-    <sortCondition descending="1" ref="C2:C72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I73" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I73" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I73">
+    <sortCondition descending="1" ref="C2:C73"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1721,7 +1721,7 @@
   </sheetPr>
   <dimension ref="B2:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -1789,7 +1789,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,G3,H3,I3,I3,J3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,G3,H3,I3,I3,J3)</f>
         <v>9.4</v>
       </c>
       <c r="D3" s="1">
@@ -1826,7 +1826,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,G4,H4,I4,I4,J4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -1862,7 +1862,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,G5,H5,I5,I5,J5)</f>
+        <f t="shared" si="0"/>
         <v>8.7312500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -1901,7 +1901,7 @@
         <v>112</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,G6,H6,I6,I6,J6)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D6" s="1">
@@ -1938,7 +1938,7 @@
         <v>93</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,G7,H7,I7,I7,J7)</f>
+        <f t="shared" si="0"/>
         <v>8.5250000000000004</v>
       </c>
       <c r="D7" s="1">
@@ -1974,7 +1974,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,G8,H8,I8,I8,J8)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D8" s="1">
@@ -2010,7 +2010,7 @@
         <v>140</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,G9,H9,I9,I9,J9)</f>
+        <f t="shared" si="0"/>
         <v>8.4124999999999996</v>
       </c>
       <c r="D9" s="1">
@@ -2046,7 +2046,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,G10,H10,I10,I10,J10)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D10" s="1">
@@ -2082,7 +2082,7 @@
         <v>7</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,G11,H11,I11,I11,J11)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D11" s="1">
@@ -2118,7 +2118,7 @@
         <v>138</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,G12,H12,I12,I12,J12)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D12" s="1">
@@ -2154,7 +2154,7 @@
         <v>28</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,G13,H13,I13,I13,J13)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D13" s="1">
@@ -2192,7 +2192,7 @@
         <v>46</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,G14,H14,I14,I14,J14)</f>
+        <f t="shared" si="0"/>
         <v>8.2625000000000011</v>
       </c>
       <c r="D14" s="1">
@@ -2228,7 +2228,7 @@
         <v>20</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,G15,H15,I15,I15,J15)</f>
+        <f t="shared" si="0"/>
         <v>8.2375000000000007</v>
       </c>
       <c r="D15" s="1">
@@ -2266,7 +2266,7 @@
         <v>10</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,G16,H16,I16,I16,J16)</f>
+        <f t="shared" si="0"/>
         <v>8.2124999999999986</v>
       </c>
       <c r="D16" s="1">
@@ -2304,7 +2304,7 @@
         <v>8</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,G17,H17,I17,I17,J17)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D17" s="1">
@@ -2342,7 +2342,7 @@
         <v>137</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,G18,H18,I18,I18,J18)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D18" s="1">
@@ -2378,7 +2378,7 @@
         <v>92</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,G19,H19,I19,I19,J19)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D19" s="1">
@@ -2414,7 +2414,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,G20,H20,I20,I20,J20)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D20" s="1">
@@ -2450,7 +2450,7 @@
         <v>33</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,G21,H21,I21,I21,J21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2486,7 +2486,7 @@
         <v>120</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,G22,H22,I22,I22,J22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2522,7 +2522,7 @@
         <v>70</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,G23,H23,I23,I23,J23)</f>
+        <f t="shared" si="0"/>
         <v>7.9749999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -2556,7 +2556,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,G24,H24,I24,I24,J24)</f>
+        <f t="shared" si="0"/>
         <v>7.9625000000000004</v>
       </c>
       <c r="D24" s="1">
@@ -2592,7 +2592,7 @@
         <v>139</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,G25,H25,I25,I25,J25)</f>
+        <f t="shared" si="0"/>
         <v>7.9375</v>
       </c>
       <c r="D25" s="1">
@@ -2628,7 +2628,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,G26,H26,I26,I26,J26)</f>
+        <f t="shared" si="0"/>
         <v>7.9124999999999996</v>
       </c>
       <c r="D26" s="1">
@@ -2664,7 +2664,7 @@
         <v>73</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,G27,H27,I27,I27,J27)</f>
+        <f t="shared" si="0"/>
         <v>7.8500000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -2702,7 +2702,7 @@
         <v>143</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,G28,H28,I28,I28,J28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2738,7 +2738,7 @@
         <v>43</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,G29,H29,I29,I29,J29)</f>
+        <f t="shared" si="0"/>
         <v>7.6875000000000009</v>
       </c>
       <c r="D29" s="1">
@@ -2774,7 +2774,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,G30,H30,I30,I30,J30)</f>
+        <f t="shared" si="0"/>
         <v>7.65</v>
       </c>
       <c r="D30" s="1">
@@ -2813,7 +2813,7 @@
         <v>105</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,G31,H31,I31,I31,J31)</f>
+        <f t="shared" si="0"/>
         <v>7.6499999999999995</v>
       </c>
       <c r="D31" s="1">
@@ -2851,7 +2851,7 @@
         <v>142</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,G32,H32,I32,I32,J32)</f>
+        <f t="shared" si="0"/>
         <v>7.6499999999999995</v>
       </c>
       <c r="D32" s="1">
@@ -2887,7 +2887,7 @@
         <v>47</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,G33,H33,I33,I33,J33)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D33" s="1">
@@ -2923,7 +2923,7 @@
         <v>80</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,G34,H34,I34,I34,J34)</f>
+        <f t="shared" si="0"/>
         <v>7.3750000000000009</v>
       </c>
       <c r="D34" s="1">
@@ -2959,7 +2959,7 @@
         <v>115</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,G35,H35,I35,I35,J35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,G35,H35,I35,I35,J35)</f>
         <v>7.375</v>
       </c>
       <c r="D35" s="1">
@@ -2995,7 +2995,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,G36,H36,I36,I36,J36)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D36" s="1">
@@ -3030,7 +3030,7 @@
         <v>29</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,G37,H37,I37,I37,J37)</f>
+        <f t="shared" si="1"/>
         <v>7.3250000000000002</v>
       </c>
       <c r="D37" s="1">
@@ -3068,7 +3068,7 @@
         <v>141</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,G38,H38,I38,I38,J38)</f>
+        <f t="shared" si="1"/>
         <v>7.3125000000000009</v>
       </c>
       <c r="D38" s="1">
@@ -3104,7 +3104,7 @@
         <v>45</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,G39,H39,I39,I39,J39)</f>
+        <f t="shared" si="1"/>
         <v>7.3125</v>
       </c>
       <c r="D39" s="1">
@@ -3140,7 +3140,7 @@
         <v>49</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,G40,H40,I40,I40,J40)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D40" s="1">
@@ -3176,7 +3176,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,G41,H41,I41,I41,J41)</f>
+        <f t="shared" si="1"/>
         <v>7.2374999999999989</v>
       </c>
       <c r="D41" s="1">
@@ -3211,7 +3211,7 @@
         <v>22</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,G42,H42,I42,I42,J42)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D42" s="1">
@@ -3246,7 +3246,7 @@
         <v>27</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,G43,H43,I43,I43,J43)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -3283,7 +3283,7 @@
         <v>44</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,G44,H44,I44,I44,J44)</f>
+        <f t="shared" si="1"/>
         <v>7.1250000000000009</v>
       </c>
       <c r="D44" s="1">
@@ -3318,7 +3318,7 @@
         <v>76</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,G45,H45,I45,I45,J45)</f>
+        <f t="shared" si="1"/>
         <v>7.0250000000000004</v>
       </c>
       <c r="D45" s="1">
@@ -3354,7 +3354,7 @@
         <v>71</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,G46,H46,I46,I46,J46)</f>
+        <f t="shared" si="1"/>
         <v>6.8500000000000005</v>
       </c>
       <c r="D46" s="1">
@@ -3392,7 +3392,7 @@
         <v>18</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,G47,H47,I47,I47,J47)</f>
+        <f t="shared" si="1"/>
         <v>6.8250000000000002</v>
       </c>
       <c r="D47" s="1">
@@ -3427,7 +3427,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,G48,H48,I48,I48,J48)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D48" s="1">
@@ -3462,7 +3462,7 @@
         <v>9</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,G49,H49,I49,I49,J49)</f>
+        <f t="shared" si="1"/>
         <v>6.6749999999999998</v>
       </c>
       <c r="D49" s="1">
@@ -3498,7 +3498,7 @@
         <v>106</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,G50,H50,I50,I50,J50)</f>
+        <f t="shared" si="1"/>
         <v>6.6125000000000007</v>
       </c>
       <c r="D50" s="1">
@@ -3536,7 +3536,7 @@
         <v>13</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,G51,H51,I51,I51,J51)</f>
+        <f t="shared" si="1"/>
         <v>6.5249999999999995</v>
       </c>
       <c r="D51" s="1">
@@ -3572,7 +3572,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,G52,H52,I52,I52,J52)</f>
+        <f t="shared" si="1"/>
         <v>6.4750000000000005</v>
       </c>
       <c r="D52" s="1">
@@ -3607,7 +3607,7 @@
         <v>32</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,G53,H53,I53,I53,J53)</f>
+        <f t="shared" si="1"/>
         <v>6.3500000000000005</v>
       </c>
       <c r="D53" s="1">
@@ -3645,7 +3645,7 @@
         <v>30</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,G54,H54,I54,I54,J54)</f>
+        <f t="shared" si="1"/>
         <v>6.2750000000000004</v>
       </c>
       <c r="D54" s="1">
@@ -3681,7 +3681,7 @@
         <v>42</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,G55,H55,I55,I55,J55)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D55" s="1">
@@ -3717,7 +3717,7 @@
         <v>89</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,G56,H56,I56,I56,J56)</f>
+        <f t="shared" si="1"/>
         <v>6.1</v>
       </c>
       <c r="D56" s="1">
@@ -3753,7 +3753,7 @@
         <v>11</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,G57,H57,I57,I57,J57)</f>
+        <f t="shared" si="1"/>
         <v>5.9124999999999996</v>
       </c>
       <c r="D57" s="1">
@@ -3789,7 +3789,7 @@
         <v>99</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,G58,H58,I58,I58,J58)</f>
+        <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
       <c r="D58" s="1">
@@ -3825,7 +3825,7 @@
         <v>91</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,G59,H59,I59,I59,J59)</f>
+        <f t="shared" si="1"/>
         <v>5.3375000000000004</v>
       </c>
       <c r="D59" s="1">
@@ -3860,7 +3860,7 @@
         <v>36</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,G60,H60,I60,I60,J60)</f>
+        <f t="shared" si="1"/>
         <v>4.7124999999999995</v>
       </c>
       <c r="D60" s="1">
@@ -3912,10 +3912,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K72"/>
+  <dimension ref="B2:K73"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K3"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H73" sqref="H73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,7 +3964,7 @@
         <v>51</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.8285714285714274</v>
       </c>
       <c r="D3" s="1">
@@ -3992,7 +3992,7 @@
         <v>79</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8142857142857149</v>
       </c>
       <c r="D4" s="1">
@@ -4019,7 +4019,7 @@
         <v>66</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="D5" s="1">
@@ -4046,7 +4046,7 @@
         <v>128</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.6</v>
       </c>
       <c r="D6" s="1">
@@ -4073,7 +4073,7 @@
         <v>124</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.571428571428573</v>
       </c>
       <c r="D7" s="1">
@@ -4100,7 +4100,7 @@
         <v>121</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.4571428571428573</v>
       </c>
       <c r="D8" s="1">
@@ -4127,7 +4127,7 @@
         <v>127</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.4285714285714288</v>
       </c>
       <c r="D9" s="1">
@@ -4154,7 +4154,7 @@
         <v>24</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.4285714285714288</v>
       </c>
       <c r="D10" s="1">
@@ -4181,7 +4181,7 @@
         <v>56</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.3571428571428577</v>
       </c>
       <c r="D11" s="1">
@@ -4208,7 +4208,7 @@
         <v>107</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.3428571428571434</v>
       </c>
       <c r="D12" s="1">
@@ -4235,7 +4235,7 @@
         <v>96</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.3285714285714274</v>
       </c>
       <c r="D13" s="1">
@@ -4262,7 +4262,7 @@
         <v>25</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.2857142857142865</v>
       </c>
       <c r="D14" s="1">
@@ -4289,7 +4289,7 @@
         <v>81</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.1857142857142868</v>
       </c>
       <c r="D15" s="1">
@@ -4316,7 +4316,7 @@
         <v>77</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1714285714285726</v>
       </c>
       <c r="D16" s="1">
@@ -4343,7 +4343,7 @@
         <v>126</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.0857142857142854</v>
       </c>
       <c r="D17" s="1">
@@ -4370,7 +4370,7 @@
         <v>58</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.0714285714285712</v>
       </c>
       <c r="D18" s="1">
@@ -4397,7 +4397,7 @@
         <v>125</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.0571428571428569</v>
       </c>
       <c r="D19" s="1">
@@ -4424,7 +4424,7 @@
         <v>54</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,F20,G20,H20,H20,I20)</f>
         <v>7.9714285714285706</v>
       </c>
       <c r="D20" s="1">
@@ -4451,7 +4451,7 @@
         <v>23</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,F21,G21,H21,H21,I21)</f>
         <v>7.9142857142857137</v>
       </c>
       <c r="D21" s="1">
@@ -4478,7 +4478,7 @@
         <v>122</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D22" s="1">
@@ -4505,7 +4505,7 @@
         <v>108</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.8857142857142852</v>
       </c>
       <c r="D23" s="1">
@@ -4532,7 +4532,7 @@
         <v>109</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.757142857142858</v>
       </c>
       <c r="D24" s="1">
@@ -4559,7 +4559,7 @@
         <v>61</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.757142857142858</v>
       </c>
       <c r="D25" s="1">
@@ -4586,7 +4586,7 @@
         <v>78</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7142857142857144</v>
       </c>
       <c r="D26" s="1">
@@ -4613,7 +4613,7 @@
         <v>60</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D27" s="1">
@@ -4640,7 +4640,7 @@
         <v>123</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.6714285714285708</v>
       </c>
       <c r="D28" s="1">
@@ -4667,7 +4667,7 @@
         <v>67</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.6571428571428575</v>
       </c>
       <c r="D29" s="1">
@@ -4694,7 +4694,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.6571428571428566</v>
       </c>
       <c r="D30" s="1">
@@ -4721,7 +4721,7 @@
         <v>55</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6428571428571415</v>
       </c>
       <c r="D31" s="1">
@@ -4748,7 +4748,7 @@
         <v>133</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.5857142857142863</v>
       </c>
       <c r="D32" s="1">
@@ -4775,7 +4775,7 @@
         <v>131</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.5285714285714294</v>
       </c>
       <c r="D33" s="1">
@@ -4802,7 +4802,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5142857142857151</v>
       </c>
       <c r="D34" s="1">
@@ -4829,7 +4829,7 @@
         <v>38</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5142857142857151</v>
       </c>
       <c r="D35" s="1">
@@ -4856,7 +4856,7 @@
         <v>94</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5142857142857133</v>
       </c>
       <c r="D36" s="1">
@@ -4883,7 +4883,7 @@
         <v>97</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5</v>
       </c>
       <c r="D37" s="1">
@@ -4910,7 +4910,7 @@
         <v>62</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5</v>
       </c>
       <c r="D38" s="1">
@@ -4937,7 +4937,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.4714285714285706</v>
       </c>
       <c r="D39" s="1">
@@ -4964,7 +4964,7 @@
         <v>69</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.4571428571428573</v>
       </c>
       <c r="D40" s="1">
@@ -4991,7 +4991,7 @@
         <v>111</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.3428571428571425</v>
       </c>
       <c r="D41" s="1">
@@ -5018,7 +5018,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.3428571428571425</v>
       </c>
       <c r="D42" s="1">
@@ -5045,7 +5045,7 @@
         <v>52</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.257142857142858</v>
       </c>
       <c r="D43" s="1">
@@ -5072,7 +5072,7 @@
         <v>59</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.257142857142858</v>
       </c>
       <c r="D44" s="1">
@@ -5099,7 +5099,7 @@
         <v>65</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.2428571428571429</v>
       </c>
       <c r="D45" s="1">
@@ -5126,7 +5126,7 @@
         <v>103</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.1714285714285717</v>
       </c>
       <c r="D46" s="1">
@@ -5153,7 +5153,7 @@
         <v>53</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.1714285714285708</v>
       </c>
       <c r="D47" s="1">
@@ -5180,7 +5180,7 @@
         <v>40</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.1428571428571441</v>
       </c>
       <c r="D48" s="1">
@@ -5207,7 +5207,7 @@
         <v>98</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.0857142857142872</v>
       </c>
       <c r="D49" s="1">
@@ -5234,7 +5234,7 @@
         <v>110</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.0857142857142863</v>
       </c>
       <c r="D50" s="1">
@@ -5257,42 +5257,42 @@
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B51" s="2" t="s">
-        <v>104</v>
+      <c r="B51" s="9" t="s">
+        <v>144</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0142857142857151</v>
+        <f>AVERAGE(D51,E51,F51,G51,H51,H51,I51)</f>
+        <v>7.0857142857142863</v>
       </c>
       <c r="D51" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G51" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H51" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="I51" s="3">
-        <v>6.7</v>
+        <v>6.5</v>
+      </c>
+      <c r="I51" s="1">
+        <v>5.6</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>39</v>
+        <v>104</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>AVERAGE(D52,E52,F52,G52,H52,H52,I52)</f>
+        <v>7.0142857142857151</v>
       </c>
       <c r="D52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" s="1">
         <v>8</v>
@@ -5301,28 +5301,28 @@
         <v>7</v>
       </c>
       <c r="G52" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H52" s="3">
-        <v>6.5</v>
+        <v>7.2</v>
       </c>
       <c r="I52" s="3">
-        <v>6</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9714285714285706</v>
+        <f>AVERAGE(D53,E53,F53,G53,H53,H53,I53)</f>
+        <v>7</v>
       </c>
       <c r="D53" s="1">
         <v>8</v>
       </c>
       <c r="E53" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F53" s="1">
         <v>7</v>
@@ -5331,46 +5331,46 @@
         <v>7</v>
       </c>
       <c r="H53" s="3">
-        <v>7.3</v>
+        <v>6.5</v>
       </c>
       <c r="I53" s="3">
-        <v>6.2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9285714285714288</v>
+        <f>AVERAGE(D54,E54,F54,G54,H54,H54,I54)</f>
+        <v>6.9714285714285706</v>
       </c>
       <c r="D54" s="1">
         <v>8</v>
       </c>
       <c r="E54" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H54" s="3">
-        <v>6.1</v>
+        <v>7.3</v>
       </c>
       <c r="I54" s="3">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8428571428571416</v>
+        <f>AVERAGE(D55,E55,F55,G55,H55,H55,I55)</f>
+        <v>6.9285714285714288</v>
       </c>
       <c r="D55" s="1">
         <v>8</v>
@@ -5382,10 +5382,10 @@
         <v>8</v>
       </c>
       <c r="G55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H55" s="3">
-        <v>6.3</v>
+        <v>6.1</v>
       </c>
       <c r="I55" s="3">
         <v>5.3</v>
@@ -5393,14 +5393,14 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,F56,G56,H56,H56,I56)</f>
         <v>6.8428571428571416</v>
       </c>
       <c r="D56" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1">
         <v>7</v>
@@ -5409,7 +5409,7 @@
         <v>8</v>
       </c>
       <c r="G56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H56" s="3">
         <v>6.3</v>
@@ -5420,11 +5420,11 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8142857142857149</v>
+        <f>AVERAGE(D57,E57,F57,G57,H57,H57,I57)</f>
+        <v>6.8428571428571416</v>
       </c>
       <c r="D57" s="1">
         <v>7</v>
@@ -5433,31 +5433,31 @@
         <v>7</v>
       </c>
       <c r="F57" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H57" s="3">
-        <v>7.1</v>
+        <v>6.3</v>
       </c>
       <c r="I57" s="3">
-        <v>6.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7999999999999989</v>
+        <f>AVERAGE(D58,E58,F58,G58,H58,H58,I58)</f>
+        <v>6.8142857142857149</v>
       </c>
       <c r="D58" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F58" s="1">
         <v>6</v>
@@ -5466,100 +5466,100 @@
         <v>7</v>
       </c>
       <c r="H58" s="3">
-        <v>7.9</v>
+        <v>7.1</v>
       </c>
       <c r="I58" s="3">
-        <v>7.8</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7857142857142856</v>
+        <f>AVERAGE(D59,E59,F59,G59,H59,H59,I59)</f>
+        <v>6.7999999999999989</v>
       </c>
       <c r="D59" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F59" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>5.5</v>
+        <v>7.9</v>
       </c>
       <c r="I59" s="3">
-        <v>4.5</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
-        <v>6.5285714285714276</v>
+        <f>AVERAGE(D60,E60,F60,G60,H60,H60,I60)</f>
+        <v>6.7857142857142856</v>
       </c>
       <c r="D60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G60" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H60" s="3">
-        <v>6.3</v>
+        <v>5.5</v>
       </c>
       <c r="I60" s="3">
-        <v>6.1</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
-        <v>6.3571428571428568</v>
+        <f>AVERAGE(D61,E61,F61,G61,H61,H61,I61)</f>
+        <v>6.5285714285714276</v>
       </c>
       <c r="D61" s="1">
         <v>7</v>
       </c>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G61" s="1">
         <v>6</v>
       </c>
       <c r="H61" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I61" s="3">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
-        <v>6.2428571428571429</v>
+        <f>AVERAGE(D62,E62,F62,G62,H62,H62,I62)</f>
+        <v>6.3571428571428568</v>
       </c>
       <c r="D62" s="1">
         <v>7</v>
@@ -5568,25 +5568,25 @@
         <v>6</v>
       </c>
       <c r="F62" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G62" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H62" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.9</v>
       </c>
       <c r="I62" s="3">
-        <v>4.5</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1714285714285717</v>
+        <f>AVERAGE(D63,E63,F63,G63,H63,H63,I63)</f>
+        <v>6.2428571428571429</v>
       </c>
       <c r="D63" s="1">
         <v>7</v>
@@ -5601,235 +5601,235 @@
         <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I63" s="3">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>64</v>
+        <v>101</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1714285714285708</v>
+        <f>AVERAGE(D64,E64,F64,G64,H64,H64,I64)</f>
+        <v>6.1714285714285717</v>
       </c>
       <c r="D64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H64" s="3">
-        <v>6.4</v>
+        <v>5</v>
       </c>
       <c r="I64" s="3">
-        <v>5.4</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1</v>
+        <f>AVERAGE(D65,E65,F65,G65,H65,H65,I65)</f>
+        <v>6.1714285714285708</v>
       </c>
       <c r="D65" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E65" s="1">
         <v>7</v>
       </c>
       <c r="F65" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H65" s="3">
-        <v>4.3</v>
+        <v>6.4</v>
       </c>
       <c r="I65" s="3">
-        <v>4.0999999999999996</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
-        <v>6.0571428571428569</v>
+        <f>AVERAGE(D66,E66,F66,G66,H66,H66,I66)</f>
+        <v>6.1</v>
       </c>
       <c r="D66" s="1">
         <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F66" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H66" s="3">
-        <v>7</v>
+        <v>4.3</v>
       </c>
       <c r="I66" s="3">
-        <v>6.4</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>113</v>
+        <v>26</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C72" si="2">AVERAGE(D67,E67,F67,G67,H67,H67,I67)</f>
-        <v>5.8428571428571425</v>
+        <f>AVERAGE(D67,E67,F67,G67,H67,H67,I67)</f>
+        <v>6.0571428571428569</v>
       </c>
       <c r="D67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
+        <v>3</v>
+      </c>
+      <c r="F67" s="1">
         <v>5</v>
       </c>
-      <c r="F67" s="1">
-        <v>4</v>
-      </c>
       <c r="G67" s="1">
         <v>6</v>
       </c>
       <c r="H67" s="3">
-        <v>6.8</v>
+        <v>7</v>
       </c>
       <c r="I67" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
-        <v>5.6428571428571432</v>
+        <f>AVERAGE(D68,E68,F68,G68,H68,H68,I68)</f>
+        <v>5.8428571428571425</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F68" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
       <c r="H68" s="3">
-        <v>4.5</v>
+        <v>6.8</v>
       </c>
       <c r="I68" s="3">
-        <v>3.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
-        <v>5.3428571428571425</v>
+        <f>AVERAGE(D69,E69,F69,G69,H69,H69,I69)</f>
+        <v>5.6428571428571432</v>
       </c>
       <c r="D69" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F69" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H69" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I69" s="3">
-        <v>5.8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>114</v>
+        <v>21</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
-        <v>5.0428571428571427</v>
+        <f>AVERAGE(D70,E70,F70,G70,H70,H70,I70)</f>
+        <v>5.3428571428571425</v>
       </c>
       <c r="D70" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F70" s="1">
         <v>2</v>
       </c>
       <c r="G70" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H70" s="3">
-        <v>8.1999999999999993</v>
+        <v>6.8</v>
       </c>
       <c r="I70" s="3">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
-        <v>4.6714285714285708</v>
+        <f>AVERAGE(D71,E71,F71,G71,H71,H71,I71)</f>
+        <v>5.0428571428571427</v>
       </c>
       <c r="D71" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E71" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F71" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G71" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H71" s="3">
-        <v>4.9000000000000004</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I71" s="3">
-        <v>3.9</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
-        <v>4.1285714285714281</v>
+        <f>AVERAGE(D72,E72,F72,G72,H72,H72,I72)</f>
+        <v>4.6714285714285708</v>
       </c>
       <c r="D72" s="1">
         <v>5</v>
@@ -5838,15 +5838,42 @@
         <v>4</v>
       </c>
       <c r="F72" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G72" s="1">
         <v>5</v>
       </c>
       <c r="H72" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I72" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" s="5">
+        <f>AVERAGE(D73,E73,F73,G73,H73,H73,I73)</f>
+        <v>4.1285714285714281</v>
+      </c>
+      <c r="D73" s="1">
+        <v>5</v>
+      </c>
+      <c r="E73" s="1">
+        <v>4</v>
+      </c>
+      <c r="F73" s="1">
+        <v>2</v>
+      </c>
+      <c r="G73" s="1">
+        <v>5</v>
+      </c>
+      <c r="H73" s="3">
         <v>4.5</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I73" s="3">
         <v>3.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 58 Estado eléctrico
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D427E3E7-EB32-4E3A-8969-D694D66DBED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5C64F5-5586-49CA-858C-7726D379424C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="147">
   <si>
     <t>Película</t>
   </si>
@@ -942,6 +942,9 @@
   </si>
   <si>
     <t>Paradise</t>
+  </si>
+  <si>
+    <t>Estado eléctrico</t>
   </si>
 </sst>
 </file>
@@ -1297,10 +1300,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I74" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I74" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I74">
-    <sortCondition descending="1" ref="C2:C74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I75" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I75" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I75">
+    <sortCondition descending="1" ref="C2:C75"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3915,10 +3918,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K74"/>
+  <dimension ref="B2:K75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5584,7 +5587,7 @@
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="2" t="s">
         <v>145</v>
       </c>
       <c r="C63" s="5">
@@ -5827,66 +5830,66 @@
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>114</v>
+      <c r="B72" s="9" t="s">
+        <v>146</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,F72,G72,H72,H72,I72)</f>
-        <v>5.0428571428571427</v>
+        <v>5.2714285714285714</v>
       </c>
       <c r="D72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F72" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G72" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H72" s="3">
-        <v>8.1999999999999993</v>
-      </c>
-      <c r="I72" s="3">
-        <v>7.9</v>
+        <v>5.9</v>
+      </c>
+      <c r="I72" s="1">
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,F73,G73,H73,H73,I73)</f>
-        <v>4.6714285714285708</v>
+        <v>5.0428571428571427</v>
       </c>
       <c r="D73" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F73" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G73" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H73" s="3">
-        <v>4.9000000000000004</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I73" s="3">
-        <v>3.9</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>68</v>
+        <v>136</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,F74,G74,H74,H74,I74)</f>
-        <v>4.1285714285714281</v>
+        <v>4.6714285714285708</v>
       </c>
       <c r="D74" s="1">
         <v>5</v>
@@ -5895,15 +5898,42 @@
         <v>4</v>
       </c>
       <c r="F74" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G74" s="1">
         <v>5</v>
       </c>
       <c r="H74" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I74" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="5">
+        <f>AVERAGE(D75,E75,F75,G75,H75,H75,I75)</f>
+        <v>4.1285714285714281</v>
+      </c>
+      <c r="D75" s="1">
+        <v>5</v>
+      </c>
+      <c r="E75" s="1">
+        <v>4</v>
+      </c>
+      <c r="F75" s="1">
+        <v>2</v>
+      </c>
+      <c r="G75" s="1">
+        <v>5</v>
+      </c>
+      <c r="H75" s="3">
         <v>4.5</v>
       </c>
-      <c r="I74" s="3">
+      <c r="I75" s="3">
         <v>3.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 65 Los hombres lobo
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197271F9-21AC-442E-A812-77B95F0870A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B63F4-EBA1-4071-91BD-11F11F278DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
   <si>
     <t>Película</t>
   </si>
@@ -1005,6 +1005,9 @@
   </si>
   <si>
     <t>El sindicato</t>
+  </si>
+  <si>
+    <t>Los hombres lobo</t>
   </si>
 </sst>
 </file>
@@ -1014,7 +1017,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1050,12 +1053,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1363,10 +1360,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I86" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I86" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I86">
-    <sortCondition descending="1" ref="C2:C86"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I87" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I87" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I87">
+    <sortCondition descending="1" ref="C2:C87"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1796,8 +1793,8 @@
   </sheetPr>
   <dimension ref="B2:O62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1861,7 +1858,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -1895,7 +1892,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -1928,7 +1925,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -1964,7 +1961,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2000,7 +1997,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2034,7 +2031,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2067,7 +2064,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D9" s="1">
@@ -2100,7 +2097,7 @@
         <v>93</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D10" s="1">
@@ -2133,7 +2130,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D11" s="1">
@@ -2168,7 +2165,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D12" s="1">
@@ -2203,7 +2200,7 @@
         <v>7</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D13" s="1">
@@ -2236,7 +2233,7 @@
         <v>137</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D14" s="1">
@@ -2269,7 +2266,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D15" s="1">
@@ -2304,7 +2301,7 @@
         <v>139</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D16" s="1">
@@ -2337,7 +2334,7 @@
         <v>46</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D17" s="1">
@@ -2370,7 +2367,7 @@
         <v>136</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D18" s="1">
@@ -2403,7 +2400,7 @@
         <v>70</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -2434,7 +2431,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D20" s="1">
@@ -2467,7 +2464,7 @@
         <v>33</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2500,7 +2497,7 @@
         <v>120</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2533,7 +2530,7 @@
         <v>5</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D23" s="1">
@@ -2566,7 +2563,7 @@
         <v>43</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D24" s="1">
@@ -2599,7 +2596,7 @@
         <v>138</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D25" s="1">
@@ -2632,7 +2629,7 @@
         <v>82</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D26" s="1">
@@ -2665,7 +2662,7 @@
         <v>73</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -2700,7 +2697,7 @@
         <v>34</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7125000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -2733,7 +2730,7 @@
         <v>142</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D29" s="1">
@@ -2766,7 +2763,7 @@
         <v>47</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D30" s="1">
@@ -2799,7 +2796,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D31" s="1">
@@ -2835,7 +2832,7 @@
         <v>105</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D32" s="1">
@@ -2870,7 +2867,7 @@
         <v>141</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -2903,7 +2900,7 @@
         <v>16</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.4874999999999989</v>
       </c>
       <c r="D34" s="1">
@@ -2935,7 +2932,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.35</v>
       </c>
       <c r="D35" s="1">
@@ -2967,7 +2964,7 @@
         <v>80</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D36" s="1">
@@ -3000,7 +2997,7 @@
         <v>115</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D37" s="1">
@@ -3033,7 +3030,7 @@
         <v>29</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D38" s="1">
@@ -3068,7 +3065,7 @@
         <v>22</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D39" s="1">
@@ -3100,7 +3097,7 @@
         <v>140</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D40" s="1">
@@ -3133,7 +3130,7 @@
         <v>45</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D41" s="1">
@@ -3166,7 +3163,7 @@
         <v>27</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -3200,7 +3197,7 @@
         <v>49</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -3233,7 +3230,7 @@
         <v>71</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D44" s="1">
@@ -3268,7 +3265,7 @@
         <v>76</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D45" s="1">
@@ -3301,7 +3298,7 @@
         <v>44</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D46" s="1">
@@ -3333,7 +3330,7 @@
         <v>48</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D47" s="1">
@@ -3365,7 +3362,7 @@
         <v>148</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -3398,7 +3395,7 @@
         <v>153</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D49" s="1">
@@ -3431,7 +3428,7 @@
         <v>17</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D50" s="1">
@@ -3463,7 +3460,7 @@
         <v>18</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D51" s="1">
@@ -3495,7 +3492,7 @@
         <v>9</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D52" s="1">
@@ -3528,7 +3525,7 @@
         <v>106</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D53" s="1">
@@ -3563,7 +3560,7 @@
         <v>30</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D54" s="1">
@@ -3596,7 +3593,7 @@
         <v>13</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -3629,7 +3626,7 @@
         <v>32</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D56" s="1">
@@ -3664,7 +3661,7 @@
         <v>42</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D57" s="1">
@@ -3697,7 +3694,7 @@
         <v>11</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D58" s="1">
@@ -3730,7 +3727,7 @@
         <v>89</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D59" s="1">
@@ -3763,7 +3760,7 @@
         <v>99</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D60" s="1">
@@ -3796,7 +3793,7 @@
         <v>91</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>5.4625000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -3828,7 +3825,7 @@
         <v>36</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D62" s="1">
@@ -3877,10 +3874,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K86"/>
+  <dimension ref="B2:K87"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3926,11 +3923,11 @@
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>107</v>
       </c>
       <c r="C3" s="5">
         <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
-        <v>8.8625000000000007</v>
+        <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
         <v>9</v>
@@ -3945,129 +3942,129 @@
         <v>10</v>
       </c>
       <c r="H3" s="3">
-        <v>8</v>
+        <v>8.1</v>
       </c>
       <c r="I3" s="3">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="K3" s="8"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="C4" s="5">
         <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
-        <v>8.85</v>
+        <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="1">
-        <v>9</v>
-      </c>
       <c r="F4" s="1">
         <v>9</v>
       </c>
       <c r="G4" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H4" s="3">
-        <v>8.4</v>
+        <v>8</v>
       </c>
       <c r="I4" s="3">
-        <v>8</v>
+        <v>6.9</v>
       </c>
       <c r="K4" s="8"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5">
         <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
-        <v>8.8375000000000004</v>
+        <v>8.85</v>
       </c>
       <c r="D5" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>9</v>
       </c>
       <c r="F5" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="1">
         <v>9</v>
       </c>
       <c r="H5" s="3">
-        <v>8.5</v>
+        <v>8.4</v>
       </c>
       <c r="I5" s="3">
-        <v>7.7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>128</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5">
         <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
-        <v>8.65</v>
+        <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1">
+        <v>9</v>
+      </c>
+      <c r="F6" s="1">
         <v>10</v>
       </c>
-      <c r="E6" s="1">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1">
-        <v>9</v>
-      </c>
       <c r="G6" s="1">
         <v>9</v>
       </c>
       <c r="H6" s="3">
-        <v>8.1</v>
+        <v>8.5</v>
       </c>
       <c r="I6" s="3">
-        <v>7</v>
+        <v>7.7</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C7" s="5">
         <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
-        <v>8.625</v>
+        <v>8.65</v>
       </c>
       <c r="D7" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1">
         <v>9</v>
       </c>
       <c r="F7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G7" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="3">
-        <v>7.7</v>
+        <v>8.1</v>
       </c>
       <c r="I7" s="3">
-        <v>6.6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="C8" s="5">
         <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
-        <v>8.5250000000000004</v>
+        <v>8.625</v>
       </c>
       <c r="D8" s="1">
         <v>9</v>
@@ -4076,7 +4073,7 @@
         <v>9</v>
       </c>
       <c r="F8" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G8" s="1">
         <v>10</v>
@@ -4085,16 +4082,16 @@
         <v>7.7</v>
       </c>
       <c r="I8" s="3">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C9" s="5">
         <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
-        <v>8.5</v>
+        <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
         <v>9</v>
@@ -4103,21 +4100,21 @@
         <v>9</v>
       </c>
       <c r="F9" s="1">
+        <v>9</v>
+      </c>
+      <c r="G9" s="1">
         <v>10</v>
-      </c>
-      <c r="G9" s="1">
-        <v>9</v>
       </c>
       <c r="H9" s="3">
         <v>7.7</v>
       </c>
       <c r="I9" s="3">
-        <v>6.6</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>127</v>
       </c>
       <c r="C10" s="5">
         <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
@@ -4130,21 +4127,21 @@
         <v>9</v>
       </c>
       <c r="F10" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G10" s="1">
         <v>9</v>
       </c>
       <c r="H10" s="3">
-        <v>8.1</v>
+        <v>7.7</v>
       </c>
       <c r="I10" s="3">
-        <v>7.8</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="5">
         <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
@@ -4154,7 +4151,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1">
         <v>8</v>
@@ -4163,49 +4160,49 @@
         <v>9</v>
       </c>
       <c r="H11" s="3">
-        <v>7.6</v>
+        <v>8.1</v>
       </c>
       <c r="I11" s="3">
-        <v>6.8</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="C12" s="5">
         <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
-        <v>8.4375</v>
+        <v>8.5</v>
       </c>
       <c r="D12" s="1">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="1">
-        <v>9</v>
-      </c>
       <c r="F12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="1">
         <v>9</v>
       </c>
       <c r="H12" s="3">
-        <v>7.5</v>
+        <v>7.6</v>
       </c>
       <c r="I12" s="3">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="C13" s="5">
         <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
-        <v>8.4124999999999996</v>
+        <v>8.4375</v>
       </c>
       <c r="D13" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1">
         <v>9</v>
@@ -4217,37 +4214,37 @@
         <v>9</v>
       </c>
       <c r="H13" s="3">
-        <v>7.8</v>
+        <v>7.5</v>
       </c>
       <c r="I13" s="3">
-        <v>6.7</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C14" s="5">
         <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
-        <v>8.3000000000000007</v>
+        <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14" s="1">
         <v>9</v>
       </c>
       <c r="G14" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="3">
-        <v>8.1</v>
+        <v>7.8</v>
       </c>
       <c r="I14" s="3">
-        <v>7.2</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
@@ -5412,7 +5409,7 @@
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C58" s="5">
@@ -5763,7 +5760,7 @@
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C71" s="5">
@@ -5790,7 +5787,7 @@
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="2" t="s">
         <v>160</v>
       </c>
       <c r="C72" s="5">
@@ -5817,7 +5814,7 @@
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="2" t="s">
         <v>159</v>
       </c>
       <c r="C73" s="5">
@@ -5952,7 +5949,7 @@
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="2" t="s">
         <v>156</v>
       </c>
       <c r="C78" s="5">
@@ -6033,7 +6030,7 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="2" t="s">
         <v>154</v>
       </c>
       <c r="C81" s="5">
@@ -6087,110 +6084,137 @@
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="2" t="s">
-        <v>114</v>
+      <c r="B83" s="9" t="s">
+        <v>161</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D83" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E83" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F83" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I83" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D84" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E84" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F84" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G84" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H84" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I84" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D85" s="1">
         <v>5</v>
       </c>
       <c r="E85" s="1">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1">
+        <v>3</v>
+      </c>
+      <c r="G85" s="1">
         <v>4</v>
       </c>
-      <c r="F85" s="1">
-        <v>2</v>
-      </c>
-      <c r="G85" s="1">
-        <v>5</v>
-      </c>
       <c r="H85" s="3">
-        <v>4.5</v>
+        <v>5.9</v>
       </c>
       <c r="I85" s="3">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="9" t="s">
-        <v>155</v>
+      <c r="B86" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D86" s="1">
+        <v>5</v>
+      </c>
+      <c r="E86" s="1">
+        <v>4</v>
+      </c>
+      <c r="F86" s="1">
+        <v>2</v>
+      </c>
+      <c r="G86" s="1">
+        <v>5</v>
+      </c>
+      <c r="H86" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I86" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B87" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C87" s="5">
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D87" s="1">
         <v>1</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E87" s="1">
         <v>1</v>
       </c>
-      <c r="F86" s="1">
+      <c r="F87" s="1">
         <v>0</v>
       </c>
-      <c r="G86" s="1">
+      <c r="G87" s="1">
         <v>1</v>
       </c>
-      <c r="H86" s="3">
+      <c r="H87" s="3">
         <v>6.7</v>
       </c>
-      <c r="I86" s="3">
+      <c r="I87" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 66 El muro negro
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E2B63F4-EBA1-4071-91BD-11F11F278DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BAE31-2A72-417B-8D0C-635C6DEA9541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="164">
   <si>
     <t>Película</t>
   </si>
@@ -1008,6 +1008,12 @@
   </si>
   <si>
     <t>Los hombres lobo</t>
+  </si>
+  <si>
+    <t>Almost cops</t>
+  </si>
+  <si>
+    <t>El muro negro</t>
   </si>
 </sst>
 </file>
@@ -1360,10 +1366,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I87" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I87" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I87">
-    <sortCondition descending="1" ref="C2:C87"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I89" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I89">
+    <sortCondition descending="1" ref="C2:C89"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -2932,7 +2938,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C62" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.35</v>
       </c>
       <c r="D35" s="1">
@@ -3874,10 +3880,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K87"/>
+  <dimension ref="B2:K89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6030,12 +6036,12 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>154</v>
+      <c r="B81" s="9" t="s">
+        <v>163</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D81" s="1">
         <v>5</v>
@@ -6044,177 +6050,231 @@
         <v>5</v>
       </c>
       <c r="F81" s="1">
+        <v>3</v>
+      </c>
+      <c r="G81" s="1">
         <v>5</v>
       </c>
-      <c r="G81" s="1">
-        <v>3</v>
-      </c>
       <c r="H81" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="I81" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="2" t="s">
-        <v>135</v>
+      <c r="B82" s="9" t="s">
+        <v>162</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>4.5874999999999995</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D82" s="1">
         <v>5</v>
       </c>
       <c r="E82" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G82" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H82" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I82" s="3">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B83" s="9" t="s">
-        <v>161</v>
+      <c r="B83" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D83" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E83" s="1">
+        <v>5</v>
+      </c>
+      <c r="F83" s="1">
+        <v>5</v>
+      </c>
+      <c r="G83" s="1">
+        <v>3</v>
+      </c>
+      <c r="H83" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I83" s="3">
         <v>4</v>
-      </c>
-      <c r="F83" s="1">
-        <v>6</v>
-      </c>
-      <c r="G83" s="1">
-        <v>5</v>
-      </c>
-      <c r="H83" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="I83" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>4.4124999999999996</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D84" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E84" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F84" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G84" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>8.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I84" s="3">
-        <v>7.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D85" s="1">
+        <v>1</v>
+      </c>
+      <c r="E85" s="1">
+        <v>4</v>
+      </c>
+      <c r="F85" s="1">
+        <v>6</v>
+      </c>
+      <c r="G85" s="1">
         <v>5</v>
       </c>
-      <c r="E85" s="1">
-        <v>3</v>
-      </c>
-      <c r="F85" s="1">
-        <v>3</v>
-      </c>
-      <c r="G85" s="1">
-        <v>4</v>
-      </c>
       <c r="H85" s="3">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="I85" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>68</v>
+        <v>114</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.1124999999999998</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D86" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F86" s="1">
         <v>2</v>
       </c>
       <c r="G86" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H86" s="3">
-        <v>4.5</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I86" s="3">
-        <v>3.9</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <v>4.3374999999999995</v>
+      </c>
+      <c r="D87" s="1">
+        <v>5</v>
+      </c>
+      <c r="E87" s="1">
+        <v>3</v>
+      </c>
+      <c r="F87" s="1">
+        <v>3</v>
+      </c>
+      <c r="G87" s="1">
+        <v>4</v>
+      </c>
+      <c r="H87" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I87" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C88" s="5">
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D88" s="1">
+        <v>5</v>
+      </c>
+      <c r="E88" s="1">
+        <v>4</v>
+      </c>
+      <c r="F88" s="1">
+        <v>2</v>
+      </c>
+      <c r="G88" s="1">
+        <v>5</v>
+      </c>
+      <c r="H88" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I88" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B89" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C89" s="5">
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D89" s="1">
         <v>1</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E89" s="1">
         <v>1</v>
       </c>
-      <c r="F87" s="1">
+      <c r="F89" s="1">
         <v>0</v>
       </c>
-      <c r="G87" s="1">
+      <c r="G89" s="1">
         <v>1</v>
       </c>
-      <c r="H87" s="3">
+      <c r="H89" s="3">
         <v>6.7</v>
       </c>
-      <c r="I87" s="3">
+      <c r="I89" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 67 Ejército de ladrones
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA5BAE31-2A72-417B-8D0C-635C6DEA9541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CF1453-684E-4047-A5D2-94B4B2E1945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,10 +57,10 @@
     <author>tc={8A943824-8E5D-48CD-A77C-A2B35F5980A3}</author>
     <author>tc={905D74EB-1C41-4120-8733-E9C8C2FF351A}</author>
     <author>tc={B4E0A9EE-3277-494F-88A8-61F8EE265DDE}</author>
+    <author>tc={97D38487-0228-4117-9D87-BCCFD4EC6983}</author>
     <author>tc={BE581C86-E71E-4F40-9F43-00EDE88FB108}</author>
     <author>tc={9C26C127-20FF-4258-B62D-B6B902EB0E98}</author>
     <author>tc={B1E35BAB-7C71-4B4F-9EE2-76495541B293}</author>
-    <author>tc={97D38487-0228-4117-9D87-BCCFD4EC6983}</author>
     <author>tc={C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}</author>
     <author>tc={E34E6F01-0047-4D5E-A9F0-76B7D80CE842}</author>
     <author>tc={162EA199-65BB-48FF-A9B1-580BDA0F2A25}</author>
@@ -231,7 +231,15 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B23" authorId="18" shapeId="0" xr:uid="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
+    <comment ref="B23" authorId="18" shapeId="0" xr:uid="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    3 temporadas</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="19" shapeId="0" xr:uid="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -239,7 +247,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B24" authorId="19" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+    <comment ref="B25" authorId="20" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -247,20 +255,12 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B27" authorId="20" shapeId="0" xr:uid="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
+    <comment ref="B28" authorId="21" shapeId="0" xr:uid="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     3 temporadas</t>
-      </text>
-    </comment>
-    <comment ref="B28" authorId="21" shapeId="0" xr:uid="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
-      <text>
-        <t>[Comentario encadenado]
-Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
-Comentario:
-    2 temporadas</t>
       </text>
     </comment>
     <comment ref="B29" authorId="22" shapeId="0" xr:uid="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>Película</t>
   </si>
@@ -1014,6 +1014,9 @@
   </si>
   <si>
     <t>El muro negro</t>
+  </si>
+  <si>
+    <t>Ejército de ladrones</t>
   </si>
 </sst>
 </file>
@@ -1366,10 +1369,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I89" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I89" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I89">
-    <sortCondition descending="1" ref="C2:C89"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I90" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I90" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I90">
+    <sortCondition descending="1" ref="C2:C90"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1704,17 +1707,17 @@
   <threadedComment ref="B22" dT="2025-02-03T22:22:50.97" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B4E0A9EE-3277-494F-88A8-61F8EE265DDE}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B23" dT="2024-07-08T19:02:11.85" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
+  <threadedComment ref="B23" dT="2024-07-08T19:03:23.53" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
+    <text>3 temporadas</text>
+  </threadedComment>
+  <threadedComment ref="B24" dT="2024-07-08T19:02:11.85" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B24" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+  <threadedComment ref="B25" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B27" dT="2024-07-08T19:01:48.87" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
+  <threadedComment ref="B28" dT="2024-07-08T19:01:48.87" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
     <text>3 temporadas</text>
-  </threadedComment>
-  <threadedComment ref="B28" dT="2024-07-08T19:03:23.53" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
-    <text>2 temporadas</text>
   </threadedComment>
   <threadedComment ref="B29" dT="2025-04-19T09:54:12.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
     <text>1 temporada</text>
@@ -1799,8 +1802,8 @@
   </sheetPr>
   <dimension ref="B2:O62"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2533,29 +2536,29 @@
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C23" s="5">
         <f t="shared" si="0"/>
-        <v>7.8750000000000009</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1">
         <v>8</v>
       </c>
       <c r="F23" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H23" s="3">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="I23" s="3">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="J23" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2566,14 +2569,14 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C24" s="5">
         <f t="shared" si="0"/>
-        <v>7.8125000000000009</v>
+        <v>7.8750000000000009</v>
       </c>
       <c r="D24" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E24" s="1">
         <v>8</v>
@@ -2585,58 +2588,58 @@
         <v>8</v>
       </c>
       <c r="H24" s="3">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="I24" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="J24" s="1"/>
-      <c r="K24" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.6</v>
+      </c>
+      <c r="J24" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="C25" s="5">
         <f t="shared" si="0"/>
-        <v>7.8125</v>
+        <v>7.8125000000000009</v>
       </c>
       <c r="D25" s="1">
         <v>8</v>
       </c>
       <c r="E25" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1">
         <v>8</v>
       </c>
       <c r="H25" s="3">
-        <v>7.5</v>
+        <v>7.2</v>
       </c>
       <c r="I25" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="J25" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K25" s="1"/>
+        <v>6.1</v>
+      </c>
+      <c r="J25" s="1"/>
+      <c r="K25" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="C26" s="5">
         <f t="shared" si="0"/>
-        <v>7.7874999999999996</v>
+        <v>7.8125</v>
       </c>
       <c r="D26" s="1">
         <v>8</v>
@@ -2648,13 +2651,13 @@
         <v>8</v>
       </c>
       <c r="G26" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H26" s="3">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="I26" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="J26" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2665,11 +2668,11 @@
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C27" s="5">
         <f t="shared" si="0"/>
-        <v>7.7250000000000005</v>
+        <v>7.7874999999999996</v>
       </c>
       <c r="D27" s="1">
         <v>8</v>
@@ -2681,53 +2684,53 @@
         <v>8</v>
       </c>
       <c r="G27" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" s="3">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="I27" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J27" s="1" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K27" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.3</v>
+      </c>
+      <c r="J27" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="C28" s="5">
         <f t="shared" si="0"/>
-        <v>7.7125000000000004</v>
+        <v>7.7250000000000005</v>
       </c>
       <c r="D28" s="1">
         <v>8</v>
       </c>
       <c r="E28" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F28" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G28" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="3">
-        <v>8</v>
+        <v>7.2</v>
       </c>
       <c r="I28" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="J28" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K28" s="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="J28" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
@@ -2938,7 +2941,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C62" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.35</v>
       </c>
       <c r="D35" s="1">
@@ -3880,10 +3883,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K89"/>
+  <dimension ref="B2:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5281,41 +5284,41 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D53" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H53" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I53" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D54" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1">
         <v>7</v>
@@ -5324,25 +5327,25 @@
         <v>8</v>
       </c>
       <c r="G54" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H54" s="3">
-        <v>6.6</v>
+        <v>7.2</v>
       </c>
       <c r="I54" s="3">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D55" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1">
         <v>7</v>
@@ -5351,25 +5354,25 @@
         <v>8</v>
       </c>
       <c r="G55" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H55" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I55" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
-        <v>6.9375</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D56" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E56" s="1">
         <v>7</v>
@@ -5378,18 +5381,18 @@
         <v>8</v>
       </c>
       <c r="G56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H56" s="3">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="I56" s="3">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
@@ -5399,7 +5402,7 @@
         <v>8</v>
       </c>
       <c r="E57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" s="1">
         <v>8</v>
@@ -5408,46 +5411,46 @@
         <v>8</v>
       </c>
       <c r="H57" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I57" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9375</v>
       </c>
       <c r="D58" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E58" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F58" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G58" s="1">
         <v>8</v>
       </c>
       <c r="H58" s="3">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="I58" s="3">
-        <v>6.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="2" t="s">
-        <v>41</v>
+      <c r="B59" s="9" t="s">
+        <v>164</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>6.8624999999999989</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D59" s="1">
         <v>8</v>
@@ -5462,91 +5465,91 @@
         <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="I59" s="3">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D60" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E60" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F60" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G60" s="1">
         <v>8</v>
       </c>
       <c r="H60" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I60" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D61" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I61" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>6.8375000000000004</v>
+        <v>6.85</v>
       </c>
       <c r="D62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1">
         <v>7</v>
       </c>
       <c r="H62" s="3">
-        <v>7.1</v>
+        <v>7.3</v>
       </c>
       <c r="I62" s="3">
-        <v>6.5</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
@@ -5578,88 +5581,88 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E64" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H64" s="3">
         <v>6.3</v>
       </c>
       <c r="I64" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.3125</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D65" s="1">
         <v>7</v>
       </c>
       <c r="E65" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F65" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G65" s="1">
         <v>6</v>
       </c>
       <c r="H65" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I65" s="3">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E66" s="1">
         <v>6</v>
       </c>
       <c r="F66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H66" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I66" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
@@ -5669,142 +5672,142 @@
         <v>6</v>
       </c>
       <c r="E67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H67" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I67" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D68" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G68" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H68" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I68" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D69" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" s="1">
         <v>8</v>
       </c>
       <c r="G69" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H69" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I69" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D70" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F70" s="1">
         <v>8</v>
       </c>
       <c r="G70" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H70" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I70" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D71" s="1">
         <v>7</v>
       </c>
       <c r="E71" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H71" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I71" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D72" s="1">
         <v>7</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" s="1">
         <v>7</v>
@@ -5813,166 +5816,166 @@
         <v>7</v>
       </c>
       <c r="H72" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I72" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1">
         <v>6</v>
       </c>
       <c r="F73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G73" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I73" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D74" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G74" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H74" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I74" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E75" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F75" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G75" s="1">
         <v>6</v>
       </c>
       <c r="H75" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I75" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D76" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F76" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G76" s="1">
         <v>6</v>
       </c>
       <c r="H76" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I76" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D77" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1">
+        <v>3</v>
+      </c>
+      <c r="F77" s="1">
         <v>5</v>
       </c>
-      <c r="F77" s="1">
-        <v>6</v>
-      </c>
       <c r="G77" s="1">
         <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I77" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D78" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E78" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F78" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G78" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H78" s="3">
         <v>5.8</v>
@@ -5983,298 +5986,325 @@
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>5.1124999999999998</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D79" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G79" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H79" s="3">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="I79" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D80" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E80" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F80" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G80" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H80" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I80" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
-        <v>163</v>
+      <c r="B81" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D81" s="1">
         <v>5</v>
       </c>
       <c r="E81" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F81" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G81" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H81" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I81" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B82" s="9" t="s">
-        <v>162</v>
+      <c r="B82" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D82" s="1">
         <v>5</v>
       </c>
       <c r="E82" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G82" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H82" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I82" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I82" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D83" s="1">
         <v>5</v>
       </c>
       <c r="E83" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H83" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I83" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D84" s="1">
         <v>5</v>
       </c>
       <c r="E84" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F84" s="1">
         <v>5</v>
       </c>
       <c r="G84" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H84" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I84" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D85" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1">
         <v>4</v>
       </c>
       <c r="F85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G85" s="1">
         <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I85" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D86" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E86" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F86" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G86" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I86" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D87" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E87" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F87" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G87" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H87" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I87" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D88" s="1">
         <v>5</v>
       </c>
       <c r="E88" s="1">
+        <v>3</v>
+      </c>
+      <c r="F88" s="1">
+        <v>3</v>
+      </c>
+      <c r="G88" s="1">
         <v>4</v>
       </c>
-      <c r="F88" s="1">
-        <v>2</v>
-      </c>
-      <c r="G88" s="1">
-        <v>5</v>
-      </c>
       <c r="H88" s="3">
-        <v>4.5</v>
+        <v>5.9</v>
       </c>
       <c r="I88" s="3">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D89" s="1">
+        <v>5</v>
+      </c>
+      <c r="E89" s="1">
+        <v>4</v>
+      </c>
+      <c r="F89" s="1">
+        <v>2</v>
+      </c>
+      <c r="G89" s="1">
+        <v>5</v>
+      </c>
+      <c r="H89" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I89" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C90" s="5">
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D90" s="1">
         <v>1</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E90" s="1">
         <v>1</v>
       </c>
-      <c r="F89" s="1">
+      <c r="F90" s="1">
         <v>0</v>
       </c>
-      <c r="G89" s="1">
+      <c r="G90" s="1">
         <v>1</v>
       </c>
-      <c r="H89" s="3">
+      <c r="H90" s="3">
         <v>6.7</v>
       </c>
-      <c r="I89" s="3">
+      <c r="I90" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 68 Rebel Ridge
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5CF1453-684E-4047-A5D2-94B4B2E1945D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A39E202-99EC-4C0F-BE44-554BBF725EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
   <si>
     <t>Película</t>
   </si>
@@ -1017,6 +1017,9 @@
   </si>
   <si>
     <t>Ejército de ladrones</t>
+  </si>
+  <si>
+    <t>Rebel Ridge</t>
   </si>
 </sst>
 </file>
@@ -1369,10 +1372,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I90" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I90" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I90">
-    <sortCondition descending="1" ref="C2:C90"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I91" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I91" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I91">
+    <sortCondition descending="1" ref="C2:C91"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -2941,7 +2944,7 @@
         <v>50</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C62" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.35</v>
       </c>
       <c r="D35" s="1">
@@ -3883,10 +3886,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K90"/>
+  <dimension ref="B2:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5013,72 +5016,72 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>111</v>
+      <c r="B43" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="C43" s="5">
         <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
-        <v>7.3</v>
+        <v>7.3249999999999993</v>
       </c>
       <c r="D43" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G43" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H43" s="3">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="I43" s="3">
-        <v>5.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
-        <v>7.2750000000000004</v>
+        <v>7.3</v>
       </c>
       <c r="D44" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F44" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G44" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H44" s="3">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="I44" s="3">
-        <v>6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
-        <v>7.2374999999999998</v>
+        <v>7.2750000000000004</v>
       </c>
       <c r="D45" s="1">
         <v>7</v>
       </c>
       <c r="E45" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F45" s="1">
         <v>8</v>
@@ -5087,265 +5090,265 @@
         <v>8</v>
       </c>
       <c r="H45" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
       <c r="I45" s="3">
-        <v>4.9000000000000004</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
-        <v>7.2250000000000005</v>
+        <v>7.2374999999999998</v>
       </c>
       <c r="D46" s="1">
         <v>7</v>
       </c>
       <c r="E46" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F46" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H46" s="3">
-        <v>8.1</v>
+        <v>6</v>
       </c>
       <c r="I46" s="3">
-        <v>7.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
-        <v>7.2125000000000004</v>
+        <v>7.2250000000000005</v>
       </c>
       <c r="D47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E47" s="1">
         <v>7</v>
       </c>
       <c r="F47" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H47" s="3">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="I47" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
-        <v>7.2124999999999995</v>
+        <v>7.2125000000000004</v>
       </c>
       <c r="D48" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E48" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F48" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G48" s="1">
         <v>8</v>
       </c>
       <c r="H48" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I48" s="3">
         <v>6.3</v>
-      </c>
-      <c r="I48" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
-        <v>7.1499999999999995</v>
+        <v>7.2124999999999995</v>
       </c>
       <c r="D49" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E49" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F49" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G49" s="1">
         <v>8</v>
       </c>
       <c r="H49" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I49" s="3">
-        <v>6.6</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
-        <v>7.1375000000000011</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D50" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F50" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G50" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H50" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I50" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D51" s="1">
         <v>7</v>
       </c>
       <c r="E51" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H51" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I51" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I51" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
-        <v>7.125</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H52" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I52" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
-        <v>7.0875000000000004</v>
+        <v>7.125</v>
       </c>
       <c r="D53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53" s="1">
         <v>8</v>
       </c>
       <c r="F53" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G53" s="1">
         <v>7</v>
       </c>
       <c r="H53" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I53" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D54" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E54" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F54" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H54" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I54" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D55" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" s="1">
         <v>7</v>
@@ -5354,25 +5357,25 @@
         <v>8</v>
       </c>
       <c r="G55" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H55" s="3">
-        <v>6.6</v>
+        <v>7.2</v>
       </c>
       <c r="I55" s="3">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D56" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E56" s="1">
         <v>7</v>
@@ -5381,25 +5384,25 @@
         <v>8</v>
       </c>
       <c r="G56" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H56" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I56" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
-        <v>6.9375</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D57" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E57" s="1">
         <v>7</v>
@@ -5408,18 +5411,18 @@
         <v>8</v>
       </c>
       <c r="G57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H57" s="3">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="I57" s="3">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
@@ -5429,7 +5432,7 @@
         <v>8</v>
       </c>
       <c r="E58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" s="1">
         <v>8</v>
@@ -5438,258 +5441,258 @@
         <v>8</v>
       </c>
       <c r="H58" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I58" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
-        <v>164</v>
+      <c r="B59" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D59" s="1">
         <v>8</v>
       </c>
       <c r="E59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
       </c>
       <c r="G59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H59" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="I59" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D60" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F60" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G60" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H60" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I60" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D61" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E61" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F61" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G61" s="1">
         <v>8</v>
       </c>
       <c r="H61" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I61" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E62" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H62" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I62" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>6.6999999999999993</v>
+        <v>6.85</v>
       </c>
       <c r="D63" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E63" s="1">
         <v>6</v>
       </c>
       <c r="F63" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G63" s="1">
         <v>7</v>
       </c>
       <c r="H63" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I63" s="3">
-        <v>7.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D64" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E64" s="1">
         <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G64" s="1">
         <v>7</v>
       </c>
       <c r="H64" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I64" s="3">
-        <v>5.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G65" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H65" s="3">
         <v>6.3</v>
       </c>
       <c r="I65" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.3125</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D66" s="1">
         <v>7</v>
       </c>
       <c r="E66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G66" s="1">
         <v>6</v>
       </c>
       <c r="H66" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I66" s="3">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E67" s="1">
         <v>6</v>
       </c>
       <c r="F67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H67" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I67" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
@@ -5699,142 +5702,142 @@
         <v>6</v>
       </c>
       <c r="E68" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H68" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I68" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H69" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I69" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D70" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E70" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" s="1">
         <v>8</v>
       </c>
       <c r="G70" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H70" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I70" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F71" s="1">
         <v>8</v>
       </c>
       <c r="G71" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H71" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I71" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D72" s="1">
         <v>7</v>
       </c>
       <c r="E72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H72" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I72" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D73" s="1">
         <v>7</v>
       </c>
       <c r="E73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" s="1">
         <v>7</v>
@@ -5843,166 +5846,166 @@
         <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I73" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E74" s="1">
         <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G74" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H74" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I74" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D75" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G75" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H75" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I75" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G76" s="1">
         <v>6</v>
       </c>
       <c r="H76" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I76" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F77" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G77" s="1">
         <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I77" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D78" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
+        <v>3</v>
+      </c>
+      <c r="F78" s="1">
         <v>5</v>
       </c>
-      <c r="F78" s="1">
-        <v>6</v>
-      </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I78" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D79" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F79" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G79" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3">
         <v>5.8</v>
@@ -6013,298 +6016,325 @@
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>5.1124999999999998</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D80" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G80" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H80" s="3">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="I80" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D81" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F81" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I81" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D82" s="1">
         <v>5</v>
       </c>
       <c r="E82" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F82" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G82" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H82" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I82" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D83" s="1">
         <v>5</v>
       </c>
       <c r="E83" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G83" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I83" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I83" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D84" s="1">
         <v>5</v>
       </c>
       <c r="E84" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G84" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H84" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I84" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D85" s="1">
         <v>5</v>
       </c>
       <c r="E85" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F85" s="1">
         <v>5</v>
       </c>
       <c r="G85" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H85" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I85" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D86" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E86" s="1">
         <v>4</v>
       </c>
       <c r="F86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G86" s="1">
         <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I86" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E87" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F87" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I87" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D88" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F88" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G88" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H88" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I88" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D89" s="1">
         <v>5</v>
       </c>
       <c r="E89" s="1">
+        <v>3</v>
+      </c>
+      <c r="F89" s="1">
+        <v>3</v>
+      </c>
+      <c r="G89" s="1">
         <v>4</v>
       </c>
-      <c r="F89" s="1">
-        <v>2</v>
-      </c>
-      <c r="G89" s="1">
-        <v>5</v>
-      </c>
       <c r="H89" s="3">
-        <v>4.5</v>
+        <v>5.9</v>
       </c>
       <c r="I89" s="3">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D90" s="1">
+        <v>5</v>
+      </c>
+      <c r="E90" s="1">
+        <v>4</v>
+      </c>
+      <c r="F90" s="1">
+        <v>2</v>
+      </c>
+      <c r="G90" s="1">
+        <v>5</v>
+      </c>
+      <c r="H90" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I90" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B91" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C91" s="5">
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D91" s="1">
         <v>1</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E91" s="1">
         <v>1</v>
       </c>
-      <c r="F90" s="1">
+      <c r="F91" s="1">
         <v>0</v>
       </c>
-      <c r="G90" s="1">
+      <c r="G91" s="1">
         <v>1</v>
       </c>
-      <c r="H90" s="3">
+      <c r="H91" s="3">
         <v>6.7</v>
       </c>
-      <c r="I90" s="3">
+      <c r="I91" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 69 La huella del mal & Alimañas
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A39E202-99EC-4C0F-BE44-554BBF725EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3666A69A-6471-44E1-B567-E83BEF11E474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="168">
   <si>
     <t>Película</t>
   </si>
@@ -1020,6 +1020,12 @@
   </si>
   <si>
     <t>Rebel Ridge</t>
+  </si>
+  <si>
+    <t>La huella del mal</t>
+  </si>
+  <si>
+    <t>Alimañas</t>
   </si>
 </sst>
 </file>
@@ -1372,10 +1378,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I91" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I91" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I91">
-    <sortCondition descending="1" ref="C2:C91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I93" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I93" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I93">
+    <sortCondition descending="1" ref="C2:C93"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1805,8 +1811,8 @@
   </sheetPr>
   <dimension ref="B2:O62"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C62"/>
+    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,10 +3892,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K91"/>
+  <dimension ref="B2:K93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5016,7 +5022,7 @@
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="2" t="s">
         <v>165</v>
       </c>
       <c r="C43" s="5">
@@ -6042,299 +6048,353 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>145</v>
+      <c r="B81" s="9" t="s">
+        <v>166</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>5.1124999999999998</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D81" s="1">
         <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F81" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G81" s="1">
         <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I81" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D82" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F82" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G82" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H82" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I82" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D83" s="1">
         <v>5</v>
       </c>
       <c r="E83" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F83" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G83" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H83" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I83" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D84" s="1">
         <v>5</v>
       </c>
       <c r="E84" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F84" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G84" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H84" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I84" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I84" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D85" s="1">
         <v>5</v>
       </c>
       <c r="E85" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G85" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H85" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I85" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D86" s="1">
         <v>5</v>
       </c>
       <c r="E86" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F86" s="1">
         <v>5</v>
       </c>
       <c r="G86" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H86" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I86" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D87" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E87" s="1">
         <v>4</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G87" s="1">
         <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I87" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D88" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E88" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F88" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I88" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D89" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E89" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G89" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H89" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I89" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>68</v>
+        <v>150</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D90" s="1">
         <v>5</v>
       </c>
       <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
+        <v>3</v>
+      </c>
+      <c r="G90" s="1">
         <v>4</v>
       </c>
-      <c r="F90" s="1">
-        <v>2</v>
-      </c>
-      <c r="G90" s="1">
-        <v>5</v>
-      </c>
       <c r="H90" s="3">
-        <v>4.5</v>
+        <v>5.9</v>
       </c>
       <c r="I90" s="3">
-        <v>3.9</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>155</v>
+      <c r="B91" s="9" t="s">
+        <v>167</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <v>4.2749999999999995</v>
+      </c>
+      <c r="D91" s="1">
+        <v>4</v>
+      </c>
+      <c r="E91" s="1">
+        <v>2</v>
+      </c>
+      <c r="F91" s="1">
+        <v>6</v>
+      </c>
+      <c r="G91" s="1">
+        <v>6</v>
+      </c>
+      <c r="H91" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I91" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B92" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C92" s="5">
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D92" s="1">
+        <v>5</v>
+      </c>
+      <c r="E92" s="1">
+        <v>4</v>
+      </c>
+      <c r="F92" s="1">
+        <v>2</v>
+      </c>
+      <c r="G92" s="1">
+        <v>5</v>
+      </c>
+      <c r="H92" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I92" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B93" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C93" s="5">
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D93" s="1">
         <v>1</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E93" s="1">
         <v>1</v>
       </c>
-      <c r="F91" s="1">
+      <c r="F93" s="1">
         <v>0</v>
       </c>
-      <c r="G91" s="1">
+      <c r="G93" s="1">
         <v>1</v>
       </c>
-      <c r="H91" s="3">
+      <c r="H93" s="3">
         <v>6.7</v>
       </c>
-      <c r="I91" s="3">
+      <c r="I93" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 71 "Mi año en Oxford"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2995C5-9A10-47FF-BEB3-CB68D20CEFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE392C1-6130-4B30-A178-11247959BAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1845" yWindow="2970" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
   <si>
     <t>Película</t>
   </si>
@@ -1029,6 +1029,9 @@
   </si>
   <si>
     <t>Chappie</t>
+  </si>
+  <si>
+    <t>Mi año en Oxford</t>
   </si>
 </sst>
 </file>
@@ -1381,10 +1384,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I94" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I94" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I94">
-    <sortCondition descending="1" ref="C2:C94"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I95" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I95" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I95">
+    <sortCondition descending="1" ref="C2:C95"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3895,10 +3898,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K94"/>
+  <dimension ref="B2:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5673,7 +5676,7 @@
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="2" t="s">
         <v>168</v>
       </c>
       <c r="C67" s="5">
@@ -6159,272 +6162,299 @@
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="2" t="s">
-        <v>163</v>
+      <c r="B85" s="9" t="s">
+        <v>169</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D85" s="1">
+        <v>6</v>
+      </c>
+      <c r="E85" s="1">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1">
         <v>5</v>
       </c>
-      <c r="E85" s="1">
-        <v>5</v>
-      </c>
-      <c r="F85" s="1">
-        <v>3</v>
-      </c>
       <c r="G85" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I85" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D86" s="1">
         <v>5</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G86" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H86" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I86" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I86" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D87" s="1">
         <v>5</v>
       </c>
       <c r="E87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H87" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I87" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D88" s="1">
         <v>5</v>
       </c>
       <c r="E88" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F88" s="1">
         <v>5</v>
       </c>
       <c r="G88" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H88" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I88" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D89" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E89" s="1">
         <v>4</v>
       </c>
       <c r="F89" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G89" s="1">
         <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I89" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D90" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E90" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F90" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G90" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I90" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D91" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E91" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G91" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H91" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I91" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D92" s="1">
+        <v>5</v>
+      </c>
+      <c r="E92" s="1">
+        <v>3</v>
+      </c>
+      <c r="F92" s="1">
+        <v>3</v>
+      </c>
+      <c r="G92" s="1">
         <v>4</v>
       </c>
-      <c r="E92" s="1">
-        <v>2</v>
-      </c>
-      <c r="F92" s="1">
-        <v>6</v>
-      </c>
-      <c r="G92" s="1">
-        <v>6</v>
-      </c>
       <c r="H92" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I92" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I92" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D93" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E93" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F93" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I93" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D94" s="1">
+        <v>5</v>
+      </c>
+      <c r="E94" s="1">
+        <v>4</v>
+      </c>
+      <c r="F94" s="1">
+        <v>2</v>
+      </c>
+      <c r="G94" s="1">
+        <v>5</v>
+      </c>
+      <c r="H94" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I94" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B95" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" s="5">
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D95" s="1">
         <v>1</v>
       </c>
-      <c r="E94" s="1">
+      <c r="E95" s="1">
         <v>1</v>
       </c>
-      <c r="F94" s="1">
+      <c r="F95" s="1">
         <v>0</v>
       </c>
-      <c r="G94" s="1">
+      <c r="G95" s="1">
         <v>1</v>
       </c>
-      <c r="H94" s="3">
+      <c r="H95" s="3">
         <v>6.7</v>
       </c>
-      <c r="I94" s="3">
+      <c r="I95" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 72 "Coach Carter"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE392C1-6130-4B30-A178-11247959BAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A31DBC-6924-4025-B598-34D7A5F99168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="2970" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="5580" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="171">
   <si>
     <t>Película</t>
   </si>
@@ -1032,6 +1032,9 @@
   </si>
   <si>
     <t>Mi año en Oxford</t>
+  </si>
+  <si>
+    <t>Coach Carter</t>
   </si>
 </sst>
 </file>
@@ -1384,10 +1387,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I95" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I95" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I95">
-    <sortCondition descending="1" ref="C2:C95"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I96" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I96" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I96">
+    <sortCondition descending="1" ref="C2:C96"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3898,10 +3901,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K95"/>
+  <dimension ref="B2:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,66 +4275,66 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>125</v>
+      <c r="B15" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="C15" s="5">
         <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
-        <v>8.1750000000000007</v>
+        <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E15" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G15" s="1">
         <v>9</v>
       </c>
       <c r="H15" s="3">
-        <v>7.5</v>
+        <v>7.3</v>
       </c>
       <c r="I15" s="3">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="C16" s="5">
         <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
-        <v>8.1624999999999996</v>
+        <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
         <v>9</v>
       </c>
       <c r="E16" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F16" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="1">
         <v>9</v>
       </c>
       <c r="H16" s="3">
-        <v>7.6</v>
+        <v>7.5</v>
       </c>
       <c r="I16" s="3">
-        <v>7.1</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5">
         <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
-        <v>8.15</v>
+        <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
         <v>9</v>
@@ -4340,79 +4343,79 @@
         <v>8</v>
       </c>
       <c r="F17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G17" s="1">
         <v>9</v>
       </c>
       <c r="H17" s="3">
-        <v>8</v>
+        <v>7.6</v>
       </c>
       <c r="I17" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C18" s="5">
         <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
-        <v>8.1</v>
+        <v>8.15</v>
       </c>
       <c r="D18" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E18" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1">
         <v>8</v>
       </c>
       <c r="G18" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H18" s="3">
         <v>8</v>
       </c>
       <c r="I18" s="3">
-        <v>6.8</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C19" s="5">
         <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
-        <v>8.0750000000000011</v>
+        <v>8.1</v>
       </c>
       <c r="D19" s="1">
         <v>8</v>
       </c>
       <c r="E19" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G19" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H19" s="3">
-        <v>7.6</v>
+        <v>8</v>
       </c>
       <c r="I19" s="3">
-        <v>6.4</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>126</v>
       </c>
       <c r="C20" s="5">
         <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
-        <v>8.0625</v>
+        <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
         <v>8</v>
@@ -4421,55 +4424,55 @@
         <v>8</v>
       </c>
       <c r="F20" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H20" s="3">
-        <v>8.1</v>
+        <v>7.6</v>
       </c>
       <c r="I20" s="3">
-        <v>7.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C21" s="5">
         <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
-        <v>7.9249999999999998</v>
+        <v>8.0625</v>
       </c>
       <c r="D21" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1">
         <v>8</v>
       </c>
       <c r="F21" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" s="3">
-        <v>7</v>
+        <v>8.1</v>
       </c>
       <c r="I21" s="3">
-        <v>6.4</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>122</v>
+        <v>23</v>
       </c>
       <c r="C22" s="5">
         <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
-        <v>7.9124999999999996</v>
+        <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E22" s="1">
         <v>8</v>
@@ -4481,19 +4484,19 @@
         <v>9</v>
       </c>
       <c r="H22" s="3">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="I22" s="3">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="C23" s="5">
         <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
-        <v>7.8999999999999995</v>
+        <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
         <v>9</v>
@@ -4502,75 +4505,75 @@
         <v>8</v>
       </c>
       <c r="F23" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H23" s="3">
         <v>7.4</v>
       </c>
       <c r="I23" s="3">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="C24" s="5">
         <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
-        <v>7.875</v>
+        <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E24" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G24" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H24" s="3">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
       <c r="I24" s="3">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="C25" s="5">
         <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
-        <v>7.7875000000000005</v>
+        <v>7.875</v>
       </c>
       <c r="D25" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F25" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G25" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H25" s="3">
-        <v>7.1</v>
+        <v>6.9</v>
       </c>
       <c r="I25" s="3">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="C26" s="5">
         <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
@@ -4586,22 +4589,22 @@
         <v>8</v>
       </c>
       <c r="G26" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H26" s="3">
-        <v>7.7</v>
+        <v>7.1</v>
       </c>
       <c r="I26" s="3">
-        <v>6.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C27" s="5">
         <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
-        <v>7.7375000000000007</v>
+        <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
         <v>8</v>
@@ -4610,75 +4613,75 @@
         <v>8</v>
       </c>
       <c r="F27" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" s="1">
         <v>8</v>
       </c>
       <c r="H27" s="3">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="I27" s="3">
-        <v>6.5</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="C28" s="5">
         <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
-        <v>7.7000000000000011</v>
+        <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
         <v>8</v>
       </c>
       <c r="E28" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F28" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G28" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H28" s="3">
         <v>7.2</v>
       </c>
       <c r="I28" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="C29" s="5">
         <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
-        <v>7.6999999999999993</v>
+        <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
         <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G29" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H29" s="3">
-        <v>7.8</v>
+        <v>7.2</v>
       </c>
       <c r="I29" s="3">
-        <v>7</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="C30" s="5">
         <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
@@ -4688,31 +4691,31 @@
         <v>8</v>
       </c>
       <c r="E30" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F30" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H30" s="3">
-        <v>6.3</v>
+        <v>7.8</v>
       </c>
       <c r="I30" s="3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C31" s="5">
         <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
-        <v>7.6875</v>
+        <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1">
         <v>9</v>
@@ -4724,79 +4727,79 @@
         <v>9</v>
       </c>
       <c r="H31" s="3">
-        <v>5.9</v>
+        <v>6.3</v>
       </c>
       <c r="I31" s="3">
-        <v>4.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="C32" s="5">
         <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
-        <v>7.5874999999999995</v>
+        <v>7.6875</v>
       </c>
       <c r="D32" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F32" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G32" s="1">
         <v>9</v>
       </c>
       <c r="H32" s="3">
-        <v>7.9</v>
+        <v>5.9</v>
       </c>
       <c r="I32" s="3">
-        <v>6.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="C33" s="5">
         <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
-        <v>7.5750000000000011</v>
+        <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F33" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G33" s="1">
         <v>9</v>
       </c>
       <c r="H33" s="3">
-        <v>7.2</v>
+        <v>7.9</v>
       </c>
       <c r="I33" s="3">
-        <v>6.2</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C34" s="5">
         <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
-        <v>7.5750000000000002</v>
+        <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E34" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F34" s="1">
         <v>8</v>
@@ -4805,130 +4808,130 @@
         <v>9</v>
       </c>
       <c r="H34" s="3">
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="I34" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C35" s="5">
         <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
-        <v>7.5625</v>
+        <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F35" s="1">
         <v>8</v>
       </c>
       <c r="G35" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H35" s="3">
         <v>7</v>
       </c>
       <c r="I35" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C36" s="5">
         <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
-        <v>7.5624999999999991</v>
+        <v>7.5625</v>
       </c>
       <c r="D36" s="1">
         <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F36" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G36" s="1">
         <v>8</v>
       </c>
       <c r="H36" s="3">
-        <v>8.3000000000000007</v>
+        <v>7</v>
       </c>
       <c r="I36" s="3">
-        <v>7.9</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C37" s="5">
         <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
-        <v>7.5250000000000004</v>
+        <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F37" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G37" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H37" s="3">
-        <v>6.7</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I37" s="3">
-        <v>5.8</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="C38" s="5">
         <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
-        <v>7.5125000000000002</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
         <v>7</v>
       </c>
       <c r="G38" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H38" s="3">
-        <v>8</v>
+        <v>6.7</v>
       </c>
       <c r="I38" s="3">
-        <v>7.1</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C39" s="5">
         <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
-        <v>7.4625000000000004</v>
+        <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1">
         <v>7</v>
@@ -4937,55 +4940,55 @@
         <v>7</v>
       </c>
       <c r="G39" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H39" s="3">
-        <v>6.7</v>
+        <v>8</v>
       </c>
       <c r="I39" s="3">
-        <v>6.3</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C40" s="5">
         <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
-        <v>7.4249999999999998</v>
+        <v>7.4625000000000004</v>
       </c>
       <c r="D40" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H40" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I40" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C41" s="5">
         <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
-        <v>7.4124999999999996</v>
+        <v>7.4249999999999998</v>
       </c>
       <c r="D41" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1">
         <v>8</v>
@@ -4994,25 +4997,25 @@
         <v>8</v>
       </c>
       <c r="H41" s="3">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="I41" s="3">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>52</v>
+        <v>131</v>
       </c>
       <c r="C42" s="5">
         <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
-        <v>7.3500000000000005</v>
+        <v>7.4124999999999996</v>
       </c>
       <c r="D42" s="1">
         <v>8</v>
       </c>
       <c r="E42" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" s="1">
         <v>8</v>
@@ -5021,19 +5024,19 @@
         <v>8</v>
       </c>
       <c r="H42" s="3">
-        <v>6.6</v>
+        <v>7.4</v>
       </c>
       <c r="I42" s="3">
-        <v>5.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C43" s="5">
         <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
-        <v>7.3249999999999993</v>
+        <v>7.3500000000000005</v>
       </c>
       <c r="D43" s="1">
         <v>8</v>
@@ -5045,82 +5048,82 @@
         <v>8</v>
       </c>
       <c r="G43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H43" s="3">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="I43" s="3">
-        <v>6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
-        <v>7.3</v>
+        <v>7.3249999999999993</v>
       </c>
       <c r="D44" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G44" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H44" s="3">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="I44" s="3">
-        <v>5.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
-        <v>7.2750000000000004</v>
+        <v>7.3</v>
       </c>
       <c r="D45" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G45" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H45" s="3">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="I45" s="3">
-        <v>6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
-        <v>7.2374999999999998</v>
+        <v>7.2750000000000004</v>
       </c>
       <c r="D46" s="1">
         <v>7</v>
       </c>
       <c r="E46" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1">
         <v>8</v>
@@ -5129,265 +5132,265 @@
         <v>8</v>
       </c>
       <c r="H46" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
       <c r="I46" s="3">
-        <v>4.9000000000000004</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
-        <v>7.2250000000000005</v>
+        <v>7.2374999999999998</v>
       </c>
       <c r="D47" s="1">
         <v>7</v>
       </c>
       <c r="E47" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F47" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G47" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H47" s="3">
-        <v>8.1</v>
+        <v>6</v>
       </c>
       <c r="I47" s="3">
-        <v>7.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
-        <v>7.2125000000000004</v>
+        <v>7.2250000000000005</v>
       </c>
       <c r="D48" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E48" s="1">
         <v>7</v>
       </c>
       <c r="F48" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G48" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H48" s="3">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="I48" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
-        <v>7.2124999999999995</v>
+        <v>7.2125000000000004</v>
       </c>
       <c r="D49" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E49" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F49" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1">
         <v>8</v>
       </c>
       <c r="H49" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I49" s="3">
         <v>6.3</v>
-      </c>
-      <c r="I49" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
-        <v>7.1499999999999995</v>
+        <v>7.2124999999999995</v>
       </c>
       <c r="D50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G50" s="1">
         <v>8</v>
       </c>
       <c r="H50" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I50" s="3">
-        <v>6.6</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
-        <v>7.1375000000000011</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D51" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G51" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H51" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I51" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D52" s="1">
         <v>7</v>
       </c>
       <c r="E52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G52" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H52" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I52" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I52" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
-        <v>7.125</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H53" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I53" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
-        <v>7.0875000000000004</v>
+        <v>7.125</v>
       </c>
       <c r="D54" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1">
         <v>8</v>
       </c>
       <c r="F54" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1">
         <v>7</v>
       </c>
       <c r="H54" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I54" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D55" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F55" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H55" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I55" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D56" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" s="1">
         <v>7</v>
@@ -5396,25 +5399,25 @@
         <v>8</v>
       </c>
       <c r="G56" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H56" s="3">
-        <v>6.6</v>
+        <v>7.2</v>
       </c>
       <c r="I56" s="3">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D57" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E57" s="1">
         <v>7</v>
@@ -5423,25 +5426,25 @@
         <v>8</v>
       </c>
       <c r="G57" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H57" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I57" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
-        <v>6.9375</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D58" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E58" s="1">
         <v>7</v>
@@ -5450,18 +5453,18 @@
         <v>8</v>
       </c>
       <c r="G58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H58" s="3">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="I58" s="3">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
@@ -5471,7 +5474,7 @@
         <v>8</v>
       </c>
       <c r="E59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
@@ -5480,214 +5483,214 @@
         <v>8</v>
       </c>
       <c r="H59" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I59" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D60" s="1">
         <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1">
         <v>8</v>
       </c>
       <c r="G60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H60" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="I60" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D61" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F61" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I61" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D62" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F62" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G62" s="1">
         <v>8</v>
       </c>
       <c r="H62" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I62" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D63" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E63" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I63" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>6.6999999999999993</v>
+        <v>6.85</v>
       </c>
       <c r="D64" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E64" s="1">
         <v>6</v>
       </c>
       <c r="F64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G64" s="1">
         <v>7</v>
       </c>
       <c r="H64" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I64" s="3">
-        <v>7.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D65" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1">
         <v>6</v>
       </c>
       <c r="F65" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G65" s="1">
         <v>7</v>
       </c>
       <c r="H65" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I65" s="3">
-        <v>5.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H66" s="3">
         <v>6.3</v>
       </c>
       <c r="I66" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D67" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F67" s="1">
         <v>7</v>
@@ -5696,69 +5699,69 @@
         <v>6</v>
       </c>
       <c r="H67" s="3">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="I67" s="3">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.3125</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D68" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E68" s="1">
         <v>6</v>
       </c>
       <c r="F68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G68" s="1">
         <v>6</v>
       </c>
       <c r="H68" s="3">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="I68" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E69" s="1">
         <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H69" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I69" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
@@ -5768,142 +5771,142 @@
         <v>6</v>
       </c>
       <c r="E70" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I70" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D71" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F71" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G71" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H71" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I71" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D72" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1">
         <v>8</v>
       </c>
       <c r="G72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H72" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I72" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D73" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" s="1">
         <v>8</v>
       </c>
       <c r="G73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I73" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D74" s="1">
         <v>7</v>
       </c>
       <c r="E74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H74" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I74" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D75" s="1">
         <v>7</v>
       </c>
       <c r="E75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F75" s="1">
         <v>7</v>
@@ -5912,166 +5915,166 @@
         <v>7</v>
       </c>
       <c r="H75" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I75" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1">
         <v>6</v>
       </c>
       <c r="F76" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H76" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I76" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G77" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H77" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I77" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F78" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I78" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F79" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G79" s="1">
         <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I79" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D80" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1">
+        <v>3</v>
+      </c>
+      <c r="F80" s="1">
         <v>5</v>
       </c>
-      <c r="F80" s="1">
-        <v>6</v>
-      </c>
       <c r="G80" s="1">
         <v>6</v>
       </c>
       <c r="H80" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I80" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D81" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G81" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3">
         <v>5.8</v>
@@ -6082,379 +6085,406 @@
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D82" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E82" s="1">
         <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I82" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>5.1124999999999998</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D83" s="1">
         <v>6</v>
       </c>
       <c r="E83" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
         <v>6</v>
       </c>
       <c r="H83" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I83" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D84" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E84" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F84" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G84" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I84" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B85" s="9" t="s">
-        <v>169</v>
+      <c r="B85" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E85" s="1">
         <v>3</v>
       </c>
       <c r="F85" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G85" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H85" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I85" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D86" s="1">
+        <v>6</v>
+      </c>
+      <c r="E86" s="1">
+        <v>3</v>
+      </c>
+      <c r="F86" s="1">
         <v>5</v>
       </c>
-      <c r="E86" s="1">
-        <v>5</v>
-      </c>
-      <c r="F86" s="1">
-        <v>3</v>
-      </c>
       <c r="G86" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I86" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D87" s="1">
         <v>5</v>
       </c>
       <c r="E87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G87" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H87" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I87" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I87" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D88" s="1">
         <v>5</v>
       </c>
       <c r="E88" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H88" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I88" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D89" s="1">
         <v>5</v>
       </c>
       <c r="E89" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F89" s="1">
         <v>5</v>
       </c>
       <c r="G89" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H89" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I89" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D90" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1">
         <v>4</v>
       </c>
       <c r="F90" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G90" s="1">
         <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I90" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D91" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E91" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F91" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G91" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I91" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D92" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F92" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G92" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H92" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I92" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D93" s="1">
+        <v>5</v>
+      </c>
+      <c r="E93" s="1">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1">
+        <v>3</v>
+      </c>
+      <c r="G93" s="1">
         <v>4</v>
       </c>
-      <c r="E93" s="1">
-        <v>2</v>
-      </c>
-      <c r="F93" s="1">
-        <v>6</v>
-      </c>
-      <c r="G93" s="1">
-        <v>6</v>
-      </c>
       <c r="H93" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I93" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I93" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D94" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E94" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F94" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I94" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D95" s="1">
+        <v>5</v>
+      </c>
+      <c r="E95" s="1">
+        <v>4</v>
+      </c>
+      <c r="F95" s="1">
+        <v>2</v>
+      </c>
+      <c r="G95" s="1">
+        <v>5</v>
+      </c>
+      <c r="H95" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I95" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B96" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C96" s="5">
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D96" s="1">
         <v>1</v>
       </c>
-      <c r="E95" s="1">
+      <c r="E96" s="1">
         <v>1</v>
       </c>
-      <c r="F95" s="1">
+      <c r="F96" s="1">
         <v>0</v>
       </c>
-      <c r="G95" s="1">
+      <c r="G96" s="1">
         <v>1</v>
       </c>
-      <c r="H95" s="3">
+      <c r="H96" s="3">
         <v>6.7</v>
       </c>
-      <c r="I95" s="3">
+      <c r="I96" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 73 "Spenser Confidential"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A31DBC-6924-4025-B598-34D7A5F99168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C43DC239-4EDD-4F9C-89A9-4809F4556FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="5580" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8280" yWindow="2940" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="172">
   <si>
     <t>Película</t>
   </si>
@@ -1035,6 +1035,9 @@
   </si>
   <si>
     <t>Coach Carter</t>
+  </si>
+  <si>
+    <t>Spenser Confidential</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1390,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I96" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I96" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I96">
-    <sortCondition descending="1" ref="C2:C96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I97" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I97" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I97">
+    <sortCondition descending="1" ref="C2:C97"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3901,10 +3904,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K96"/>
+  <dimension ref="B2:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4275,7 +4278,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C15" s="5">
@@ -5409,42 +5412,42 @@
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B57" s="2" t="s">
-        <v>110</v>
+      <c r="B57" s="9" t="s">
+        <v>171</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1">
         <v>8</v>
       </c>
       <c r="G57" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H57" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="I57" s="3">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D58" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
         <v>7</v>
@@ -5453,25 +5456,25 @@
         <v>8</v>
       </c>
       <c r="G58" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H58" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I58" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>6.9375</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D59" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59" s="1">
         <v>7</v>
@@ -5480,18 +5483,18 @@
         <v>8</v>
       </c>
       <c r="G59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="I59" s="3">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
@@ -5501,7 +5504,7 @@
         <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F60" s="1">
         <v>8</v>
@@ -5510,214 +5513,214 @@
         <v>8</v>
       </c>
       <c r="H60" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I60" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D61" s="1">
         <v>8</v>
       </c>
       <c r="E61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F61" s="1">
         <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="I61" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D62" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H62" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I62" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D63" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E63" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F63" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G63" s="1">
         <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I63" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D64" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H64" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I64" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.6999999999999993</v>
+        <v>6.85</v>
       </c>
       <c r="D65" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1">
         <v>6</v>
       </c>
       <c r="F65" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G65" s="1">
         <v>7</v>
       </c>
       <c r="H65" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I65" s="3">
-        <v>7.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D66" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E66" s="1">
         <v>6</v>
       </c>
       <c r="F66" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G66" s="1">
         <v>7</v>
       </c>
       <c r="H66" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I66" s="3">
-        <v>5.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H67" s="3">
         <v>6.3</v>
       </c>
       <c r="I67" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" s="1">
         <v>7</v>
@@ -5726,69 +5729,69 @@
         <v>6</v>
       </c>
       <c r="H68" s="3">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="I68" s="3">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.3125</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D69" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
         <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G69" s="1">
         <v>6</v>
       </c>
       <c r="H69" s="3">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="I69" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E70" s="1">
         <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G70" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H70" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I70" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
@@ -5798,142 +5801,142 @@
         <v>6</v>
       </c>
       <c r="E71" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H71" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I71" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G72" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H72" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I72" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" s="1">
         <v>8</v>
       </c>
       <c r="G73" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H73" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I73" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F74" s="1">
         <v>8</v>
       </c>
       <c r="G74" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H74" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I74" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D75" s="1">
         <v>7</v>
       </c>
       <c r="E75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H75" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I75" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D76" s="1">
         <v>7</v>
       </c>
       <c r="E76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
         <v>7</v>
@@ -5942,166 +5945,166 @@
         <v>7</v>
       </c>
       <c r="H76" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I76" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
         <v>6</v>
       </c>
       <c r="F77" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G77" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H77" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I77" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D78" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G78" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H78" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I78" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D79" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E79" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G79" s="1">
         <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I79" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E80" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F80" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G80" s="1">
         <v>6</v>
       </c>
       <c r="H80" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I80" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D81" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1">
+        <v>3</v>
+      </c>
+      <c r="F81" s="1">
         <v>5</v>
       </c>
-      <c r="F81" s="1">
-        <v>6</v>
-      </c>
       <c r="G81" s="1">
         <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I81" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D82" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F82" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G82" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H82" s="3">
         <v>5.8</v>
@@ -6112,379 +6115,406 @@
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D83" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E83" s="1">
         <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G83" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I83" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>5.1124999999999998</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D84" s="1">
         <v>6</v>
       </c>
       <c r="E84" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G84" s="1">
         <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I84" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D85" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F85" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G85" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I85" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E86" s="1">
         <v>3</v>
       </c>
       <c r="F86" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G86" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H86" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I86" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D87" s="1">
+        <v>6</v>
+      </c>
+      <c r="E87" s="1">
+        <v>3</v>
+      </c>
+      <c r="F87" s="1">
         <v>5</v>
       </c>
-      <c r="E87" s="1">
-        <v>5</v>
-      </c>
-      <c r="F87" s="1">
-        <v>3</v>
-      </c>
       <c r="G87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I87" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D88" s="1">
         <v>5</v>
       </c>
       <c r="E88" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G88" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H88" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I88" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I88" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D89" s="1">
         <v>5</v>
       </c>
       <c r="E89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H89" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I89" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D90" s="1">
         <v>5</v>
       </c>
       <c r="E90" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F90" s="1">
         <v>5</v>
       </c>
       <c r="G90" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H90" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I90" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D91" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1">
         <v>4</v>
       </c>
       <c r="F91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G91" s="1">
         <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I91" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D92" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E92" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F92" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G92" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I92" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D93" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E93" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F93" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G93" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H93" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I93" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D94" s="1">
+        <v>5</v>
+      </c>
+      <c r="E94" s="1">
+        <v>3</v>
+      </c>
+      <c r="F94" s="1">
+        <v>3</v>
+      </c>
+      <c r="G94" s="1">
         <v>4</v>
       </c>
-      <c r="E94" s="1">
-        <v>2</v>
-      </c>
-      <c r="F94" s="1">
-        <v>6</v>
-      </c>
-      <c r="G94" s="1">
-        <v>6</v>
-      </c>
       <c r="H94" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I94" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I94" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D95" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E95" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F95" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I95" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D96" s="1">
+        <v>5</v>
+      </c>
+      <c r="E96" s="1">
+        <v>4</v>
+      </c>
+      <c r="F96" s="1">
+        <v>2</v>
+      </c>
+      <c r="G96" s="1">
+        <v>5</v>
+      </c>
+      <c r="H96" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I96" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B97" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C97" s="5">
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D97" s="1">
         <v>1</v>
       </c>
-      <c r="E96" s="1">
+      <c r="E97" s="1">
         <v>1</v>
       </c>
-      <c r="F96" s="1">
+      <c r="F97" s="1">
         <v>0</v>
       </c>
-      <c r="G96" s="1">
+      <c r="G97" s="1">
         <v>1</v>
       </c>
-      <c r="H96" s="3">
+      <c r="H97" s="3">
         <v>6.7</v>
       </c>
-      <c r="I96" s="3">
+      <c r="I97" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 75 "A descubierto"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347BC8A0-27D8-4242-AAD2-223D5500D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0384457-B82C-4969-8D3F-6F3F9BD00595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4110" yWindow="4110" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="174">
   <si>
     <t>Película</t>
   </si>
@@ -1041,6 +1041,9 @@
   </si>
   <si>
     <t>Garra</t>
+  </si>
+  <si>
+    <t>A descubierto</t>
   </si>
 </sst>
 </file>
@@ -1393,10 +1396,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I98" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I98" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I98">
-    <sortCondition descending="1" ref="C2:C98"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I99" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I99" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I99">
+    <sortCondition descending="1" ref="C2:C99"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3907,10 +3910,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K98"/>
+  <dimension ref="B2:K99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4956,7 +4959,7 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C40" s="5">
@@ -6468,83 +6471,110 @@
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B96" s="2" t="s">
-        <v>167</v>
+      <c r="B96" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D96" s="1">
+        <v>3</v>
+      </c>
+      <c r="E96" s="1">
         <v>4</v>
       </c>
-      <c r="E96" s="1">
-        <v>2</v>
-      </c>
       <c r="F96" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G96" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H96" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I96" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D97" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E97" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F97" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I97" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D98" s="1">
+        <v>5</v>
+      </c>
+      <c r="E98" s="1">
+        <v>4</v>
+      </c>
+      <c r="F98" s="1">
+        <v>2</v>
+      </c>
+      <c r="G98" s="1">
+        <v>5</v>
+      </c>
+      <c r="H98" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I98" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B99" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C99" s="5">
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>2.9124999999999996</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D99" s="1">
         <v>1</v>
       </c>
-      <c r="E98" s="1">
+      <c r="E99" s="1">
         <v>1</v>
       </c>
-      <c r="F98" s="1">
+      <c r="F99" s="1">
         <v>0</v>
       </c>
-      <c r="G98" s="1">
+      <c r="G99" s="1">
         <v>1</v>
       </c>
-      <c r="H98" s="3">
+      <c r="H99" s="3">
         <v>6.7</v>
       </c>
-      <c r="I98" s="3">
+      <c r="I99" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 77 "Jack el caza gigantes" & "Mamá o papá"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E28870-B46C-4EF7-8CCF-391DB1AFE5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBF3811-A5D3-4A61-BE88-6C2461C9EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="4110" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5370" yWindow="4710" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
   <si>
     <t>Película</t>
   </si>
@@ -1047,6 +1047,12 @@
   </si>
   <si>
     <t>Supersalidos</t>
+  </si>
+  <si>
+    <t>Jack el caza gigantes</t>
+  </si>
+  <si>
+    <t>Mamá o papá</t>
   </si>
 </sst>
 </file>
@@ -1399,10 +1405,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I100" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I100" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I100">
-    <sortCondition descending="1" ref="C2:C100"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I102" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I102" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I102">
+    <sortCondition descending="1" ref="C2:C102"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3913,10 +3919,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K100"/>
+  <dimension ref="B2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H100" sqref="H100"/>
+    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5070,12 +5076,12 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
-        <v>52</v>
+      <c r="B44" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
-        <v>7.3500000000000005</v>
+        <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
         <v>8</v>
@@ -5084,25 +5090,25 @@
         <v>8</v>
       </c>
       <c r="F44" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G44" s="1">
         <v>8</v>
       </c>
       <c r="H44" s="3">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="I44" s="3">
-        <v>5.6</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
-        <v>7.3249999999999993</v>
+        <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
         <v>8</v>
@@ -5114,82 +5120,82 @@
         <v>8</v>
       </c>
       <c r="G45" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H45" s="3">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="I45" s="3">
-        <v>6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
-        <v>7.3</v>
+        <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E46" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F46" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H46" s="3">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="I46" s="3">
-        <v>5.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
-        <v>7.2750000000000004</v>
+        <v>7.3</v>
       </c>
       <c r="D47" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F47" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G47" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H47" s="3">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="I47" s="3">
-        <v>6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
-        <v>7.2374999999999998</v>
+        <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
         <v>7</v>
       </c>
       <c r="E48" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1">
         <v>8</v>
@@ -5198,319 +5204,319 @@
         <v>8</v>
       </c>
       <c r="H48" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
       <c r="I48" s="3">
-        <v>4.9000000000000004</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
-        <v>7.2250000000000005</v>
+        <v>7.2374999999999998</v>
       </c>
       <c r="D49" s="1">
         <v>7</v>
       </c>
       <c r="E49" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F49" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G49" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H49" s="3">
-        <v>8.1</v>
+        <v>6</v>
       </c>
       <c r="I49" s="3">
-        <v>7.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
-        <v>7.2125000000000004</v>
+        <v>7.2250000000000005</v>
       </c>
       <c r="D50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E50" s="1">
         <v>7</v>
       </c>
       <c r="F50" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H50" s="3">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="I50" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
-        <v>7.2124999999999995</v>
+        <v>7.2125000000000004</v>
       </c>
       <c r="D51" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F51" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1">
         <v>8</v>
       </c>
       <c r="H51" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I51" s="3">
         <v>6.3</v>
-      </c>
-      <c r="I51" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
-        <v>7.1499999999999995</v>
+        <v>7.2124999999999995</v>
       </c>
       <c r="D52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F52" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G52" s="1">
         <v>8</v>
       </c>
       <c r="H52" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I52" s="3">
-        <v>6.6</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
-        <v>7.1375000000000011</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F53" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G53" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H53" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I53" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D54" s="1">
         <v>7</v>
       </c>
       <c r="E54" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H54" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I54" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I54" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
-        <v>7.125</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H55" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I55" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
-        <v>7.0875000000000004</v>
+        <v>7.125</v>
       </c>
       <c r="D56" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1">
         <v>8</v>
       </c>
       <c r="F56" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G56" s="1">
         <v>7</v>
       </c>
       <c r="H56" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I56" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D57" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H57" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I57" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D58" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" s="1">
         <v>8</v>
       </c>
       <c r="G58" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H58" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I58" s="3">
         <v>6.2</v>
-      </c>
-      <c r="I58" s="3">
-        <v>5.2</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
       </c>
       <c r="G59" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="I59" s="3">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D60" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E60" s="1">
         <v>7</v>
@@ -5519,25 +5525,25 @@
         <v>8</v>
       </c>
       <c r="G60" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H60" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I60" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>6.9375</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E61" s="1">
         <v>7</v>
@@ -5546,22 +5552,22 @@
         <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" s="3">
-        <v>6.1</v>
+        <v>6.5</v>
       </c>
       <c r="I61" s="3">
-        <v>5.3</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="2" t="s">
-        <v>87</v>
+      <c r="B62" s="9" t="s">
+        <v>176</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>6.9375</v>
+        <v>7.05</v>
       </c>
       <c r="D62" s="1">
         <v>8</v>
@@ -5570,25 +5576,25 @@
         <v>8</v>
       </c>
       <c r="F62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G62" s="1">
         <v>8</v>
       </c>
       <c r="H62" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I62" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D63" s="1">
         <v>8</v>
@@ -5600,52 +5606,52 @@
         <v>8</v>
       </c>
       <c r="G63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="I63" s="3">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9375</v>
       </c>
       <c r="D64" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E64" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F64" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1">
         <v>8</v>
       </c>
       <c r="H64" s="3">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="I64" s="3">
-        <v>6.4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>88</v>
+        <v>164</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.8624999999999989</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1">
         <v>7</v>
@@ -5654,76 +5660,76 @@
         <v>8</v>
       </c>
       <c r="G65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H65" s="3">
-        <v>6.3</v>
+        <v>6.4</v>
       </c>
       <c r="I65" s="3">
-        <v>5.3</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.85</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D66" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E66" s="1">
         <v>6</v>
       </c>
       <c r="F66" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H66" s="3">
-        <v>7.3</v>
+        <v>6.9</v>
       </c>
       <c r="I66" s="3">
-        <v>6.2</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.6999999999999993</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D67" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F67" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H67" s="3">
-        <v>7.9</v>
+        <v>6.3</v>
       </c>
       <c r="I67" s="3">
-        <v>7.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.6124999999999989</v>
+        <v>6.85</v>
       </c>
       <c r="D68" s="1">
         <v>8</v>
@@ -5732,52 +5738,52 @@
         <v>6</v>
       </c>
       <c r="F68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G68" s="1">
         <v>7</v>
       </c>
       <c r="H68" s="3">
-        <v>6.3</v>
+        <v>7.3</v>
       </c>
       <c r="I68" s="3">
-        <v>5.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>117</v>
+        <v>57</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D69" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H69" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I69" s="3">
-        <v>6.1</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.5499999999999989</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D70" s="1">
         <v>8</v>
@@ -5786,55 +5792,55 @@
         <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H70" s="3">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="I70" s="3">
-        <v>5.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.3125</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D71" s="1">
         <v>7</v>
       </c>
       <c r="E71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G71" s="1">
         <v>6</v>
       </c>
       <c r="H71" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I71" s="3">
-        <v>5.7</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.2749999999999995</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D72" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1">
         <v>6</v>
@@ -5843,28 +5849,28 @@
         <v>7</v>
       </c>
       <c r="G72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H72" s="3">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
       <c r="I72" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" s="1">
         <v>6</v>
@@ -5873,73 +5879,73 @@
         <v>6</v>
       </c>
       <c r="H73" s="3">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="I73" s="3">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E74" s="1">
         <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G74" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H74" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="I74" s="3">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D75" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E75" s="1">
         <v>7</v>
       </c>
       <c r="F75" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H75" s="3">
-        <v>4.3</v>
+        <v>6.4</v>
       </c>
       <c r="I75" s="3">
-        <v>4.0999999999999996</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.15</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D76" s="1">
         <v>7</v>
@@ -5954,34 +5960,34 @@
         <v>8</v>
       </c>
       <c r="H76" s="3">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I76" s="3">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>6.0874999999999995</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D77" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1">
         <v>7</v>
       </c>
       <c r="F77" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G77" s="1">
         <v>7</v>
       </c>
       <c r="H77" s="3">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="I77" s="3">
         <v>4.0999999999999996</v>
@@ -5989,11 +5995,11 @@
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>160</v>
+        <v>101</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>6.05</v>
+        <v>6.15</v>
       </c>
       <c r="D78" s="1">
         <v>7</v>
@@ -6002,193 +6008,193 @@
         <v>6</v>
       </c>
       <c r="F78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H78" s="3">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="I78" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>5.9499999999999993</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G79" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H79" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I79" s="3">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>74</v>
+        <v>160</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>5.8125</v>
+        <v>6.05</v>
       </c>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E80" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
       <c r="I80" s="3">
-        <v>3.5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>5.7374999999999989</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
+        <v>6</v>
+      </c>
+      <c r="F81" s="1">
+        <v>8</v>
+      </c>
+      <c r="G81" s="1">
         <v>5</v>
       </c>
-      <c r="F81" s="1">
-        <v>4</v>
-      </c>
-      <c r="G81" s="1">
-        <v>6</v>
-      </c>
       <c r="H81" s="3">
-        <v>6.8</v>
+        <v>5.8</v>
       </c>
       <c r="I81" s="3">
-        <v>5.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>5.6749999999999998</v>
+        <v>5.8125</v>
       </c>
       <c r="D82" s="1">
         <v>8</v>
       </c>
       <c r="E82" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F82" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G82" s="1">
         <v>6</v>
       </c>
       <c r="H82" s="3">
-        <v>7</v>
+        <v>4.5</v>
       </c>
       <c r="I82" s="3">
-        <v>6.4</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>5.5624999999999991</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E83" s="1">
         <v>5</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G83" s="1">
         <v>6</v>
       </c>
       <c r="H83" s="3">
-        <v>5.8</v>
+        <v>6.8</v>
       </c>
       <c r="I83" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D84" s="1">
+        <v>8</v>
+      </c>
+      <c r="E84" s="1">
         <v>3</v>
       </c>
-      <c r="E84" s="1">
-        <v>6</v>
-      </c>
       <c r="F84" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G84" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I84" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D85" s="1">
         <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F85" s="1">
         <v>6</v>
@@ -6197,154 +6203,154 @@
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I85" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>5.1124999999999998</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E86" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F86" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H86" s="3">
-        <v>5.9</v>
+        <v>5.8</v>
       </c>
       <c r="I86" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>21</v>
+        <v>166</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>5.05</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>6.8</v>
+        <v>4.8</v>
       </c>
       <c r="I87" s="3">
-        <v>5.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>4.9874999999999998</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D88" s="1">
         <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F88" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G88" s="1">
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="I88" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D89" s="1">
         <v>5</v>
       </c>
       <c r="E89" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F89" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G89" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H89" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I89" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.7875000000000005</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D90" s="1">
+        <v>6</v>
+      </c>
+      <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
         <v>5</v>
       </c>
-      <c r="E90" s="1">
-        <v>6</v>
-      </c>
-      <c r="F90" s="1">
-        <v>6</v>
-      </c>
       <c r="G90" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H90" s="3">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="I90" s="3">
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D91" s="1">
         <v>5</v>
@@ -6353,258 +6359,312 @@
         <v>5</v>
       </c>
       <c r="F91" s="1">
+        <v>3</v>
+      </c>
+      <c r="G91" s="1">
         <v>5</v>
       </c>
-      <c r="G91" s="1">
-        <v>3</v>
-      </c>
       <c r="H91" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="I91" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>4.5874999999999995</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D92" s="1">
         <v>5</v>
       </c>
       <c r="E92" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G92" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H92" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I92" s="3">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D93" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E93" s="1">
+        <v>5</v>
+      </c>
+      <c r="F93" s="1">
+        <v>5</v>
+      </c>
+      <c r="G93" s="1">
+        <v>3</v>
+      </c>
+      <c r="H93" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I93" s="3">
         <v>4</v>
-      </c>
-      <c r="F93" s="1">
-        <v>6</v>
-      </c>
-      <c r="G93" s="1">
-        <v>5</v>
-      </c>
-      <c r="H93" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="I93" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.4124999999999996</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D94" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F94" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G94" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>8.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I94" s="3">
-        <v>7.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D95" s="1">
+        <v>1</v>
+      </c>
+      <c r="E95" s="1">
+        <v>4</v>
+      </c>
+      <c r="F95" s="1">
+        <v>6</v>
+      </c>
+      <c r="G95" s="1">
         <v>5</v>
       </c>
-      <c r="E95" s="1">
-        <v>3</v>
-      </c>
-      <c r="F95" s="1">
-        <v>3</v>
-      </c>
-      <c r="G95" s="1">
-        <v>4</v>
-      </c>
       <c r="H95" s="3">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="I95" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>4.3125</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D96" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E96" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F96" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G96" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H96" s="3">
-        <v>5.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I96" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D97" s="1">
+        <v>5</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1">
+        <v>3</v>
+      </c>
+      <c r="G97" s="1">
         <v>4</v>
       </c>
-      <c r="E97" s="1">
-        <v>2</v>
-      </c>
-      <c r="F97" s="1">
-        <v>6</v>
-      </c>
-      <c r="G97" s="1">
-        <v>6</v>
-      </c>
       <c r="H97" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I97" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I97" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3125</v>
       </c>
       <c r="D98" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E98" s="1">
         <v>4</v>
       </c>
       <c r="F98" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H98" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
       <c r="I98" s="3">
-        <v>3.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>2.9124999999999996</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D99" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E99" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F99" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>6.7</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I99" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B100" s="9" t="s">
-        <v>174</v>
+      <c r="B100" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>4.1124999999999998</v>
+      </c>
+      <c r="D100" s="1">
+        <v>5</v>
+      </c>
+      <c r="E100" s="1">
+        <v>4</v>
+      </c>
+      <c r="F100" s="1">
+        <v>2</v>
+      </c>
+      <c r="G100" s="1">
+        <v>5</v>
+      </c>
+      <c r="H100" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="I100" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C101" s="5">
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>2.9124999999999996</v>
+      </c>
+      <c r="D101" s="1">
+        <v>1</v>
+      </c>
+      <c r="E101" s="1">
+        <v>1</v>
+      </c>
+      <c r="F101" s="1">
+        <v>0</v>
+      </c>
+      <c r="G101" s="1">
+        <v>1</v>
+      </c>
+      <c r="H101" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I101" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C102" s="5">
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
         <v>2.6375000000000002</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D102" s="1">
         <v>0</v>
       </c>
-      <c r="E100" s="1">
+      <c r="E102" s="1">
         <v>0</v>
       </c>
-      <c r="F100" s="1">
+      <c r="F102" s="1">
         <v>0</v>
       </c>
-      <c r="G100" s="1">
+      <c r="G102" s="1">
         <v>0</v>
       </c>
-      <c r="H100" s="3">
+      <c r="H102" s="3">
         <v>7.6</v>
       </c>
-      <c r="I100" s="3">
+      <c r="I102" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 78 "Capitán América: el primer vengador"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBF3811-A5D3-4A61-BE88-6C2461C9EEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24619E5D-26E1-405B-A6B4-4FFF8E125391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="4710" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5715" yWindow="5055" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -522,7 +522,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
   <si>
     <t>Película</t>
   </si>
@@ -1053,6 +1053,9 @@
   </si>
   <si>
     <t>Mamá o papá</t>
+  </si>
+  <si>
+    <t>Capitán América: el primer vengador</t>
   </si>
 </sst>
 </file>
@@ -1405,10 +1408,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I102" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I102" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I102">
-    <sortCondition descending="1" ref="C2:C102"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I103" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I103" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I103">
+    <sortCondition descending="1" ref="C2:C103"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3919,10 +3922,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K102"/>
+  <dimension ref="B2:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5076,7 +5079,7 @@
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="2" t="s">
         <v>175</v>
       </c>
       <c r="C44" s="5">
@@ -5563,17 +5566,17 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>7.05</v>
+        <v>7.0749999999999993</v>
       </c>
       <c r="D62" s="1">
         <v>8</v>
       </c>
       <c r="E62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
         <v>7</v>
@@ -5582,42 +5585,42 @@
         <v>8</v>
       </c>
       <c r="H62" s="3">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="I62" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>6.9375</v>
+        <v>7.05</v>
       </c>
       <c r="D63" s="1">
         <v>8</v>
       </c>
       <c r="E63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F63" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G63" s="1">
         <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I63" s="3">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
@@ -5627,7 +5630,7 @@
         <v>8</v>
       </c>
       <c r="E64" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F64" s="1">
         <v>8</v>
@@ -5636,214 +5639,214 @@
         <v>8</v>
       </c>
       <c r="H64" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I64" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D65" s="1">
         <v>8</v>
       </c>
       <c r="E65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F65" s="1">
         <v>8</v>
       </c>
       <c r="G65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H65" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="I65" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D66" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F66" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G66" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H66" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I66" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D67" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E67" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F67" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G67" s="1">
         <v>8</v>
       </c>
       <c r="H67" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I67" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G68" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H68" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I68" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.6999999999999993</v>
+        <v>6.85</v>
       </c>
       <c r="D69" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
         <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G69" s="1">
         <v>7</v>
       </c>
       <c r="H69" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I69" s="3">
-        <v>7.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D70" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E70" s="1">
         <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G70" s="1">
         <v>7</v>
       </c>
       <c r="H70" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I70" s="3">
-        <v>5.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H71" s="3">
         <v>6.3</v>
       </c>
       <c r="I71" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D72" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" s="1">
         <v>7</v>
@@ -5852,69 +5855,69 @@
         <v>6</v>
       </c>
       <c r="H72" s="3">
-        <v>6.8</v>
+        <v>6.3</v>
       </c>
       <c r="I72" s="3">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.3125</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D73" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1">
         <v>6</v>
       </c>
       <c r="F73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G73" s="1">
         <v>6</v>
       </c>
       <c r="H73" s="3">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="I73" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E74" s="1">
         <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H74" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I74" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
@@ -5924,142 +5927,142 @@
         <v>6</v>
       </c>
       <c r="E75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H75" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I75" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G76" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H76" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I76" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" s="1">
         <v>8</v>
       </c>
       <c r="G77" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H77" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I77" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F78" s="1">
         <v>8</v>
       </c>
       <c r="G78" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H78" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I78" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D79" s="1">
         <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G79" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H79" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I79" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D80" s="1">
         <v>7</v>
       </c>
       <c r="E80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F80" s="1">
         <v>7</v>
@@ -6068,166 +6071,166 @@
         <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I80" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E81" s="1">
         <v>6</v>
       </c>
       <c r="F81" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G81" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H81" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I81" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D82" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H82" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I82" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D83" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
         <v>6</v>
       </c>
       <c r="H83" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I83" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D84" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E84" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F84" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G84" s="1">
         <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I84" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1">
+        <v>3</v>
+      </c>
+      <c r="F85" s="1">
         <v>5</v>
       </c>
-      <c r="F85" s="1">
-        <v>6</v>
-      </c>
       <c r="G85" s="1">
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I85" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D86" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F86" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G86" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H86" s="3">
         <v>5.8</v>
@@ -6238,433 +6241,460 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D87" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E87" s="1">
         <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H87" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I87" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>5.1124999999999998</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D88" s="1">
         <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I88" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F89" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G89" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I89" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D90" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E90" s="1">
         <v>3</v>
       </c>
       <c r="F90" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G90" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H90" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I90" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D91" s="1">
+        <v>6</v>
+      </c>
+      <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1">
         <v>5</v>
       </c>
-      <c r="E91" s="1">
-        <v>5</v>
-      </c>
-      <c r="F91" s="1">
-        <v>3</v>
-      </c>
       <c r="G91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I91" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D92" s="1">
         <v>5</v>
       </c>
       <c r="E92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G92" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H92" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I92" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I92" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D93" s="1">
         <v>5</v>
       </c>
       <c r="E93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G93" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H93" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I93" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D94" s="1">
         <v>5</v>
       </c>
       <c r="E94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1">
         <v>5</v>
       </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H94" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I94" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D95" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1">
         <v>4</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
         <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I95" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D96" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E96" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F96" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I96" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D97" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E97" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F97" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G97" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H97" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I97" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D98" s="1">
+        <v>5</v>
+      </c>
+      <c r="E98" s="1">
         <v>3</v>
       </c>
-      <c r="E98" s="1">
-        <v>4</v>
-      </c>
       <c r="F98" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G98" s="1">
         <v>4</v>
       </c>
       <c r="H98" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I98" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D99" s="1">
+        <v>3</v>
+      </c>
+      <c r="E99" s="1">
         <v>4</v>
       </c>
-      <c r="E99" s="1">
-        <v>2</v>
-      </c>
       <c r="F99" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G99" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H99" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I99" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D100" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E100" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F100" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I100" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>2.9124999999999996</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D101" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F101" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G101" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I101" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F102" s="1">
         <v>0</v>
       </c>
       <c r="G102" s="1">
+        <v>1</v>
+      </c>
+      <c r="H102" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I102" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C103" s="5">
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D103" s="1">
         <v>0</v>
       </c>
-      <c r="H102" s="3">
+      <c r="E103" s="1">
+        <v>0</v>
+      </c>
+      <c r="F103" s="1">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0</v>
+      </c>
+      <c r="H103" s="3">
         <v>7.6</v>
       </c>
-      <c r="I102" s="3">
+      <c r="I103" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 79 "The Gentleman"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24619E5D-26E1-405B-A6B4-4FFF8E125391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8945D2DB-AF55-4097-938E-B9006B7F9A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5715" yWindow="5055" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -45,6 +45,7 @@
     <author>tc={496D87B0-3602-4EB1-A1C5-F64705C70B5D}</author>
     <author>tc={26FE7985-915B-4289-94F0-5860019BF56A}</author>
     <author>tc={3683BF2F-E1C6-4C4E-9996-83C1478A99F6}</author>
+    <author>tc={407FABE6-5267-4AAF-9F2A-B5863409AB12}</author>
     <author>tc={C8511A46-7B58-42AB-8C3C-2EFE3DE84018}</author>
     <author>tc={AA204F5A-5DAA-4465-A50C-898D09DAFD15}</author>
     <author>tc={2E945918-DD73-456D-BDDD-CC865E675D1A}</author>
@@ -135,7 +136,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B9" authorId="6" shapeId="0" xr:uid="{C8511A46-7B58-42AB-8C3C-2EFE3DE84018}">
+    <comment ref="B9" authorId="6" shapeId="0" xr:uid="{407FABE6-5267-4AAF-9F2A-B5863409AB12}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -143,7 +144,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B10" authorId="7" shapeId="0" xr:uid="{AA204F5A-5DAA-4465-A50C-898D09DAFD15}">
+    <comment ref="B10" authorId="7" shapeId="0" xr:uid="{C8511A46-7B58-42AB-8C3C-2EFE3DE84018}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -151,7 +152,15 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B11" authorId="8" shapeId="0" xr:uid="{2E945918-DD73-456D-BDDD-CC865E675D1A}">
+    <comment ref="B11" authorId="8" shapeId="0" xr:uid="{AA204F5A-5DAA-4465-A50C-898D09DAFD15}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    1 temporada</t>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="9" shapeId="0" xr:uid="{2E945918-DD73-456D-BDDD-CC865E675D1A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -159,7 +168,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B12" authorId="9" shapeId="0" xr:uid="{C13EA9AF-3198-4E5B-8448-9249F961D0EF}">
+    <comment ref="B13" authorId="10" shapeId="0" xr:uid="{C13EA9AF-3198-4E5B-8448-9249F961D0EF}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -167,7 +176,7 @@
     8 temporadas</t>
       </text>
     </comment>
-    <comment ref="B13" authorId="10" shapeId="0" xr:uid="{881D7872-46EB-4733-BFC5-0312B38EBAB5}">
+    <comment ref="B14" authorId="11" shapeId="0" xr:uid="{881D7872-46EB-4733-BFC5-0312B38EBAB5}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -175,7 +184,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B14" authorId="11" shapeId="0" xr:uid="{BF2DB552-17AA-4BD2-BF9A-A99B472BF7ED}">
+    <comment ref="B15" authorId="12" shapeId="0" xr:uid="{BF2DB552-17AA-4BD2-BF9A-A99B472BF7ED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -183,7 +192,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B15" authorId="12" shapeId="0" xr:uid="{BC451F18-8F5A-406D-8BBC-03C0BFA2AAEA}">
+    <comment ref="B16" authorId="13" shapeId="0" xr:uid="{BC451F18-8F5A-406D-8BBC-03C0BFA2AAEA}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -191,7 +200,7 @@
     5 temporadas</t>
       </text>
     </comment>
-    <comment ref="B18" authorId="13" shapeId="0" xr:uid="{00485B95-C329-4B85-9804-A48D96CD4982}">
+    <comment ref="B19" authorId="14" shapeId="0" xr:uid="{00485B95-C329-4B85-9804-A48D96CD4982}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -199,7 +208,7 @@
     9 temporadas</t>
       </text>
     </comment>
-    <comment ref="B19" authorId="14" shapeId="0" xr:uid="{E767B4D9-B138-43E0-903B-85823960EFBB}">
+    <comment ref="B20" authorId="15" shapeId="0" xr:uid="{E767B4D9-B138-43E0-903B-85823960EFBB}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -207,7 +216,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B20" authorId="15" shapeId="0" xr:uid="{8A943824-8E5D-48CD-A77C-A2B35F5980A3}">
+    <comment ref="B21" authorId="16" shapeId="0" xr:uid="{8A943824-8E5D-48CD-A77C-A2B35F5980A3}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -215,7 +224,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="16" shapeId="0" xr:uid="{905D74EB-1C41-4120-8733-E9C8C2FF351A}">
+    <comment ref="B22" authorId="17" shapeId="0" xr:uid="{905D74EB-1C41-4120-8733-E9C8C2FF351A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -223,7 +232,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B22" authorId="17" shapeId="0" xr:uid="{B4E0A9EE-3277-494F-88A8-61F8EE265DDE}">
+    <comment ref="B23" authorId="18" shapeId="0" xr:uid="{B4E0A9EE-3277-494F-88A8-61F8EE265DDE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -231,7 +240,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B23" authorId="18" shapeId="0" xr:uid="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
+    <comment ref="B24" authorId="19" shapeId="0" xr:uid="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -239,7 +248,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B24" authorId="19" shapeId="0" xr:uid="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
+    <comment ref="B25" authorId="20" shapeId="0" xr:uid="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -247,7 +256,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B25" authorId="20" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+    <comment ref="B26" authorId="21" shapeId="0" xr:uid="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -255,7 +264,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B28" authorId="21" shapeId="0" xr:uid="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
+    <comment ref="B29" authorId="22" shapeId="0" xr:uid="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -263,7 +272,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B29" authorId="22" shapeId="0" xr:uid="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
+    <comment ref="B30" authorId="23" shapeId="0" xr:uid="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -271,7 +280,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B30" authorId="23" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -279,7 +288,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B31" authorId="24" shapeId="0" xr:uid="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
+    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -287,7 +296,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B32" authorId="25" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -295,7 +304,7 @@
     10 temporadas</t>
       </text>
     </comment>
-    <comment ref="B33" authorId="26" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+    <comment ref="B34" authorId="27" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -303,7 +312,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B34" authorId="27" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+    <comment ref="B35" authorId="28" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -311,7 +320,7 @@
     5 temporadas</t>
       </text>
     </comment>
-    <comment ref="B36" authorId="28" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+    <comment ref="B37" authorId="29" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -319,7 +328,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="29" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+    <comment ref="B38" authorId="30" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -327,7 +336,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B39" authorId="30" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+    <comment ref="B40" authorId="31" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -335,7 +344,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B40" authorId="31" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+    <comment ref="B41" authorId="32" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -343,7 +352,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B41" authorId="32" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+    <comment ref="B42" authorId="33" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -351,7 +360,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="33" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+    <comment ref="B43" authorId="34" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -359,7 +368,7 @@
     14 temporadas</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="34" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+    <comment ref="B45" authorId="35" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -367,7 +376,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B45" authorId="35" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+    <comment ref="B46" authorId="36" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -375,7 +384,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B48" authorId="36" shapeId="0" xr:uid="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
+    <comment ref="B49" authorId="37" shapeId="0" xr:uid="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -383,7 +392,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B49" authorId="37" shapeId="0" xr:uid="{96839C2B-31B6-4DC0-88B7-37E650032258}">
+    <comment ref="B50" authorId="38" shapeId="0" xr:uid="{96839C2B-31B6-4DC0-88B7-37E650032258}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -391,7 +400,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B50" authorId="38" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+    <comment ref="B51" authorId="39" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -399,7 +408,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B51" authorId="39" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+    <comment ref="B52" authorId="40" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -407,7 +416,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B52" authorId="40" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+    <comment ref="B53" authorId="41" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -415,7 +424,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B58" authorId="41" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+    <comment ref="B59" authorId="42" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -423,7 +432,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B59" authorId="42" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+    <comment ref="B60" authorId="43" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -431,7 +440,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B60" authorId="43" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+    <comment ref="B61" authorId="44" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -439,7 +448,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B61" authorId="44" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <comment ref="B62" authorId="45" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -447,7 +456,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B62" authorId="45" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+    <comment ref="B63" authorId="46" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -522,7 +531,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="179">
   <si>
     <t>Película</t>
   </si>
@@ -1056,6 +1065,9 @@
   </si>
   <si>
     <t>Capitán América: el primer vengador</t>
+  </si>
+  <si>
+    <t>The Gentlemen</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1077,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1101,6 +1113,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1144,7 +1162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1167,9 +1185,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1382,10 +1397,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M62" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B2:M62" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M62">
-    <sortCondition descending="1" ref="C2:C62"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M63" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:M63" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M63">
+    <sortCondition descending="1" ref="C2:C63"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="21"/>
@@ -1710,124 +1725,127 @@
   <threadedComment ref="B8" dT="2024-07-08T19:02:24.70" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3683BF2F-E1C6-4C4E-9996-83C1478A99F6}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B9" dT="2024-07-08T19:01:35.63" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C8511A46-7B58-42AB-8C3C-2EFE3DE84018}">
+  <threadedComment ref="B9" dT="2025-09-29T15:07:42.51" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{407FABE6-5267-4AAF-9F2A-B5863409AB12}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B10" dT="2024-07-18T18:33:23.80" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AA204F5A-5DAA-4465-A50C-898D09DAFD15}">
+  <threadedComment ref="B10" dT="2024-07-08T19:01:35.63" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C8511A46-7B58-42AB-8C3C-2EFE3DE84018}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B11" dT="2024-07-08T19:06:15.06" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{2E945918-DD73-456D-BDDD-CC865E675D1A}">
+  <threadedComment ref="B11" dT="2024-07-18T18:33:23.80" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AA204F5A-5DAA-4465-A50C-898D09DAFD15}">
+    <text>1 temporada</text>
+  </threadedComment>
+  <threadedComment ref="B12" dT="2024-07-08T19:06:15.06" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{2E945918-DD73-456D-BDDD-CC865E675D1A}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B12" dT="2024-07-08T19:05:46.15" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C13EA9AF-3198-4E5B-8448-9249F961D0EF}">
+  <threadedComment ref="B13" dT="2024-07-08T19:05:46.15" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C13EA9AF-3198-4E5B-8448-9249F961D0EF}">
     <text>8 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B13" dT="2024-07-08T19:00:39.41" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{881D7872-46EB-4733-BFC5-0312B38EBAB5}">
+  <threadedComment ref="B14" dT="2024-07-08T19:00:39.41" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{881D7872-46EB-4733-BFC5-0312B38EBAB5}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B14" dT="2025-03-06T21:44:17.70" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BF2DB552-17AA-4BD2-BF9A-A99B472BF7ED}">
+  <threadedComment ref="B15" dT="2025-03-06T21:44:17.70" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BF2DB552-17AA-4BD2-BF9A-A99B472BF7ED}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B15" dT="2024-07-08T19:00:57.65" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC451F18-8F5A-406D-8BBC-03C0BFA2AAEA}">
+  <threadedComment ref="B16" dT="2024-07-08T19:00:57.65" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC451F18-8F5A-406D-8BBC-03C0BFA2AAEA}">
     <text>5 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B18" dT="2024-07-08T19:03:36.33" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{00485B95-C329-4B85-9804-A48D96CD4982}">
+  <threadedComment ref="B19" dT="2024-07-08T19:03:36.33" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{00485B95-C329-4B85-9804-A48D96CD4982}">
     <text>9 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B19" dT="2024-07-08T19:01:23.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E767B4D9-B138-43E0-903B-85823960EFBB}">
+  <threadedComment ref="B20" dT="2024-07-08T19:01:23.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E767B4D9-B138-43E0-903B-85823960EFBB}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B20" dT="2024-07-13T10:17:23.07" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8A943824-8E5D-48CD-A77C-A2B35F5980A3}">
+  <threadedComment ref="B21" dT="2024-07-13T10:17:23.07" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8A943824-8E5D-48CD-A77C-A2B35F5980A3}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B21" dT="2024-07-08T19:05:06.84" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{905D74EB-1C41-4120-8733-E9C8C2FF351A}">
+  <threadedComment ref="B22" dT="2024-07-08T19:05:06.84" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{905D74EB-1C41-4120-8733-E9C8C2FF351A}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B22" dT="2025-02-03T22:22:50.97" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B4E0A9EE-3277-494F-88A8-61F8EE265DDE}">
+  <threadedComment ref="B23" dT="2025-02-03T22:22:50.97" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B4E0A9EE-3277-494F-88A8-61F8EE265DDE}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B23" dT="2024-07-08T19:03:23.53" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
+  <threadedComment ref="B24" dT="2024-07-08T19:03:23.53" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{97D38487-0228-4117-9D87-BCCFD4EC6983}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B24" dT="2024-07-08T19:02:11.85" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
+  <threadedComment ref="B25" dT="2024-07-08T19:02:11.85" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BE581C86-E71E-4F40-9F43-00EDE88FB108}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B25" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
+  <threadedComment ref="B26" dT="2024-07-08T19:03:46.50" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{9C26C127-20FF-4258-B62D-B6B902EB0E98}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B28" dT="2024-07-08T19:01:48.87" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
+  <threadedComment ref="B29" dT="2024-07-08T19:01:48.87" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1E35BAB-7C71-4B4F-9EE2-76495541B293}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B29" dT="2025-04-19T09:54:12.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
+  <threadedComment ref="B30" dT="2025-04-19T09:54:12.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C7D97E8C-DE70-4119-AC31-C6C9E2D35A59}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B30" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
+  <threadedComment ref="B31" dT="2024-07-08T19:08:09.20" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{E34E6F01-0047-4D5E-A9F0-76B7D80CE842}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B31" dT="2024-07-08T19:06:42.39" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
+  <threadedComment ref="B32" dT="2024-07-08T19:06:42.39" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B32" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+  <threadedComment ref="B33" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
     <text>10 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B33" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+  <threadedComment ref="B34" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B34" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+  <threadedComment ref="B35" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
     <text>5 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B36" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+  <threadedComment ref="B37" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B37" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+  <threadedComment ref="B38" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B39" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+  <threadedComment ref="B40" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B40" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+  <threadedComment ref="B41" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B41" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+  <threadedComment ref="B42" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B42" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+  <threadedComment ref="B43" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
     <text>14 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B44" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+  <threadedComment ref="B45" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+  <threadedComment ref="B46" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B48" dT="2025-06-14T16:15:11.96" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
+  <threadedComment ref="B49" dT="2025-06-14T16:15:11.96" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B49" dT="2025-07-02T22:08:33.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{96839C2B-31B6-4DC0-88B7-37E650032258}">
+  <threadedComment ref="B50" dT="2025-07-02T22:08:33.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{96839C2B-31B6-4DC0-88B7-37E650032258}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B50" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+  <threadedComment ref="B51" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B51" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+  <threadedComment ref="B52" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B52" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+  <threadedComment ref="B53" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B58" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+  <threadedComment ref="B59" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B59" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+  <threadedComment ref="B60" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B60" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+  <threadedComment ref="B61" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B61" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+  <threadedComment ref="B62" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B62" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+  <threadedComment ref="B63" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
     <text>4 temporadas</text>
   </threadedComment>
 </ThreadedComments>
@@ -1839,10 +1857,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O62"/>
+  <dimension ref="B2:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M62" sqref="M62"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -1940,7 +1958,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -1973,7 +1991,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2009,7 +2027,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2045,7 +2063,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2079,7 +2097,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2109,14 +2127,14 @@
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
-        <v>8.4875000000000007</v>
+        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>9</v>
@@ -2125,15 +2143,15 @@
         <v>9</v>
       </c>
       <c r="G9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H9" s="3">
-        <v>8.1</v>
+        <v>8</v>
       </c>
       <c r="I9" s="3">
-        <v>6.7</v>
-      </c>
-      <c r="J9" s="1" t="e" vm="4">
+        <v>7.1</v>
+      </c>
+      <c r="J9" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="K9" s="1"/>
@@ -2142,11 +2160,11 @@
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
-        <v>8.4</v>
+        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
@@ -2155,37 +2173,37 @@
         <v>9</v>
       </c>
       <c r="F10" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" s="1">
         <v>9</v>
       </c>
       <c r="H10" s="3">
-        <v>8.4</v>
+        <v>8.1</v>
       </c>
       <c r="I10" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="J10" s="1"/>
-      <c r="K10" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.7</v>
+      </c>
+      <c r="J10" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
-        <v>8.3875000000000011</v>
+        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <v>8.4</v>
       </c>
       <c r="D11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1">
         <v>8</v>
@@ -2194,14 +2212,12 @@
         <v>9</v>
       </c>
       <c r="H11" s="3">
-        <v>9.1</v>
+        <v>8.4</v>
       </c>
       <c r="I11" s="3">
-        <v>7.9</v>
-      </c>
-      <c r="J11" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J11" s="1"/>
       <c r="K11" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -2210,97 +2226,99 @@
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
-        <v>8.3625000000000007</v>
+        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
         <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F12" s="1">
         <v>8</v>
       </c>
       <c r="G12" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H12" s="3">
-        <v>9.1999999999999993</v>
+        <v>9.1</v>
       </c>
       <c r="I12" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="J12" s="1"/>
+        <v>7.9</v>
+      </c>
+      <c r="J12" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K12" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="L12" s="1"/>
-      <c r="M12" s="1" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M12" s="1"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
-        <v>8.3624999999999989</v>
+        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
         <v>9</v>
       </c>
       <c r="F13" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="1">
         <v>7</v>
       </c>
       <c r="H13" s="3">
-        <v>8.3000000000000007</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="I13" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="J13" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K13" s="1"/>
+        <v>8.5</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+      <c r="M13" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>137</v>
+        <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
-        <v>8.3125</v>
+        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>9</v>
       </c>
       <c r="F14" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" s="3">
-        <v>8.8000000000000007</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I14" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="J14" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2311,11 +2329,11 @@
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
-        <v>8.2875000000000014</v>
+        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <v>8.3125</v>
       </c>
       <c r="D15" s="1">
         <v>8</v>
@@ -2327,33 +2345,31 @@
         <v>8</v>
       </c>
       <c r="G15" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H15" s="3">
-        <v>8.1999999999999993</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="I15" s="3">
-        <v>6.9</v>
+        <v>7.9</v>
       </c>
       <c r="J15" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K15" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>139</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
-        <v>8.2874999999999996</v>
+        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1">
         <v>9</v>
@@ -2362,34 +2378,36 @@
         <v>8</v>
       </c>
       <c r="G16" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H16" s="3">
-        <v>8.3000000000000007</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I16" s="3">
-        <v>7.7</v>
+        <v>6.9</v>
       </c>
       <c r="J16" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K16" s="1"/>
+      <c r="K16" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>46</v>
+        <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
-        <v>8.1375000000000011</v>
+        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E17" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F17" s="1">
         <v>8</v>
@@ -2398,64 +2416,64 @@
         <v>8</v>
       </c>
       <c r="H17" s="3">
-        <v>8.6999999999999993</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I17" s="3">
         <v>7.7</v>
       </c>
-      <c r="J17" s="1"/>
-      <c r="K17" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="J17" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>136</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
-        <v>8.125</v>
+        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1">
         <v>8</v>
       </c>
       <c r="F18" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="1">
         <v>8</v>
       </c>
       <c r="H18" s="3">
-        <v>8.4</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I18" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="J18" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K18" s="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>70</v>
+        <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
-        <v>8.1</v>
+        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <v>8.125</v>
       </c>
       <c r="D19" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1">
         <v>9</v>
@@ -2464,121 +2482,121 @@
         <v>8</v>
       </c>
       <c r="H19" s="3">
-        <v>7.3</v>
+        <v>8.4</v>
       </c>
       <c r="I19" s="3">
-        <v>6.2</v>
+        <v>7.2</v>
+      </c>
+      <c r="J19" t="e" vm="1">
+        <v>#VALUE!</v>
       </c>
       <c r="K19" s="1"/>
-      <c r="L19" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <v>8.1</v>
       </c>
       <c r="D20" s="1">
         <v>9</v>
       </c>
       <c r="E20" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F20" s="1">
         <v>9</v>
       </c>
       <c r="G20" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H20" s="3">
-        <v>7.4</v>
+        <v>7.3</v>
       </c>
       <c r="I20" s="3">
         <v>6.2</v>
       </c>
-      <c r="J20" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
       <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+      <c r="L20" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
         <v>8</v>
       </c>
       <c r="D21" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E21" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F21" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G21" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H21" s="3">
-        <v>8.4</v>
+        <v>7.4</v>
       </c>
       <c r="I21" s="3">
-        <v>7.2</v>
-      </c>
-      <c r="J21" s="1"/>
-      <c r="K21" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.2</v>
+      </c>
+      <c r="J21" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
         <v>8</v>
       </c>
       <c r="D22" s="1">
         <v>8</v>
       </c>
       <c r="E22" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F22" s="1">
         <v>8</v>
       </c>
       <c r="G22" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H22" s="3">
-        <v>9</v>
+        <v>8.4</v>
       </c>
       <c r="I22" s="3">
-        <v>8</v>
-      </c>
-      <c r="J22" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K22" s="1"/>
+        <v>7.2</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2591,13 +2609,13 @@
         <v>8</v>
       </c>
       <c r="G23" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H23" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I23" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J23" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2608,29 +2626,29 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
-        <v>7.8750000000000009</v>
+        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <v>8</v>
       </c>
       <c r="D24" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1">
         <v>8</v>
       </c>
       <c r="F24" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H24" s="3">
-        <v>7.7</v>
+        <v>8</v>
       </c>
       <c r="I24" s="3">
-        <v>6.6</v>
+        <v>7</v>
       </c>
       <c r="J24" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2641,14 +2659,14 @@
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
-        <v>7.8125000000000009</v>
+        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E25" s="1">
         <v>8</v>
@@ -2660,58 +2678,58 @@
         <v>8</v>
       </c>
       <c r="H25" s="3">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="I25" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="J25" s="1"/>
-      <c r="K25" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.6</v>
+      </c>
+      <c r="J25" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>138</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
-        <v>7.8125</v>
+        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
         <v>8</v>
       </c>
       <c r="E26" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G26" s="1">
         <v>8</v>
       </c>
       <c r="H26" s="3">
-        <v>7.5</v>
+        <v>7.2</v>
       </c>
       <c r="I26" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="J26" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K26" s="1"/>
+        <v>6.1</v>
+      </c>
+      <c r="J26" s="1"/>
+      <c r="K26" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
-        <v>7.7874999999999996</v>
+        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <v>7.8125</v>
       </c>
       <c r="D27" s="1">
         <v>8</v>
@@ -2723,13 +2741,13 @@
         <v>8</v>
       </c>
       <c r="G27" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H27" s="3">
-        <v>8</v>
+        <v>7.5</v>
       </c>
       <c r="I27" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="J27" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2740,11 +2758,11 @@
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
-        <v>7.7250000000000005</v>
+        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
         <v>8</v>
@@ -2756,36 +2774,34 @@
         <v>8</v>
       </c>
       <c r="G28" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H28" s="3">
-        <v>7.2</v>
+        <v>8</v>
       </c>
       <c r="I28" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J28" s="1" t="e" vm="4">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K28" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.3</v>
+      </c>
+      <c r="J28" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>142</v>
+        <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
-        <v>7.6624999999999996</v>
+        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1">
         <v>8</v>
@@ -2794,112 +2810,111 @@
         <v>8</v>
       </c>
       <c r="H29" s="3">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="I29" s="3">
-        <v>6.5</v>
-      </c>
-      <c r="J29" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K29" s="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="J29" s="1" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K29" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>47</v>
+        <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
-        <v>7.6000000000000005</v>
+        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E30" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F30" s="1">
         <v>8</v>
       </c>
       <c r="G30" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H30" s="3">
-        <v>8.6</v>
+        <v>7.4</v>
       </c>
       <c r="I30" s="3">
-        <v>7.6</v>
-      </c>
-      <c r="J30" s="1"/>
-      <c r="K30" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.5</v>
+      </c>
+      <c r="J30" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
-        <v>7.5250000000000004</v>
+        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <v>7.6000000000000005</v>
       </c>
       <c r="D31" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F31" s="1">
         <v>8</v>
       </c>
       <c r="G31" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H31" s="3">
-        <v>8.1</v>
+        <v>8.6</v>
       </c>
       <c r="I31" s="3">
-        <v>7</v>
-      </c>
-      <c r="J31" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.6</v>
+      </c>
+      <c r="J31" s="1"/>
       <c r="K31" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L31" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
-        <v>7.5249999999999995</v>
+        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <v>7.5250000000000004</v>
       </c>
       <c r="D32" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G32" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" s="3">
-        <v>7.9</v>
+        <v>8.1</v>
       </c>
       <c r="I32" s="3">
-        <v>6.4</v>
+        <v>7</v>
       </c>
       <c r="J32" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2907,99 +2922,103 @@
       <c r="K32" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="L32" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
         <v>8</v>
       </c>
       <c r="E33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1">
         <v>7</v>
       </c>
       <c r="G33" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H33" s="3">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="I33" s="3">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="J33" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K33" s="1"/>
+      <c r="K33" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
-        <v>7.4874999999999989</v>
+        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <v>7.5249999999999995</v>
       </c>
       <c r="D34" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F34" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34" s="1">
         <v>7</v>
       </c>
       <c r="H34" s="3">
-        <v>8.3000000000000007</v>
+        <v>7.8</v>
       </c>
       <c r="I34" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="J34" s="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="J34" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K34" s="1"/>
-      <c r="L34" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C62" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
-        <v>7.35</v>
+        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E35" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G35" s="1">
         <v>7</v>
       </c>
       <c r="H35" s="3">
-        <v>8.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I35" s="3">
-        <v>7.8</v>
+        <v>7.3</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -3009,62 +3028,61 @@
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2500000000000009</v>
+        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <v>7.35</v>
       </c>
       <c r="D36" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F36" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G36" s="1">
         <v>7</v>
       </c>
       <c r="H36" s="3">
-        <v>6.7</v>
+        <v>8.5</v>
       </c>
       <c r="I36" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="J36" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.8</v>
+      </c>
+      <c r="J36" s="1"/>
       <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="L36" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
-        <v>7.25</v>
+        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <v>7.2500000000000009</v>
       </c>
       <c r="D37" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E37" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G37" s="1">
         <v>7</v>
       </c>
       <c r="H37" s="3">
-        <v>8.4</v>
+        <v>6.7</v>
       </c>
       <c r="I37" s="3">
-        <v>7.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J37" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3075,129 +3093,129 @@
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <v>7.25</v>
+      </c>
+      <c r="D38" s="1">
+        <v>8</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5</v>
+      </c>
+      <c r="F38" s="1">
+        <v>7</v>
+      </c>
+      <c r="G38" s="1">
+        <v>7</v>
+      </c>
+      <c r="H38" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="I38" s="3">
         <v>7.2</v>
       </c>
-      <c r="D38" s="1">
-        <v>8</v>
-      </c>
-      <c r="E38" s="1">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1">
-        <v>7</v>
-      </c>
-      <c r="G38" s="1">
-        <v>5</v>
-      </c>
-      <c r="H38" s="3">
-        <v>8</v>
-      </c>
-      <c r="I38" s="3">
-        <v>6.6</v>
-      </c>
       <c r="J38" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K38" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K38" s="1"/>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
         <v>7.2</v>
       </c>
       <c r="D39" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F39" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G39" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H39" s="3">
-        <v>8.6</v>
+        <v>8</v>
       </c>
       <c r="I39" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+        <v>6.6</v>
+      </c>
+      <c r="J39" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K39" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1875000000000009</v>
+        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <v>7.2</v>
       </c>
       <c r="D40" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1">
         <v>7</v>
       </c>
       <c r="F40" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G40" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H40" s="3">
-        <v>6.7</v>
+        <v>8.6</v>
       </c>
       <c r="I40" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="J40" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J40" s="1"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="1"/>
-      <c r="M40" s="1"/>
+      <c r="L40" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1875</v>
+        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <v>7.1875000000000009</v>
       </c>
       <c r="D41" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F41" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H41" s="3">
-        <v>9.1</v>
+        <v>6.7</v>
       </c>
       <c r="I41" s="3">
-        <v>8.3000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="J41" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3208,100 +3226,98 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1749999999999998</v>
+        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <v>7.1875</v>
       </c>
       <c r="D42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E42" s="1">
         <v>6</v>
       </c>
       <c r="F42" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G42" s="1">
         <v>7</v>
       </c>
       <c r="H42" s="3">
-        <v>7.5</v>
+        <v>9.1</v>
       </c>
       <c r="I42" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="J42" s="1"/>
-      <c r="K42" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
-      <c r="L42" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J42" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F43" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G43" s="1">
         <v>7</v>
       </c>
       <c r="H43" s="3">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="I43" s="3">
-        <v>7.4</v>
+        <v>5.4</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L43" s="1"/>
-      <c r="M43" s="1"/>
+      <c r="L43" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9750000000000005</v>
+        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <v>7.1749999999999998</v>
       </c>
       <c r="D44" s="1">
         <v>6</v>
       </c>
       <c r="E44" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G44" s="1">
         <v>7</v>
       </c>
       <c r="H44" s="3">
-        <v>7.7</v>
+        <v>8.5</v>
       </c>
       <c r="I44" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J44" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J44" s="1"/>
       <c r="K44" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3310,94 +3326,97 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9</v>
+        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <v>6.9750000000000005</v>
       </c>
       <c r="D45" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F45" s="1">
         <v>7</v>
       </c>
       <c r="G45" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H45" s="3">
-        <v>8</v>
+        <v>7.7</v>
       </c>
       <c r="I45" s="3">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
       <c r="J45" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K45" s="1"/>
+      <c r="K45" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8750000000000009</v>
+        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <v>6.9</v>
       </c>
       <c r="D46" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E46" s="1">
         <v>6</v>
       </c>
       <c r="F46" s="1">
+        <v>7</v>
+      </c>
+      <c r="G46" s="1">
         <v>5</v>
       </c>
-      <c r="G46" s="1">
-        <v>7</v>
-      </c>
       <c r="H46" s="3">
-        <v>8.6999999999999993</v>
+        <v>8</v>
       </c>
       <c r="I46" s="3">
-        <v>8.6</v>
-      </c>
-      <c r="J46" s="1"/>
+        <v>7.2</v>
+      </c>
+      <c r="J46" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K46" s="1"/>
-      <c r="L46" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8</v>
+        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <v>6.8750000000000009</v>
       </c>
       <c r="D47" s="1">
         <v>6</v>
       </c>
       <c r="E47" s="1">
+        <v>6</v>
+      </c>
+      <c r="F47" s="1">
         <v>5</v>
       </c>
-      <c r="F47" s="1">
-        <v>6</v>
-      </c>
       <c r="G47" s="1">
         <v>7</v>
       </c>
       <c r="H47" s="3">
-        <v>8.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I47" s="3">
-        <v>7.4</v>
+        <v>8.6</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -3407,17 +3426,17 @@
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7750000000000004</v>
+        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <v>6.8</v>
       </c>
       <c r="D48" s="1">
         <v>6</v>
       </c>
       <c r="E48" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F48" s="1">
         <v>6</v>
@@ -3426,43 +3445,42 @@
         <v>7</v>
       </c>
       <c r="H48" s="3">
-        <v>7.7</v>
+        <v>8.5</v>
       </c>
       <c r="I48" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="J48" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J48" s="1"/>
       <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
-      <c r="M48" s="1"/>
+      <c r="L48" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
-        <v>6.75</v>
+        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <v>6.7750000000000004</v>
       </c>
       <c r="D49" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F49" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G49" s="1">
         <v>7</v>
       </c>
       <c r="H49" s="3">
-        <v>5.9</v>
+        <v>7.7</v>
       </c>
       <c r="I49" s="3">
-        <v>4.2</v>
+        <v>6.8</v>
       </c>
       <c r="J49" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3473,61 +3491,62 @@
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7250000000000005</v>
+        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <v>6.75</v>
       </c>
       <c r="D50" s="1">
         <v>8</v>
       </c>
       <c r="E50" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F50" s="1">
         <v>7</v>
       </c>
       <c r="G50" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H50" s="3">
-        <v>7.7</v>
+        <v>5.9</v>
       </c>
       <c r="I50" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J50" s="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="J50" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K50" s="1"/>
-      <c r="L50" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7</v>
+        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <v>6.7250000000000005</v>
       </c>
       <c r="D51" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E51" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F51" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G51" s="1">
         <v>6</v>
       </c>
       <c r="H51" s="3">
-        <v>8.6</v>
+        <v>7.7</v>
       </c>
       <c r="I51" s="3">
-        <v>7.4</v>
+        <v>6.4</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3537,79 +3556,76 @@
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
-        <v>6.55</v>
+        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <v>6.7</v>
       </c>
       <c r="D52" s="1">
         <v>5</v>
       </c>
       <c r="E52" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F52" s="1">
         <v>6</v>
       </c>
       <c r="G52" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H52" s="3">
-        <v>7</v>
+        <v>8.6</v>
       </c>
       <c r="I52" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="J52" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J52" s="1"/>
       <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
+      <c r="L52" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
-        <v>6.4875000000000007</v>
+        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <v>6.55</v>
       </c>
       <c r="D53" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E53" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F53" s="1">
         <v>6</v>
       </c>
       <c r="G53" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H53" s="3">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="I53" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="J53" s="1"/>
-      <c r="K53" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+        <v>5.4</v>
+      </c>
+      <c r="J53" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-      <c r="M53" s="1" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M53" s="1"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
-        <v>6.4</v>
+        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <v>6.4875000000000007</v>
       </c>
       <c r="D54" s="1">
         <v>6</v>
@@ -3621,46 +3637,48 @@
         <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H54" s="3">
         <v>8.1</v>
       </c>
       <c r="I54" s="3">
-        <v>6</v>
-      </c>
-      <c r="J54" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K54" s="1"/>
+        <v>7.7</v>
+      </c>
+      <c r="J54" s="1"/>
+      <c r="K54" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
+      <c r="M54" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
-        <v>6.3999999999999995</v>
+        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <v>6.4</v>
       </c>
       <c r="D55" s="1">
         <v>6</v>
       </c>
       <c r="E55" s="1">
+        <v>6</v>
+      </c>
+      <c r="F55" s="1">
+        <v>6</v>
+      </c>
+      <c r="G55" s="1">
         <v>5</v>
       </c>
-      <c r="F55" s="1">
-        <v>6</v>
-      </c>
-      <c r="G55" s="1">
-        <v>6</v>
-      </c>
       <c r="H55" s="3">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="I55" s="3">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="J55" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3671,66 +3689,66 @@
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
-        <v>6.2250000000000005</v>
+        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D56" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E56" s="1">
         <v>5</v>
       </c>
       <c r="F56" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G56" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H56" s="3">
-        <v>8.1999999999999993</v>
+        <v>7.8</v>
       </c>
       <c r="I56" s="3">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="J56" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K56" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1750000000000007</v>
+        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <v>6.2250000000000005</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1">
         <v>5</v>
       </c>
       <c r="F57" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G57" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H57" s="3">
-        <v>6.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I57" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="J57" s="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="J57" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K57" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3739,62 +3757,62 @@
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1624999999999996</v>
+        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <v>6.1750000000000007</v>
       </c>
       <c r="D58" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F58" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G58" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H58" s="3">
-        <v>7.5</v>
+        <v>6.6</v>
       </c>
       <c r="I58" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="J58" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K58" s="1"/>
+        <v>6.2</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L58" s="1"/>
       <c r="M58" s="1"/>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
-        <v>5.9749999999999996</v>
+        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <v>6.1624999999999996</v>
       </c>
       <c r="D59" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E59" s="1">
         <v>7</v>
       </c>
       <c r="F59" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G59" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="I59" s="3">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="J59" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3805,29 +3823,29 @@
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
-        <v>5.7750000000000004</v>
+        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <v>5.9749999999999996</v>
       </c>
       <c r="D60" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E60" s="1">
         <v>7</v>
       </c>
       <c r="F60" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G60" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H60" s="3">
-        <v>6.1</v>
+        <v>7.3</v>
       </c>
       <c r="I60" s="3">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="J60" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3838,11 +3856,11 @@
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
-        <v>5.4625000000000004</v>
+        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <v>5.7750000000000004</v>
       </c>
       <c r="D61" s="1">
         <v>5</v>
@@ -3851,55 +3869,88 @@
         <v>7</v>
       </c>
       <c r="F61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H61" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.1</v>
       </c>
       <c r="I61" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="J61" s="1"/>
+        <v>5</v>
+      </c>
+      <c r="J61" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K61" s="1"/>
-      <c r="L61" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="5">
+        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <v>5.4625000000000004</v>
+      </c>
+      <c r="D62" s="1">
+        <v>5</v>
+      </c>
+      <c r="E62" s="1">
+        <v>7</v>
+      </c>
+      <c r="F62" s="1">
+        <v>6</v>
+      </c>
+      <c r="G62" s="1">
+        <v>7</v>
+      </c>
+      <c r="H62" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I62" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B63" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C62" s="5">
-        <f t="shared" si="1"/>
+      <c r="C63" s="5">
+        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
         <v>4.5874999999999995</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D63" s="1">
         <v>2</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E63" s="1">
         <v>4</v>
       </c>
-      <c r="F62" s="1">
+      <c r="F63" s="1">
         <v>2</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G63" s="1">
         <v>5</v>
       </c>
-      <c r="H62" s="3">
+      <c r="H63" s="3">
         <v>7.7</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I63" s="3">
         <v>6.3</v>
       </c>
-      <c r="J62" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K62" s="1"/>
-      <c r="L62" s="1"/>
-      <c r="M62" s="1"/>
+      <c r="J63" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3908,7 +3959,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="53" orientation="landscape" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -3924,7 +3975,7 @@
   </sheetPr>
   <dimension ref="B2:K103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A65" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
@@ -3974,7 +4025,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4002,7 +4053,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4030,7 +4081,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4057,7 +4108,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4084,7 +4135,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4111,7 +4162,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4138,7 +4189,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4165,7 +4216,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4192,7 +4243,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4219,7 +4270,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4246,7 +4297,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4273,7 +4324,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4300,7 +4351,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4327,7 +4378,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4354,7 +4405,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4381,7 +4432,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4408,7 +4459,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4435,7 +4486,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4462,7 +4513,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4489,7 +4540,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4516,7 +4567,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4543,7 +4594,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4570,7 +4621,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4597,7 +4648,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4624,7 +4675,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4651,7 +4702,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
@@ -4678,7 +4729,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
@@ -4705,7 +4756,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D30" s="1">
@@ -4732,7 +4783,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4759,7 +4810,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.6875</v>
       </c>
       <c r="D32" s="1">
@@ -4786,7 +4837,7 @@
         <v>123</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -4813,7 +4864,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
@@ -4840,7 +4891,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
@@ -4867,7 +4918,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5625</v>
       </c>
       <c r="D36" s="1">
@@ -4894,7 +4945,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
@@ -4921,7 +4972,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -4948,7 +4999,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -4975,7 +5026,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
@@ -5002,7 +5053,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
@@ -5029,7 +5080,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.4249999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -5056,7 +5107,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.4124999999999996</v>
       </c>
       <c r="D43" s="1">
@@ -5083,7 +5134,7 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
@@ -5110,7 +5161,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -5137,7 +5188,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
@@ -5164,7 +5215,7 @@
         <v>111</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D47" s="1">
@@ -5191,7 +5242,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -5218,7 +5269,7 @@
         <v>147</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>7.2374999999999998</v>
       </c>
       <c r="D49" s="1">
@@ -5245,7 +5296,7 @@
         <v>59</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>7.2250000000000005</v>
       </c>
       <c r="D50" s="1">
@@ -5272,7 +5323,7 @@
         <v>65</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>7.2125000000000004</v>
       </c>
       <c r="D51" s="1">
@@ -5299,7 +5350,7 @@
         <v>146</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>7.2124999999999995</v>
       </c>
       <c r="D52" s="1">
@@ -5326,7 +5377,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>7.1499999999999995</v>
       </c>
       <c r="D53" s="1">
@@ -5353,7 +5404,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>7.1375000000000011</v>
       </c>
       <c r="D54" s="1">
@@ -5380,7 +5431,7 @@
         <v>40</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>7.1250000000000009</v>
       </c>
       <c r="D55" s="1">
@@ -5407,7 +5458,7 @@
         <v>39</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>7.125</v>
       </c>
       <c r="D56" s="1">
@@ -5434,7 +5485,7 @@
         <v>133</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>7.0875000000000004</v>
       </c>
       <c r="D57" s="1">
@@ -5461,7 +5512,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D58" s="1">
@@ -5488,7 +5539,7 @@
         <v>171</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
@@ -5515,7 +5566,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D60" s="1">
@@ -5542,7 +5593,7 @@
         <v>143</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
@@ -5565,11 +5616,11 @@
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="2" t="s">
         <v>177</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>7.0749999999999993</v>
       </c>
       <c r="D62" s="1">
@@ -5596,7 +5647,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>7.05</v>
       </c>
       <c r="D63" s="1">
@@ -5623,7 +5674,7 @@
         <v>95</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>6.9375</v>
       </c>
       <c r="D64" s="1">
@@ -5650,7 +5701,7 @@
         <v>87</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>6.9375</v>
       </c>
       <c r="D65" s="1">
@@ -5677,7 +5728,7 @@
         <v>164</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>6.9124999999999996</v>
       </c>
       <c r="D66" s="1">
@@ -5704,7 +5755,7 @@
         <v>157</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -5731,7 +5782,7 @@
         <v>88</v>
       </c>
       <c r="C68" s="5">
-        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D68" s="1">
@@ -5758,7 +5809,7 @@
         <v>119</v>
       </c>
       <c r="C69" s="5">
-        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
+        <f t="shared" si="2"/>
         <v>6.85</v>
       </c>
       <c r="D69" s="1">
@@ -5785,7 +5836,7 @@
         <v>57</v>
       </c>
       <c r="C70" s="5">
-        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
+        <f t="shared" si="2"/>
         <v>6.6999999999999993</v>
       </c>
       <c r="D70" s="1">
@@ -5812,7 +5863,7 @@
         <v>41</v>
       </c>
       <c r="C71" s="5">
-        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
+        <f t="shared" si="2"/>
         <v>6.6124999999999989</v>
       </c>
       <c r="D71" s="1">
@@ -5839,7 +5890,7 @@
         <v>117</v>
       </c>
       <c r="C72" s="5">
-        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D72" s="1">
@@ -5866,7 +5917,7 @@
         <v>168</v>
       </c>
       <c r="C73" s="5">
-        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
+        <f t="shared" si="2"/>
         <v>6.5499999999999989</v>
       </c>
       <c r="D73" s="1">
@@ -5893,7 +5944,7 @@
         <v>134</v>
       </c>
       <c r="C74" s="5">
-        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <f t="shared" si="2"/>
         <v>6.3125</v>
       </c>
       <c r="D74" s="1">
@@ -5920,7 +5971,7 @@
         <v>144</v>
       </c>
       <c r="C75" s="5">
-        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D75" s="1">
@@ -5947,7 +5998,7 @@
         <v>64</v>
       </c>
       <c r="C76" s="5">
-        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D76" s="1">
@@ -5974,7 +6025,7 @@
         <v>75</v>
       </c>
       <c r="C77" s="5">
-        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <f t="shared" si="2"/>
         <v>6.2125000000000004</v>
       </c>
       <c r="D77" s="1">
@@ -6001,7 +6052,7 @@
         <v>19</v>
       </c>
       <c r="C78" s="5">
-        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <f t="shared" si="2"/>
         <v>6.2124999999999995</v>
       </c>
       <c r="D78" s="1">
@@ -6028,7 +6079,7 @@
         <v>101</v>
       </c>
       <c r="C79" s="5">
-        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <f t="shared" si="2"/>
         <v>6.15</v>
       </c>
       <c r="D79" s="1">
@@ -6055,7 +6106,7 @@
         <v>158</v>
       </c>
       <c r="C80" s="5">
-        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <f t="shared" si="2"/>
         <v>6.0874999999999995</v>
       </c>
       <c r="D80" s="1">
@@ -6082,7 +6133,7 @@
         <v>160</v>
       </c>
       <c r="C81" s="5">
-        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
       <c r="D81" s="1">
@@ -6109,7 +6160,7 @@
         <v>159</v>
       </c>
       <c r="C82" s="5">
-        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <f t="shared" si="2"/>
         <v>5.9499999999999993</v>
       </c>
       <c r="D82" s="1">
@@ -6136,7 +6187,7 @@
         <v>74</v>
       </c>
       <c r="C83" s="5">
-        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <f t="shared" si="2"/>
         <v>5.8125</v>
       </c>
       <c r="D83" s="1">
@@ -6163,7 +6214,7 @@
         <v>113</v>
       </c>
       <c r="C84" s="5">
-        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <f t="shared" si="2"/>
         <v>5.7374999999999989</v>
       </c>
       <c r="D84" s="1">
@@ -6190,7 +6241,7 @@
         <v>26</v>
       </c>
       <c r="C85" s="5">
-        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <f t="shared" si="2"/>
         <v>5.6749999999999998</v>
       </c>
       <c r="D85" s="1">
@@ -6217,7 +6268,7 @@
         <v>149</v>
       </c>
       <c r="C86" s="5">
-        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D86" s="1">
@@ -6244,7 +6295,7 @@
         <v>156</v>
       </c>
       <c r="C87" s="5">
-        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D87" s="1">
@@ -6271,7 +6322,7 @@
         <v>166</v>
       </c>
       <c r="C88" s="5">
-        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <f t="shared" si="2"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D88" s="1">
@@ -6298,7 +6349,7 @@
         <v>145</v>
       </c>
       <c r="C89" s="5">
-        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <f t="shared" si="2"/>
         <v>5.1124999999999998</v>
       </c>
       <c r="D89" s="1">
@@ -6325,7 +6376,7 @@
         <v>21</v>
       </c>
       <c r="C90" s="5">
-        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <f t="shared" si="2"/>
         <v>5.05</v>
       </c>
       <c r="D90" s="1">
@@ -6352,7 +6403,7 @@
         <v>169</v>
       </c>
       <c r="C91" s="5">
-        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <f t="shared" si="2"/>
         <v>4.9874999999999998</v>
       </c>
       <c r="D91" s="1">
@@ -6379,7 +6430,7 @@
         <v>163</v>
       </c>
       <c r="C92" s="5">
-        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <f t="shared" si="2"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="D92" s="1">
@@ -6406,7 +6457,7 @@
         <v>162</v>
       </c>
       <c r="C93" s="5">
-        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <f t="shared" si="2"/>
         <v>4.7875000000000005</v>
       </c>
       <c r="D93" s="1">
@@ -6433,7 +6484,7 @@
         <v>154</v>
       </c>
       <c r="C94" s="5">
-        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <f t="shared" si="2"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="D94" s="1">
@@ -6460,7 +6511,7 @@
         <v>135</v>
       </c>
       <c r="C95" s="5">
-        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <f t="shared" si="2"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D95" s="1">
@@ -6487,7 +6538,7 @@
         <v>161</v>
       </c>
       <c r="C96" s="5">
-        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <f t="shared" si="2"/>
         <v>4.4249999999999998</v>
       </c>
       <c r="D96" s="1">
@@ -6514,7 +6565,7 @@
         <v>114</v>
       </c>
       <c r="C97" s="5">
-        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <f t="shared" si="2"/>
         <v>4.4124999999999996</v>
       </c>
       <c r="D97" s="1">
@@ -6541,7 +6592,7 @@
         <v>150</v>
       </c>
       <c r="C98" s="5">
-        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <f t="shared" si="2"/>
         <v>4.3374999999999995</v>
       </c>
       <c r="D98" s="1">
@@ -6568,7 +6619,7 @@
         <v>173</v>
       </c>
       <c r="C99" s="5">
-        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>4.3125</v>
       </c>
       <c r="D99" s="1">
@@ -6595,7 +6646,7 @@
         <v>167</v>
       </c>
       <c r="C100" s="5">
-        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <f t="shared" si="3"/>
         <v>4.2749999999999995</v>
       </c>
       <c r="D100" s="1">
@@ -6622,7 +6673,7 @@
         <v>68</v>
       </c>
       <c r="C101" s="5">
-        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <f t="shared" si="3"/>
         <v>4.1124999999999998</v>
       </c>
       <c r="D101" s="1">
@@ -6649,7 +6700,7 @@
         <v>155</v>
       </c>
       <c r="C102" s="5">
-        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <f t="shared" si="3"/>
         <v>2.9124999999999996</v>
       </c>
       <c r="D102" s="1">
@@ -6676,7 +6727,7 @@
         <v>174</v>
       </c>
       <c r="C103" s="5">
-        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <f t="shared" si="3"/>
         <v>2.6375000000000002</v>
       </c>
       <c r="D103" s="1">

</xml_diff>

<commit_message>
V. 80 "Expediente Warren: El último rito"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8945D2DB-AF55-4097-938E-B9006B7F9A54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89542707-F88B-4477-9A36-5D79C2A66429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -531,7 +531,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
   <si>
     <t>Película</t>
   </si>
@@ -1068,6 +1068,9 @@
   </si>
   <si>
     <t>The Gentlemen</t>
+  </si>
+  <si>
+    <t>Expediente Warren: El último rito</t>
   </si>
 </sst>
 </file>
@@ -1077,7 +1080,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1113,12 +1116,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1162,7 +1159,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1185,6 +1182,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1423,10 +1423,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I103" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I103" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I103">
-    <sortCondition descending="1" ref="C2:C103"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I104" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I104" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I104">
+    <sortCondition descending="1" ref="C2:C104"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1859,7 +1859,7 @@
   </sheetPr>
   <dimension ref="B2:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1924,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -1958,7 +1958,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -1991,7 +1991,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2027,7 +2027,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2063,7 +2063,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2097,7 +2097,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2130,7 +2130,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2163,7 +2163,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2196,7 +2196,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2229,7 +2229,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2264,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2299,7 +2299,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2332,7 +2332,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2365,7 +2365,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2400,7 +2400,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2433,7 +2433,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2466,7 +2466,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2499,7 +2499,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2530,7 +2530,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2563,7 +2563,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2596,7 +2596,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2629,7 +2629,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2662,7 +2662,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2695,7 +2695,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2728,7 +2728,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2761,7 +2761,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2794,7 +2794,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2829,7 +2829,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -2862,7 +2862,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D31" s="1">
@@ -2895,7 +2895,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D32" s="1">
@@ -2931,7 +2931,7 @@
         <v>105</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -2966,7 +2966,7 @@
         <v>141</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -2999,7 +2999,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -3031,7 +3031,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D36" s="1">
@@ -3063,7 +3063,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D37" s="1">
@@ -3096,7 +3096,7 @@
         <v>115</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D38" s="1">
@@ -3129,7 +3129,7 @@
         <v>29</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D39" s="1">
@@ -3164,7 +3164,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D40" s="1">
@@ -3196,7 +3196,7 @@
         <v>140</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D41" s="1">
@@ -3229,7 +3229,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D42" s="1">
@@ -3262,7 +3262,7 @@
         <v>27</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -3296,7 +3296,7 @@
         <v>49</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -3329,7 +3329,7 @@
         <v>71</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -3364,7 +3364,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D46" s="1">
@@ -3397,7 +3397,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D47" s="1">
@@ -3429,7 +3429,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D48" s="1">
@@ -3461,7 +3461,7 @@
         <v>148</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -3494,7 +3494,7 @@
         <v>153</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D50" s="1">
@@ -3527,7 +3527,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D51" s="1">
@@ -3559,7 +3559,7 @@
         <v>18</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D52" s="1">
@@ -3591,7 +3591,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D53" s="1">
@@ -3624,7 +3624,7 @@
         <v>106</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D54" s="1">
@@ -3659,7 +3659,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D55" s="1">
@@ -3692,7 +3692,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D56" s="1">
@@ -3725,7 +3725,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D57" s="1">
@@ -3760,7 +3760,7 @@
         <v>42</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D58" s="1">
@@ -3793,7 +3793,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D59" s="1">
@@ -3826,7 +3826,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D60" s="1">
@@ -3859,7 +3859,7 @@
         <v>99</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -3892,7 +3892,7 @@
         <v>91</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>5.4625000000000004</v>
       </c>
       <c r="D62" s="1">
@@ -3924,7 +3924,7 @@
         <v>36</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D63" s="1">
@@ -3973,10 +3973,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K103"/>
+  <dimension ref="B2:K104"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4025,7 +4025,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4053,7 +4053,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4081,7 +4081,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4108,7 +4108,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4135,7 +4135,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4162,7 +4162,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4189,7 +4189,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4216,7 +4216,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4243,7 +4243,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4270,7 +4270,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4297,7 +4297,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4324,7 +4324,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4351,7 +4351,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4378,7 +4378,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4405,7 +4405,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4432,7 +4432,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4459,7 +4459,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4486,7 +4486,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4513,7 +4513,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4540,7 +4540,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4567,7 +4567,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4594,7 +4594,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4621,7 +4621,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4648,7 +4648,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4675,7 +4675,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4702,7 +4702,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
@@ -4729,7 +4729,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
@@ -4756,7 +4756,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D30" s="1">
@@ -4783,7 +4783,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4810,7 +4810,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.6875</v>
       </c>
       <c r="D32" s="1">
@@ -4837,7 +4837,7 @@
         <v>123</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -4864,7 +4864,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
@@ -4891,7 +4891,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
@@ -4918,7 +4918,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5625</v>
       </c>
       <c r="D36" s="1">
@@ -4945,7 +4945,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
@@ -4972,7 +4972,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -4999,7 +4999,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5026,7 +5026,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
@@ -5053,7 +5053,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
@@ -5080,7 +5080,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -5107,7 +5107,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D43" s="1">
@@ -5134,7 +5134,7 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
@@ -5161,7 +5161,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -5188,7 +5188,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
@@ -5215,7 +5215,7 @@
         <v>111</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3</v>
       </c>
       <c r="D47" s="1">
@@ -5242,7 +5242,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -5269,7 +5269,7 @@
         <v>147</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.2374999999999998</v>
       </c>
       <c r="D49" s="1">
@@ -5296,7 +5296,7 @@
         <v>59</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2250000000000005</v>
       </c>
       <c r="D50" s="1">
@@ -5323,7 +5323,7 @@
         <v>65</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
         <v>7.2125000000000004</v>
       </c>
       <c r="D51" s="1">
@@ -5350,7 +5350,7 @@
         <v>146</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
         <v>7.2124999999999995</v>
       </c>
       <c r="D52" s="1">
@@ -5377,7 +5377,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="D53" s="1">
@@ -5404,7 +5404,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
         <v>7.1375000000000011</v>
       </c>
       <c r="D54" s="1">
@@ -5431,7 +5431,7 @@
         <v>40</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.1250000000000009</v>
       </c>
       <c r="D55" s="1">
@@ -5458,7 +5458,7 @@
         <v>39</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.125</v>
       </c>
       <c r="D56" s="1">
@@ -5485,7 +5485,7 @@
         <v>133</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.0875000000000004</v>
       </c>
       <c r="D57" s="1">
@@ -5512,7 +5512,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D58" s="1">
@@ -5539,7 +5539,7 @@
         <v>171</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
@@ -5566,7 +5566,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D60" s="1">
@@ -5593,7 +5593,7 @@
         <v>143</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
@@ -5620,7 +5620,7 @@
         <v>177</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0749999999999993</v>
       </c>
       <c r="D62" s="1">
@@ -5647,7 +5647,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.05</v>
       </c>
       <c r="D63" s="1">
@@ -5674,7 +5674,7 @@
         <v>95</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>6.9375</v>
       </c>
       <c r="D64" s="1">
@@ -5701,7 +5701,7 @@
         <v>87</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>6.9375</v>
       </c>
       <c r="D65" s="1">
@@ -5728,7 +5728,7 @@
         <v>164</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D66" s="1">
@@ -5755,7 +5755,7 @@
         <v>157</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -5782,7 +5782,7 @@
         <v>88</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D68" s="1">
@@ -5809,7 +5809,7 @@
         <v>119</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
         <v>6.85</v>
       </c>
       <c r="D69" s="1">
@@ -5836,7 +5836,7 @@
         <v>57</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
         <v>6.6999999999999993</v>
       </c>
       <c r="D70" s="1">
@@ -5863,7 +5863,7 @@
         <v>41</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
         <v>6.6124999999999989</v>
       </c>
       <c r="D71" s="1">
@@ -5890,7 +5890,7 @@
         <v>117</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D72" s="1">
@@ -5913,12 +5913,12 @@
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="2" t="s">
-        <v>168</v>
+      <c r="B73" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5499999999999989</v>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D73" s="1">
         <v>8</v>
@@ -5930,217 +5930,217 @@
         <v>7</v>
       </c>
       <c r="G73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I73" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3125</v>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1">
         <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G74" s="1">
         <v>6</v>
       </c>
       <c r="H74" s="3">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="I74" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2749999999999995</v>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <v>6.3125</v>
       </c>
       <c r="D75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E75" s="1">
         <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H75" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I75" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D76" s="1">
         <v>6</v>
       </c>
       <c r="E76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H76" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I76" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2125000000000004</v>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F77" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G77" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I77" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2124999999999995</v>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D78" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1">
         <v>8</v>
       </c>
       <c r="G78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H78" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I78" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
-        <v>6.15</v>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D79" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
         <v>8</v>
       </c>
       <c r="G79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H79" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I79" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
-        <v>6.0874999999999995</v>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <v>6.15</v>
       </c>
       <c r="D80" s="1">
         <v>7</v>
       </c>
       <c r="E80" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H80" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I80" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
-        <v>6.05</v>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D81" s="1">
         <v>7</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
@@ -6149,166 +6149,166 @@
         <v>7</v>
       </c>
       <c r="H81" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I81" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
-        <v>5.9499999999999993</v>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <v>6.05</v>
       </c>
       <c r="D82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E82" s="1">
         <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H82" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I82" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8125</v>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D83" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G83" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H83" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I83" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
-        <v>5.7374999999999989</v>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <v>5.8125</v>
       </c>
       <c r="D84" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E84" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F84" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G84" s="1">
         <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I84" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
-        <v>5.6749999999999998</v>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D85" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E85" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F85" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G85" s="1">
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I85" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
-        <v>5.5624999999999991</v>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E86" s="1">
+        <v>3</v>
+      </c>
+      <c r="F86" s="1">
         <v>5</v>
       </c>
-      <c r="F86" s="1">
-        <v>6</v>
-      </c>
       <c r="G86" s="1">
         <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I86" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D87" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H87" s="3">
         <v>5.8</v>
@@ -6319,433 +6319,460 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
-        <v>5.4874999999999989</v>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D88" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E88" s="1">
         <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G88" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H88" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I88" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
-        <v>5.1124999999999998</v>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D89" s="1">
         <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
         <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I89" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
-        <v>5.05</v>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D90" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E90" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F90" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G90" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H90" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I90" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
-        <v>4.9874999999999998</v>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <v>5.05</v>
       </c>
       <c r="D91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1">
         <v>3</v>
       </c>
       <c r="F91" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G91" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H91" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I91" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D92" s="1">
+        <v>6</v>
+      </c>
+      <c r="E92" s="1">
+        <v>3</v>
+      </c>
+      <c r="F92" s="1">
         <v>5</v>
       </c>
-      <c r="E92" s="1">
-        <v>5</v>
-      </c>
-      <c r="F92" s="1">
-        <v>3</v>
-      </c>
       <c r="G92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H92" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I92" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
-        <v>4.7875000000000005</v>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D93" s="1">
         <v>5</v>
       </c>
       <c r="E93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F93" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G93" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H93" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I93" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I93" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
-        <v>4.5999999999999996</v>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D94" s="1">
         <v>5</v>
       </c>
       <c r="E94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H94" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I94" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
-        <v>4.5874999999999995</v>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D95" s="1">
         <v>5</v>
       </c>
       <c r="E95" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1">
         <v>5</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H95" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I95" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
-        <v>4.4249999999999998</v>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D96" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E96" s="1">
         <v>4</v>
       </c>
       <c r="F96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G96" s="1">
         <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I96" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
-        <v>4.4124999999999996</v>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D97" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E97" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F97" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I97" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
-        <v>4.3374999999999995</v>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D98" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E98" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F98" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G98" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H98" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I98" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.3125</v>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D99" s="1">
+        <v>5</v>
+      </c>
+      <c r="E99" s="1">
         <v>3</v>
       </c>
-      <c r="E99" s="1">
-        <v>4</v>
-      </c>
       <c r="F99" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G99" s="1">
         <v>4</v>
       </c>
       <c r="H99" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I99" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2749999999999995</v>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>4.3125</v>
       </c>
       <c r="D100" s="1">
+        <v>3</v>
+      </c>
+      <c r="E100" s="1">
         <v>4</v>
       </c>
-      <c r="E100" s="1">
-        <v>2</v>
-      </c>
       <c r="F100" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G100" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H100" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I100" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1124999999999998</v>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D101" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E101" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F101" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I101" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D102" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F102" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G102" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I102" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F103" s="1">
         <v>0</v>
       </c>
       <c r="G103" s="1">
+        <v>1</v>
+      </c>
+      <c r="H103" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I103" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C104" s="5">
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D104" s="1">
         <v>0</v>
       </c>
-      <c r="H103" s="3">
+      <c r="E104" s="1">
+        <v>0</v>
+      </c>
+      <c r="F104" s="1">
+        <v>0</v>
+      </c>
+      <c r="G104" s="1">
+        <v>0</v>
+      </c>
+      <c r="H104" s="3">
         <v>7.6</v>
       </c>
-      <c r="I103" s="3">
+      <c r="I104" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 81 "El refugio atómico"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89542707-F88B-4477-9A36-5D79C2A66429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FFF64F-6B9F-41EC-9930-3758C7E4B973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -84,6 +84,7 @@
     <author>tc={ED84D32D-B87E-494D-BC5A-D963B24A65B4}</author>
     <author>tc={25B82680-662E-4149-A9D4-D7D343B29E09}</author>
     <author>tc={8D955452-5474-4D7F-9EFB-C317CB8E77C7}</author>
+    <author>tc={3955FC3A-5089-4113-A6FF-7CA6DD36C98F}</author>
     <author>tc={C6F778D8-6F01-47AB-B632-8939C5C0B507}</author>
     <author>tc={B1297543-A2F2-4625-BBB2-C2604CA16AED}</author>
   </authors>
@@ -448,7 +449,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B62" authorId="45" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <comment ref="B62" authorId="45" shapeId="0" xr:uid="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -456,7 +457,15 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B63" authorId="46" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+    <comment ref="B63" authorId="46" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    1 temporada</t>
+      </text>
+    </comment>
+    <comment ref="B64" authorId="47" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -531,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="181">
   <si>
     <t>Película</t>
   </si>
@@ -1071,6 +1080,9 @@
   </si>
   <si>
     <t>Expediente Warren: El último rito</t>
+  </si>
+  <si>
+    <t>El refugio atómico</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1092,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1116,6 +1128,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1159,7 +1177,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1182,9 +1200,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1397,10 +1412,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M63" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B2:M63" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M63">
-    <sortCondition descending="1" ref="C2:C63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M64" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:M64" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M64">
+    <sortCondition descending="1" ref="C2:C64"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="21"/>
@@ -1842,10 +1857,13 @@
   <threadedComment ref="B61" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B62" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+  <threadedComment ref="B62" dT="2025-10-07T18:49:36.71" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B63" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+  <threadedComment ref="B63" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <text>1 temporada</text>
+  </threadedComment>
+  <threadedComment ref="B64" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
     <text>4 temporadas</text>
   </threadedComment>
 </ThreadedComments>
@@ -1857,10 +1875,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O63"/>
+  <dimension ref="B2:O64"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,7 +1942,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -1958,7 +1976,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -1991,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2027,7 +2045,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2063,7 +2081,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2097,7 +2115,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2130,7 +2148,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2163,7 +2181,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2196,7 +2214,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2229,7 +2247,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2264,7 +2282,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2299,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2332,7 +2350,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2365,7 +2383,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2400,7 +2418,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2433,7 +2451,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2466,7 +2484,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2499,7 +2517,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2530,7 +2548,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2563,7 +2581,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2596,7 +2614,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2629,7 +2647,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2662,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2695,7 +2713,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2728,7 +2746,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2761,7 +2779,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2794,7 +2812,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2829,7 +2847,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -2862,7 +2880,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="D31" s="1">
@@ -2895,7 +2913,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D32" s="1">
@@ -2931,7 +2949,7 @@
         <v>105</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -2966,7 +2984,7 @@
         <v>141</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
         <v>7.5249999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -2999,7 +3017,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -3031,7 +3049,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
         <v>7.35</v>
       </c>
       <c r="D36" s="1">
@@ -3063,7 +3081,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
         <v>7.2500000000000009</v>
       </c>
       <c r="D37" s="1">
@@ -3096,7 +3114,7 @@
         <v>115</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
         <v>7.25</v>
       </c>
       <c r="D38" s="1">
@@ -3129,7 +3147,7 @@
         <v>29</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
         <v>7.2</v>
       </c>
       <c r="D39" s="1">
@@ -3164,7 +3182,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
         <v>7.2</v>
       </c>
       <c r="D40" s="1">
@@ -3196,7 +3214,7 @@
         <v>140</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
         <v>7.1875000000000009</v>
       </c>
       <c r="D41" s="1">
@@ -3229,7 +3247,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
         <v>7.1875</v>
       </c>
       <c r="D42" s="1">
@@ -3262,7 +3280,7 @@
         <v>27</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -3296,7 +3314,7 @@
         <v>49</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
         <v>7.1749999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -3329,7 +3347,7 @@
         <v>71</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
         <v>6.9750000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -3364,7 +3382,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
         <v>6.9</v>
       </c>
       <c r="D46" s="1">
@@ -3397,7 +3415,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
         <v>6.8750000000000009</v>
       </c>
       <c r="D47" s="1">
@@ -3429,7 +3447,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
         <v>6.8</v>
       </c>
       <c r="D48" s="1">
@@ -3461,7 +3479,7 @@
         <v>148</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
         <v>6.7750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -3494,7 +3512,7 @@
         <v>153</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
         <v>6.75</v>
       </c>
       <c r="D50" s="1">
@@ -3527,7 +3545,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
         <v>6.7250000000000005</v>
       </c>
       <c r="D51" s="1">
@@ -3559,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
         <v>6.7</v>
       </c>
       <c r="D52" s="1">
@@ -3591,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
         <v>6.55</v>
       </c>
       <c r="D53" s="1">
@@ -3624,7 +3642,7 @@
         <v>106</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
         <v>6.4875000000000007</v>
       </c>
       <c r="D54" s="1">
@@ -3659,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
         <v>6.4</v>
       </c>
       <c r="D55" s="1">
@@ -3692,7 +3710,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
         <v>6.3999999999999995</v>
       </c>
       <c r="D56" s="1">
@@ -3725,7 +3743,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
         <v>6.2250000000000005</v>
       </c>
       <c r="D57" s="1">
@@ -3760,7 +3778,7 @@
         <v>42</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
         <v>6.1750000000000007</v>
       </c>
       <c r="D58" s="1">
@@ -3793,7 +3811,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
         <v>6.1624999999999996</v>
       </c>
       <c r="D59" s="1">
@@ -3826,7 +3844,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
         <v>5.9749999999999996</v>
       </c>
       <c r="D60" s="1">
@@ -3859,7 +3877,7 @@
         <v>99</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
         <v>5.7750000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -3889,68 +3907,101 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
-        <v>5.4625000000000004</v>
+        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <v>5.7625000000000002</v>
       </c>
       <c r="D62" s="1">
+        <v>8</v>
+      </c>
+      <c r="E62" s="1">
+        <v>8</v>
+      </c>
+      <c r="F62" s="1">
         <v>5</v>
       </c>
-      <c r="E62" s="1">
-        <v>7</v>
-      </c>
-      <c r="F62" s="1">
-        <v>6</v>
-      </c>
       <c r="G62" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H62" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I62" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I62" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="J62" s="1"/>
+      <c r="J62" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K62" s="1"/>
-      <c r="L62" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" s="5">
+        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <v>5.4625000000000004</v>
+      </c>
+      <c r="D63" s="1">
+        <v>5</v>
+      </c>
+      <c r="E63" s="1">
+        <v>7</v>
+      </c>
+      <c r="F63" s="1">
+        <v>6</v>
+      </c>
+      <c r="G63" s="1">
+        <v>7</v>
+      </c>
+      <c r="H63" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I63" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="5">
-        <f t="shared" si="1"/>
+      <c r="C64" s="5">
+        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
         <v>4.5874999999999995</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D64" s="1">
         <v>2</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E64" s="1">
         <v>4</v>
       </c>
-      <c r="F63" s="1">
+      <c r="F64" s="1">
         <v>2</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G64" s="1">
         <v>5</v>
       </c>
-      <c r="H63" s="3">
+      <c r="H64" s="3">
         <v>7.7</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I64" s="3">
         <v>6.3</v>
       </c>
-      <c r="J63" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
-      <c r="K63" s="1"/>
-      <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
+      <c r="J64" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -3975,7 +4026,7 @@
   </sheetPr>
   <dimension ref="B2:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -4025,7 +4076,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4053,7 +4104,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4081,7 +4132,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4108,7 +4159,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4135,7 +4186,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4162,7 +4213,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4189,7 +4240,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4216,7 +4267,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4243,7 +4294,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4270,7 +4321,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4297,7 +4348,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4324,7 +4375,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4351,7 +4402,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4378,7 +4429,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4405,7 +4456,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4432,7 +4483,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4459,7 +4510,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4486,7 +4537,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4513,7 +4564,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4540,7 +4591,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4567,7 +4618,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4594,7 +4645,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4621,7 +4672,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4648,7 +4699,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4675,7 +4726,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4702,7 +4753,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
@@ -4729,7 +4780,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
@@ -4756,7 +4807,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D30" s="1">
@@ -4783,7 +4834,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4810,7 +4861,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.6875</v>
       </c>
       <c r="D32" s="1">
@@ -4837,7 +4888,7 @@
         <v>123</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -4864,7 +4915,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
@@ -4891,7 +4942,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
@@ -4918,7 +4969,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5625</v>
       </c>
       <c r="D36" s="1">
@@ -4945,7 +4996,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
@@ -4972,7 +5023,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -4999,7 +5050,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5026,7 +5077,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
@@ -5053,7 +5104,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
@@ -5080,7 +5131,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.4249999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -5107,7 +5158,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.4124999999999996</v>
       </c>
       <c r="D43" s="1">
@@ -5134,7 +5185,7 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
@@ -5161,7 +5212,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -5188,7 +5239,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
@@ -5215,7 +5266,7 @@
         <v>111</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D47" s="1">
@@ -5242,7 +5293,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -5269,7 +5320,7 @@
         <v>147</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>7.2374999999999998</v>
       </c>
       <c r="D49" s="1">
@@ -5296,7 +5347,7 @@
         <v>59</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>7.2250000000000005</v>
       </c>
       <c r="D50" s="1">
@@ -5323,7 +5374,7 @@
         <v>65</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>7.2125000000000004</v>
       </c>
       <c r="D51" s="1">
@@ -5350,7 +5401,7 @@
         <v>146</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>7.2124999999999995</v>
       </c>
       <c r="D52" s="1">
@@ -5377,7 +5428,7 @@
         <v>53</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>7.1499999999999995</v>
       </c>
       <c r="D53" s="1">
@@ -5404,7 +5455,7 @@
         <v>104</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>7.1375000000000011</v>
       </c>
       <c r="D54" s="1">
@@ -5431,7 +5482,7 @@
         <v>40</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>7.1250000000000009</v>
       </c>
       <c r="D55" s="1">
@@ -5458,7 +5509,7 @@
         <v>39</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>7.125</v>
       </c>
       <c r="D56" s="1">
@@ -5485,7 +5536,7 @@
         <v>133</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>7.0875000000000004</v>
       </c>
       <c r="D57" s="1">
@@ -5512,7 +5563,7 @@
         <v>98</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D58" s="1">
@@ -5539,7 +5590,7 @@
         <v>171</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
@@ -5566,7 +5617,7 @@
         <v>110</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D60" s="1">
@@ -5593,7 +5644,7 @@
         <v>143</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
@@ -5620,7 +5671,7 @@
         <v>177</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>7.0749999999999993</v>
       </c>
       <c r="D62" s="1">
@@ -5647,7 +5698,7 @@
         <v>176</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>7.05</v>
       </c>
       <c r="D63" s="1">
@@ -5674,7 +5725,7 @@
         <v>95</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>6.9375</v>
       </c>
       <c r="D64" s="1">
@@ -5701,7 +5752,7 @@
         <v>87</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>6.9375</v>
       </c>
       <c r="D65" s="1">
@@ -5728,7 +5779,7 @@
         <v>164</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>6.9124999999999996</v>
       </c>
       <c r="D66" s="1">
@@ -5755,7 +5806,7 @@
         <v>157</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -5782,7 +5833,7 @@
         <v>88</v>
       </c>
       <c r="C68" s="5">
-        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D68" s="1">
@@ -5809,7 +5860,7 @@
         <v>119</v>
       </c>
       <c r="C69" s="5">
-        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
+        <f t="shared" si="2"/>
         <v>6.85</v>
       </c>
       <c r="D69" s="1">
@@ -5836,7 +5887,7 @@
         <v>57</v>
       </c>
       <c r="C70" s="5">
-        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
+        <f t="shared" si="2"/>
         <v>6.6999999999999993</v>
       </c>
       <c r="D70" s="1">
@@ -5863,7 +5914,7 @@
         <v>41</v>
       </c>
       <c r="C71" s="5">
-        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
+        <f t="shared" si="2"/>
         <v>6.6124999999999989</v>
       </c>
       <c r="D71" s="1">
@@ -5890,7 +5941,7 @@
         <v>117</v>
       </c>
       <c r="C72" s="5">
-        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D72" s="1">
@@ -5913,11 +5964,11 @@
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="2" t="s">
         <v>179</v>
       </c>
       <c r="C73" s="5">
-        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D73" s="1">
@@ -5944,7 +5995,7 @@
         <v>168</v>
       </c>
       <c r="C74" s="5">
-        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <f t="shared" si="2"/>
         <v>6.5499999999999989</v>
       </c>
       <c r="D74" s="1">
@@ -5971,7 +6022,7 @@
         <v>134</v>
       </c>
       <c r="C75" s="5">
-        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <f t="shared" si="2"/>
         <v>6.3125</v>
       </c>
       <c r="D75" s="1">
@@ -5998,7 +6049,7 @@
         <v>144</v>
       </c>
       <c r="C76" s="5">
-        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D76" s="1">
@@ -6025,7 +6076,7 @@
         <v>64</v>
       </c>
       <c r="C77" s="5">
-        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D77" s="1">
@@ -6052,7 +6103,7 @@
         <v>75</v>
       </c>
       <c r="C78" s="5">
-        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <f t="shared" si="2"/>
         <v>6.2125000000000004</v>
       </c>
       <c r="D78" s="1">
@@ -6079,7 +6130,7 @@
         <v>19</v>
       </c>
       <c r="C79" s="5">
-        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <f t="shared" si="2"/>
         <v>6.2124999999999995</v>
       </c>
       <c r="D79" s="1">
@@ -6106,7 +6157,7 @@
         <v>101</v>
       </c>
       <c r="C80" s="5">
-        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <f t="shared" si="2"/>
         <v>6.15</v>
       </c>
       <c r="D80" s="1">
@@ -6133,7 +6184,7 @@
         <v>158</v>
       </c>
       <c r="C81" s="5">
-        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <f t="shared" si="2"/>
         <v>6.0874999999999995</v>
       </c>
       <c r="D81" s="1">
@@ -6160,7 +6211,7 @@
         <v>160</v>
       </c>
       <c r="C82" s="5">
-        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
       <c r="D82" s="1">
@@ -6187,7 +6238,7 @@
         <v>159</v>
       </c>
       <c r="C83" s="5">
-        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <f t="shared" si="2"/>
         <v>5.9499999999999993</v>
       </c>
       <c r="D83" s="1">
@@ -6214,7 +6265,7 @@
         <v>74</v>
       </c>
       <c r="C84" s="5">
-        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <f t="shared" si="2"/>
         <v>5.8125</v>
       </c>
       <c r="D84" s="1">
@@ -6241,7 +6292,7 @@
         <v>113</v>
       </c>
       <c r="C85" s="5">
-        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <f t="shared" si="2"/>
         <v>5.7374999999999989</v>
       </c>
       <c r="D85" s="1">
@@ -6268,7 +6319,7 @@
         <v>26</v>
       </c>
       <c r="C86" s="5">
-        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <f t="shared" si="2"/>
         <v>5.6749999999999998</v>
       </c>
       <c r="D86" s="1">
@@ -6295,7 +6346,7 @@
         <v>149</v>
       </c>
       <c r="C87" s="5">
-        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D87" s="1">
@@ -6322,7 +6373,7 @@
         <v>156</v>
       </c>
       <c r="C88" s="5">
-        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D88" s="1">
@@ -6349,7 +6400,7 @@
         <v>166</v>
       </c>
       <c r="C89" s="5">
-        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <f t="shared" si="2"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D89" s="1">
@@ -6376,7 +6427,7 @@
         <v>145</v>
       </c>
       <c r="C90" s="5">
-        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <f t="shared" si="2"/>
         <v>5.1124999999999998</v>
       </c>
       <c r="D90" s="1">
@@ -6403,7 +6454,7 @@
         <v>21</v>
       </c>
       <c r="C91" s="5">
-        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <f t="shared" si="2"/>
         <v>5.05</v>
       </c>
       <c r="D91" s="1">
@@ -6430,7 +6481,7 @@
         <v>169</v>
       </c>
       <c r="C92" s="5">
-        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <f t="shared" si="2"/>
         <v>4.9874999999999998</v>
       </c>
       <c r="D92" s="1">
@@ -6457,7 +6508,7 @@
         <v>163</v>
       </c>
       <c r="C93" s="5">
-        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <f t="shared" si="2"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="D93" s="1">
@@ -6484,7 +6535,7 @@
         <v>162</v>
       </c>
       <c r="C94" s="5">
-        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <f t="shared" si="2"/>
         <v>4.7875000000000005</v>
       </c>
       <c r="D94" s="1">
@@ -6511,7 +6562,7 @@
         <v>154</v>
       </c>
       <c r="C95" s="5">
-        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <f t="shared" si="2"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="D95" s="1">
@@ -6538,7 +6589,7 @@
         <v>135</v>
       </c>
       <c r="C96" s="5">
-        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <f t="shared" si="2"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D96" s="1">
@@ -6565,7 +6616,7 @@
         <v>161</v>
       </c>
       <c r="C97" s="5">
-        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <f t="shared" si="2"/>
         <v>4.4249999999999998</v>
       </c>
       <c r="D97" s="1">
@@ -6592,7 +6643,7 @@
         <v>114</v>
       </c>
       <c r="C98" s="5">
-        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <f t="shared" si="2"/>
         <v>4.4124999999999996</v>
       </c>
       <c r="D98" s="1">
@@ -6619,7 +6670,7 @@
         <v>150</v>
       </c>
       <c r="C99" s="5">
-        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>4.3374999999999995</v>
       </c>
       <c r="D99" s="1">
@@ -6646,7 +6697,7 @@
         <v>173</v>
       </c>
       <c r="C100" s="5">
-        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <f t="shared" si="3"/>
         <v>4.3125</v>
       </c>
       <c r="D100" s="1">
@@ -6673,7 +6724,7 @@
         <v>167</v>
       </c>
       <c r="C101" s="5">
-        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <f t="shared" si="3"/>
         <v>4.2749999999999995</v>
       </c>
       <c r="D101" s="1">
@@ -6700,7 +6751,7 @@
         <v>68</v>
       </c>
       <c r="C102" s="5">
-        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <f t="shared" si="3"/>
         <v>4.1124999999999998</v>
       </c>
       <c r="D102" s="1">
@@ -6727,7 +6778,7 @@
         <v>155</v>
       </c>
       <c r="C103" s="5">
-        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <f t="shared" si="3"/>
         <v>2.9124999999999996</v>
       </c>
       <c r="D103" s="1">
@@ -6754,7 +6805,7 @@
         <v>174</v>
       </c>
       <c r="C104" s="5">
-        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <f t="shared" si="3"/>
         <v>2.6375000000000002</v>
       </c>
       <c r="D104" s="1">

</xml_diff>

<commit_message>
V. 82 "Capitana Marvel"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1FFF64F-6B9F-41EC-9930-3758C7E4B973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4D7BE7-74B3-43BE-9BDA-0C1391B8D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="182">
   <si>
     <t>Película</t>
   </si>
@@ -1083,6 +1083,9 @@
   </si>
   <si>
     <t>El refugio atómico</t>
+  </si>
+  <si>
+    <t>Capitana Marvel</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1095,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1128,12 +1131,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1177,7 +1174,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1200,6 +1197,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1438,10 +1438,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I104" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I104" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I104">
-    <sortCondition descending="1" ref="C2:C104"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I105" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I105" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I105">
+    <sortCondition descending="1" ref="C2:C105"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1877,7 +1877,7 @@
   </sheetPr>
   <dimension ref="B2:O64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
@@ -1942,7 +1942,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -1976,7 +1976,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -2009,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2045,7 +2045,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2081,7 +2081,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2115,7 +2115,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2148,7 +2148,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2181,7 +2181,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2214,7 +2214,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2247,7 +2247,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2282,7 +2282,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2317,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2350,7 +2350,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2383,7 +2383,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2418,7 +2418,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2451,7 +2451,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2484,7 +2484,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2517,7 +2517,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2548,7 +2548,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2581,7 +2581,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2614,7 +2614,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2647,7 +2647,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2680,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2713,7 +2713,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2746,7 +2746,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2779,7 +2779,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2812,7 +2812,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2847,7 +2847,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -2880,7 +2880,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D31" s="1">
@@ -2913,7 +2913,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D32" s="1">
@@ -2949,7 +2949,7 @@
         <v>105</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -2984,7 +2984,7 @@
         <v>141</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -3017,7 +3017,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -3049,7 +3049,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D36" s="1">
@@ -3081,7 +3081,7 @@
         <v>80</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D37" s="1">
@@ -3114,7 +3114,7 @@
         <v>115</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D38" s="1">
@@ -3147,7 +3147,7 @@
         <v>29</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D39" s="1">
@@ -3182,7 +3182,7 @@
         <v>22</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D40" s="1">
@@ -3214,7 +3214,7 @@
         <v>140</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D41" s="1">
@@ -3247,7 +3247,7 @@
         <v>45</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D42" s="1">
@@ -3280,7 +3280,7 @@
         <v>27</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -3314,7 +3314,7 @@
         <v>49</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -3347,7 +3347,7 @@
         <v>71</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -3382,7 +3382,7 @@
         <v>76</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D46" s="1">
@@ -3415,7 +3415,7 @@
         <v>44</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D47" s="1">
@@ -3447,7 +3447,7 @@
         <v>48</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D48" s="1">
@@ -3479,7 +3479,7 @@
         <v>148</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -3512,7 +3512,7 @@
         <v>153</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D50" s="1">
@@ -3545,7 +3545,7 @@
         <v>17</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D51" s="1">
@@ -3577,7 +3577,7 @@
         <v>18</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D52" s="1">
@@ -3609,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D53" s="1">
@@ -3642,7 +3642,7 @@
         <v>106</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D54" s="1">
@@ -3677,7 +3677,7 @@
         <v>30</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D55" s="1">
@@ -3710,7 +3710,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D56" s="1">
@@ -3743,7 +3743,7 @@
         <v>32</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D57" s="1">
@@ -3778,7 +3778,7 @@
         <v>42</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D58" s="1">
@@ -3811,7 +3811,7 @@
         <v>11</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D59" s="1">
@@ -3844,7 +3844,7 @@
         <v>89</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D60" s="1">
@@ -3877,7 +3877,7 @@
         <v>99</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -3910,7 +3910,7 @@
         <v>180</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>5.7625000000000002</v>
       </c>
       <c r="D62" s="1">
@@ -3943,7 +3943,7 @@
         <v>91</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>5.4625000000000004</v>
       </c>
       <c r="D63" s="1">
@@ -3975,7 +3975,7 @@
         <v>36</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D64" s="1">
@@ -4024,10 +4024,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K104"/>
+  <dimension ref="B2:K105"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4076,7 +4076,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4104,7 +4104,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4132,7 +4132,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4159,7 +4159,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4186,7 +4186,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4213,7 +4213,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4240,7 +4240,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4267,7 +4267,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4294,7 +4294,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4321,7 +4321,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4348,7 +4348,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4375,7 +4375,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4402,7 +4402,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4429,7 +4429,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4456,7 +4456,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4483,7 +4483,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4510,7 +4510,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4537,7 +4537,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4564,7 +4564,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4591,7 +4591,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4618,7 +4618,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4645,7 +4645,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4672,7 +4672,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4699,7 +4699,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4726,7 +4726,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4753,7 +4753,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
@@ -4780,7 +4780,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
@@ -4807,7 +4807,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D30" s="1">
@@ -4834,7 +4834,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4861,7 +4861,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.6875</v>
       </c>
       <c r="D32" s="1">
@@ -4888,7 +4888,7 @@
         <v>123</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -4915,7 +4915,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
@@ -4942,7 +4942,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
@@ -4969,7 +4969,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5625</v>
       </c>
       <c r="D36" s="1">
@@ -4996,7 +4996,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
@@ -5023,7 +5023,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -5050,7 +5050,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5077,7 +5077,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
@@ -5104,7 +5104,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
@@ -5131,7 +5131,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -5158,7 +5158,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D43" s="1">
@@ -5185,7 +5185,7 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
@@ -5212,7 +5212,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -5239,7 +5239,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
@@ -5266,7 +5266,7 @@
         <v>111</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3</v>
       </c>
       <c r="D47" s="1">
@@ -5293,7 +5293,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -5316,18 +5316,18 @@
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>147</v>
+      <c r="B49" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2374999999999998</v>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
+        <v>7.2750000000000004</v>
       </c>
       <c r="D49" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E49" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F49" s="1">
         <v>8</v>
@@ -5336,319 +5336,319 @@
         <v>8</v>
       </c>
       <c r="H49" s="3">
-        <v>6</v>
+        <v>6.7</v>
       </c>
       <c r="I49" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2250000000000005</v>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
+        <v>7.2374999999999998</v>
       </c>
       <c r="D50" s="1">
         <v>7</v>
       </c>
       <c r="E50" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F50" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G50" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H50" s="3">
-        <v>8.1</v>
+        <v>6</v>
       </c>
       <c r="I50" s="3">
-        <v>7.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2125000000000004</v>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
+        <v>7.2250000000000005</v>
       </c>
       <c r="D51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E51" s="1">
         <v>7</v>
       </c>
       <c r="F51" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G51" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H51" s="3">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="I51" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2124999999999995</v>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
+        <v>7.2125000000000004</v>
       </c>
       <c r="D52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E52" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F52" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G52" s="1">
         <v>8</v>
       </c>
       <c r="H52" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I52" s="3">
         <v>6.3</v>
-      </c>
-      <c r="I52" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>53</v>
+        <v>146</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1499999999999995</v>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
+        <v>7.2124999999999995</v>
       </c>
       <c r="D53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F53" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G53" s="1">
         <v>8</v>
       </c>
       <c r="H53" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I53" s="3">
-        <v>6.6</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1375000000000011</v>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D54" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G54" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H54" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I54" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1250000000000009</v>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D55" s="1">
         <v>7</v>
       </c>
       <c r="E55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G55" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H55" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I55" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I55" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
-        <v>7.125</v>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G56" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H56" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I56" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0875000000000004</v>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
+        <v>7.125</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57" s="1">
         <v>8</v>
       </c>
       <c r="F57" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1">
         <v>7</v>
       </c>
       <c r="H57" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I57" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0750000000000011</v>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D58" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F58" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H58" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I58" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" s="1">
         <v>8</v>
       </c>
       <c r="G59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H59" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I59" s="3">
         <v>6.2</v>
-      </c>
-      <c r="I59" s="3">
-        <v>5.2</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0750000000000002</v>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1">
         <v>8</v>
       </c>
       <c r="G60" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H60" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="I60" s="3">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1">
         <v>7</v>
@@ -5657,55 +5657,55 @@
         <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H61" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I61" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0749999999999993</v>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D62" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E62" s="1">
         <v>7</v>
       </c>
       <c r="F62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H62" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I62" s="3">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
-        <v>7.05</v>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
+        <v>7.0749999999999993</v>
       </c>
       <c r="D63" s="1">
         <v>8</v>
       </c>
       <c r="E63" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F63" s="1">
         <v>7</v>
@@ -5714,52 +5714,52 @@
         <v>8</v>
       </c>
       <c r="H63" s="3">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="I63" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9375</v>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
+        <v>7.05</v>
       </c>
       <c r="D64" s="1">
         <v>8</v>
       </c>
       <c r="E64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F64" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G64" s="1">
         <v>8</v>
       </c>
       <c r="H64" s="3">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I64" s="3">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>6.9375</v>
       </c>
       <c r="D65" s="1">
         <v>8</v>
       </c>
       <c r="E65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" s="1">
         <v>8</v>
@@ -5768,235 +5768,235 @@
         <v>8</v>
       </c>
       <c r="H65" s="3">
-        <v>5.5</v>
+        <v>6.1</v>
       </c>
       <c r="I65" s="3">
-        <v>4.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>164</v>
+        <v>87</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9124999999999996</v>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
+        <v>6.9375</v>
       </c>
       <c r="D66" s="1">
         <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F66" s="1">
         <v>8</v>
       </c>
       <c r="G66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H66" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
       <c r="I66" s="3">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.8999999999999995</v>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D67" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E67" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F67" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G67" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H67" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I67" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
-        <v>6.8624999999999989</v>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D68" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E68" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F68" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G68" s="1">
         <v>8</v>
       </c>
       <c r="H68" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I68" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
-        <v>6.85</v>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D69" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F69" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G69" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H69" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I69" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
-        <v>6.6999999999999993</v>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
+        <v>6.85</v>
       </c>
       <c r="D70" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E70" s="1">
         <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G70" s="1">
         <v>7</v>
       </c>
       <c r="H70" s="3">
-        <v>7.9</v>
+        <v>7.3</v>
       </c>
       <c r="I70" s="3">
-        <v>7.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
-        <v>6.6124999999999989</v>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D71" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E71" s="1">
         <v>6</v>
       </c>
       <c r="F71" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G71" s="1">
         <v>7</v>
       </c>
       <c r="H71" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I71" s="3">
-        <v>5.3</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5874999999999995</v>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H72" s="3">
         <v>6.3</v>
       </c>
       <c r="I72" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" s="1">
         <v>7</v>
       </c>
       <c r="G73" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H73" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I73" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5499999999999989</v>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D74" s="1">
         <v>8</v>
@@ -6008,217 +6008,217 @@
         <v>7</v>
       </c>
       <c r="G74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H74" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I74" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3125</v>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E75" s="1">
         <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G75" s="1">
         <v>6</v>
       </c>
       <c r="H75" s="3">
-        <v>6.9</v>
+        <v>6.8</v>
       </c>
       <c r="I75" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2749999999999995</v>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
+        <v>6.3125</v>
       </c>
       <c r="D76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1">
         <v>6</v>
       </c>
       <c r="F76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H76" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I76" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D77" s="1">
         <v>6</v>
       </c>
       <c r="E77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H77" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I77" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2125000000000004</v>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F78" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G78" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I78" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2124999999999995</v>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1">
         <v>8</v>
       </c>
       <c r="G79" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H79" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I79" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
-        <v>6.15</v>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F80" s="1">
         <v>8</v>
       </c>
       <c r="G80" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I80" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
-        <v>6.0874999999999995</v>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <v>6.15</v>
       </c>
       <c r="D81" s="1">
         <v>7</v>
       </c>
       <c r="E81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G81" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H81" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I81" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
-        <v>6.05</v>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D82" s="1">
         <v>7</v>
       </c>
       <c r="E82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F82" s="1">
         <v>7</v>
@@ -6227,166 +6227,166 @@
         <v>7</v>
       </c>
       <c r="H82" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I82" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
-        <v>5.9499999999999993</v>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <v>6.05</v>
       </c>
       <c r="D83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E83" s="1">
         <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I83" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8125</v>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D84" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G84" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H84" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I84" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
-        <v>5.7374999999999989</v>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <v>5.8125</v>
       </c>
       <c r="D85" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F85" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G85" s="1">
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I85" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
-        <v>5.6749999999999998</v>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D86" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F86" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G86" s="1">
         <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I86" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
-        <v>5.5624999999999991</v>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D87" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E87" s="1">
+        <v>3</v>
+      </c>
+      <c r="F87" s="1">
         <v>5</v>
       </c>
-      <c r="F87" s="1">
-        <v>6</v>
-      </c>
       <c r="G87" s="1">
         <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I87" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D88" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H88" s="3">
         <v>5.8</v>
@@ -6397,433 +6397,460 @@
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
-        <v>5.4874999999999989</v>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D89" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E89" s="1">
         <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G89" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I89" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>145</v>
+        <v>166</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
-        <v>5.1124999999999998</v>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D90" s="1">
         <v>6</v>
       </c>
       <c r="E90" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F90" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G90" s="1">
         <v>6</v>
       </c>
       <c r="H90" s="3">
-        <v>5.9</v>
+        <v>4.8</v>
       </c>
       <c r="I90" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
-        <v>5.05</v>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F91" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I91" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
-        <v>4.9874999999999998</v>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>5.05</v>
       </c>
       <c r="D92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1">
         <v>3</v>
       </c>
       <c r="F92" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G92" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H92" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I92" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D93" s="1">
+        <v>6</v>
+      </c>
+      <c r="E93" s="1">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1">
         <v>5</v>
       </c>
-      <c r="E93" s="1">
-        <v>5</v>
-      </c>
-      <c r="F93" s="1">
-        <v>3</v>
-      </c>
       <c r="G93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I93" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
-        <v>4.7875000000000005</v>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D94" s="1">
         <v>5</v>
       </c>
       <c r="E94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G94" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H94" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I94" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I94" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
-        <v>4.5999999999999996</v>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D95" s="1">
         <v>5</v>
       </c>
       <c r="E95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H95" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I95" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
-        <v>4.5874999999999995</v>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D96" s="1">
         <v>5</v>
       </c>
       <c r="E96" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F96" s="1">
         <v>5</v>
       </c>
       <c r="G96" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H96" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I96" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
-        <v>4.4249999999999998</v>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D97" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E97" s="1">
         <v>4</v>
       </c>
       <c r="F97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G97" s="1">
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I97" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
-        <v>4.4124999999999996</v>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D98" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E98" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F98" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I98" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.3374999999999995</v>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D99" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E99" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F99" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H99" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I99" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3125</v>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D100" s="1">
+        <v>5</v>
+      </c>
+      <c r="E100" s="1">
         <v>3</v>
       </c>
-      <c r="E100" s="1">
-        <v>4</v>
-      </c>
       <c r="F100" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G100" s="1">
         <v>4</v>
       </c>
       <c r="H100" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I100" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2749999999999995</v>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>4.3125</v>
       </c>
       <c r="D101" s="1">
+        <v>3</v>
+      </c>
+      <c r="E101" s="1">
         <v>4</v>
       </c>
-      <c r="E101" s="1">
-        <v>2</v>
-      </c>
       <c r="F101" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G101" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H101" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I101" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1124999999999998</v>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D102" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E102" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F102" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H102" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I102" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D103" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E103" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F103" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G103" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I103" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C104" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D104" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104" s="1">
         <v>0</v>
       </c>
       <c r="G104" s="1">
+        <v>1</v>
+      </c>
+      <c r="H104" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I104" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C105" s="5">
+        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D105" s="1">
         <v>0</v>
       </c>
-      <c r="H104" s="3">
+      <c r="E105" s="1">
+        <v>0</v>
+      </c>
+      <c r="F105" s="1">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0</v>
+      </c>
+      <c r="H105" s="3">
         <v>7.6</v>
       </c>
-      <c r="I104" s="3">
+      <c r="I105" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 83 "6 en la sombra"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4D7BE7-74B3-43BE-9BDA-0C1391B8D3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF31AF0-EFFC-4A17-9193-3E9B405A3D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="183">
   <si>
     <t>Película</t>
   </si>
@@ -1086,6 +1086,9 @@
   </si>
   <si>
     <t>Capitana Marvel</t>
+  </si>
+  <si>
+    <t>6 en la sombra</t>
   </si>
 </sst>
 </file>
@@ -1438,10 +1441,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I105" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I105" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I105">
-    <sortCondition descending="1" ref="C2:C105"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I106" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I106" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I106">
+    <sortCondition descending="1" ref="C2:C106"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3017,7 +3020,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C64" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -4024,10 +4027,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K105"/>
+  <dimension ref="B2:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5316,7 +5319,7 @@
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="2" t="s">
         <v>181</v>
       </c>
       <c r="C49" s="5">
@@ -6450,27 +6453,27 @@
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="2" t="s">
-        <v>145</v>
+      <c r="B91" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.1124999999999998</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E91" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F91" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H91" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="I91" s="3">
         <v>5.0999999999999996</v>
@@ -6478,379 +6481,406 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E92" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F92" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G92" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H92" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I92" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E93" s="1">
         <v>3</v>
       </c>
       <c r="F93" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G93" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H93" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I93" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D94" s="1">
+        <v>6</v>
+      </c>
+      <c r="E94" s="1">
+        <v>3</v>
+      </c>
+      <c r="F94" s="1">
         <v>5</v>
       </c>
-      <c r="E94" s="1">
-        <v>5</v>
-      </c>
-      <c r="F94" s="1">
-        <v>3</v>
-      </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I94" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D95" s="1">
         <v>5</v>
       </c>
       <c r="E95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G95" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I95" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I95" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D96" s="1">
         <v>5</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H96" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I96" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D97" s="1">
         <v>5</v>
       </c>
       <c r="E97" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F97" s="1">
         <v>5</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H97" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I97" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D98" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E98" s="1">
         <v>4</v>
       </c>
       <c r="F98" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
         <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I98" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D99" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E99" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F99" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I99" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D100" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E100" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F100" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G100" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H100" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I100" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D101" s="1">
+        <v>5</v>
+      </c>
+      <c r="E101" s="1">
         <v>3</v>
       </c>
-      <c r="E101" s="1">
-        <v>4</v>
-      </c>
       <c r="F101" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G101" s="1">
         <v>4</v>
       </c>
       <c r="H101" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I101" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D102" s="1">
+        <v>3</v>
+      </c>
+      <c r="E102" s="1">
         <v>4</v>
       </c>
-      <c r="E102" s="1">
-        <v>2</v>
-      </c>
       <c r="F102" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G102" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H102" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I102" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D103" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E103" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F103" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I103" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>2.9124999999999996</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D104" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E104" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F104" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G104" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I104" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D105" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" s="1">
         <v>0</v>
       </c>
       <c r="G105" s="1">
+        <v>1</v>
+      </c>
+      <c r="H105" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I105" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C106" s="5">
+        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D106" s="1">
         <v>0</v>
       </c>
-      <c r="H105" s="3">
+      <c r="E106" s="1">
+        <v>0</v>
+      </c>
+      <c r="F106" s="1">
+        <v>0</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
+      </c>
+      <c r="H106" s="3">
         <v>7.6</v>
       </c>
-      <c r="I105" s="3">
+      <c r="I106" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 84 "La mujer del camarote 10"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF31AF0-EFFC-4A17-9193-3E9B405A3D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FAF6769-AD9F-4F56-BEAB-06E9F3133965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -540,7 +540,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="184">
   <si>
     <t>Película</t>
   </si>
@@ -1089,6 +1089,9 @@
   </si>
   <si>
     <t>6 en la sombra</t>
+  </si>
+  <si>
+    <t>La mujer del camarote 10</t>
   </si>
 </sst>
 </file>
@@ -1441,10 +1444,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I106" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I106" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I106">
-    <sortCondition descending="1" ref="C2:C106"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I107" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I107" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I107">
+    <sortCondition descending="1" ref="C2:C107"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4027,10 +4030,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K106"/>
+  <dimension ref="B2:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6048,62 +6051,62 @@
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
-        <v>134</v>
+      <c r="B76" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.3125</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1">
         <v>6</v>
       </c>
       <c r="F76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H76" s="3">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="I76" s="3">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
         <v>6</v>
       </c>
       <c r="F77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I77" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
@@ -6113,142 +6116,142 @@
         <v>6</v>
       </c>
       <c r="E78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H78" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I78" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G79" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I79" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E80" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
         <v>8</v>
       </c>
       <c r="G80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H80" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I80" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D81" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
         <v>8</v>
       </c>
       <c r="G81" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H81" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I81" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D82" s="1">
         <v>7</v>
       </c>
       <c r="E82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G82" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H82" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I82" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D83" s="1">
         <v>7</v>
       </c>
       <c r="E83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
         <v>7</v>
@@ -6257,166 +6260,166 @@
         <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I83" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E84" s="1">
         <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G84" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H84" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I84" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>74</v>
+        <v>159</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>5.8125</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D85" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G85" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H85" s="3">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="I85" s="3">
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125</v>
       </c>
       <c r="D86" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E86" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F86" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G86" s="1">
         <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I86" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D87" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E87" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G87" s="1">
         <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I87" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D88" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E88" s="1">
+        <v>3</v>
+      </c>
+      <c r="F88" s="1">
         <v>5</v>
       </c>
-      <c r="F88" s="1">
-        <v>6</v>
-      </c>
       <c r="G88" s="1">
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I88" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D89" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F89" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
         <v>5.8</v>
@@ -6427,80 +6430,80 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D90" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E90" s="1">
         <v>6</v>
       </c>
       <c r="F90" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G90" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H90" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I90" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B91" s="9" t="s">
-        <v>182</v>
+      <c r="B91" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.2875000000000005</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>6.1</v>
+        <v>4.8</v>
       </c>
       <c r="I91" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>5.1124999999999998</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="I92" s="3">
         <v>5.0999999999999996</v>
@@ -6508,379 +6511,406 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E93" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F93" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G93" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I93" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1">
         <v>3</v>
       </c>
       <c r="F94" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G94" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H94" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I94" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D95" s="1">
+        <v>6</v>
+      </c>
+      <c r="E95" s="1">
+        <v>3</v>
+      </c>
+      <c r="F95" s="1">
         <v>5</v>
       </c>
-      <c r="E95" s="1">
-        <v>5</v>
-      </c>
-      <c r="F95" s="1">
-        <v>3</v>
-      </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I95" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D96" s="1">
         <v>5</v>
       </c>
       <c r="E96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G96" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H96" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I96" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I96" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D97" s="1">
         <v>5</v>
       </c>
       <c r="E97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H97" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I97" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D98" s="1">
         <v>5</v>
       </c>
       <c r="E98" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1">
         <v>5</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H98" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I98" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D99" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E99" s="1">
         <v>4</v>
       </c>
       <c r="F99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G99" s="1">
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I99" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D100" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E100" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F100" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I100" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D101" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E101" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F101" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G101" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H101" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I101" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D102" s="1">
+        <v>5</v>
+      </c>
+      <c r="E102" s="1">
         <v>3</v>
       </c>
-      <c r="E102" s="1">
-        <v>4</v>
-      </c>
       <c r="F102" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G102" s="1">
         <v>4</v>
       </c>
       <c r="H102" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I102" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D103" s="1">
+        <v>3</v>
+      </c>
+      <c r="E103" s="1">
         <v>4</v>
       </c>
-      <c r="E103" s="1">
-        <v>2</v>
-      </c>
       <c r="F103" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G103" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H103" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I103" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D104" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E104" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F104" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H104" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I104" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>2.9124999999999996</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D105" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F105" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G105" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I105" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D106" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F106" s="1">
         <v>0</v>
       </c>
       <c r="G106" s="1">
+        <v>1</v>
+      </c>
+      <c r="H106" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I106" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B107" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C107" s="5">
+        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D107" s="1">
         <v>0</v>
       </c>
-      <c r="H106" s="3">
+      <c r="E107" s="1">
+        <v>0</v>
+      </c>
+      <c r="F107" s="1">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="3">
         <v>7.6</v>
       </c>
-      <c r="I106" s="3">
+      <c r="I107" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 87 "Furioza 2"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F929837-89A2-4DA9-82BF-4074998EFD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3A7265-F2F8-4A0D-9899-8B6AFDEF51B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
   <si>
     <t>Película</t>
   </si>
@@ -1107,6 +1107,9 @@
   </si>
   <si>
     <t>Animal</t>
+  </si>
+  <si>
+    <t>Furioza 2</t>
   </si>
 </sst>
 </file>
@@ -1116,7 +1119,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1152,12 +1155,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1201,7 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1224,6 +1221,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1462,10 +1462,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I108" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I108" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I108">
-    <sortCondition descending="1" ref="C2:C108"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I109" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I109" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I109">
+    <sortCondition descending="1" ref="C2:C109"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -1904,7 +1904,7 @@
   </sheetPr>
   <dimension ref="B2:O65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -1969,7 +1969,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -2003,7 +2003,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -2036,7 +2036,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2072,7 +2072,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2108,7 +2108,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2142,7 +2142,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2175,7 +2175,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2208,7 +2208,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2241,7 +2241,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2274,7 +2274,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2309,7 +2309,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2344,7 +2344,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2377,7 +2377,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2410,7 +2410,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2445,7 +2445,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2478,7 +2478,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2511,7 +2511,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2544,7 +2544,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2575,7 +2575,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2608,7 +2608,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2641,7 +2641,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2674,7 +2674,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2707,7 +2707,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2740,7 +2740,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2773,7 +2773,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2806,7 +2806,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2839,7 +2839,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2874,7 +2874,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -2907,7 +2907,7 @@
         <v>47</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D31" s="1">
@@ -2940,7 +2940,7 @@
         <v>15</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D32" s="1">
@@ -2976,7 +2976,7 @@
         <v>105</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -3011,7 +3011,7 @@
         <v>141</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -3044,7 +3044,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -3076,7 +3076,7 @@
         <v>50</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D36" s="1">
@@ -3108,7 +3108,7 @@
         <v>185</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D37" s="1">
@@ -3141,7 +3141,7 @@
         <v>80</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D38" s="1">
@@ -3174,7 +3174,7 @@
         <v>115</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D39" s="1">
@@ -3207,7 +3207,7 @@
         <v>29</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D40" s="1">
@@ -3242,7 +3242,7 @@
         <v>22</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D41" s="1">
@@ -3274,7 +3274,7 @@
         <v>140</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D42" s="1">
@@ -3307,7 +3307,7 @@
         <v>45</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D43" s="1">
@@ -3340,7 +3340,7 @@
         <v>27</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -3374,7 +3374,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D45" s="1">
@@ -3407,7 +3407,7 @@
         <v>71</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D46" s="1">
@@ -3442,7 +3442,7 @@
         <v>76</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D47" s="1">
@@ -3475,7 +3475,7 @@
         <v>44</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D48" s="1">
@@ -3507,7 +3507,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D49" s="1">
@@ -3539,7 +3539,7 @@
         <v>148</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -3572,7 +3572,7 @@
         <v>153</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D51" s="1">
@@ -3605,7 +3605,7 @@
         <v>17</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D52" s="1">
@@ -3637,7 +3637,7 @@
         <v>18</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D53" s="1">
@@ -3669,7 +3669,7 @@
         <v>9</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D54" s="1">
@@ -3702,7 +3702,7 @@
         <v>106</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D55" s="1">
@@ -3737,7 +3737,7 @@
         <v>30</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D56" s="1">
@@ -3770,7 +3770,7 @@
         <v>13</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D57" s="1">
@@ -3803,7 +3803,7 @@
         <v>32</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D58" s="1">
@@ -3838,7 +3838,7 @@
         <v>42</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D59" s="1">
@@ -3871,7 +3871,7 @@
         <v>11</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D60" s="1">
@@ -3904,7 +3904,7 @@
         <v>89</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D61" s="1">
@@ -3937,7 +3937,7 @@
         <v>99</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D62" s="1">
@@ -3970,7 +3970,7 @@
         <v>180</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>5.7625000000000002</v>
       </c>
       <c r="D63" s="1">
@@ -4003,7 +4003,7 @@
         <v>91</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>5.4625000000000004</v>
       </c>
       <c r="D64" s="1">
@@ -4035,7 +4035,7 @@
         <v>36</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,F65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D65" s="1">
@@ -4084,10 +4084,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K108"/>
+  <dimension ref="B2:K109"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C88" sqref="C88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,7 +4136,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4164,7 +4164,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4192,7 +4192,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4219,7 +4219,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4246,7 +4246,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4273,7 +4273,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4300,7 +4300,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4327,7 +4327,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4354,7 +4354,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4381,7 +4381,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4408,7 +4408,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4435,7 +4435,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4462,7 +4462,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4489,7 +4489,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4516,7 +4516,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4543,7 +4543,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4570,7 +4570,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4597,7 +4597,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4624,7 +4624,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4651,7 +4651,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4678,7 +4678,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4705,7 +4705,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4732,7 +4732,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4759,7 +4759,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4786,7 +4786,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4813,7 +4813,7 @@
         <v>60</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D28" s="1">
@@ -4840,7 +4840,7 @@
         <v>38</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D29" s="1">
@@ -4867,7 +4867,7 @@
         <v>63</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D30" s="1">
@@ -4894,7 +4894,7 @@
         <v>94</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4921,7 +4921,7 @@
         <v>97</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.6875</v>
       </c>
       <c r="D32" s="1">
@@ -4948,7 +4948,7 @@
         <v>123</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D33" s="1">
@@ -4975,7 +4975,7 @@
         <v>37</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D34" s="1">
@@ -5002,7 +5002,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D35" s="1">
@@ -5029,7 +5029,7 @@
         <v>62</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5625</v>
       </c>
       <c r="D36" s="1">
@@ -5056,7 +5056,7 @@
         <v>55</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D37" s="1">
@@ -5083,7 +5083,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -5110,7 +5110,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5137,7 +5137,7 @@
         <v>172</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
@@ -5164,7 +5164,7 @@
         <v>130</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
@@ -5191,7 +5191,7 @@
         <v>100</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D42" s="1">
@@ -5218,7 +5218,7 @@
         <v>131</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D43" s="1">
@@ -5245,7 +5245,7 @@
         <v>175</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D44" s="1">
@@ -5272,7 +5272,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D45" s="1">
@@ -5299,7 +5299,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D46" s="1">
@@ -5326,7 +5326,7 @@
         <v>111</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3</v>
       </c>
       <c r="D47" s="1">
@@ -5353,7 +5353,7 @@
         <v>103</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D48" s="1">
@@ -5380,7 +5380,7 @@
         <v>181</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -5407,7 +5407,7 @@
         <v>147</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2374999999999998</v>
       </c>
       <c r="D50" s="1">
@@ -5434,7 +5434,7 @@
         <v>59</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
         <v>7.2250000000000005</v>
       </c>
       <c r="D51" s="1">
@@ -5461,7 +5461,7 @@
         <v>65</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
         <v>7.2125000000000004</v>
       </c>
       <c r="D52" s="1">
@@ -5488,7 +5488,7 @@
         <v>146</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
         <v>7.2124999999999995</v>
       </c>
       <c r="D53" s="1">
@@ -5515,7 +5515,7 @@
         <v>53</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="D54" s="1">
@@ -5542,7 +5542,7 @@
         <v>104</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.1375000000000011</v>
       </c>
       <c r="D55" s="1">
@@ -5569,7 +5569,7 @@
         <v>40</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.1250000000000009</v>
       </c>
       <c r="D56" s="1">
@@ -5596,7 +5596,7 @@
         <v>39</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.125</v>
       </c>
       <c r="D57" s="1">
@@ -5623,7 +5623,7 @@
         <v>133</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.0875000000000004</v>
       </c>
       <c r="D58" s="1">
@@ -5650,7 +5650,7 @@
         <v>98</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D59" s="1">
@@ -5677,7 +5677,7 @@
         <v>171</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D60" s="1">
@@ -5704,7 +5704,7 @@
         <v>110</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D61" s="1">
@@ -5731,7 +5731,7 @@
         <v>143</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D62" s="1">
@@ -5758,7 +5758,7 @@
         <v>177</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.0749999999999993</v>
       </c>
       <c r="D63" s="1">
@@ -5785,7 +5785,7 @@
         <v>176</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>7.05</v>
       </c>
       <c r="D64" s="1">
@@ -5812,7 +5812,7 @@
         <v>95</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>6.9375</v>
       </c>
       <c r="D65" s="1">
@@ -5839,7 +5839,7 @@
         <v>164</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D66" s="1">
@@ -5866,7 +5866,7 @@
         <v>157</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -5893,7 +5893,7 @@
         <v>88</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D68" s="1">
@@ -5920,7 +5920,7 @@
         <v>184</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D69" s="1">
@@ -5947,7 +5947,7 @@
         <v>119</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
         <v>6.85</v>
       </c>
       <c r="D70" s="1">
@@ -5974,7 +5974,7 @@
         <v>57</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
         <v>6.6999999999999993</v>
       </c>
       <c r="D71" s="1">
@@ -6001,7 +6001,7 @@
         <v>87</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
         <v>6.6875</v>
       </c>
       <c r="D72" s="1">
@@ -6028,7 +6028,7 @@
         <v>41</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
         <v>6.6124999999999989</v>
       </c>
       <c r="D73" s="1">
@@ -6055,7 +6055,7 @@
         <v>117</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D74" s="1">
@@ -6082,7 +6082,7 @@
         <v>179</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D75" s="1">
@@ -6109,7 +6109,7 @@
         <v>168</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.5499999999999989</v>
       </c>
       <c r="D76" s="1">
@@ -6136,7 +6136,7 @@
         <v>183</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D77" s="1">
@@ -6163,7 +6163,7 @@
         <v>134</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
         <v>6.3125</v>
       </c>
       <c r="D78" s="1">
@@ -6190,7 +6190,7 @@
         <v>144</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D79" s="1">
@@ -6217,7 +6217,7 @@
         <v>64</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D80" s="1">
@@ -6244,7 +6244,7 @@
         <v>75</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
         <v>6.2125000000000004</v>
       </c>
       <c r="D81" s="1">
@@ -6271,7 +6271,7 @@
         <v>19</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
         <v>6.2124999999999995</v>
       </c>
       <c r="D82" s="1">
@@ -6298,7 +6298,7 @@
         <v>101</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
         <v>6.15</v>
       </c>
       <c r="D83" s="1">
@@ -6325,7 +6325,7 @@
         <v>158</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
         <v>6.0874999999999995</v>
       </c>
       <c r="D84" s="1">
@@ -6352,7 +6352,7 @@
         <v>160</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
         <v>6.05</v>
       </c>
       <c r="D85" s="1">
@@ -6379,7 +6379,7 @@
         <v>159</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
         <v>5.9499999999999993</v>
       </c>
       <c r="D86" s="1">
@@ -6402,132 +6402,132 @@
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="2" t="s">
-        <v>74</v>
+      <c r="B87" s="9" t="s">
+        <v>186</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8125</v>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D87" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E87" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H87" s="3">
-        <v>4.5</v>
+        <v>6.2</v>
       </c>
       <c r="I87" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
-        <v>5.7374999999999989</v>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <v>5.8125</v>
       </c>
       <c r="D88" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E88" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F88" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I88" s="3">
-        <v>5.3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
-        <v>5.6749999999999998</v>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D89" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F89" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G89" s="1">
         <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I89" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
-        <v>5.5624999999999991</v>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D90" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1">
+        <v>3</v>
+      </c>
+      <c r="F90" s="1">
         <v>5</v>
       </c>
-      <c r="F90" s="1">
-        <v>6</v>
-      </c>
       <c r="G90" s="1">
         <v>6</v>
       </c>
       <c r="H90" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I90" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D91" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
         <v>5.8</v>
@@ -6538,80 +6538,80 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
-        <v>5.4874999999999989</v>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D92" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E92" s="1">
         <v>6</v>
       </c>
       <c r="F92" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H92" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I92" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
-        <v>5.2875000000000005</v>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G93" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>6.1</v>
+        <v>4.8</v>
       </c>
       <c r="I93" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
-        <v>5.1124999999999998</v>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="I94" s="3">
         <v>5.0999999999999996</v>
@@ -6619,379 +6619,406 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
-        <v>5.05</v>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E95" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F95" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G95" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I95" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
-        <v>4.9874999999999998</v>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <v>5.05</v>
       </c>
       <c r="D96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E96" s="1">
         <v>3</v>
       </c>
       <c r="F96" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G96" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H96" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I96" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
-        <v>4.8499999999999996</v>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D97" s="1">
+        <v>6</v>
+      </c>
+      <c r="E97" s="1">
+        <v>3</v>
+      </c>
+      <c r="F97" s="1">
         <v>5</v>
       </c>
-      <c r="E97" s="1">
-        <v>5</v>
-      </c>
-      <c r="F97" s="1">
-        <v>3</v>
-      </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I97" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
-        <v>4.7875000000000005</v>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D98" s="1">
         <v>5</v>
       </c>
       <c r="E98" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G98" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H98" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I98" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I98" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.5999999999999996</v>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D99" s="1">
         <v>5</v>
       </c>
       <c r="E99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H99" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I99" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5874999999999995</v>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D100" s="1">
         <v>5</v>
       </c>
       <c r="E100" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
         <v>5</v>
       </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H100" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I100" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4249999999999998</v>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D101" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1">
         <v>4</v>
       </c>
       <c r="F101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G101" s="1">
         <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I101" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4124999999999996</v>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D102" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E102" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F102" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I102" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3374999999999995</v>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D103" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E103" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F103" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G103" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H103" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I103" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C104" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3125</v>
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D104" s="1">
+        <v>5</v>
+      </c>
+      <c r="E104" s="1">
         <v>3</v>
       </c>
-      <c r="E104" s="1">
-        <v>4</v>
-      </c>
       <c r="F104" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G104" s="1">
         <v>4</v>
       </c>
       <c r="H104" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I104" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C105" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2749999999999995</v>
+        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <v>4.3125</v>
       </c>
       <c r="D105" s="1">
+        <v>3</v>
+      </c>
+      <c r="E105" s="1">
         <v>4</v>
       </c>
-      <c r="E105" s="1">
-        <v>2</v>
-      </c>
       <c r="F105" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G105" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H105" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I105" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C106" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1124999999999998</v>
+        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D106" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E106" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F106" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H106" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I106" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C107" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D107" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F107" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G107" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I107" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C108" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" s="1">
         <v>0</v>
       </c>
       <c r="G108" s="1">
+        <v>1</v>
+      </c>
+      <c r="H108" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I108" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B109" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C109" s="5">
+        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D109" s="1">
         <v>0</v>
       </c>
-      <c r="H108" s="3">
+      <c r="E109" s="1">
+        <v>0</v>
+      </c>
+      <c r="F109" s="1">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0</v>
+      </c>
+      <c r="H109" s="3">
         <v>7.6</v>
       </c>
-      <c r="I108" s="3">
+      <c r="I109" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 88 "Una casa llena de dinamita"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3A7265-F2F8-4A0D-9899-8B6AFDEF51B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FD8BE2-72B5-4D20-971C-9F077159DB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="188">
   <si>
     <t>Película</t>
   </si>
@@ -1110,6 +1110,9 @@
   </si>
   <si>
     <t>Furioza 2</t>
+  </si>
+  <si>
+    <t>Una casa llena de dinamita</t>
   </si>
 </sst>
 </file>
@@ -1462,10 +1465,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I109" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I109" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I109">
-    <sortCondition descending="1" ref="C2:C109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I110" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I110" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I110">
+    <sortCondition descending="1" ref="C2:C110"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -3044,7 +3047,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C65" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.4874999999999989</v>
       </c>
       <c r="D35" s="1">
@@ -4084,10 +4087,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K109"/>
+  <dimension ref="B2:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6402,7 +6405,7 @@
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C87" s="5">
@@ -6430,38 +6433,38 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>74</v>
+        <v>113</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>5.8125</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D88" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G88" s="1">
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>4.5</v>
+        <v>6.8</v>
       </c>
       <c r="I88" s="3">
-        <v>3.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>113</v>
+      <c r="B89" s="9" t="s">
+        <v>187</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>5.7374999999999989</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D89" s="1">
         <v>7</v>
@@ -6473,13 +6476,13 @@
         <v>4</v>
       </c>
       <c r="G89" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H89" s="3">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="I89" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
@@ -6619,406 +6622,433 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D95" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E95" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
         <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I95" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E96" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F96" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G96" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I96" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E97" s="1">
         <v>3</v>
       </c>
       <c r="F97" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G97" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H97" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I97" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D98" s="1">
+        <v>6</v>
+      </c>
+      <c r="E98" s="1">
+        <v>3</v>
+      </c>
+      <c r="F98" s="1">
         <v>5</v>
       </c>
-      <c r="E98" s="1">
-        <v>5</v>
-      </c>
-      <c r="F98" s="1">
-        <v>3</v>
-      </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I98" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D99" s="1">
         <v>5</v>
       </c>
       <c r="E99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G99" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H99" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I99" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I99" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D100" s="1">
         <v>5</v>
       </c>
       <c r="E100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H100" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I100" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D101" s="1">
         <v>5</v>
       </c>
       <c r="E101" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F101" s="1">
         <v>5</v>
       </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H101" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I101" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D102" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
         <v>4</v>
       </c>
       <c r="F102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G102" s="1">
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I102" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D103" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E103" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F103" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I103" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D104" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E104" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F104" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G104" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H104" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I104" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D105" s="1">
+        <v>5</v>
+      </c>
+      <c r="E105" s="1">
         <v>3</v>
       </c>
-      <c r="E105" s="1">
-        <v>4</v>
-      </c>
       <c r="F105" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G105" s="1">
         <v>4</v>
       </c>
       <c r="H105" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I105" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D106" s="1">
+        <v>3</v>
+      </c>
+      <c r="E106" s="1">
         <v>4</v>
       </c>
-      <c r="E106" s="1">
-        <v>2</v>
-      </c>
       <c r="F106" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G106" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H106" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I106" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D107" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E107" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F107" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H107" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I107" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>2.9124999999999996</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D108" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F108" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G108" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I108" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D109" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F109" s="1">
         <v>0</v>
       </c>
       <c r="G109" s="1">
+        <v>1</v>
+      </c>
+      <c r="H109" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I109" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B110" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C110" s="5">
+        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D110" s="1">
         <v>0</v>
       </c>
-      <c r="H109" s="3">
+      <c r="E110" s="1">
+        <v>0</v>
+      </c>
+      <c r="F110" s="1">
+        <v>0</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0</v>
+      </c>
+      <c r="H110" s="3">
         <v>7.6</v>
       </c>
-      <c r="I109" s="3">
+      <c r="I110" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 89 "Triple frontera"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87FD8BE2-72B5-4D20-971C-9F077159DB95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEED945B-FD13-49A3-A1E5-10C68EC46783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
   <si>
     <t>Película</t>
   </si>
@@ -1113,6 +1113,9 @@
   </si>
   <si>
     <t>Una casa llena de dinamita</t>
+  </si>
+  <si>
+    <t>Triple frontera</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1468,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I110" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I110" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I110">
-    <sortCondition descending="1" ref="C2:C110"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I111" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I111" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I111">
+    <sortCondition descending="1" ref="C2:C111"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4087,10 +4090,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K110"/>
+  <dimension ref="B2:K111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C110" sqref="C110"/>
+      <selection activeCell="H111" sqref="H111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6162,12 +6165,12 @@
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="2" t="s">
-        <v>134</v>
+      <c r="B78" s="9" t="s">
+        <v>188</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>6.3125</v>
+        <v>6.35</v>
       </c>
       <c r="D78" s="1">
         <v>7</v>
@@ -6176,48 +6179,48 @@
         <v>6</v>
       </c>
       <c r="F78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G78" s="1">
         <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I78" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
         <v>6</v>
       </c>
       <c r="F79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I79" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
@@ -6227,142 +6230,142 @@
         <v>6</v>
       </c>
       <c r="E80" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I80" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I81" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D82" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
         <v>8</v>
       </c>
       <c r="G82" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H82" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I82" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D83" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
         <v>8</v>
       </c>
       <c r="G83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I83" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D84" s="1">
         <v>7</v>
       </c>
       <c r="E84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G84" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H84" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I84" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D85" s="1">
         <v>7</v>
       </c>
       <c r="E85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F85" s="1">
         <v>7</v>
@@ -6371,73 +6374,73 @@
         <v>7</v>
       </c>
       <c r="H85" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I85" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
         <v>6</v>
       </c>
       <c r="F86" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G86" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H86" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I86" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>5.8125000000000009</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
+        <v>6</v>
+      </c>
+      <c r="F87" s="1">
+        <v>8</v>
+      </c>
+      <c r="G87" s="1">
         <v>5</v>
       </c>
-      <c r="F87" s="1">
+      <c r="H87" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="I87" s="3">
         <v>5</v>
-      </c>
-      <c r="G87" s="1">
-        <v>7</v>
-      </c>
-      <c r="H87" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="I87" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D88" s="1">
         <v>7</v>
@@ -6446,25 +6449,25 @@
         <v>5</v>
       </c>
       <c r="F88" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H88" s="3">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="I88" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="9" t="s">
-        <v>187</v>
+      <c r="B89" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D89" s="1">
         <v>7</v>
@@ -6476,37 +6479,37 @@
         <v>4</v>
       </c>
       <c r="G89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I89" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D90" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E90" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F90" s="1">
+        <v>4</v>
+      </c>
+      <c r="G90" s="1">
         <v>5</v>
       </c>
-      <c r="G90" s="1">
-        <v>6</v>
-      </c>
       <c r="H90" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I90" s="3">
         <v>6.4</v>
@@ -6514,50 +6517,50 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D91" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1">
+        <v>3</v>
+      </c>
+      <c r="F91" s="1">
         <v>5</v>
       </c>
-      <c r="F91" s="1">
-        <v>6</v>
-      </c>
       <c r="G91" s="1">
         <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I91" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D92" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H92" s="3">
         <v>5.8</v>
@@ -6568,487 +6571,514 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D93" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E93" s="1">
         <v>6</v>
       </c>
       <c r="F93" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H93" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I93" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>5.2875000000000005</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94" s="3">
-        <v>6.1</v>
+        <v>4.8</v>
       </c>
       <c r="I94" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D95" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1">
         <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I95" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D96" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E96" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
         <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I96" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E97" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F97" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G97" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I97" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D98" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E98" s="1">
         <v>3</v>
       </c>
       <c r="F98" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G98" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H98" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I98" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D99" s="1">
+        <v>6</v>
+      </c>
+      <c r="E99" s="1">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1">
         <v>5</v>
       </c>
-      <c r="E99" s="1">
-        <v>5</v>
-      </c>
-      <c r="F99" s="1">
-        <v>3</v>
-      </c>
       <c r="G99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I99" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D100" s="1">
         <v>5</v>
       </c>
       <c r="E100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G100" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H100" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I100" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I100" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D101" s="1">
         <v>5</v>
       </c>
       <c r="E101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G101" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H101" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I101" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D102" s="1">
         <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
       </c>
       <c r="G102" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H102" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I102" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D103" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E103" s="1">
         <v>4</v>
       </c>
       <c r="F103" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G103" s="1">
         <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I103" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D104" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E104" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F104" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I104" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D105" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E105" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F105" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G105" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H105" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I105" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D106" s="1">
+        <v>5</v>
+      </c>
+      <c r="E106" s="1">
         <v>3</v>
       </c>
-      <c r="E106" s="1">
-        <v>4</v>
-      </c>
       <c r="F106" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G106" s="1">
         <v>4</v>
       </c>
       <c r="H106" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I106" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D107" s="1">
+        <v>3</v>
+      </c>
+      <c r="E107" s="1">
         <v>4</v>
       </c>
-      <c r="E107" s="1">
-        <v>2</v>
-      </c>
       <c r="F107" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G107" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H107" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I107" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D108" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E108" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F108" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I108" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>155</v>
+        <v>68</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>2.9124999999999996</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D109" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F109" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G109" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>6.7</v>
+        <v>4.5</v>
       </c>
       <c r="I109" s="3">
-        <v>5.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F110" s="1">
         <v>0</v>
       </c>
       <c r="G110" s="1">
+        <v>1</v>
+      </c>
+      <c r="H110" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I110" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B111" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C111" s="5">
+        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D111" s="1">
         <v>0</v>
       </c>
-      <c r="H110" s="3">
+      <c r="E111" s="1">
+        <v>0</v>
+      </c>
+      <c r="F111" s="1">
+        <v>0</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0</v>
+      </c>
+      <c r="H111" s="3">
         <v>7.6</v>
       </c>
-      <c r="I110" s="3">
+      <c r="I111" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 90 "Maldita suerte"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEED945B-FD13-49A3-A1E5-10C68EC46783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66663373-672C-42EB-ACA4-14C075C3160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="190">
   <si>
     <t>Película</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>Triple frontera</t>
+  </si>
+  <si>
+    <t>Maldita suerte</t>
   </si>
 </sst>
 </file>
@@ -1468,10 +1471,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I111" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I111" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I111">
-    <sortCondition descending="1" ref="C2:C111"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I112" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I112" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I112">
+    <sortCondition descending="1" ref="C2:C112"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4090,10 +4093,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K111"/>
+  <dimension ref="B2:K112"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H111" sqref="H111"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6165,7 +6168,7 @@
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="2" t="s">
         <v>188</v>
       </c>
       <c r="C78" s="5">
@@ -7029,56 +7032,83 @@
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B110" s="2" t="s">
-        <v>155</v>
+      <c r="B110" s="9" t="s">
+        <v>189</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>2.9124999999999996</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D110" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E110" s="1">
         <v>1</v>
       </c>
       <c r="F110" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G110" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H110" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I110" s="3">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F111" s="1">
         <v>0</v>
       </c>
       <c r="G111" s="1">
+        <v>1</v>
+      </c>
+      <c r="H111" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I111" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B112" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C112" s="5">
+        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D112" s="1">
         <v>0</v>
       </c>
-      <c r="H111" s="3">
+      <c r="E112" s="1">
+        <v>0</v>
+      </c>
+      <c r="F112" s="1">
+        <v>0</v>
+      </c>
+      <c r="G112" s="1">
+        <v>0</v>
+      </c>
+      <c r="H112" s="3">
         <v>7.6</v>
       </c>
-      <c r="I111" s="3">
+      <c r="I112" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 91 "Inside man: most wanted"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66663373-672C-42EB-ACA4-14C075C3160E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84A0CDF-4346-4AFA-B40E-2F024CBADD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
   <si>
     <t>Película</t>
   </si>
@@ -1119,6 +1119,9 @@
   </si>
   <si>
     <t>Maldita suerte</t>
+  </si>
+  <si>
+    <t>Inside man: most wanted</t>
   </si>
 </sst>
 </file>
@@ -1471,10 +1474,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I112" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I112" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I112">
-    <sortCondition descending="1" ref="C2:C112"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I113" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I113">
+    <sortCondition descending="1" ref="C2:C113"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4093,10 +4096,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K112"/>
+  <dimension ref="B2:K113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B112" sqref="B112"/>
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6627,488 +6630,515 @@
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>182</v>
+      <c r="B95" s="9" t="s">
+        <v>190</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D95" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I95" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D96" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E96" s="1">
         <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H96" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I96" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D97" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E97" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
         <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I97" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E98" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F98" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G98" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I98" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E99" s="1">
         <v>3</v>
       </c>
       <c r="F99" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G99" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H99" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I99" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D100" s="1">
+        <v>6</v>
+      </c>
+      <c r="E100" s="1">
+        <v>3</v>
+      </c>
+      <c r="F100" s="1">
         <v>5</v>
       </c>
-      <c r="E100" s="1">
-        <v>5</v>
-      </c>
-      <c r="F100" s="1">
-        <v>3</v>
-      </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I100" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D101" s="1">
         <v>5</v>
       </c>
       <c r="E101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F101" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G101" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H101" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I101" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I101" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D102" s="1">
         <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H102" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I102" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D103" s="1">
         <v>5</v>
       </c>
       <c r="E103" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F103" s="1">
         <v>5</v>
       </c>
       <c r="G103" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H103" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I103" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D104" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E104" s="1">
         <v>4</v>
       </c>
       <c r="F104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G104" s="1">
         <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I104" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D105" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E105" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F105" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I105" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D106" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E106" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F106" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G106" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H106" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I106" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D107" s="1">
+        <v>5</v>
+      </c>
+      <c r="E107" s="1">
         <v>3</v>
       </c>
-      <c r="E107" s="1">
-        <v>4</v>
-      </c>
       <c r="F107" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G107" s="1">
         <v>4</v>
       </c>
       <c r="H107" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I107" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D108" s="1">
+        <v>3</v>
+      </c>
+      <c r="E108" s="1">
         <v>4</v>
       </c>
-      <c r="E108" s="1">
-        <v>2</v>
-      </c>
       <c r="F108" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G108" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H108" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I108" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D109" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E109" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F109" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H109" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I109" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B110" s="9" t="s">
-        <v>189</v>
+      <c r="B110" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>3.3250000000000002</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D110" s="1">
+        <v>5</v>
+      </c>
+      <c r="E110" s="1">
         <v>4</v>
-      </c>
-      <c r="E110" s="1">
-        <v>1</v>
       </c>
       <c r="F110" s="1">
         <v>2</v>
       </c>
       <c r="G110" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="I110" s="3">
-        <v>5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>2.9124999999999996</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D111" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E111" s="1">
         <v>1</v>
       </c>
       <c r="F111" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G111" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H111" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I111" s="3">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F112" s="1">
         <v>0</v>
       </c>
       <c r="G112" s="1">
+        <v>1</v>
+      </c>
+      <c r="H112" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I112" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B113" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C113" s="5">
+        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D113" s="1">
         <v>0</v>
       </c>
-      <c r="H112" s="3">
+      <c r="E113" s="1">
+        <v>0</v>
+      </c>
+      <c r="F113" s="1">
+        <v>0</v>
+      </c>
+      <c r="G113" s="1">
+        <v>0</v>
+      </c>
+      <c r="H113" s="3">
         <v>7.6</v>
       </c>
-      <c r="I112" s="3">
+      <c r="I113" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 92 "Vida a lo grande"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84A0CDF-4346-4AFA-B40E-2F024CBADD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9572405-CF4E-4A4D-B2F1-16F225CDFE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,7 +549,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="192">
   <si>
     <t>Película</t>
   </si>
@@ -1122,6 +1122,9 @@
   </si>
   <si>
     <t>Inside man: most wanted</t>
+  </si>
+  <si>
+    <t>Vida a lo grande</t>
   </si>
 </sst>
 </file>
@@ -1474,10 +1477,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I113" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I113" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I113">
-    <sortCondition descending="1" ref="C2:C113"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I114" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I114" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I114">
+    <sortCondition descending="1" ref="C2:C114"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4096,10 +4099,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K113"/>
+  <dimension ref="B2:K114"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A76" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6631,514 +6634,541 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.375</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D95" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E95" s="1">
         <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="I95" s="3">
-        <v>4.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D96" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I96" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D97" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E97" s="1">
         <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I97" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D98" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E98" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
         <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I98" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E99" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F99" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G99" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I99" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E100" s="1">
         <v>3</v>
       </c>
       <c r="F100" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G100" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H100" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I100" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D101" s="1">
+        <v>6</v>
+      </c>
+      <c r="E101" s="1">
+        <v>3</v>
+      </c>
+      <c r="F101" s="1">
         <v>5</v>
       </c>
-      <c r="E101" s="1">
-        <v>5</v>
-      </c>
-      <c r="F101" s="1">
-        <v>3</v>
-      </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I101" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D102" s="1">
         <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F102" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G102" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H102" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I102" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I102" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D103" s="1">
         <v>5</v>
       </c>
       <c r="E103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H103" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I103" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D104" s="1">
         <v>5</v>
       </c>
       <c r="E104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
         <v>5</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H104" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I104" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D105" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1">
         <v>4</v>
       </c>
       <c r="F105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G105" s="1">
         <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I105" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D106" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E106" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F106" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I106" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D107" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E107" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F107" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H107" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I107" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D108" s="1">
+        <v>5</v>
+      </c>
+      <c r="E108" s="1">
         <v>3</v>
       </c>
-      <c r="E108" s="1">
-        <v>4</v>
-      </c>
       <c r="F108" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G108" s="1">
         <v>4</v>
       </c>
       <c r="H108" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I108" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D109" s="1">
+        <v>3</v>
+      </c>
+      <c r="E109" s="1">
         <v>4</v>
       </c>
-      <c r="E109" s="1">
-        <v>2</v>
-      </c>
       <c r="F109" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G109" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H109" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I109" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D110" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E110" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F110" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I110" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>3.3250000000000002</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D111" s="1">
+        <v>5</v>
+      </c>
+      <c r="E111" s="1">
         <v>4</v>
-      </c>
-      <c r="E111" s="1">
-        <v>1</v>
       </c>
       <c r="F111" s="1">
         <v>2</v>
       </c>
       <c r="G111" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="I111" s="3">
-        <v>5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>2.9124999999999996</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D112" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E112" s="1">
         <v>1</v>
       </c>
       <c r="F112" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G112" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H112" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I112" s="3">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D113" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F113" s="1">
         <v>0</v>
       </c>
       <c r="G113" s="1">
+        <v>1</v>
+      </c>
+      <c r="H113" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I113" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B114" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C114" s="5">
+        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D114" s="1">
         <v>0</v>
       </c>
-      <c r="H113" s="3">
+      <c r="E114" s="1">
+        <v>0</v>
+      </c>
+      <c r="F114" s="1">
+        <v>0</v>
+      </c>
+      <c r="G114" s="1">
+        <v>0</v>
+      </c>
+      <c r="H114" s="3">
         <v>7.6</v>
       </c>
-      <c r="I113" s="3">
+      <c r="I114" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 95 "Una navidad ex-cepcional"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189DAEDF-9321-485C-9EF3-4BD8E78B3459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B7EEB-6487-4223-9E8B-0A98C1DB6DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="195">
   <si>
     <t>Película</t>
   </si>
@@ -1140,6 +1140,9 @@
   </si>
   <si>
     <t>Frankenstein</t>
+  </si>
+  <si>
+    <t>Una navidad ex-cepcional</t>
   </si>
 </sst>
 </file>
@@ -1228,7 +1231,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1251,9 +1254,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1492,10 +1492,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I115" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I115" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I115">
-    <sortCondition descending="1" ref="C2:C115"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I116" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I116" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I116">
+    <sortCondition descending="1" ref="C2:C116"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4150,10 +4150,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K115"/>
+  <dimension ref="B2:K116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,7 +4202,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4230,7 +4230,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4258,7 +4258,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4285,7 +4285,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4312,7 +4312,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4339,7 +4339,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4366,7 +4366,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4393,7 +4393,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4420,7 +4420,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4447,7 +4447,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4474,7 +4474,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4501,7 +4501,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4528,7 +4528,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4555,7 +4555,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4582,7 +4582,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4609,7 +4609,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4636,7 +4636,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4663,7 +4663,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4690,7 +4690,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4717,7 +4717,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4744,7 +4744,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4771,7 +4771,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4798,7 +4798,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4825,7 +4825,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4852,7 +4852,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4875,11 +4875,11 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="2" t="s">
         <v>193</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7750000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -4906,7 +4906,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7375000000000007</v>
       </c>
       <c r="D29" s="1">
@@ -4933,7 +4933,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000011</v>
       </c>
       <c r="D30" s="1">
@@ -4960,7 +4960,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4987,7 +4987,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D32" s="1">
@@ -5014,7 +5014,7 @@
         <v>97</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.6875</v>
       </c>
       <c r="D33" s="1">
@@ -5041,7 +5041,7 @@
         <v>123</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5874999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -5068,7 +5068,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D35" s="1">
@@ -5095,7 +5095,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5750000000000002</v>
       </c>
       <c r="D36" s="1">
@@ -5122,7 +5122,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.5625</v>
       </c>
       <c r="D37" s="1">
@@ -5149,7 +5149,7 @@
         <v>55</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.5624999999999991</v>
       </c>
       <c r="D38" s="1">
@@ -5176,7 +5176,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D39" s="1">
@@ -5203,7 +5203,7 @@
         <v>132</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.5125000000000002</v>
       </c>
       <c r="D40" s="1">
@@ -5230,7 +5230,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
@@ -5257,7 +5257,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
@@ -5284,7 +5284,7 @@
         <v>100</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.4249999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -5311,7 +5311,7 @@
         <v>131</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.4124999999999996</v>
       </c>
       <c r="D44" s="1">
@@ -5338,7 +5338,7 @@
         <v>175</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.3624999999999989</v>
       </c>
       <c r="D45" s="1">
@@ -5365,7 +5365,7 @@
         <v>52</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.3500000000000005</v>
       </c>
       <c r="D46" s="1">
@@ -5392,7 +5392,7 @@
         <v>165</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.3249999999999993</v>
       </c>
       <c r="D47" s="1">
@@ -5419,7 +5419,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D48" s="1">
@@ -5446,7 +5446,7 @@
         <v>103</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -5473,7 +5473,7 @@
         <v>181</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -5500,7 +5500,7 @@
         <v>147</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>7.2374999999999998</v>
       </c>
       <c r="D51" s="1">
@@ -5527,7 +5527,7 @@
         <v>59</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>7.2250000000000005</v>
       </c>
       <c r="D52" s="1">
@@ -5554,7 +5554,7 @@
         <v>65</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>7.2125000000000004</v>
       </c>
       <c r="D53" s="1">
@@ -5581,7 +5581,7 @@
         <v>146</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>7.2124999999999995</v>
       </c>
       <c r="D54" s="1">
@@ -5608,7 +5608,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>7.1499999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -5635,7 +5635,7 @@
         <v>104</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>7.1375000000000011</v>
       </c>
       <c r="D56" s="1">
@@ -5662,7 +5662,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>7.1250000000000009</v>
       </c>
       <c r="D57" s="1">
@@ -5689,7 +5689,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>7.125</v>
       </c>
       <c r="D58" s="1">
@@ -5716,7 +5716,7 @@
         <v>133</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>7.0875000000000004</v>
       </c>
       <c r="D59" s="1">
@@ -5743,7 +5743,7 @@
         <v>98</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D60" s="1">
@@ -5770,7 +5770,7 @@
         <v>171</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D61" s="1">
@@ -5797,7 +5797,7 @@
         <v>110</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D62" s="1">
@@ -5824,7 +5824,7 @@
         <v>143</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D63" s="1">
@@ -5851,7 +5851,7 @@
         <v>177</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>7.0749999999999993</v>
       </c>
       <c r="D64" s="1">
@@ -5878,7 +5878,7 @@
         <v>176</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>7.05</v>
       </c>
       <c r="D65" s="1">
@@ -5905,7 +5905,7 @@
         <v>95</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>6.9375</v>
       </c>
       <c r="D66" s="1">
@@ -5932,7 +5932,7 @@
         <v>164</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D67" s="1">
@@ -5959,7 +5959,7 @@
         <v>157</v>
       </c>
       <c r="C68" s="5">
-        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
+        <f t="shared" si="2"/>
         <v>6.8999999999999995</v>
       </c>
       <c r="D68" s="1">
@@ -5986,7 +5986,7 @@
         <v>88</v>
       </c>
       <c r="C69" s="5">
-        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D69" s="1">
@@ -6013,7 +6013,7 @@
         <v>184</v>
       </c>
       <c r="C70" s="5">
-        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D70" s="1">
@@ -6040,7 +6040,7 @@
         <v>119</v>
       </c>
       <c r="C71" s="5">
-        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
+        <f t="shared" si="2"/>
         <v>6.85</v>
       </c>
       <c r="D71" s="1">
@@ -6067,7 +6067,7 @@
         <v>57</v>
       </c>
       <c r="C72" s="5">
-        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
+        <f t="shared" si="2"/>
         <v>6.6999999999999993</v>
       </c>
       <c r="D72" s="1">
@@ -6094,7 +6094,7 @@
         <v>87</v>
       </c>
       <c r="C73" s="5">
-        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
+        <f t="shared" si="2"/>
         <v>6.6875</v>
       </c>
       <c r="D73" s="1">
@@ -6121,7 +6121,7 @@
         <v>41</v>
       </c>
       <c r="C74" s="5">
-        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <f t="shared" si="2"/>
         <v>6.6124999999999989</v>
       </c>
       <c r="D74" s="1">
@@ -6148,7 +6148,7 @@
         <v>117</v>
       </c>
       <c r="C75" s="5">
-        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D75" s="1">
@@ -6175,7 +6175,7 @@
         <v>179</v>
       </c>
       <c r="C76" s="5">
-        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D76" s="1">
@@ -6202,7 +6202,7 @@
         <v>168</v>
       </c>
       <c r="C77" s="5">
-        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <f t="shared" si="2"/>
         <v>6.5499999999999989</v>
       </c>
       <c r="D77" s="1">
@@ -6229,7 +6229,7 @@
         <v>183</v>
       </c>
       <c r="C78" s="5">
-        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <f t="shared" si="2"/>
         <v>6.3624999999999998</v>
       </c>
       <c r="D78" s="1">
@@ -6256,7 +6256,7 @@
         <v>188</v>
       </c>
       <c r="C79" s="5">
-        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <f t="shared" si="2"/>
         <v>6.35</v>
       </c>
       <c r="D79" s="1">
@@ -6283,7 +6283,7 @@
         <v>134</v>
       </c>
       <c r="C80" s="5">
-        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <f t="shared" si="2"/>
         <v>6.3125</v>
       </c>
       <c r="D80" s="1">
@@ -6310,7 +6310,7 @@
         <v>144</v>
       </c>
       <c r="C81" s="5">
-        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D81" s="1">
@@ -6337,7 +6337,7 @@
         <v>64</v>
       </c>
       <c r="C82" s="5">
-        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D82" s="1">
@@ -6364,7 +6364,7 @@
         <v>75</v>
       </c>
       <c r="C83" s="5">
-        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <f t="shared" si="2"/>
         <v>6.2125000000000004</v>
       </c>
       <c r="D83" s="1">
@@ -6391,7 +6391,7 @@
         <v>19</v>
       </c>
       <c r="C84" s="5">
-        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <f t="shared" si="2"/>
         <v>6.2124999999999995</v>
       </c>
       <c r="D84" s="1">
@@ -6418,7 +6418,7 @@
         <v>101</v>
       </c>
       <c r="C85" s="5">
-        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <f t="shared" si="2"/>
         <v>6.15</v>
       </c>
       <c r="D85" s="1">
@@ -6445,7 +6445,7 @@
         <v>158</v>
       </c>
       <c r="C86" s="5">
-        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <f t="shared" si="2"/>
         <v>6.0874999999999995</v>
       </c>
       <c r="D86" s="1">
@@ -6472,7 +6472,7 @@
         <v>160</v>
       </c>
       <c r="C87" s="5">
-        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
       <c r="D87" s="1">
@@ -6499,7 +6499,7 @@
         <v>159</v>
       </c>
       <c r="C88" s="5">
-        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <f t="shared" si="2"/>
         <v>5.9499999999999993</v>
       </c>
       <c r="D88" s="1">
@@ -6526,7 +6526,7 @@
         <v>186</v>
       </c>
       <c r="C89" s="5">
-        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <f t="shared" si="2"/>
         <v>5.8125000000000009</v>
       </c>
       <c r="D89" s="1">
@@ -6553,7 +6553,7 @@
         <v>113</v>
       </c>
       <c r="C90" s="5">
-        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <f t="shared" si="2"/>
         <v>5.7374999999999989</v>
       </c>
       <c r="D90" s="1">
@@ -6580,7 +6580,7 @@
         <v>187</v>
       </c>
       <c r="C91" s="5">
-        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <f t="shared" si="2"/>
         <v>5.7250000000000005</v>
       </c>
       <c r="D91" s="1">
@@ -6607,7 +6607,7 @@
         <v>26</v>
       </c>
       <c r="C92" s="5">
-        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <f t="shared" si="2"/>
         <v>5.6749999999999998</v>
       </c>
       <c r="D92" s="1">
@@ -6634,7 +6634,7 @@
         <v>149</v>
       </c>
       <c r="C93" s="5">
-        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D93" s="1">
@@ -6661,7 +6661,7 @@
         <v>156</v>
       </c>
       <c r="C94" s="5">
-        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <f t="shared" si="2"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D94" s="1">
@@ -6688,7 +6688,7 @@
         <v>166</v>
       </c>
       <c r="C95" s="5">
-        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <f t="shared" si="2"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D95" s="1">
@@ -6715,7 +6715,7 @@
         <v>191</v>
       </c>
       <c r="C96" s="5">
-        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <f t="shared" si="2"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D96" s="1">
@@ -6742,7 +6742,7 @@
         <v>190</v>
       </c>
       <c r="C97" s="5">
-        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <f t="shared" si="2"/>
         <v>5.375</v>
       </c>
       <c r="D97" s="1">
@@ -6769,7 +6769,7 @@
         <v>182</v>
       </c>
       <c r="C98" s="5">
-        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <f t="shared" si="2"/>
         <v>5.2875000000000005</v>
       </c>
       <c r="D98" s="1">
@@ -6796,7 +6796,7 @@
         <v>74</v>
       </c>
       <c r="C99" s="5">
-        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>5.1875</v>
       </c>
       <c r="D99" s="1">
@@ -6823,7 +6823,7 @@
         <v>145</v>
       </c>
       <c r="C100" s="5">
-        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <f t="shared" si="3"/>
         <v>5.1124999999999998</v>
       </c>
       <c r="D100" s="1">
@@ -6850,7 +6850,7 @@
         <v>21</v>
       </c>
       <c r="C101" s="5">
-        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <f t="shared" si="3"/>
         <v>5.05</v>
       </c>
       <c r="D101" s="1">
@@ -6877,7 +6877,7 @@
         <v>169</v>
       </c>
       <c r="C102" s="5">
-        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <f t="shared" si="3"/>
         <v>4.9874999999999998</v>
       </c>
       <c r="D102" s="1">
@@ -6904,7 +6904,7 @@
         <v>163</v>
       </c>
       <c r="C103" s="5">
-        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <f t="shared" si="3"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="D103" s="1">
@@ -6931,7 +6931,7 @@
         <v>162</v>
       </c>
       <c r="C104" s="5">
-        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <f t="shared" si="3"/>
         <v>4.7875000000000005</v>
       </c>
       <c r="D104" s="1">
@@ -6958,7 +6958,7 @@
         <v>154</v>
       </c>
       <c r="C105" s="5">
-        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <f t="shared" si="3"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="D105" s="1">
@@ -6985,7 +6985,7 @@
         <v>135</v>
       </c>
       <c r="C106" s="5">
-        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
+        <f t="shared" si="3"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D106" s="1">
@@ -7012,7 +7012,7 @@
         <v>161</v>
       </c>
       <c r="C107" s="5">
-        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <f t="shared" si="3"/>
         <v>4.4249999999999998</v>
       </c>
       <c r="D107" s="1">
@@ -7039,7 +7039,7 @@
         <v>114</v>
       </c>
       <c r="C108" s="5">
-        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
+        <f t="shared" si="3"/>
         <v>4.4124999999999996</v>
       </c>
       <c r="D108" s="1">
@@ -7066,7 +7066,7 @@
         <v>150</v>
       </c>
       <c r="C109" s="5">
-        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
+        <f t="shared" si="3"/>
         <v>4.3374999999999995</v>
       </c>
       <c r="D109" s="1">
@@ -7093,7 +7093,7 @@
         <v>173</v>
       </c>
       <c r="C110" s="5">
-        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
+        <f t="shared" si="3"/>
         <v>4.3125</v>
       </c>
       <c r="D110" s="1">
@@ -7120,7 +7120,7 @@
         <v>167</v>
       </c>
       <c r="C111" s="5">
-        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
+        <f t="shared" si="3"/>
         <v>4.2749999999999995</v>
       </c>
       <c r="D111" s="1">
@@ -7147,7 +7147,7 @@
         <v>68</v>
       </c>
       <c r="C112" s="5">
-        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
+        <f t="shared" si="3"/>
         <v>4.1124999999999998</v>
       </c>
       <c r="D112" s="1">
@@ -7174,7 +7174,7 @@
         <v>189</v>
       </c>
       <c r="C113" s="5">
-        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
+        <f t="shared" si="3"/>
         <v>3.3250000000000002</v>
       </c>
       <c r="D113" s="1">
@@ -7198,55 +7198,82 @@
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C114" s="5">
-        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>2.9124999999999996</v>
+        <f t="shared" si="3"/>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D114" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E114" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F114" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G114" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H114" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I114" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C115" s="5">
-        <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>2.6375000000000002</v>
+        <f t="shared" si="3"/>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D115" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E115" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F115" s="1">
         <v>0</v>
       </c>
       <c r="G115" s="1">
+        <v>1</v>
+      </c>
+      <c r="H115" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I115" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B116" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C116" s="5">
+        <f t="shared" si="3"/>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D116" s="1">
         <v>0</v>
       </c>
-      <c r="H115" s="3">
+      <c r="E116" s="1">
+        <v>0</v>
+      </c>
+      <c r="F116" s="1">
+        <v>0</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0</v>
+      </c>
+      <c r="H116" s="3">
         <v>7.6</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I116" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 96 "El chico que salvó la navidad"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587B7EEB-6487-4223-9E8B-0A98C1DB6DC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624C2209-C1E7-45C5-B236-B40CF8E6F169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="196">
   <si>
     <t>Película</t>
   </si>
@@ -1143,6 +1143,9 @@
   </si>
   <si>
     <t>Una navidad ex-cepcional</t>
+  </si>
+  <si>
+    <t>El chico que salvó la navidad</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1254,6 +1257,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1492,10 +1498,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I116" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I116" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I116">
-    <sortCondition descending="1" ref="C2:C116"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I117" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I117" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I117">
+    <sortCondition descending="1" ref="C2:C117"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4150,10 +4156,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K116"/>
+  <dimension ref="B2:K117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C117" sqref="C117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4202,7 +4208,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4230,7 +4236,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4258,7 +4264,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4285,7 +4291,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4312,7 +4318,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4339,7 +4345,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4366,7 +4372,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4393,7 +4399,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4420,7 +4426,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4447,7 +4453,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4474,7 +4480,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4501,7 +4507,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4528,7 +4534,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4555,7 +4561,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4582,7 +4588,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4609,7 +4615,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4636,7 +4642,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4663,7 +4669,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4690,7 +4696,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4717,7 +4723,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4744,7 +4750,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4771,7 +4777,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4798,7 +4804,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4825,7 +4831,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4852,7 +4858,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4879,7 +4885,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7750000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -4906,7 +4912,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D29" s="1">
@@ -4933,7 +4939,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D30" s="1">
@@ -4960,7 +4966,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -4987,7 +4993,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D32" s="1">
@@ -5014,7 +5020,7 @@
         <v>97</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.6875</v>
       </c>
       <c r="D33" s="1">
@@ -5041,7 +5047,7 @@
         <v>123</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -5068,7 +5074,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D35" s="1">
@@ -5095,7 +5101,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D36" s="1">
@@ -5122,7 +5128,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5625</v>
       </c>
       <c r="D37" s="1">
@@ -5149,7 +5155,7 @@
         <v>55</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D38" s="1">
@@ -5176,7 +5182,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D39" s="1">
@@ -5203,7 +5209,7 @@
         <v>132</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D40" s="1">
@@ -5230,7 +5236,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
@@ -5257,7 +5263,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
@@ -5284,7 +5290,7 @@
         <v>100</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -5311,7 +5317,7 @@
         <v>131</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D44" s="1">
@@ -5338,7 +5344,7 @@
         <v>175</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D45" s="1">
@@ -5365,7 +5371,7 @@
         <v>52</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D46" s="1">
@@ -5392,7 +5398,7 @@
         <v>165</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D47" s="1">
@@ -5419,7 +5425,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.3</v>
       </c>
       <c r="D48" s="1">
@@ -5446,7 +5452,7 @@
         <v>103</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -5473,7 +5479,7 @@
         <v>181</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -5500,7 +5506,7 @@
         <v>147</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
         <v>7.2374999999999998</v>
       </c>
       <c r="D51" s="1">
@@ -5527,7 +5533,7 @@
         <v>59</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
         <v>7.2250000000000005</v>
       </c>
       <c r="D52" s="1">
@@ -5554,7 +5560,7 @@
         <v>65</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
         <v>7.2125000000000004</v>
       </c>
       <c r="D53" s="1">
@@ -5581,7 +5587,7 @@
         <v>146</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
         <v>7.2124999999999995</v>
       </c>
       <c r="D54" s="1">
@@ -5608,7 +5614,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -5635,7 +5641,7 @@
         <v>104</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.1375000000000011</v>
       </c>
       <c r="D56" s="1">
@@ -5662,7 +5668,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.1250000000000009</v>
       </c>
       <c r="D57" s="1">
@@ -5689,7 +5695,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.125</v>
       </c>
       <c r="D58" s="1">
@@ -5716,7 +5722,7 @@
         <v>133</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.0875000000000004</v>
       </c>
       <c r="D59" s="1">
@@ -5743,7 +5749,7 @@
         <v>98</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D60" s="1">
@@ -5770,7 +5776,7 @@
         <v>171</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D61" s="1">
@@ -5797,7 +5803,7 @@
         <v>110</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D62" s="1">
@@ -5824,7 +5830,7 @@
         <v>143</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D63" s="1">
@@ -5851,7 +5857,7 @@
         <v>177</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>7.0749999999999993</v>
       </c>
       <c r="D64" s="1">
@@ -5878,7 +5884,7 @@
         <v>176</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>7.05</v>
       </c>
       <c r="D65" s="1">
@@ -5905,7 +5911,7 @@
         <v>95</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
         <v>6.9375</v>
       </c>
       <c r="D66" s="1">
@@ -5932,7 +5938,7 @@
         <v>164</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D67" s="1">
@@ -5959,7 +5965,7 @@
         <v>157</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D68" s="1">
@@ -5986,7 +5992,7 @@
         <v>88</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D69" s="1">
@@ -6013,7 +6019,7 @@
         <v>184</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D70" s="1">
@@ -6040,7 +6046,7 @@
         <v>119</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
         <v>6.85</v>
       </c>
       <c r="D71" s="1">
@@ -6067,7 +6073,7 @@
         <v>57</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
         <v>6.6999999999999993</v>
       </c>
       <c r="D72" s="1">
@@ -6094,7 +6100,7 @@
         <v>87</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
         <v>6.6875</v>
       </c>
       <c r="D73" s="1">
@@ -6121,7 +6127,7 @@
         <v>41</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
         <v>6.6124999999999989</v>
       </c>
       <c r="D74" s="1">
@@ -6148,7 +6154,7 @@
         <v>117</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D75" s="1">
@@ -6175,7 +6181,7 @@
         <v>179</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D76" s="1">
@@ -6202,7 +6208,7 @@
         <v>168</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
         <v>6.5499999999999989</v>
       </c>
       <c r="D77" s="1">
@@ -6229,7 +6235,7 @@
         <v>183</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D78" s="1">
@@ -6256,7 +6262,7 @@
         <v>188</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
         <v>6.35</v>
       </c>
       <c r="D79" s="1">
@@ -6283,7 +6289,7 @@
         <v>134</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
         <v>6.3125</v>
       </c>
       <c r="D80" s="1">
@@ -6310,7 +6316,7 @@
         <v>144</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D81" s="1">
@@ -6337,7 +6343,7 @@
         <v>64</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D82" s="1">
@@ -6364,7 +6370,7 @@
         <v>75</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
         <v>6.2125000000000004</v>
       </c>
       <c r="D83" s="1">
@@ -6391,7 +6397,7 @@
         <v>19</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
         <v>6.2124999999999995</v>
       </c>
       <c r="D84" s="1">
@@ -6418,7 +6424,7 @@
         <v>101</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
         <v>6.15</v>
       </c>
       <c r="D85" s="1">
@@ -6445,7 +6451,7 @@
         <v>158</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
         <v>6.0874999999999995</v>
       </c>
       <c r="D86" s="1">
@@ -6472,7 +6478,7 @@
         <v>160</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
         <v>6.05</v>
       </c>
       <c r="D87" s="1">
@@ -6499,7 +6505,7 @@
         <v>159</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
         <v>5.9499999999999993</v>
       </c>
       <c r="D88" s="1">
@@ -6522,39 +6528,39 @@
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="2" t="s">
-        <v>186</v>
+      <c r="B89" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8125000000000009</v>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="1">
         <v>5</v>
       </c>
       <c r="F89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I89" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
-        <v>5.7374999999999989</v>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D90" s="1">
         <v>7</v>
@@ -6563,25 +6569,25 @@
         <v>5</v>
       </c>
       <c r="F90" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H90" s="3">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="I90" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
-        <v>5.7250000000000005</v>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D91" s="1">
         <v>7</v>
@@ -6593,37 +6599,37 @@
         <v>4</v>
       </c>
       <c r="G91" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I91" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
-        <v>5.6749999999999998</v>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D92" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F92" s="1">
+        <v>4</v>
+      </c>
+      <c r="G92" s="1">
         <v>5</v>
       </c>
-      <c r="G92" s="1">
-        <v>6</v>
-      </c>
       <c r="H92" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I92" s="3">
         <v>6.4</v>
@@ -6631,50 +6637,50 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
-        <v>5.5624999999999991</v>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D93" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E93" s="1">
+        <v>3</v>
+      </c>
+      <c r="F93" s="1">
         <v>5</v>
       </c>
-      <c r="F93" s="1">
-        <v>6</v>
-      </c>
       <c r="G93" s="1">
         <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I93" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D94" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94" s="3">
         <v>5.8</v>
@@ -6685,595 +6691,622 @@
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
-        <v>5.4874999999999989</v>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D95" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E95" s="1">
         <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H95" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I95" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E96" s="1">
         <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I96" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
-        <v>5.375</v>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D97" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E97" s="1">
         <v>6</v>
       </c>
       <c r="F97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="I97" s="3">
-        <v>4.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
-        <v>5.2875000000000005</v>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>5.375</v>
       </c>
       <c r="D98" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I98" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.1875</v>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D99" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E99" s="1">
         <v>5</v>
       </c>
       <c r="F99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I99" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
-        <v>5.1124999999999998</v>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>5.1875</v>
       </c>
       <c r="D100" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E100" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
         <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I100" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
-        <v>5.05</v>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E101" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F101" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G101" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I101" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9874999999999998</v>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <v>5.05</v>
       </c>
       <c r="D102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
         <v>3</v>
       </c>
       <c r="F102" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G102" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H102" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I102" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
-        <v>4.8499999999999996</v>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D103" s="1">
+        <v>6</v>
+      </c>
+      <c r="E103" s="1">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1">
         <v>5</v>
       </c>
-      <c r="E103" s="1">
-        <v>5</v>
-      </c>
-      <c r="F103" s="1">
-        <v>3</v>
-      </c>
       <c r="G103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I103" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C104" s="5">
-        <f t="shared" si="3"/>
-        <v>4.7875000000000005</v>
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D104" s="1">
         <v>5</v>
       </c>
       <c r="E104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G104" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H104" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I104" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I104" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C105" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5999999999999996</v>
+        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D105" s="1">
         <v>5</v>
       </c>
       <c r="E105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H105" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I105" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C106" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5874999999999995</v>
+        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D106" s="1">
         <v>5</v>
       </c>
       <c r="E106" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1">
         <v>5</v>
       </c>
       <c r="G106" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H106" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I106" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C107" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4249999999999998</v>
+        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D107" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1">
         <v>4</v>
       </c>
       <c r="F107" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G107" s="1">
         <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I107" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C108" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4124999999999996</v>
+        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D108" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E108" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F108" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I108" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C109" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3374999999999995</v>
+        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D109" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E109" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F109" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G109" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H109" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I109" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C110" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3125</v>
+        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D110" s="1">
+        <v>5</v>
+      </c>
+      <c r="E110" s="1">
         <v>3</v>
       </c>
-      <c r="E110" s="1">
-        <v>4</v>
-      </c>
       <c r="F110" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G110" s="1">
         <v>4</v>
       </c>
       <c r="H110" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I110" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C111" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2749999999999995</v>
+        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
+        <v>4.3125</v>
       </c>
       <c r="D111" s="1">
+        <v>3</v>
+      </c>
+      <c r="E111" s="1">
         <v>4</v>
       </c>
-      <c r="E111" s="1">
-        <v>2</v>
-      </c>
       <c r="F111" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G111" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H111" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I111" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C112" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1124999999999998</v>
+        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D112" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E112" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F112" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G112" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H112" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I112" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="C113" s="5">
-        <f t="shared" si="3"/>
-        <v>3.3250000000000002</v>
+        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D113" s="1">
+        <v>5</v>
+      </c>
+      <c r="E113" s="1">
         <v>4</v>
-      </c>
-      <c r="E113" s="1">
-        <v>1</v>
       </c>
       <c r="F113" s="1">
         <v>2</v>
       </c>
       <c r="G113" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="I113" s="3">
-        <v>5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C114" s="5">
-        <f t="shared" si="3"/>
-        <v>3.2749999999999995</v>
+        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D114" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E114" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F114" s="1">
         <v>2</v>
       </c>
       <c r="G114" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H114" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I114" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C115" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D115" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E115" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F115" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G115" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H115" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I115" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C116" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D116" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" s="1">
         <v>0</v>
       </c>
       <c r="G116" s="1">
+        <v>1</v>
+      </c>
+      <c r="H116" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I116" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B117" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117" s="5">
+        <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D117" s="1">
         <v>0</v>
       </c>
-      <c r="H116" s="3">
+      <c r="E117" s="1">
+        <v>0</v>
+      </c>
+      <c r="F117" s="1">
+        <v>0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>0</v>
+      </c>
+      <c r="H117" s="3">
         <v>7.6</v>
       </c>
-      <c r="I116" s="3">
+      <c r="I117" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 97 "Caramelo" & "Troll"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624C2209-C1E7-45C5-B236-B40CF8E6F169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFF2DE5-C70B-4513-BC62-338B2C613E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -558,7 +558,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="198">
   <si>
     <t>Película</t>
   </si>
@@ -1146,6 +1146,12 @@
   </si>
   <si>
     <t>El chico que salvó la navidad</t>
+  </si>
+  <si>
+    <t>Troll</t>
+  </si>
+  <si>
+    <t>Caramelo</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1504,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I117" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I117" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I117">
-    <sortCondition descending="1" ref="C2:C117"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I119" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I119" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I119">
+    <sortCondition descending="1" ref="C2:C119"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4156,10 +4162,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K117"/>
+  <dimension ref="B2:K119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C117" sqref="C117"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C119" sqref="C119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6069,147 +6075,147 @@
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B72" s="2" t="s">
-        <v>57</v>
+      <c r="B72" s="9" t="s">
+        <v>196</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.6999999999999993</v>
+        <v>6.7999999999999989</v>
       </c>
       <c r="D72" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H72" s="3">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
       <c r="I72" s="3">
-        <v>7.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.6875</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D73" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E73" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>5.5</v>
+        <v>7.9</v>
       </c>
       <c r="I73" s="3">
-        <v>4.5</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6875</v>
       </c>
       <c r="D74" s="1">
         <v>8</v>
       </c>
       <c r="E74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F74" s="1">
         <v>8</v>
       </c>
       <c r="G74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H74" s="3">
-        <v>6.3</v>
+        <v>5.5</v>
       </c>
       <c r="I74" s="3">
-        <v>5.3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H75" s="3">
         <v>6.3</v>
       </c>
       <c r="I75" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D76" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
         <v>7</v>
       </c>
       <c r="G76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H76" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I76" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D77" s="1">
         <v>8</v>
@@ -6221,22 +6227,22 @@
         <v>7</v>
       </c>
       <c r="G77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H77" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I77" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>6.3624999999999998</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D78" s="1">
         <v>8</v>
@@ -6248,79 +6254,79 @@
         <v>7</v>
       </c>
       <c r="G78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>5.9</v>
+        <v>6.8</v>
       </c>
       <c r="I78" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B79" s="2" t="s">
-        <v>188</v>
+      <c r="B79" s="9" t="s">
+        <v>197</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.35</v>
+        <v>6.5375000000000005</v>
       </c>
       <c r="D79" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
         <v>7</v>
       </c>
       <c r="G79" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H79" s="3">
-        <v>6.5</v>
+        <v>7.1</v>
       </c>
       <c r="I79" s="3">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>6.3125</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1">
         <v>6</v>
       </c>
       <c r="F80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>6.9</v>
+        <v>5.9</v>
       </c>
       <c r="I80" s="3">
-        <v>5.7</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.2749999999999995</v>
+        <v>6.35</v>
       </c>
       <c r="D81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E81" s="1">
         <v>6</v>
@@ -6329,28 +6335,28 @@
         <v>7</v>
       </c>
       <c r="G81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="I81" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
         <v>6</v>
@@ -6359,73 +6365,73 @@
         <v>6</v>
       </c>
       <c r="H82" s="3">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="I82" s="3">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E83" s="1">
         <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="I83" s="3">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D84" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E84" s="1">
         <v>7</v>
       </c>
       <c r="F84" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>4.3</v>
+        <v>6.4</v>
       </c>
       <c r="I84" s="3">
-        <v>4.0999999999999996</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>6.15</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D85" s="1">
         <v>7</v>
@@ -6440,34 +6446,34 @@
         <v>8</v>
       </c>
       <c r="H85" s="3">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I85" s="3">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.0874999999999995</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D86" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E86" s="1">
         <v>7</v>
       </c>
       <c r="F86" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G86" s="1">
         <v>7</v>
       </c>
       <c r="H86" s="3">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="I86" s="3">
         <v>4.0999999999999996</v>
@@ -6475,11 +6481,11 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>160</v>
+        <v>101</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>6.05</v>
+        <v>6.15</v>
       </c>
       <c r="D87" s="1">
         <v>7</v>
@@ -6488,133 +6494,133 @@
         <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G87" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H87" s="3">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="I87" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>5.9499999999999993</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G88" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H88" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I88" s="3">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B89" s="9" t="s">
-        <v>195</v>
+      <c r="B89" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>5.8875000000000011</v>
+        <v>6.05</v>
       </c>
       <c r="D89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E89" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H89" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I89" s="3">
-        <v>5.7</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>5.8125000000000009</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D90" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E90" s="1">
+        <v>6</v>
+      </c>
+      <c r="F90" s="1">
+        <v>8</v>
+      </c>
+      <c r="G90" s="1">
         <v>5</v>
       </c>
-      <c r="F90" s="1">
+      <c r="H90" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="I90" s="3">
         <v>5</v>
-      </c>
-      <c r="G90" s="1">
-        <v>7</v>
-      </c>
-      <c r="H90" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="I90" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D91" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
         <v>5</v>
       </c>
       <c r="F91" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G91" s="1">
         <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="I91" s="3">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>5.7250000000000005</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D92" s="1">
         <v>7</v>
@@ -6623,112 +6629,112 @@
         <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G92" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H92" s="3">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="I92" s="3">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D93" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E93" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F93" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G93" s="1">
         <v>6</v>
       </c>
       <c r="H93" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I93" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>5.5624999999999991</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E94" s="1">
         <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G94" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H94" s="3">
-        <v>5.8</v>
+        <v>6.7</v>
       </c>
       <c r="I94" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D95" s="1">
+        <v>8</v>
+      </c>
+      <c r="E95" s="1">
         <v>3</v>
       </c>
-      <c r="E95" s="1">
-        <v>6</v>
-      </c>
       <c r="F95" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I95" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D96" s="1">
         <v>6</v>
       </c>
       <c r="E96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F96" s="1">
         <v>6</v>
@@ -6737,28 +6743,28 @@
         <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I96" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D97" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E97" s="1">
         <v>6</v>
       </c>
       <c r="F97" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G97" s="1">
         <v>5</v>
@@ -6767,19 +6773,19 @@
         <v>5.8</v>
       </c>
       <c r="I97" s="3">
-        <v>5.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.375</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D98" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E98" s="1">
         <v>6</v>
@@ -6791,25 +6797,25 @@
         <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="I98" s="3">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.2875000000000005</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D99" s="1">
         <v>5</v>
       </c>
       <c r="E99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
@@ -6818,25 +6824,25 @@
         <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="I99" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.1875</v>
+        <v>5.375</v>
       </c>
       <c r="D100" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F100" s="1">
         <v>6</v>
@@ -6845,34 +6851,34 @@
         <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
       <c r="I100" s="3">
-        <v>3.5</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.1124999999999998</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E101" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F101" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="I101" s="3">
         <v>5.0999999999999996</v>
@@ -6880,119 +6886,119 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.05</v>
+        <v>5.1875</v>
       </c>
       <c r="D102" s="1">
+        <v>7</v>
+      </c>
+      <c r="E102" s="1">
         <v>5</v>
       </c>
-      <c r="E102" s="1">
-        <v>3</v>
-      </c>
       <c r="F102" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H102" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I102" s="3">
-        <v>5.8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>4.9874999999999998</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D103" s="1">
         <v>6</v>
       </c>
       <c r="E103" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F103" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G103" s="1">
         <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="I103" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D104" s="1">
         <v>5</v>
       </c>
       <c r="E104" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F104" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H104" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I104" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.7875000000000005</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D105" s="1">
+        <v>6</v>
+      </c>
+      <c r="E105" s="1">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1">
         <v>5</v>
       </c>
-      <c r="E105" s="1">
-        <v>6</v>
-      </c>
-      <c r="F105" s="1">
-        <v>6</v>
-      </c>
       <c r="G105" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H105" s="3">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="I105" s="3">
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D106" s="1">
         <v>5</v>
@@ -7001,312 +7007,366 @@
         <v>5</v>
       </c>
       <c r="F106" s="1">
+        <v>3</v>
+      </c>
+      <c r="G106" s="1">
         <v>5</v>
       </c>
-      <c r="G106" s="1">
-        <v>3</v>
-      </c>
       <c r="H106" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="I106" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.5874999999999995</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D107" s="1">
         <v>5</v>
       </c>
       <c r="E107" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H107" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I107" s="3">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D108" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1">
+        <v>5</v>
+      </c>
+      <c r="F108" s="1">
+        <v>5</v>
+      </c>
+      <c r="G108" s="1">
+        <v>3</v>
+      </c>
+      <c r="H108" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I108" s="3">
         <v>4</v>
-      </c>
-      <c r="F108" s="1">
-        <v>6</v>
-      </c>
-      <c r="G108" s="1">
-        <v>5</v>
-      </c>
-      <c r="H108" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="I108" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.4124999999999996</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D109" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F109" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G109" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>8.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I109" s="3">
-        <v>7.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D110" s="1">
+        <v>1</v>
+      </c>
+      <c r="E110" s="1">
+        <v>4</v>
+      </c>
+      <c r="F110" s="1">
+        <v>6</v>
+      </c>
+      <c r="G110" s="1">
         <v>5</v>
       </c>
-      <c r="E110" s="1">
-        <v>3</v>
-      </c>
-      <c r="F110" s="1">
-        <v>3</v>
-      </c>
-      <c r="G110" s="1">
-        <v>4</v>
-      </c>
       <c r="H110" s="3">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="I110" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.3125</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D111" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E111" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F111" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G111" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H111" s="3">
-        <v>5.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I111" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D112" s="1">
+        <v>5</v>
+      </c>
+      <c r="E112" s="1">
+        <v>3</v>
+      </c>
+      <c r="F112" s="1">
+        <v>3</v>
+      </c>
+      <c r="G112" s="1">
         <v>4</v>
       </c>
-      <c r="E112" s="1">
-        <v>2</v>
-      </c>
-      <c r="F112" s="1">
-        <v>6</v>
-      </c>
-      <c r="G112" s="1">
-        <v>6</v>
-      </c>
       <c r="H112" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I112" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I112" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3125</v>
       </c>
       <c r="D113" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E113" s="1">
         <v>4</v>
       </c>
       <c r="F113" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G113" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H113" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
       <c r="I113" s="3">
-        <v>3.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>3.3250000000000002</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D114" s="1">
         <v>4</v>
       </c>
       <c r="E114" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F114" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G114" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H114" s="3">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I114" s="3">
-        <v>5</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>194</v>
+        <v>68</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>3.2749999999999995</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D115" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E115" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F115" s="1">
         <v>2</v>
       </c>
       <c r="G115" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>5.4</v>
+        <v>4.5</v>
       </c>
       <c r="I115" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>2.9124999999999996</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D116" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E116" s="1">
         <v>1</v>
       </c>
       <c r="F116" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G116" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H116" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I116" s="3">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
+        <v>3.2749999999999995</v>
+      </c>
+      <c r="D117" s="1">
+        <v>2</v>
+      </c>
+      <c r="E117" s="1">
+        <v>2</v>
+      </c>
+      <c r="F117" s="1">
+        <v>2</v>
+      </c>
+      <c r="G117" s="1">
+        <v>3</v>
+      </c>
+      <c r="H117" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="I117" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B118" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C118" s="5">
+        <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
+        <v>2.9124999999999996</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1</v>
+      </c>
+      <c r="E118" s="1">
+        <v>1</v>
+      </c>
+      <c r="F118" s="1">
+        <v>0</v>
+      </c>
+      <c r="G118" s="1">
+        <v>1</v>
+      </c>
+      <c r="H118" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I118" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B119" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C119" s="5">
+        <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
         <v>2.6375000000000002</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D119" s="1">
         <v>0</v>
       </c>
-      <c r="E117" s="1">
+      <c r="E119" s="1">
         <v>0</v>
       </c>
-      <c r="F117" s="1">
+      <c r="F119" s="1">
         <v>0</v>
       </c>
-      <c r="G117" s="1">
+      <c r="G119" s="1">
         <v>0</v>
       </c>
-      <c r="H117" s="3">
+      <c r="H119" s="3">
         <v>7.6</v>
       </c>
-      <c r="I117" s="3">
+      <c r="I119" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 99 "Ladrones con clase"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CB9AFF-3BED-4C8D-8644-23835D78455F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DC0781-2B61-4081-970E-75598A6F0673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="200">
   <si>
     <t>Película</t>
   </si>
@@ -1164,6 +1164,9 @@
   </si>
   <si>
     <t>Recluta</t>
+  </si>
+  <si>
+    <t>Ladrones con clase</t>
   </si>
 </sst>
 </file>
@@ -1173,7 +1176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1209,12 +1212,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1258,7 +1255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1282,51 +1279,15 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1367,6 +1328,45 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1493,48 +1493,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M67" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M67" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B2:M67" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M67">
     <sortCondition descending="1" ref="C2:C67"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{D20FF574-119A-4C5C-B6E2-E6116B88CECE}" name="Puntuación total" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{D20FF574-119A-4C5C-B6E2-E6116B88CECE}" name="Puntuación total" dataDxfId="10">
       <calculatedColumnFormula>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8DEB5362-455C-4BD9-AC5C-697A0CD42F56}" name="Adicción" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{E96E9843-A8C4-46F1-B720-AECB465AA377}" name="Visualmente" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{4403B32D-52FF-4AC4-9D4C-D3F597FF7C4A}" name="Impresión personal" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{98819486-D7B4-49C2-9DBA-8EF8CB45E089}" name="Audio" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{AE89980C-F672-4D83-BC6C-9D834B9DCB47}" name="IMDb" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{CDFF34D7-6389-437E-B3A8-EABF3538508F}" name="Filmaffinity" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{56E55214-A8DF-4868-B9DD-DE618A22CB0B}" name="N" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{B4467319-F04C-4E05-AF98-FABFAC9071D9}" name="P" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{9719DF8A-39E9-4708-BA0C-589DA380A38E}" name="D" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{500D2897-05EF-4DC7-9723-D302899DED5C}" name="M" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{8DEB5362-455C-4BD9-AC5C-697A0CD42F56}" name="Adicción" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{E96E9843-A8C4-46F1-B720-AECB465AA377}" name="Visualmente" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{4403B32D-52FF-4AC4-9D4C-D3F597FF7C4A}" name="Impresión personal" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{98819486-D7B4-49C2-9DBA-8EF8CB45E089}" name="Audio" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{AE89980C-F672-4D83-BC6C-9D834B9DCB47}" name="IMDb" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{CDFF34D7-6389-437E-B3A8-EABF3538508F}" name="Filmaffinity" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{56E55214-A8DF-4868-B9DD-DE618A22CB0B}" name="N" dataDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{B4467319-F04C-4E05-AF98-FABFAC9071D9}" name="P" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{9719DF8A-39E9-4708-BA0C-589DA380A38E}" name="D" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{500D2897-05EF-4DC7-9723-D302899DED5C}" name="M" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I119" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I119" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I119">
-    <sortCondition descending="1" ref="C2:C119"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I120" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:I120" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I120">
+    <sortCondition descending="1" ref="C2:C120"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{6C6ED398-D2C9-428D-BF53-EA4F14903295}" name="Puntuación total" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{6C6ED398-D2C9-428D-BF53-EA4F14903295}" name="Puntuación total" dataDxfId="20">
       <calculatedColumnFormula>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{23B9D8F5-026D-4193-8AE6-5F1DA8430A6D}" name="Visualmente" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{6D046514-7226-41C1-B7E5-3CDF91CE1FE6}" name="Impresión personal" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{31F9BA2E-487F-484E-8E53-40465539C756}" name="Ritmo" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{64A01C2F-A4B0-4AD2-9AFC-C73A75D660A7}" name="Audio" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{1D59F2E8-C7B0-4BBF-94F0-20411C4104C9}" name="IMDb" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{29CE3653-810C-46DD-B239-92B468054CBE}" name="Filmaffinity" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{23B9D8F5-026D-4193-8AE6-5F1DA8430A6D}" name="Visualmente" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{6D046514-7226-41C1-B7E5-3CDF91CE1FE6}" name="Impresión personal" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{31F9BA2E-487F-484E-8E53-40465539C756}" name="Ritmo" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{64A01C2F-A4B0-4AD2-9AFC-C73A75D660A7}" name="Audio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{1D59F2E8-C7B0-4BBF-94F0-20411C4104C9}" name="IMDb" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{29CE3653-810C-46DD-B239-92B468054CBE}" name="Filmaffinity" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1967,8 +1967,8 @@
   </sheetPr>
   <dimension ref="B2:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M67" sqref="M67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2032,7 +2032,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -2066,7 +2066,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -2099,7 +2099,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2135,7 +2135,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2171,7 +2171,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2205,7 +2205,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2238,7 +2238,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2271,7 +2271,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2304,7 +2304,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2337,7 +2337,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2372,7 +2372,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2407,7 +2407,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2440,7 +2440,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2473,7 +2473,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2508,7 +2508,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2541,7 +2541,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2574,7 +2574,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2607,7 +2607,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2638,7 +2638,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2671,7 +2671,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2704,7 +2704,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2737,7 +2737,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2770,7 +2770,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2803,7 +2803,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2836,7 +2836,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2869,7 +2869,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2902,7 +2902,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2937,7 +2937,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -2970,7 +2970,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D31" s="1">
@@ -3003,7 +3003,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D32" s="1">
@@ -3036,7 +3036,7 @@
         <v>198</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5625</v>
       </c>
       <c r="D33" s="1">
@@ -3069,7 +3069,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D34" s="1">
@@ -3105,7 +3105,7 @@
         <v>105</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.5249999999999995</v>
       </c>
       <c r="D35" s="1">
@@ -3140,7 +3140,7 @@
         <v>141</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D36" s="1">
@@ -3173,7 +3173,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.4874999999999989</v>
       </c>
       <c r="D37" s="1">
@@ -3205,7 +3205,7 @@
         <v>50</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D38" s="1">
@@ -3237,7 +3237,7 @@
         <v>185</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D39" s="1">
@@ -3270,7 +3270,7 @@
         <v>80</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D40" s="1">
@@ -3303,7 +3303,7 @@
         <v>115</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D41" s="1">
@@ -3336,7 +3336,7 @@
         <v>29</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D42" s="1">
@@ -3371,7 +3371,7 @@
         <v>22</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D43" s="1">
@@ -3403,7 +3403,7 @@
         <v>140</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D44" s="1">
@@ -3436,7 +3436,7 @@
         <v>45</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D45" s="1">
@@ -3469,7 +3469,7 @@
         <v>27</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D46" s="1">
@@ -3503,7 +3503,7 @@
         <v>49</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D47" s="1">
@@ -3536,7 +3536,7 @@
         <v>71</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D48" s="1">
@@ -3571,7 +3571,7 @@
         <v>76</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D49" s="1">
@@ -3604,7 +3604,7 @@
         <v>44</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D50" s="1">
@@ -3636,7 +3636,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D51" s="1">
@@ -3668,7 +3668,7 @@
         <v>148</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D52" s="1">
@@ -3701,7 +3701,7 @@
         <v>153</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D53" s="1">
@@ -3734,7 +3734,7 @@
         <v>17</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D54" s="1">
@@ -3766,7 +3766,7 @@
         <v>18</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D55" s="1">
@@ -3798,7 +3798,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D56" s="1">
@@ -3831,7 +3831,7 @@
         <v>106</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D57" s="1">
@@ -3866,7 +3866,7 @@
         <v>30</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D58" s="1">
@@ -3899,7 +3899,7 @@
         <v>13</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D59" s="1">
@@ -3932,7 +3932,7 @@
         <v>32</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D60" s="1">
@@ -3967,7 +3967,7 @@
         <v>42</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D61" s="1">
@@ -4000,7 +4000,7 @@
         <v>11</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D62" s="1">
@@ -4033,7 +4033,7 @@
         <v>89</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D63" s="1">
@@ -4066,7 +4066,7 @@
         <v>99</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D64" s="1">
@@ -4099,7 +4099,7 @@
         <v>180</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,F65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>5.7625000000000002</v>
       </c>
       <c r="D65" s="1">
@@ -4132,7 +4132,7 @@
         <v>91</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,F66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>5.4625000000000004</v>
       </c>
       <c r="D66" s="1">
@@ -4164,7 +4164,7 @@
         <v>36</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
         <v>4.5874999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -4213,10 +4213,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K119"/>
+  <dimension ref="B2:K120"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C119" sqref="C119"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4265,7 +4265,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4293,7 +4293,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4321,7 +4321,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4348,7 +4348,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4375,7 +4375,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4402,7 +4402,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4429,7 +4429,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4456,7 +4456,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4483,7 +4483,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4510,7 +4510,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4537,7 +4537,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4564,7 +4564,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4591,7 +4591,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4618,7 +4618,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4645,7 +4645,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4672,7 +4672,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4699,7 +4699,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4726,7 +4726,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4753,7 +4753,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4780,7 +4780,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4807,7 +4807,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4834,7 +4834,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4861,7 +4861,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4888,7 +4888,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4915,7 +4915,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4942,7 +4942,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7750000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -4969,7 +4969,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D29" s="1">
@@ -4996,7 +4996,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D30" s="1">
@@ -5023,7 +5023,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -5050,7 +5050,7 @@
         <v>94</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D32" s="1">
@@ -5077,7 +5077,7 @@
         <v>97</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.6875</v>
       </c>
       <c r="D33" s="1">
@@ -5104,7 +5104,7 @@
         <v>123</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D34" s="1">
@@ -5131,7 +5131,7 @@
         <v>37</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D35" s="1">
@@ -5158,7 +5158,7 @@
         <v>67</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D36" s="1">
@@ -5185,7 +5185,7 @@
         <v>62</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.5625</v>
       </c>
       <c r="D37" s="1">
@@ -5212,7 +5212,7 @@
         <v>55</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D38" s="1">
@@ -5239,7 +5239,7 @@
         <v>69</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D39" s="1">
@@ -5266,7 +5266,7 @@
         <v>132</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D40" s="1">
@@ -5293,7 +5293,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
@@ -5320,7 +5320,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
@@ -5347,7 +5347,7 @@
         <v>100</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D43" s="1">
@@ -5374,7 +5374,7 @@
         <v>131</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D44" s="1">
@@ -5401,7 +5401,7 @@
         <v>175</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D45" s="1">
@@ -5428,7 +5428,7 @@
         <v>52</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D46" s="1">
@@ -5455,7 +5455,7 @@
         <v>165</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D47" s="1">
@@ -5482,7 +5482,7 @@
         <v>111</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.3</v>
       </c>
       <c r="D48" s="1">
@@ -5509,7 +5509,7 @@
         <v>103</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D49" s="1">
@@ -5536,7 +5536,7 @@
         <v>181</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -5563,7 +5563,7 @@
         <v>147</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
         <v>7.2374999999999998</v>
       </c>
       <c r="D51" s="1">
@@ -5590,7 +5590,7 @@
         <v>59</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
         <v>7.2250000000000005</v>
       </c>
       <c r="D52" s="1">
@@ -5617,7 +5617,7 @@
         <v>65</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
         <v>7.2125000000000004</v>
       </c>
       <c r="D53" s="1">
@@ -5644,7 +5644,7 @@
         <v>146</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
         <v>7.2124999999999995</v>
       </c>
       <c r="D54" s="1">
@@ -5671,7 +5671,7 @@
         <v>53</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -5698,7 +5698,7 @@
         <v>104</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.1375000000000011</v>
       </c>
       <c r="D56" s="1">
@@ -5725,7 +5725,7 @@
         <v>40</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.1250000000000009</v>
       </c>
       <c r="D57" s="1">
@@ -5752,7 +5752,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.125</v>
       </c>
       <c r="D58" s="1">
@@ -5779,7 +5779,7 @@
         <v>133</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.0875000000000004</v>
       </c>
       <c r="D59" s="1">
@@ -5806,7 +5806,7 @@
         <v>98</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D60" s="1">
@@ -5833,7 +5833,7 @@
         <v>171</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D61" s="1">
@@ -5860,7 +5860,7 @@
         <v>110</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D62" s="1">
@@ -5887,7 +5887,7 @@
         <v>143</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D63" s="1">
@@ -5914,7 +5914,7 @@
         <v>177</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>7.0749999999999993</v>
       </c>
       <c r="D64" s="1">
@@ -5941,7 +5941,7 @@
         <v>176</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>7.05</v>
       </c>
       <c r="D65" s="1">
@@ -5968,7 +5968,7 @@
         <v>95</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
         <v>6.9375</v>
       </c>
       <c r="D66" s="1">
@@ -5995,7 +5995,7 @@
         <v>164</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D67" s="1">
@@ -6022,7 +6022,7 @@
         <v>157</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D68" s="1">
@@ -6049,7 +6049,7 @@
         <v>88</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D69" s="1">
@@ -6076,7 +6076,7 @@
         <v>184</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D70" s="1">
@@ -6103,7 +6103,7 @@
         <v>119</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
         <v>6.85</v>
       </c>
       <c r="D71" s="1">
@@ -6130,7 +6130,7 @@
         <v>196</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
         <v>6.7999999999999989</v>
       </c>
       <c r="D72" s="1">
@@ -6157,7 +6157,7 @@
         <v>57</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
         <v>6.6999999999999993</v>
       </c>
       <c r="D73" s="1">
@@ -6184,7 +6184,7 @@
         <v>87</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
         <v>6.6875</v>
       </c>
       <c r="D74" s="1">
@@ -6211,7 +6211,7 @@
         <v>41</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
         <v>6.6124999999999989</v>
       </c>
       <c r="D75" s="1">
@@ -6238,7 +6238,7 @@
         <v>117</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D76" s="1">
@@ -6265,7 +6265,7 @@
         <v>179</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D77" s="1">
@@ -6292,7 +6292,7 @@
         <v>168</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
         <v>6.5499999999999989</v>
       </c>
       <c r="D78" s="1">
@@ -6319,7 +6319,7 @@
         <v>197</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
         <v>6.5375000000000005</v>
       </c>
       <c r="D79" s="1">
@@ -6346,7 +6346,7 @@
         <v>183</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D80" s="1">
@@ -6373,7 +6373,7 @@
         <v>188</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
         <v>6.35</v>
       </c>
       <c r="D81" s="1">
@@ -6400,7 +6400,7 @@
         <v>134</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
         <v>6.3125</v>
       </c>
       <c r="D82" s="1">
@@ -6427,7 +6427,7 @@
         <v>144</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D83" s="1">
@@ -6454,7 +6454,7 @@
         <v>64</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D84" s="1">
@@ -6481,7 +6481,7 @@
         <v>75</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
         <v>6.2125000000000004</v>
       </c>
       <c r="D85" s="1">
@@ -6508,7 +6508,7 @@
         <v>19</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
         <v>6.2124999999999995</v>
       </c>
       <c r="D86" s="1">
@@ -6535,7 +6535,7 @@
         <v>101</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
         <v>6.15</v>
       </c>
       <c r="D87" s="1">
@@ -6562,7 +6562,7 @@
         <v>158</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
         <v>6.0874999999999995</v>
       </c>
       <c r="D88" s="1">
@@ -6589,7 +6589,7 @@
         <v>160</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
         <v>6.05</v>
       </c>
       <c r="D89" s="1">
@@ -6616,7 +6616,7 @@
         <v>159</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
         <v>5.9499999999999993</v>
       </c>
       <c r="D90" s="1">
@@ -6643,7 +6643,7 @@
         <v>195</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
         <v>5.8875000000000011</v>
       </c>
       <c r="D91" s="1">
@@ -6670,7 +6670,7 @@
         <v>186</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
         <v>5.8125000000000009</v>
       </c>
       <c r="D92" s="1">
@@ -6697,7 +6697,7 @@
         <v>113</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
         <v>5.7374999999999989</v>
       </c>
       <c r="D93" s="1">
@@ -6724,7 +6724,7 @@
         <v>187</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
         <v>5.7250000000000005</v>
       </c>
       <c r="D94" s="1">
@@ -6751,7 +6751,7 @@
         <v>26</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
         <v>5.6749999999999998</v>
       </c>
       <c r="D95" s="1">
@@ -6778,7 +6778,7 @@
         <v>149</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D96" s="1">
@@ -6805,7 +6805,7 @@
         <v>156</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D97" s="1">
@@ -6832,7 +6832,7 @@
         <v>166</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D98" s="1">
@@ -6859,7 +6859,7 @@
         <v>191</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D99" s="1">
@@ -6886,7 +6886,7 @@
         <v>190</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
         <v>5.375</v>
       </c>
       <c r="D100" s="1">
@@ -6913,7 +6913,7 @@
         <v>182</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
         <v>5.2875000000000005</v>
       </c>
       <c r="D101" s="1">
@@ -6940,7 +6940,7 @@
         <v>74</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
         <v>5.1875</v>
       </c>
       <c r="D102" s="1">
@@ -6967,7 +6967,7 @@
         <v>145</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
         <v>5.1124999999999998</v>
       </c>
       <c r="D103" s="1">
@@ -6994,7 +6994,7 @@
         <v>21</v>
       </c>
       <c r="C104" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
         <v>5.05</v>
       </c>
       <c r="D104" s="1">
@@ -7021,7 +7021,7 @@
         <v>169</v>
       </c>
       <c r="C105" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
         <v>4.9874999999999998</v>
       </c>
       <c r="D105" s="1">
@@ -7048,7 +7048,7 @@
         <v>163</v>
       </c>
       <c r="C106" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
         <v>4.8499999999999996</v>
       </c>
       <c r="D106" s="1">
@@ -7075,7 +7075,7 @@
         <v>162</v>
       </c>
       <c r="C107" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
         <v>4.7875000000000005</v>
       </c>
       <c r="D107" s="1">
@@ -7102,7 +7102,7 @@
         <v>154</v>
       </c>
       <c r="C108" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
         <v>4.5999999999999996</v>
       </c>
       <c r="D108" s="1">
@@ -7129,7 +7129,7 @@
         <v>135</v>
       </c>
       <c r="C109" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
         <v>4.5874999999999995</v>
       </c>
       <c r="D109" s="1">
@@ -7156,7 +7156,7 @@
         <v>161</v>
       </c>
       <c r="C110" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
         <v>4.4249999999999998</v>
       </c>
       <c r="D110" s="1">
@@ -7183,7 +7183,7 @@
         <v>114</v>
       </c>
       <c r="C111" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
         <v>4.4124999999999996</v>
       </c>
       <c r="D111" s="1">
@@ -7210,7 +7210,7 @@
         <v>150</v>
       </c>
       <c r="C112" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
         <v>4.3374999999999995</v>
       </c>
       <c r="D112" s="1">
@@ -7237,7 +7237,7 @@
         <v>173</v>
       </c>
       <c r="C113" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
         <v>4.3125</v>
       </c>
       <c r="D113" s="1">
@@ -7264,7 +7264,7 @@
         <v>167</v>
       </c>
       <c r="C114" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
         <v>4.2749999999999995</v>
       </c>
       <c r="D114" s="1">
@@ -7291,7 +7291,7 @@
         <v>68</v>
       </c>
       <c r="C115" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
         <v>4.1124999999999998</v>
       </c>
       <c r="D115" s="1">
@@ -7314,110 +7314,137 @@
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="2" t="s">
-        <v>189</v>
+      <c r="B116" s="9" t="s">
+        <v>199</v>
       </c>
       <c r="C116" s="5">
-        <f t="shared" si="3"/>
-        <v>3.3250000000000002</v>
+        <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D116" s="1">
+        <v>3</v>
+      </c>
+      <c r="E116" s="1">
+        <v>3</v>
+      </c>
+      <c r="F116" s="1">
+        <v>3</v>
+      </c>
+      <c r="G116" s="1">
         <v>4</v>
       </c>
-      <c r="E116" s="1">
-        <v>1</v>
-      </c>
-      <c r="F116" s="1">
-        <v>2</v>
-      </c>
-      <c r="G116" s="1">
-        <v>2</v>
-      </c>
       <c r="H116" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I116" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C117" s="5">
-        <f t="shared" si="3"/>
-        <v>3.2749999999999995</v>
+        <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D117" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E117" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F117" s="1">
         <v>2</v>
       </c>
       <c r="G117" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H117" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I117" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C118" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D118" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E118" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F118" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G118" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H118" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I118" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C119" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F119" s="1">
         <v>0</v>
       </c>
       <c r="G119" s="1">
+        <v>1</v>
+      </c>
+      <c r="H119" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I119" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B120" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C120" s="5">
+        <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D120" s="1">
         <v>0</v>
       </c>
-      <c r="H119" s="3">
+      <c r="E120" s="1">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1">
+        <v>0</v>
+      </c>
+      <c r="G120" s="1">
+        <v>0</v>
+      </c>
+      <c r="H120" s="3">
         <v>7.6</v>
       </c>
-      <c r="I119" s="3">
+      <c r="I120" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 100 "Troll 2"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DC0781-2B61-4081-970E-75598A6F0673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4ECC1F-3122-4245-BA62-8D404FDF3623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="201">
   <si>
     <t>Película</t>
   </si>
@@ -1167,6 +1167,9 @@
   </si>
   <si>
     <t>Ladrones con clase</t>
+  </si>
+  <si>
+    <t>Troll 2</t>
   </si>
 </sst>
 </file>
@@ -1255,7 +1258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1279,15 +1282,51 @@
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Énfasis1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i val="0"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1328,45 +1367,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <i val="0"/>
-      </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1493,48 +1493,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M67" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M67" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="B2:M67" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M67">
     <sortCondition descending="1" ref="C2:C67"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D20FF574-119A-4C5C-B6E2-E6116B88CECE}" name="Puntuación total" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{D20FF574-119A-4C5C-B6E2-E6116B88CECE}" name="Puntuación total" dataDxfId="20">
       <calculatedColumnFormula>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8DEB5362-455C-4BD9-AC5C-697A0CD42F56}" name="Adicción" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E96E9843-A8C4-46F1-B720-AECB465AA377}" name="Visualmente" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{4403B32D-52FF-4AC4-9D4C-D3F597FF7C4A}" name="Impresión personal" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{98819486-D7B4-49C2-9DBA-8EF8CB45E089}" name="Audio" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{AE89980C-F672-4D83-BC6C-9D834B9DCB47}" name="IMDb" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{CDFF34D7-6389-437E-B3A8-EABF3538508F}" name="Filmaffinity" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{56E55214-A8DF-4868-B9DD-DE618A22CB0B}" name="N" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{B4467319-F04C-4E05-AF98-FABFAC9071D9}" name="P" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{9719DF8A-39E9-4708-BA0C-589DA380A38E}" name="D" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{500D2897-05EF-4DC7-9723-D302899DED5C}" name="M" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{8DEB5362-455C-4BD9-AC5C-697A0CD42F56}" name="Adicción" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{E96E9843-A8C4-46F1-B720-AECB465AA377}" name="Visualmente" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{4403B32D-52FF-4AC4-9D4C-D3F597FF7C4A}" name="Impresión personal" dataDxfId="17"/>
+    <tableColumn id="7" xr3:uid="{98819486-D7B4-49C2-9DBA-8EF8CB45E089}" name="Audio" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{AE89980C-F672-4D83-BC6C-9D834B9DCB47}" name="IMDb" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{CDFF34D7-6389-437E-B3A8-EABF3538508F}" name="Filmaffinity" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{56E55214-A8DF-4868-B9DD-DE618A22CB0B}" name="N" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{B4467319-F04C-4E05-AF98-FABFAC9071D9}" name="P" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{9719DF8A-39E9-4708-BA0C-589DA380A38E}" name="D" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{500D2897-05EF-4DC7-9723-D302899DED5C}" name="M" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I120" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B2:I120" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I120">
-    <sortCondition descending="1" ref="C2:C120"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I121" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I121" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I121">
+    <sortCondition descending="1" ref="C2:C121"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{6C6ED398-D2C9-428D-BF53-EA4F14903295}" name="Puntuación total" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{6C6ED398-D2C9-428D-BF53-EA4F14903295}" name="Puntuación total" dataDxfId="6">
       <calculatedColumnFormula>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{23B9D8F5-026D-4193-8AE6-5F1DA8430A6D}" name="Visualmente" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{6D046514-7226-41C1-B7E5-3CDF91CE1FE6}" name="Impresión personal" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{31F9BA2E-487F-484E-8E53-40465539C756}" name="Ritmo" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{64A01C2F-A4B0-4AD2-9AFC-C73A75D660A7}" name="Audio" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1D59F2E8-C7B0-4BBF-94F0-20411C4104C9}" name="IMDb" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{29CE3653-810C-46DD-B239-92B468054CBE}" name="Filmaffinity" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{23B9D8F5-026D-4193-8AE6-5F1DA8430A6D}" name="Visualmente" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6D046514-7226-41C1-B7E5-3CDF91CE1FE6}" name="Impresión personal" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{31F9BA2E-487F-484E-8E53-40465539C756}" name="Ritmo" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{64A01C2F-A4B0-4AD2-9AFC-C73A75D660A7}" name="Audio" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{1D59F2E8-C7B0-4BBF-94F0-20411C4104C9}" name="IMDb" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{29CE3653-810C-46DD-B239-92B468054CBE}" name="Filmaffinity" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4164,7 +4164,7 @@
         <v>36</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
         <v>4.5874999999999995</v>
       </c>
       <c r="D67" s="1">
@@ -4213,10 +4213,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K120"/>
+  <dimension ref="B2:K121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+      <selection activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6370,38 +6370,38 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.35</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D81" s="1">
         <v>7</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
       </c>
       <c r="G81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H81" s="3">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="I81" s="3">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.3125</v>
+        <v>6.35</v>
       </c>
       <c r="D82" s="1">
         <v>7</v>
@@ -6410,48 +6410,48 @@
         <v>6</v>
       </c>
       <c r="F82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G82" s="1">
         <v>6</v>
       </c>
       <c r="H82" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I82" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E83" s="1">
         <v>6</v>
       </c>
       <c r="F83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H83" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I83" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
@@ -6461,142 +6461,142 @@
         <v>6</v>
       </c>
       <c r="E84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H84" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I84" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D85" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F85" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G85" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I85" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D86" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" s="1">
         <v>8</v>
       </c>
       <c r="G86" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H86" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I86" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F87" s="1">
         <v>8</v>
       </c>
       <c r="G87" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H87" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I87" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D88" s="1">
         <v>7</v>
       </c>
       <c r="E88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G88" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H88" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I88" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D89" s="1">
         <v>7</v>
       </c>
       <c r="E89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F89" s="1">
         <v>7</v>
@@ -6605,100 +6605,100 @@
         <v>7</v>
       </c>
       <c r="H89" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I89" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E90" s="1">
         <v>6</v>
       </c>
       <c r="F90" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G90" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H90" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I90" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.8875000000000011</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D91" s="1">
         <v>6</v>
       </c>
       <c r="E91" s="1">
+        <v>6</v>
+      </c>
+      <c r="F91" s="1">
+        <v>8</v>
+      </c>
+      <c r="G91" s="1">
         <v>5</v>
       </c>
-      <c r="F91" s="1">
-        <v>6</v>
-      </c>
-      <c r="G91" s="1">
-        <v>6</v>
-      </c>
       <c r="H91" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I91" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>5.8125000000000009</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D92" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E92" s="1">
         <v>5</v>
       </c>
       <c r="F92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G92" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H92" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I92" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D93" s="1">
         <v>7</v>
@@ -6707,25 +6707,25 @@
         <v>5</v>
       </c>
       <c r="F93" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G93" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H93" s="3">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="I93" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D94" s="1">
         <v>7</v>
@@ -6737,37 +6737,37 @@
         <v>4</v>
       </c>
       <c r="G94" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H94" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I94" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D95" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E95" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F95" s="1">
+        <v>4</v>
+      </c>
+      <c r="G95" s="1">
         <v>5</v>
       </c>
-      <c r="G95" s="1">
-        <v>6</v>
-      </c>
       <c r="H95" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I95" s="3">
         <v>6.4</v>
@@ -6775,50 +6775,50 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D96" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E96" s="1">
+        <v>3</v>
+      </c>
+      <c r="F96" s="1">
         <v>5</v>
       </c>
-      <c r="F96" s="1">
-        <v>6</v>
-      </c>
       <c r="G96" s="1">
         <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I96" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D97" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
         <v>5.8</v>
@@ -6829,622 +6829,649 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D98" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E98" s="1">
         <v>6</v>
       </c>
       <c r="F98" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G98" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H98" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I98" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E99" s="1">
         <v>6</v>
       </c>
       <c r="F99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I99" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.375</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D100" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E100" s="1">
         <v>6</v>
       </c>
       <c r="F100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
       <c r="I100" s="3">
-        <v>4.8</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D101" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I101" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D102" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E102" s="1">
         <v>5</v>
       </c>
       <c r="F102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I102" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E103" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F103" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
         <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I103" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F104" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G104" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H104" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I104" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>169</v>
+        <v>21</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>4.9874999999999998</v>
+        <v>5.05</v>
       </c>
       <c r="D105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1">
         <v>3</v>
       </c>
       <c r="F105" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G105" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H105" s="3">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="I105" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D106" s="1">
+        <v>6</v>
+      </c>
+      <c r="E106" s="1">
+        <v>3</v>
+      </c>
+      <c r="F106" s="1">
         <v>5</v>
       </c>
-      <c r="E106" s="1">
-        <v>5</v>
-      </c>
-      <c r="F106" s="1">
-        <v>3</v>
-      </c>
       <c r="G106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H106" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I106" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D107" s="1">
         <v>5</v>
       </c>
       <c r="E107" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F107" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G107" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H107" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I107" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I107" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D108" s="1">
         <v>5</v>
       </c>
       <c r="E108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H108" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I108" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D109" s="1">
         <v>5</v>
       </c>
       <c r="E109" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1">
         <v>5</v>
       </c>
       <c r="G109" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H109" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I109" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D110" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E110" s="1">
         <v>4</v>
       </c>
       <c r="F110" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G110" s="1">
         <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I110" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D111" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E111" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F111" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G111" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I111" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D112" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E112" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F112" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G112" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H112" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I112" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D113" s="1">
+        <v>5</v>
+      </c>
+      <c r="E113" s="1">
         <v>3</v>
       </c>
-      <c r="E113" s="1">
-        <v>4</v>
-      </c>
       <c r="F113" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G113" s="1">
         <v>4</v>
       </c>
       <c r="H113" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I113" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D114" s="1">
+        <v>3</v>
+      </c>
+      <c r="E114" s="1">
         <v>4</v>
       </c>
-      <c r="E114" s="1">
-        <v>2</v>
-      </c>
       <c r="F114" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G114" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H114" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I114" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D115" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E115" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F115" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G115" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H115" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I115" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B116" s="9" t="s">
-        <v>199</v>
+      <c r="B116" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D116" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E116" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F116" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G116" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I116" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D117" s="1">
+        <v>3</v>
+      </c>
+      <c r="E117" s="1">
+        <v>3</v>
+      </c>
+      <c r="F117" s="1">
+        <v>3</v>
+      </c>
+      <c r="G117" s="1">
         <v>4</v>
       </c>
-      <c r="E117" s="1">
-        <v>1</v>
-      </c>
-      <c r="F117" s="1">
-        <v>2</v>
-      </c>
-      <c r="G117" s="1">
-        <v>2</v>
-      </c>
       <c r="H117" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I117" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D118" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E118" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F118" s="1">
         <v>2</v>
       </c>
       <c r="G118" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H118" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I118" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D119" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E119" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F119" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G119" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H119" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I119" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F120" s="1">
         <v>0</v>
       </c>
       <c r="G120" s="1">
+        <v>1</v>
+      </c>
+      <c r="H120" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I120" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B121" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" s="5">
+        <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D121" s="1">
         <v>0</v>
       </c>
-      <c r="H120" s="3">
+      <c r="E121" s="1">
+        <v>0</v>
+      </c>
+      <c r="F121" s="1">
+        <v>0</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0</v>
+      </c>
+      <c r="H121" s="3">
         <v>7.6</v>
       </c>
-      <c r="I120" s="3">
+      <c r="I121" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 101 "Ironman" & "El Grinch"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4ECC1F-3122-4245-BA62-8D404FDF3623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31949C0-EE7F-4191-A7CA-402651386FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="203">
   <si>
     <t>Película</t>
   </si>
@@ -1170,6 +1170,12 @@
   </si>
   <si>
     <t>Troll 2</t>
+  </si>
+  <si>
+    <t>Ironman</t>
+  </si>
+  <si>
+    <t>El Grinch</t>
   </si>
 </sst>
 </file>
@@ -1258,7 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1281,6 +1287,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1519,10 +1528,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I121" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I121" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I121">
-    <sortCondition descending="1" ref="C2:C121"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I123" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I123" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I123">
+    <sortCondition descending="1" ref="C2:C123"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4213,10 +4222,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K121"/>
+  <dimension ref="B2:K123"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C121" sqref="C121"/>
+      <selection activeCell="H123" sqref="H123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5047,95 +5056,95 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="C32" s="5">
         <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
-        <v>7.6999999999999993</v>
+        <v>7.5874999999999995</v>
       </c>
       <c r="D32" s="1">
         <v>8</v>
       </c>
       <c r="E32" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F32" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G32" s="1">
         <v>9</v>
       </c>
       <c r="H32" s="3">
-        <v>6.3</v>
+        <v>7.9</v>
       </c>
       <c r="I32" s="3">
-        <v>5</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>37</v>
       </c>
       <c r="C33" s="5">
         <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
-        <v>7.6875</v>
+        <v>7.5750000000000011</v>
       </c>
       <c r="D33" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" s="1">
         <v>9</v>
       </c>
       <c r="H33" s="3">
-        <v>5.9</v>
+        <v>7.2</v>
       </c>
       <c r="I33" s="3">
-        <v>4.7</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>123</v>
+        <v>67</v>
       </c>
       <c r="C34" s="5">
         <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
-        <v>7.5874999999999995</v>
+        <v>7.5750000000000002</v>
       </c>
       <c r="D34" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E34" s="1">
         <v>7</v>
       </c>
       <c r="F34" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G34" s="1">
         <v>9</v>
       </c>
       <c r="H34" s="3">
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="I34" s="3">
-        <v>6.9</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="C35" s="5">
         <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
-        <v>7.5750000000000011</v>
+        <v>7.5625</v>
       </c>
       <c r="D35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
         <v>8</v>
@@ -5144,202 +5153,202 @@
         <v>8</v>
       </c>
       <c r="G35" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H35" s="3">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="I35" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C36" s="5">
         <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
-        <v>7.5750000000000002</v>
+        <v>7.5624999999999991</v>
       </c>
       <c r="D36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1">
         <v>7</v>
       </c>
       <c r="F36" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H36" s="3">
-        <v>7</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I36" s="3">
-        <v>6.6</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
-        <v>62</v>
+      <c r="B37" s="9" t="s">
+        <v>201</v>
       </c>
       <c r="C37" s="5">
         <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
-        <v>7.5625</v>
+        <v>7.55</v>
       </c>
       <c r="D37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E37" s="1">
         <v>8</v>
       </c>
       <c r="F37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1">
         <v>8</v>
       </c>
       <c r="H37" s="3">
-        <v>7</v>
+        <v>7.9</v>
       </c>
       <c r="I37" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C38" s="5">
         <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
-        <v>7.5624999999999991</v>
+        <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E38" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F38" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G38" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H38" s="3">
-        <v>8.3000000000000007</v>
+        <v>6.7</v>
       </c>
       <c r="I38" s="3">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
       <c r="C39" s="5">
         <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
-        <v>7.5250000000000004</v>
+        <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E39" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" s="1">
         <v>7</v>
       </c>
       <c r="G39" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H39" s="3">
-        <v>6.7</v>
+        <v>8</v>
       </c>
       <c r="I39" s="3">
-        <v>5.8</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>132</v>
+        <v>172</v>
       </c>
       <c r="C40" s="5">
         <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
-        <v>7.5125000000000002</v>
+        <v>7.4749999999999996</v>
       </c>
       <c r="D40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F40" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G40" s="1">
         <v>8</v>
       </c>
       <c r="H40" s="3">
-        <v>8</v>
+        <v>7.3</v>
       </c>
       <c r="I40" s="3">
-        <v>7.1</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="C41" s="5">
         <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
-        <v>7.4749999999999996</v>
+        <v>7.4625000000000004</v>
       </c>
       <c r="D41" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E41" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F41" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G41" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H41" s="3">
-        <v>7.3</v>
+        <v>6.7</v>
       </c>
       <c r="I41" s="3">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C42" s="5">
         <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
-        <v>7.4625000000000004</v>
+        <v>7.4375</v>
       </c>
       <c r="D42" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E42" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F42" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G42" s="1">
         <v>9</v>
       </c>
       <c r="H42" s="3">
-        <v>6.7</v>
+        <v>5.9</v>
       </c>
       <c r="I42" s="3">
-        <v>6.3</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
@@ -5668,11 +5677,11 @@
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
-        <v>7.1499999999999995</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="D55" s="1">
         <v>8</v>
@@ -5681,217 +5690,217 @@
         <v>7</v>
       </c>
       <c r="F55" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G55" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H55" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I55" s="3">
-        <v>6.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
-        <v>7.1375000000000011</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D56" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E56" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F56" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G56" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H56" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I56" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D57" s="1">
         <v>7</v>
       </c>
       <c r="E57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G57" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H57" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I57" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I57" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
-        <v>7.125</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F58" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G58" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H58" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I58" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>7.0875000000000004</v>
+        <v>7.125</v>
       </c>
       <c r="D59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E59" s="1">
         <v>8</v>
       </c>
       <c r="F59" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G59" s="1">
         <v>7</v>
       </c>
       <c r="H59" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I59" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D60" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F60" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G60" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H60" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I60" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D61" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E61" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F61" s="1">
         <v>8</v>
       </c>
       <c r="G61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H61" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I61" s="3">
         <v>6.2</v>
-      </c>
-      <c r="I61" s="3">
-        <v>5.2</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F62" s="1">
         <v>8</v>
       </c>
       <c r="G62" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H62" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="I62" s="3">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D63" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E63" s="1">
         <v>7</v>
@@ -5900,55 +5909,55 @@
         <v>8</v>
       </c>
       <c r="G63" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H63" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I63" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
-        <v>7.0749999999999993</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D64" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E64" s="1">
         <v>7</v>
       </c>
       <c r="F64" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G64" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H64" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I64" s="3">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>7.05</v>
+        <v>7.0749999999999993</v>
       </c>
       <c r="D65" s="1">
         <v>8</v>
       </c>
       <c r="E65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" s="1">
         <v>7</v>
@@ -5957,46 +5966,46 @@
         <v>8</v>
       </c>
       <c r="H65" s="3">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="I65" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>6.9375</v>
+        <v>7.05</v>
       </c>
       <c r="D66" s="1">
         <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F66" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G66" s="1">
         <v>8</v>
       </c>
       <c r="H66" s="3">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I66" s="3">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D67" s="1">
         <v>8</v>
@@ -6008,72 +6017,72 @@
         <v>8</v>
       </c>
       <c r="G67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H67" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="I67" s="3">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D68" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E68" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F68" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G68" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H68" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I68" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D69" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E69" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F69" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G69" s="1">
         <v>8</v>
       </c>
       <c r="H69" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I69" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
@@ -6100,200 +6109,200 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D71" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E71" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G71" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H71" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I71" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.7999999999999989</v>
+        <v>6.85</v>
       </c>
       <c r="D72" s="1">
         <v>8</v>
       </c>
       <c r="E72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F72" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G72" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H72" s="3">
-        <v>5.8</v>
+        <v>7.3</v>
       </c>
       <c r="I72" s="3">
-        <v>4.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>57</v>
+        <v>196</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.6999999999999993</v>
+        <v>6.7999999999999989</v>
       </c>
       <c r="D73" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E73" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F73" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G73" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H73" s="3">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
       <c r="I73" s="3">
-        <v>7.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.6875</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D74" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E74" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F74" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G74" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H74" s="3">
-        <v>5.5</v>
+        <v>7.9</v>
       </c>
       <c r="I74" s="3">
-        <v>4.5</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6875</v>
       </c>
       <c r="D75" s="1">
         <v>8</v>
       </c>
       <c r="E75" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F75" s="1">
         <v>8</v>
       </c>
       <c r="G75" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H75" s="3">
-        <v>6.3</v>
+        <v>5.5</v>
       </c>
       <c r="I75" s="3">
-        <v>5.3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H76" s="3">
         <v>6.3</v>
       </c>
       <c r="I76" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F77" s="1">
         <v>7</v>
       </c>
       <c r="G77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I77" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D78" s="1">
         <v>8</v>
@@ -6305,82 +6314,82 @@
         <v>7</v>
       </c>
       <c r="G78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H78" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I78" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.5375000000000005</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D79" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F79" s="1">
         <v>7</v>
       </c>
       <c r="G79" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="I79" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>6.3624999999999998</v>
+        <v>6.5375000000000005</v>
       </c>
       <c r="D80" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F80" s="1">
         <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H80" s="3">
-        <v>5.9</v>
+        <v>7.1</v>
       </c>
       <c r="I80" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>200</v>
+      <c r="B81" s="9" t="s">
+        <v>202</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.3624999999999998</v>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
@@ -6389,22 +6398,22 @@
         <v>7</v>
       </c>
       <c r="H81" s="3">
-        <v>5.5</v>
+        <v>6.4</v>
       </c>
       <c r="I81" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.35</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D82" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E82" s="1">
         <v>6</v>
@@ -6413,52 +6422,52 @@
         <v>7</v>
       </c>
       <c r="G82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H82" s="3">
-        <v>6.5</v>
+        <v>5.9</v>
       </c>
       <c r="I82" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>134</v>
+        <v>200</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.3125</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D83" s="1">
         <v>7</v>
       </c>
       <c r="E83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>6.9</v>
+        <v>5.5</v>
       </c>
       <c r="I83" s="3">
-        <v>5.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>144</v>
+        <v>188</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>6.2749999999999995</v>
+        <v>6.35</v>
       </c>
       <c r="D84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E84" s="1">
         <v>6</v>
@@ -6467,28 +6476,28 @@
         <v>7</v>
       </c>
       <c r="G84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H84" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="I84" s="3">
-        <v>5.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>64</v>
+        <v>134</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E85" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
         <v>6</v>
@@ -6497,73 +6506,73 @@
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="I85" s="3">
-        <v>5.4</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E86" s="1">
         <v>6</v>
       </c>
       <c r="F86" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G86" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H86" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.3</v>
       </c>
       <c r="I86" s="3">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D87" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
         <v>7</v>
       </c>
       <c r="F87" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>4.3</v>
+        <v>6.4</v>
       </c>
       <c r="I87" s="3">
-        <v>4.0999999999999996</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>6.15</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D88" s="1">
         <v>7</v>
@@ -6578,34 +6587,34 @@
         <v>8</v>
       </c>
       <c r="H88" s="3">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I88" s="3">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>158</v>
+        <v>19</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>6.0874999999999995</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D89" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E89" s="1">
         <v>7</v>
       </c>
       <c r="F89" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G89" s="1">
         <v>7</v>
       </c>
       <c r="H89" s="3">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
       <c r="I89" s="3">
         <v>4.0999999999999996</v>
@@ -6613,11 +6622,11 @@
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>160</v>
+        <v>101</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>6.05</v>
+        <v>6.15</v>
       </c>
       <c r="D90" s="1">
         <v>7</v>
@@ -6626,133 +6635,133 @@
         <v>6</v>
       </c>
       <c r="F90" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G90" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H90" s="3">
-        <v>5.4</v>
+        <v>5</v>
       </c>
       <c r="I90" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>5.9499999999999993</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D91" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E91" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F91" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G91" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H91" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I91" s="3">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>195</v>
+        <v>160</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>5.8875000000000011</v>
+        <v>6.05</v>
       </c>
       <c r="D92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H92" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I92" s="3">
-        <v>5.7</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.8125000000000009</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D93" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E93" s="1">
+        <v>6</v>
+      </c>
+      <c r="F93" s="1">
+        <v>8</v>
+      </c>
+      <c r="G93" s="1">
         <v>5</v>
       </c>
-      <c r="F93" s="1">
+      <c r="H93" s="3">
+        <v>5.8</v>
+      </c>
+      <c r="I93" s="3">
         <v>5</v>
-      </c>
-      <c r="G93" s="1">
-        <v>7</v>
-      </c>
-      <c r="H93" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="I93" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D94" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E94" s="1">
         <v>5</v>
       </c>
       <c r="F94" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G94" s="1">
         <v>6</v>
       </c>
       <c r="H94" s="3">
-        <v>6.8</v>
+        <v>6.7</v>
       </c>
       <c r="I94" s="3">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.7250000000000005</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D95" s="1">
         <v>7</v>
@@ -6761,112 +6770,112 @@
         <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H95" s="3">
-        <v>6.7</v>
+        <v>6.2</v>
       </c>
       <c r="I95" s="3">
-        <v>6.4</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D96" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E96" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G96" s="1">
         <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="I96" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.5624999999999991</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D97" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E97" s="1">
         <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G97" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H97" s="3">
-        <v>5.8</v>
+        <v>6.7</v>
       </c>
       <c r="I97" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D98" s="1">
+        <v>8</v>
+      </c>
+      <c r="E98" s="1">
         <v>3</v>
       </c>
-      <c r="E98" s="1">
-        <v>6</v>
-      </c>
       <c r="F98" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I98" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D99" s="1">
         <v>6</v>
       </c>
       <c r="E99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" s="1">
         <v>6</v>
@@ -6875,28 +6884,28 @@
         <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I99" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D100" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E100" s="1">
         <v>6</v>
       </c>
       <c r="F100" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G100" s="1">
         <v>5</v>
@@ -6905,19 +6914,19 @@
         <v>5.8</v>
       </c>
       <c r="I100" s="3">
-        <v>5.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.375</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D101" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E101" s="1">
         <v>6</v>
@@ -6929,25 +6938,25 @@
         <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>5.6</v>
+        <v>4.8</v>
       </c>
       <c r="I101" s="3">
-        <v>4.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.2875000000000005</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D102" s="1">
         <v>5</v>
       </c>
       <c r="E102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F102" s="1">
         <v>5</v>
@@ -6956,25 +6965,25 @@
         <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
       <c r="I102" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>74</v>
+        <v>190</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.1875</v>
+        <v>5.375</v>
       </c>
       <c r="D103" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F103" s="1">
         <v>6</v>
@@ -6983,34 +6992,34 @@
         <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>4.5</v>
+        <v>5.6</v>
       </c>
       <c r="I103" s="3">
-        <v>3.5</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>145</v>
+        <v>182</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.1124999999999998</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="I104" s="3">
         <v>5.0999999999999996</v>
@@ -7018,119 +7027,119 @@
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>5.05</v>
+        <v>5.1875</v>
       </c>
       <c r="D105" s="1">
+        <v>7</v>
+      </c>
+      <c r="E105" s="1">
         <v>5</v>
       </c>
-      <c r="E105" s="1">
-        <v>3</v>
-      </c>
       <c r="F105" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H105" s="3">
-        <v>6.8</v>
+        <v>4.5</v>
       </c>
       <c r="I105" s="3">
-        <v>5.8</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>4.9874999999999998</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D106" s="1">
         <v>6</v>
       </c>
       <c r="E106" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F106" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G106" s="1">
         <v>6</v>
       </c>
       <c r="H106" s="3">
-        <v>6</v>
+        <v>5.9</v>
       </c>
       <c r="I106" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>163</v>
+        <v>21</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>4.8499999999999996</v>
+        <v>5.05</v>
       </c>
       <c r="D107" s="1">
         <v>5</v>
       </c>
       <c r="E107" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F107" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="H107" s="3">
-        <v>5.5</v>
+        <v>6.8</v>
       </c>
       <c r="I107" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.7875000000000005</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D108" s="1">
+        <v>6</v>
+      </c>
+      <c r="E108" s="1">
+        <v>3</v>
+      </c>
+      <c r="F108" s="1">
         <v>5</v>
       </c>
-      <c r="E108" s="1">
-        <v>6</v>
-      </c>
-      <c r="F108" s="1">
-        <v>6</v>
-      </c>
       <c r="G108" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>4.8</v>
+        <v>6</v>
       </c>
       <c r="I108" s="3">
-        <v>3.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.5999999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D109" s="1">
         <v>5</v>
@@ -7139,339 +7148,393 @@
         <v>5</v>
       </c>
       <c r="F109" s="1">
+        <v>3</v>
+      </c>
+      <c r="G109" s="1">
         <v>5</v>
       </c>
-      <c r="G109" s="1">
-        <v>3</v>
-      </c>
       <c r="H109" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.5</v>
       </c>
       <c r="I109" s="3">
-        <v>4</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.5874999999999995</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D110" s="1">
         <v>5</v>
       </c>
       <c r="E110" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G110" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H110" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I110" s="3">
-        <v>3.9</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D111" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E111" s="1">
+        <v>5</v>
+      </c>
+      <c r="F111" s="1">
+        <v>5</v>
+      </c>
+      <c r="G111" s="1">
+        <v>3</v>
+      </c>
+      <c r="H111" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I111" s="3">
         <v>4</v>
-      </c>
-      <c r="F111" s="1">
-        <v>6</v>
-      </c>
-      <c r="G111" s="1">
-        <v>5</v>
-      </c>
-      <c r="H111" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="I111" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.4124999999999996</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D112" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E112" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F112" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G112" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>8.1999999999999993</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I112" s="3">
-        <v>7.9</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D113" s="1">
+        <v>1</v>
+      </c>
+      <c r="E113" s="1">
+        <v>4</v>
+      </c>
+      <c r="F113" s="1">
+        <v>6</v>
+      </c>
+      <c r="G113" s="1">
         <v>5</v>
       </c>
-      <c r="E113" s="1">
-        <v>3</v>
-      </c>
-      <c r="F113" s="1">
-        <v>3</v>
-      </c>
-      <c r="G113" s="1">
-        <v>4</v>
-      </c>
       <c r="H113" s="3">
-        <v>5.9</v>
+        <v>5.5</v>
       </c>
       <c r="I113" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.3125</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D114" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E114" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F114" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G114" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H114" s="3">
-        <v>5.4</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I114" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D115" s="1">
+        <v>5</v>
+      </c>
+      <c r="E115" s="1">
+        <v>3</v>
+      </c>
+      <c r="F115" s="1">
+        <v>3</v>
+      </c>
+      <c r="G115" s="1">
         <v>4</v>
       </c>
-      <c r="E115" s="1">
-        <v>2</v>
-      </c>
-      <c r="F115" s="1">
-        <v>6</v>
-      </c>
-      <c r="G115" s="1">
-        <v>6</v>
-      </c>
       <c r="H115" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I115" s="3">
         <v>4.9000000000000004</v>
-      </c>
-      <c r="I115" s="3">
-        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.1124999999999998</v>
+        <v>4.3125</v>
       </c>
       <c r="D116" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E116" s="1">
         <v>4</v>
       </c>
       <c r="F116" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G116" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H116" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
       <c r="I116" s="3">
-        <v>3.9</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>199</v>
+        <v>167</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>3.7375000000000003</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D117" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E117" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F117" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G117" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H117" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I117" s="3">
-        <v>4.3</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>189</v>
+        <v>68</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>3.3250000000000002</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D118" s="1">
+        <v>5</v>
+      </c>
+      <c r="E118" s="1">
         <v>4</v>
-      </c>
-      <c r="E118" s="1">
-        <v>1</v>
       </c>
       <c r="F118" s="1">
         <v>2</v>
       </c>
       <c r="G118" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>5.8</v>
+        <v>4.5</v>
       </c>
       <c r="I118" s="3">
-        <v>5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>3.2749999999999995</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D119" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E119" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F119" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G119" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H119" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I119" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>2.9124999999999996</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D120" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E120" s="1">
         <v>1</v>
       </c>
       <c r="F120" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G120" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H120" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I120" s="3">
-        <v>5.9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
+        <v>3.2749999999999995</v>
+      </c>
+      <c r="D121" s="1">
+        <v>2</v>
+      </c>
+      <c r="E121" s="1">
+        <v>2</v>
+      </c>
+      <c r="F121" s="1">
+        <v>2</v>
+      </c>
+      <c r="G121" s="1">
+        <v>3</v>
+      </c>
+      <c r="H121" s="3">
+        <v>5.4</v>
+      </c>
+      <c r="I121" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B122" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C122" s="5">
+        <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
+        <v>2.9124999999999996</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1</v>
+      </c>
+      <c r="E122" s="1">
+        <v>1</v>
+      </c>
+      <c r="F122" s="1">
+        <v>0</v>
+      </c>
+      <c r="G122" s="1">
+        <v>1</v>
+      </c>
+      <c r="H122" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I122" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B123" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C123" s="5">
+        <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
         <v>2.6375000000000002</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D123" s="1">
         <v>0</v>
       </c>
-      <c r="E121" s="1">
+      <c r="E123" s="1">
         <v>0</v>
       </c>
-      <c r="F121" s="1">
+      <c r="F123" s="1">
         <v>0</v>
       </c>
-      <c r="G121" s="1">
+      <c r="G123" s="1">
         <v>0</v>
       </c>
-      <c r="H121" s="3">
+      <c r="H123" s="3">
         <v>7.6</v>
       </c>
-      <c r="I121" s="3">
+      <c r="I123" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 102 "Madame Web"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31949C0-EE7F-4191-A7CA-402651386FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA02B0-A3C7-4A8F-8D0F-EE0CBCA009CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="204">
   <si>
     <t>Película</t>
   </si>
@@ -1176,6 +1176,9 @@
   </si>
   <si>
     <t>El Grinch</t>
+  </si>
+  <si>
+    <t>Madame Web</t>
   </si>
 </sst>
 </file>
@@ -1528,10 +1531,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I123" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I123" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I123">
-    <sortCondition descending="1" ref="C2:C123"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I124" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I124" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I124">
+    <sortCondition descending="1" ref="C2:C124"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4222,10 +4225,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K123"/>
+  <dimension ref="B2:K124"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H123" sqref="H123"/>
+      <selection activeCell="H124" sqref="H124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5190,7 +5193,7 @@
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="2" t="s">
         <v>201</v>
       </c>
       <c r="C37" s="5">
@@ -6378,7 +6381,7 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="2" t="s">
         <v>202</v>
       </c>
       <c r="C81" s="5">
@@ -7107,18 +7110,18 @@
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="2" t="s">
-        <v>169</v>
+      <c r="B108" s="9" t="s">
+        <v>203</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D108" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E108" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F108" s="1">
         <v>5</v>
@@ -7127,414 +7130,441 @@
         <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I108" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D109" s="1">
+        <v>6</v>
+      </c>
+      <c r="E109" s="1">
+        <v>3</v>
+      </c>
+      <c r="F109" s="1">
         <v>5</v>
       </c>
-      <c r="E109" s="1">
-        <v>5</v>
-      </c>
-      <c r="F109" s="1">
-        <v>3</v>
-      </c>
       <c r="G109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H109" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I109" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D110" s="1">
         <v>5</v>
       </c>
       <c r="E110" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F110" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G110" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H110" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I110" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I110" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D111" s="1">
         <v>5</v>
       </c>
       <c r="E111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G111" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H111" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I111" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D112" s="1">
         <v>5</v>
       </c>
       <c r="E112" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1">
         <v>5</v>
       </c>
       <c r="G112" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H112" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I112" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D113" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E113" s="1">
         <v>4</v>
       </c>
       <c r="F113" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G113" s="1">
         <v>5</v>
       </c>
       <c r="H113" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I113" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D114" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E114" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F114" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G114" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I114" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D115" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E115" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F115" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G115" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H115" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I115" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D116" s="1">
+        <v>5</v>
+      </c>
+      <c r="E116" s="1">
         <v>3</v>
       </c>
-      <c r="E116" s="1">
-        <v>4</v>
-      </c>
       <c r="F116" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G116" s="1">
         <v>4</v>
       </c>
       <c r="H116" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I116" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D117" s="1">
+        <v>3</v>
+      </c>
+      <c r="E117" s="1">
         <v>4</v>
       </c>
-      <c r="E117" s="1">
-        <v>2</v>
-      </c>
       <c r="F117" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G117" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H117" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I117" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D118" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E118" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F118" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G118" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H118" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I118" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D119" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E119" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F119" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G119" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I119" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D120" s="1">
+        <v>3</v>
+      </c>
+      <c r="E120" s="1">
+        <v>3</v>
+      </c>
+      <c r="F120" s="1">
+        <v>3</v>
+      </c>
+      <c r="G120" s="1">
         <v>4</v>
       </c>
-      <c r="E120" s="1">
-        <v>1</v>
-      </c>
-      <c r="F120" s="1">
-        <v>2</v>
-      </c>
-      <c r="G120" s="1">
-        <v>2</v>
-      </c>
       <c r="H120" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I120" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D121" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E121" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F121" s="1">
         <v>2</v>
       </c>
       <c r="G121" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H121" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I121" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D122" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E122" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F122" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G122" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H122" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I122" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F123" s="1">
         <v>0</v>
       </c>
       <c r="G123" s="1">
+        <v>1</v>
+      </c>
+      <c r="H123" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I123" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B124" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C124" s="5">
+        <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D124" s="1">
         <v>0</v>
       </c>
-      <c r="H123" s="3">
+      <c r="E124" s="1">
+        <v>0</v>
+      </c>
+      <c r="F124" s="1">
+        <v>0</v>
+      </c>
+      <c r="G124" s="1">
+        <v>0</v>
+      </c>
+      <c r="H124" s="3">
         <v>7.6</v>
       </c>
-      <c r="I123" s="3">
+      <c r="I124" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 103 "Las Ratas: Una historia de The Witcher"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DA02B0-A3C7-4A8F-8D0F-EE0CBCA009CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA763CC3-96A5-4CEB-948C-BFE035CC7087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="205">
   <si>
     <t>Película</t>
   </si>
@@ -1179,6 +1179,9 @@
   </si>
   <si>
     <t>Madame Web</t>
+  </si>
+  <si>
+    <t>Las Ratas: Una historia de The Witcher</t>
   </si>
 </sst>
 </file>
@@ -1531,10 +1534,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I124" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I124" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I124">
-    <sortCondition descending="1" ref="C2:C124"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I125" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I125" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I125">
+    <sortCondition descending="1" ref="C2:C125"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4225,10 +4228,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K124"/>
+  <dimension ref="B2:K125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H124" sqref="H124"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K115" sqref="K115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6975,180 +6978,180 @@
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="2" t="s">
-        <v>190</v>
+      <c r="B103" s="9" t="s">
+        <v>204</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D103" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E103" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F103" s="1">
         <v>6</v>
       </c>
       <c r="G103" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H103" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I103" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D104" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H104" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I104" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D105" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1">
         <v>5</v>
       </c>
       <c r="F105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I105" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D106" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E106" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
         <v>6</v>
       </c>
       <c r="H106" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I106" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E107" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F107" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G107" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H107" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I107" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B108" s="9" t="s">
-        <v>203</v>
+      <c r="B108" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D108" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F108" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G108" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H108" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I108" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D109" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E109" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1">
         <v>5</v>
@@ -7157,414 +7160,441 @@
         <v>6</v>
       </c>
       <c r="H109" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I109" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D110" s="1">
+        <v>6</v>
+      </c>
+      <c r="E110" s="1">
+        <v>3</v>
+      </c>
+      <c r="F110" s="1">
         <v>5</v>
       </c>
-      <c r="E110" s="1">
-        <v>5</v>
-      </c>
-      <c r="F110" s="1">
-        <v>3</v>
-      </c>
       <c r="G110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I110" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D111" s="1">
         <v>5</v>
       </c>
       <c r="E111" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F111" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G111" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H111" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I111" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I111" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D112" s="1">
         <v>5</v>
       </c>
       <c r="E112" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F112" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G112" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H112" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I112" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D113" s="1">
         <v>5</v>
       </c>
       <c r="E113" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1">
         <v>5</v>
       </c>
       <c r="G113" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H113" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I113" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D114" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E114" s="1">
         <v>4</v>
       </c>
       <c r="F114" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G114" s="1">
         <v>5</v>
       </c>
       <c r="H114" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I114" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D115" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E115" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F115" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G115" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I115" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D116" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E116" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F116" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G116" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H116" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I116" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D117" s="1">
+        <v>5</v>
+      </c>
+      <c r="E117" s="1">
         <v>3</v>
       </c>
-      <c r="E117" s="1">
-        <v>4</v>
-      </c>
       <c r="F117" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G117" s="1">
         <v>4</v>
       </c>
       <c r="H117" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I117" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D118" s="1">
+        <v>3</v>
+      </c>
+      <c r="E118" s="1">
         <v>4</v>
       </c>
-      <c r="E118" s="1">
-        <v>2</v>
-      </c>
       <c r="F118" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G118" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H118" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I118" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D119" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E119" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F119" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G119" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H119" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I119" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D120" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E120" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F120" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G120" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I120" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D121" s="1">
+        <v>3</v>
+      </c>
+      <c r="E121" s="1">
+        <v>3</v>
+      </c>
+      <c r="F121" s="1">
+        <v>3</v>
+      </c>
+      <c r="G121" s="1">
         <v>4</v>
       </c>
-      <c r="E121" s="1">
-        <v>1</v>
-      </c>
-      <c r="F121" s="1">
-        <v>2</v>
-      </c>
-      <c r="G121" s="1">
-        <v>2</v>
-      </c>
       <c r="H121" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I121" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D122" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E122" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F122" s="1">
         <v>2</v>
       </c>
       <c r="G122" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H122" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I122" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D123" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E123" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F123" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G123" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H123" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I123" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124" s="1">
         <v>0</v>
       </c>
       <c r="G124" s="1">
+        <v>1</v>
+      </c>
+      <c r="H124" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I124" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B125" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C125" s="5">
+        <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D125" s="1">
         <v>0</v>
       </c>
-      <c r="H124" s="3">
+      <c r="E125" s="1">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1">
+        <v>0</v>
+      </c>
+      <c r="G125" s="1">
+        <v>0</v>
+      </c>
+      <c r="H125" s="3">
         <v>7.6</v>
       </c>
-      <c r="I124" s="3">
+      <c r="I125" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 104 "Una mente maravillosa"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA763CC3-96A5-4CEB-948C-BFE035CC7087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188B33C6-C438-445C-A302-865584F2F8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="206">
   <si>
     <t>Película</t>
   </si>
@@ -1182,6 +1182,9 @@
   </si>
   <si>
     <t>Las Ratas: Una historia de The Witcher</t>
+  </si>
+  <si>
+    <t>Una mente maravillosa</t>
   </si>
 </sst>
 </file>
@@ -1534,10 +1537,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I125" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I125" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I125">
-    <sortCondition descending="1" ref="C2:C125"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I126" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I126" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I126">
+    <sortCondition descending="1" ref="C2:C126"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4228,10 +4231,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K125"/>
+  <dimension ref="B2:K126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K115" sqref="K115"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H126" sqref="H126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5277,126 +5280,126 @@
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>172</v>
+      <c r="B40" s="9" t="s">
+        <v>205</v>
       </c>
       <c r="C40" s="5">
         <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
-        <v>7.4749999999999996</v>
+        <v>7.4875000000000007</v>
       </c>
       <c r="D40" s="1">
         <v>7</v>
       </c>
       <c r="E40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1">
         <v>8</v>
       </c>
       <c r="H40" s="3">
-        <v>7.3</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I40" s="3">
-        <v>6.2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>130</v>
+        <v>172</v>
       </c>
       <c r="C41" s="5">
         <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
-        <v>7.4625000000000004</v>
+        <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E41" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H41" s="3">
-        <v>6.7</v>
+        <v>7.3</v>
       </c>
       <c r="I41" s="3">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="C42" s="5">
         <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
-        <v>7.4375</v>
+        <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E42" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F42" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G42" s="1">
         <v>9</v>
       </c>
       <c r="H42" s="3">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="I42" s="3">
-        <v>4.7</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C43" s="5">
         <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
-        <v>7.4249999999999998</v>
+        <v>7.4375</v>
       </c>
       <c r="D43" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1">
         <v>8</v>
       </c>
       <c r="F43" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G43" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H43" s="3">
-        <v>7</v>
+        <v>5.9</v>
       </c>
       <c r="I43" s="3">
-        <v>6.4</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5">
         <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
-        <v>7.4124999999999996</v>
+        <v>7.4249999999999998</v>
       </c>
       <c r="D44" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F44" s="1">
         <v>8</v>
@@ -5405,46 +5408,46 @@
         <v>8</v>
       </c>
       <c r="H44" s="3">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="I44" s="3">
-        <v>6.5</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="C45" s="5">
         <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
-        <v>7.3624999999999989</v>
+        <v>7.4124999999999996</v>
       </c>
       <c r="D45" s="1">
         <v>8</v>
       </c>
       <c r="E45" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F45" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" s="1">
         <v>8</v>
       </c>
       <c r="H45" s="3">
-        <v>6.3</v>
+        <v>7.4</v>
       </c>
       <c r="I45" s="3">
-        <v>5.3</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>175</v>
       </c>
       <c r="C46" s="5">
         <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
-        <v>7.3500000000000005</v>
+        <v>7.3624999999999989</v>
       </c>
       <c r="D46" s="1">
         <v>8</v>
@@ -5453,25 +5456,25 @@
         <v>8</v>
       </c>
       <c r="F46" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G46" s="1">
         <v>8</v>
       </c>
       <c r="H46" s="3">
-        <v>6.6</v>
+        <v>6.3</v>
       </c>
       <c r="I46" s="3">
-        <v>5.6</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>165</v>
+        <v>52</v>
       </c>
       <c r="C47" s="5">
         <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
-        <v>7.3249999999999993</v>
+        <v>7.3500000000000005</v>
       </c>
       <c r="D47" s="1">
         <v>8</v>
@@ -5483,82 +5486,82 @@
         <v>8</v>
       </c>
       <c r="G47" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H47" s="3">
-        <v>6.8</v>
+        <v>6.6</v>
       </c>
       <c r="I47" s="3">
-        <v>6</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="C48" s="5">
         <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
-        <v>7.3</v>
+        <v>7.3249999999999993</v>
       </c>
       <c r="D48" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E48" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G48" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H48" s="3">
-        <v>6.5</v>
+        <v>6.8</v>
       </c>
       <c r="I48" s="3">
-        <v>5.4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="C49" s="5">
         <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
-        <v>7.2750000000000004</v>
+        <v>7.3</v>
       </c>
       <c r="D49" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E49" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F49" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H49" s="3">
-        <v>6.6</v>
+        <v>6.5</v>
       </c>
       <c r="I49" s="3">
-        <v>6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>181</v>
+        <v>103</v>
       </c>
       <c r="C50" s="5">
         <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E50" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F50" s="1">
         <v>8</v>
@@ -5567,25 +5570,25 @@
         <v>8</v>
       </c>
       <c r="H50" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
       <c r="I50" s="3">
-        <v>5.8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>147</v>
+        <v>181</v>
       </c>
       <c r="C51" s="5">
         <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
-        <v>7.2374999999999998</v>
+        <v>7.2750000000000004</v>
       </c>
       <c r="D51" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E51" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F51" s="1">
         <v>8</v>
@@ -5594,127 +5597,127 @@
         <v>8</v>
       </c>
       <c r="H51" s="3">
-        <v>6</v>
+        <v>6.7</v>
       </c>
       <c r="I51" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>59</v>
+        <v>147</v>
       </c>
       <c r="C52" s="5">
         <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
-        <v>7.2250000000000005</v>
+        <v>7.2374999999999998</v>
       </c>
       <c r="D52" s="1">
         <v>7</v>
       </c>
       <c r="E52" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F52" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G52" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H52" s="3">
-        <v>8.1</v>
+        <v>6</v>
       </c>
       <c r="I52" s="3">
-        <v>7.6</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C53" s="5">
         <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
-        <v>7.2125000000000004</v>
+        <v>7.2250000000000005</v>
       </c>
       <c r="D53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E53" s="1">
         <v>7</v>
       </c>
       <c r="F53" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G53" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H53" s="3">
-        <v>7.2</v>
+        <v>8.1</v>
       </c>
       <c r="I53" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>146</v>
+        <v>65</v>
       </c>
       <c r="C54" s="5">
         <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
-        <v>7.2124999999999995</v>
+        <v>7.2125000000000004</v>
       </c>
       <c r="D54" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F54" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G54" s="1">
         <v>8</v>
       </c>
       <c r="H54" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I54" s="3">
         <v>6.3</v>
-      </c>
-      <c r="I54" s="3">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>94</v>
+        <v>146</v>
       </c>
       <c r="C55" s="5">
         <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
-        <v>7.1999999999999993</v>
+        <v>7.2124999999999995</v>
       </c>
       <c r="D55" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E55" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F55" s="1">
         <v>9</v>
       </c>
       <c r="G55" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H55" s="3">
         <v>6.3</v>
       </c>
       <c r="I55" s="3">
-        <v>5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
       <c r="C56" s="5">
         <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
-        <v>7.1499999999999995</v>
+        <v>7.1999999999999993</v>
       </c>
       <c r="D56" s="1">
         <v>8</v>
@@ -5723,217 +5726,217 @@
         <v>7</v>
       </c>
       <c r="F56" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G56" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H56" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I56" s="3">
-        <v>6.6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C57" s="5">
         <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
-        <v>7.1375000000000011</v>
+        <v>7.1499999999999995</v>
       </c>
       <c r="D57" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E57" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F57" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G57" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H57" s="3">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="I57" s="3">
-        <v>6.7</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>40</v>
+        <v>104</v>
       </c>
       <c r="C58" s="5">
         <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
-        <v>7.1250000000000009</v>
+        <v>7.1375000000000011</v>
       </c>
       <c r="D58" s="1">
         <v>7</v>
       </c>
       <c r="E58" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F58" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G58" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H58" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I58" s="3">
         <v>6.7</v>
-      </c>
-      <c r="I58" s="3">
-        <v>6.6</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C59" s="5">
         <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
-        <v>7.125</v>
+        <v>7.1250000000000009</v>
       </c>
       <c r="D59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E59" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G59" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H59" s="3">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="I59" s="3">
-        <v>6</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>133</v>
+        <v>39</v>
       </c>
       <c r="C60" s="5">
         <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
-        <v>7.0875000000000004</v>
+        <v>7.125</v>
       </c>
       <c r="D60" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E60" s="1">
         <v>8</v>
       </c>
       <c r="F60" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G60" s="1">
         <v>7</v>
       </c>
       <c r="H60" s="3">
-        <v>7.1</v>
+        <v>6.5</v>
       </c>
       <c r="I60" s="3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="C61" s="5">
         <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
-        <v>7.0750000000000011</v>
+        <v>7.0875000000000004</v>
       </c>
       <c r="D61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E61" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F61" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G61" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H61" s="3">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="I61" s="3">
-        <v>6.2</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>171</v>
+        <v>98</v>
       </c>
       <c r="C62" s="5">
         <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D62" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E62" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F62" s="1">
         <v>8</v>
       </c>
       <c r="G62" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H62" s="3">
+        <v>7.2</v>
+      </c>
+      <c r="I62" s="3">
         <v>6.2</v>
-      </c>
-      <c r="I62" s="3">
-        <v>5.2</v>
       </c>
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>110</v>
+        <v>171</v>
       </c>
       <c r="C63" s="5">
         <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
-        <v>7.0750000000000002</v>
+        <v>7.0750000000000011</v>
       </c>
       <c r="D63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E63" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F63" s="1">
         <v>8</v>
       </c>
       <c r="G63" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H63" s="3">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="I63" s="3">
-        <v>5.4</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C64" s="5">
         <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D64" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E64" s="1">
         <v>7</v>
@@ -5942,55 +5945,55 @@
         <v>8</v>
       </c>
       <c r="G64" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H64" s="3">
-        <v>6.5</v>
+        <v>6.6</v>
       </c>
       <c r="I64" s="3">
-        <v>5.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="C65" s="5">
         <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
-        <v>7.0749999999999993</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D65" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E65" s="1">
         <v>7</v>
       </c>
       <c r="F65" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H65" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I65" s="3">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C66" s="5">
         <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
-        <v>7.05</v>
+        <v>7.0749999999999993</v>
       </c>
       <c r="D66" s="1">
         <v>8</v>
       </c>
       <c r="E66" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F66" s="1">
         <v>7</v>
@@ -5999,46 +6002,46 @@
         <v>8</v>
       </c>
       <c r="H66" s="3">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="I66" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
-        <v>95</v>
+        <v>176</v>
       </c>
       <c r="C67" s="5">
         <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
-        <v>6.9375</v>
+        <v>7.05</v>
       </c>
       <c r="D67" s="1">
         <v>8</v>
       </c>
       <c r="E67" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F67" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G67" s="1">
         <v>8</v>
       </c>
       <c r="H67" s="3">
-        <v>6.1</v>
+        <v>6</v>
       </c>
       <c r="I67" s="3">
-        <v>5.3</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" s="2" t="s">
-        <v>164</v>
+        <v>95</v>
       </c>
       <c r="C68" s="5">
         <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
-        <v>6.9124999999999996</v>
+        <v>6.9375</v>
       </c>
       <c r="D68" s="1">
         <v>8</v>
@@ -6050,72 +6053,72 @@
         <v>8</v>
       </c>
       <c r="G68" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H68" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="I68" s="3">
-        <v>5.5</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" s="2" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C69" s="5">
         <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
-        <v>6.8999999999999995</v>
+        <v>6.9124999999999996</v>
       </c>
       <c r="D69" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E69" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F69" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G69" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H69" s="3">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="I69" s="3">
-        <v>6.4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" s="2" t="s">
-        <v>88</v>
+        <v>157</v>
       </c>
       <c r="C70" s="5">
         <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
-        <v>6.8624999999999989</v>
+        <v>6.8999999999999995</v>
       </c>
       <c r="D70" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E70" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F70" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G70" s="1">
         <v>8</v>
       </c>
       <c r="H70" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I70" s="3">
-        <v>5.3</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" s="2" t="s">
-        <v>184</v>
+        <v>88</v>
       </c>
       <c r="C71" s="5">
         <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
@@ -6142,200 +6145,200 @@
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" s="2" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="C72" s="5">
         <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
-        <v>6.85</v>
+        <v>6.8624999999999989</v>
       </c>
       <c r="D72" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E72" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G72" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H72" s="3">
-        <v>7.3</v>
+        <v>6.3</v>
       </c>
       <c r="I72" s="3">
-        <v>6.2</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" s="2" t="s">
-        <v>196</v>
+        <v>119</v>
       </c>
       <c r="C73" s="5">
         <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
-        <v>6.7999999999999989</v>
+        <v>6.85</v>
       </c>
       <c r="D73" s="1">
         <v>8</v>
       </c>
       <c r="E73" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G73" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H73" s="3">
-        <v>5.8</v>
+        <v>7.3</v>
       </c>
       <c r="I73" s="3">
-        <v>4.8</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>57</v>
+        <v>196</v>
       </c>
       <c r="C74" s="5">
         <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
-        <v>6.6999999999999993</v>
+        <v>6.7999999999999989</v>
       </c>
       <c r="D74" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E74" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F74" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G74" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H74" s="3">
-        <v>7.9</v>
+        <v>5.8</v>
       </c>
       <c r="I74" s="3">
-        <v>7.8</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" s="2" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="C75" s="5">
         <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
-        <v>6.6875</v>
+        <v>6.6999999999999993</v>
       </c>
       <c r="D75" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E75" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F75" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G75" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H75" s="3">
-        <v>5.5</v>
+        <v>7.9</v>
       </c>
       <c r="I75" s="3">
-        <v>4.5</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
-        <v>41</v>
+        <v>87</v>
       </c>
       <c r="C76" s="5">
         <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
-        <v>6.6124999999999989</v>
+        <v>6.6875</v>
       </c>
       <c r="D76" s="1">
         <v>8</v>
       </c>
       <c r="E76" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F76" s="1">
         <v>8</v>
       </c>
       <c r="G76" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H76" s="3">
-        <v>6.3</v>
+        <v>5.5</v>
       </c>
       <c r="I76" s="3">
-        <v>5.3</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C77" s="5">
         <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
-        <v>6.5874999999999995</v>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D77" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F77" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H77" s="3">
         <v>6.3</v>
       </c>
       <c r="I77" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C78" s="5">
         <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D78" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F78" s="1">
         <v>7</v>
       </c>
       <c r="G78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H78" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I78" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C79" s="5">
         <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D79" s="1">
         <v>8</v>
@@ -6347,79 +6350,79 @@
         <v>7</v>
       </c>
       <c r="G79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H79" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I79" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C80" s="5">
         <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
-        <v>6.5375000000000005</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D80" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E80" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F80" s="1">
         <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H80" s="3">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="I80" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.3999999999999995</v>
+        <v>6.5375000000000005</v>
       </c>
       <c r="D81" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
       </c>
       <c r="G81" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H81" s="3">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="I81" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.3624999999999998</v>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D82" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E82" s="1">
         <v>6</v>
@@ -6431,25 +6434,25 @@
         <v>7</v>
       </c>
       <c r="H82" s="3">
-        <v>5.9</v>
+        <v>6.4</v>
       </c>
       <c r="I82" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D83" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E83" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F83" s="1">
         <v>7</v>
@@ -6458,46 +6461,46 @@
         <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="I83" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>6.35</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D84" s="1">
         <v>7</v>
       </c>
       <c r="E84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F84" s="1">
         <v>7</v>
       </c>
       <c r="G84" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H84" s="3">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="I84" s="3">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
-        <v>6.3125</v>
+        <v>6.35</v>
       </c>
       <c r="D85" s="1">
         <v>7</v>
@@ -6506,48 +6509,48 @@
         <v>6</v>
       </c>
       <c r="F85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G85" s="1">
         <v>6</v>
       </c>
       <c r="H85" s="3">
-        <v>6.9</v>
+        <v>6.5</v>
       </c>
       <c r="I85" s="3">
-        <v>5.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
         <v>6</v>
       </c>
       <c r="F86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I86" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
@@ -6557,142 +6560,142 @@
         <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H87" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I87" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I88" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D89" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
         <v>8</v>
       </c>
       <c r="G89" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H89" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I89" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D90" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F90" s="1">
         <v>8</v>
       </c>
       <c r="G90" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H90" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I90" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D91" s="1">
         <v>7</v>
       </c>
       <c r="E91" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G91" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H91" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I91" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D92" s="1">
         <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F92" s="1">
         <v>7</v>
@@ -6701,100 +6704,100 @@
         <v>7</v>
       </c>
       <c r="H92" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I92" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D93" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E93" s="1">
         <v>6</v>
       </c>
       <c r="F93" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G93" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H93" s="3">
-        <v>5.8</v>
+        <v>5.4</v>
       </c>
       <c r="I93" s="3">
-        <v>5</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>5.8875000000000011</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D94" s="1">
         <v>6</v>
       </c>
       <c r="E94" s="1">
+        <v>6</v>
+      </c>
+      <c r="F94" s="1">
+        <v>8</v>
+      </c>
+      <c r="G94" s="1">
         <v>5</v>
       </c>
-      <c r="F94" s="1">
-        <v>6</v>
-      </c>
-      <c r="G94" s="1">
-        <v>6</v>
-      </c>
       <c r="H94" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I94" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.8125000000000009</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D95" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E95" s="1">
         <v>5</v>
       </c>
       <c r="F95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I95" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D96" s="1">
         <v>7</v>
@@ -6803,25 +6806,25 @@
         <v>5</v>
       </c>
       <c r="F96" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G96" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H96" s="3">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="I96" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D97" s="1">
         <v>7</v>
@@ -6833,37 +6836,37 @@
         <v>4</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I97" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D98" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E98" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F98" s="1">
+        <v>4</v>
+      </c>
+      <c r="G98" s="1">
         <v>5</v>
       </c>
-      <c r="G98" s="1">
-        <v>6</v>
-      </c>
       <c r="H98" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I98" s="3">
         <v>6.4</v>
@@ -6871,50 +6874,50 @@
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D99" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E99" s="1">
+        <v>3</v>
+      </c>
+      <c r="F99" s="1">
         <v>5</v>
       </c>
-      <c r="F99" s="1">
-        <v>6</v>
-      </c>
       <c r="G99" s="1">
         <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I99" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D100" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H100" s="3">
         <v>5.8</v>
@@ -6925,260 +6928,260 @@
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D101" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E101" s="1">
         <v>6</v>
       </c>
       <c r="F101" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I101" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E102" s="1">
         <v>6</v>
       </c>
       <c r="F102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H102" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I102" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B103" s="9" t="s">
-        <v>204</v>
+      <c r="B103" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.3750000000000009</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E103" s="1">
+        <v>6</v>
+      </c>
+      <c r="F103" s="1">
         <v>5</v>
       </c>
-      <c r="F103" s="1">
-        <v>6</v>
-      </c>
       <c r="G103" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I103" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D104" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
         <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H104" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I104" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D105" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H105" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I105" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D106" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E106" s="1">
         <v>5</v>
       </c>
       <c r="F106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I106" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D107" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E107" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F107" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
         <v>6</v>
       </c>
       <c r="H107" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I107" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E108" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F108" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G108" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I108" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D109" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F109" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G109" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H109" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I109" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D110" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E110" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F110" s="1">
         <v>5</v>
@@ -7187,414 +7190,441 @@
         <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I110" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D111" s="1">
+        <v>6</v>
+      </c>
+      <c r="E111" s="1">
+        <v>3</v>
+      </c>
+      <c r="F111" s="1">
         <v>5</v>
       </c>
-      <c r="E111" s="1">
-        <v>5</v>
-      </c>
-      <c r="F111" s="1">
-        <v>3</v>
-      </c>
       <c r="G111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H111" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I111" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D112" s="1">
         <v>5</v>
       </c>
       <c r="E112" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G112" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H112" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I112" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I112" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D113" s="1">
         <v>5</v>
       </c>
       <c r="E113" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F113" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G113" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H113" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I113" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D114" s="1">
         <v>5</v>
       </c>
       <c r="E114" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F114" s="1">
         <v>5</v>
       </c>
       <c r="G114" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H114" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I114" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D115" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E115" s="1">
         <v>4</v>
       </c>
       <c r="F115" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G115" s="1">
         <v>5</v>
       </c>
       <c r="H115" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I115" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D116" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E116" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F116" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G116" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H116" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I116" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.3374999999999995</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D117" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E117" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F117" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G117" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H117" s="3">
-        <v>5.9</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I117" s="3">
-        <v>4.9000000000000004</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D118" s="1">
+        <v>5</v>
+      </c>
+      <c r="E118" s="1">
         <v>3</v>
       </c>
-      <c r="E118" s="1">
-        <v>4</v>
-      </c>
       <c r="F118" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G118" s="1">
         <v>4</v>
       </c>
       <c r="H118" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I118" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D119" s="1">
+        <v>3</v>
+      </c>
+      <c r="E119" s="1">
         <v>4</v>
       </c>
-      <c r="E119" s="1">
-        <v>2</v>
-      </c>
       <c r="F119" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G119" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H119" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I119" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D120" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E120" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F120" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G120" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H120" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I120" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D121" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E121" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F121" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G121" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I121" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D122" s="1">
+        <v>3</v>
+      </c>
+      <c r="E122" s="1">
+        <v>3</v>
+      </c>
+      <c r="F122" s="1">
+        <v>3</v>
+      </c>
+      <c r="G122" s="1">
         <v>4</v>
       </c>
-      <c r="E122" s="1">
-        <v>1</v>
-      </c>
-      <c r="F122" s="1">
-        <v>2</v>
-      </c>
-      <c r="G122" s="1">
-        <v>2</v>
-      </c>
       <c r="H122" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I122" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D123" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E123" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F123" s="1">
         <v>2</v>
       </c>
       <c r="G123" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H123" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I123" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D124" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E124" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F124" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G124" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H124" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I124" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F125" s="1">
         <v>0</v>
       </c>
       <c r="G125" s="1">
+        <v>1</v>
+      </c>
+      <c r="H125" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I125" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B126" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C126" s="5">
+        <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D126" s="1">
         <v>0</v>
       </c>
-      <c r="H125" s="3">
+      <c r="E126" s="1">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1">
+        <v>0</v>
+      </c>
+      <c r="G126" s="1">
+        <v>0</v>
+      </c>
+      <c r="H126" s="3">
         <v>7.6</v>
       </c>
-      <c r="I125" s="3">
+      <c r="I126" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 106 "Dale duro"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448B8003-8DBE-4760-89E5-1BE977709686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7D3A2D-6EB8-48A5-A9B5-12ED290A1097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="208">
   <si>
     <t>Película</t>
   </si>
@@ -1188,6 +1188,9 @@
   </si>
   <si>
     <t>Eternal</t>
+  </si>
+  <si>
+    <t>Dale duro</t>
   </si>
 </sst>
 </file>
@@ -1540,10 +1543,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I127" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I127" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I127">
-    <sortCondition descending="1" ref="C2:C127"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I128" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I128" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I128">
+    <sortCondition descending="1" ref="C2:C128"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4234,10 +4237,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K127"/>
+  <dimension ref="B2:K128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C127" sqref="C127"/>
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6741,7 +6744,7 @@
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C94" s="5">
@@ -7416,245 +7419,272 @@
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B119" s="2" t="s">
-        <v>150</v>
+      <c r="B119" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D119" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E119" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F119" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G119" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H119" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I119" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D120" s="1">
+        <v>5</v>
+      </c>
+      <c r="E120" s="1">
         <v>3</v>
       </c>
-      <c r="E120" s="1">
-        <v>4</v>
-      </c>
       <c r="F120" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G120" s="1">
         <v>4</v>
       </c>
       <c r="H120" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I120" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D121" s="1">
+        <v>3</v>
+      </c>
+      <c r="E121" s="1">
         <v>4</v>
       </c>
-      <c r="E121" s="1">
-        <v>2</v>
-      </c>
       <c r="F121" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G121" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H121" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I121" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D122" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E122" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F122" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G122" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H122" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I122" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D123" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E123" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F123" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G123" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I123" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D124" s="1">
+        <v>3</v>
+      </c>
+      <c r="E124" s="1">
+        <v>3</v>
+      </c>
+      <c r="F124" s="1">
+        <v>3</v>
+      </c>
+      <c r="G124" s="1">
         <v>4</v>
       </c>
-      <c r="E124" s="1">
-        <v>1</v>
-      </c>
-      <c r="F124" s="1">
-        <v>2</v>
-      </c>
-      <c r="G124" s="1">
-        <v>2</v>
-      </c>
       <c r="H124" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I124" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D125" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E125" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F125" s="1">
         <v>2</v>
       </c>
       <c r="G125" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H125" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I125" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D126" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E126" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F126" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G126" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H126" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I126" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F127" s="1">
         <v>0</v>
       </c>
       <c r="G127" s="1">
+        <v>1</v>
+      </c>
+      <c r="H127" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I127" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B128" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C128" s="5">
+        <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D128" s="1">
         <v>0</v>
       </c>
-      <c r="H127" s="3">
+      <c r="E128" s="1">
+        <v>0</v>
+      </c>
+      <c r="F128" s="1">
+        <v>0</v>
+      </c>
+      <c r="G128" s="1">
+        <v>0</v>
+      </c>
+      <c r="H128" s="3">
         <v>7.6</v>
       </c>
-      <c r="I127" s="3">
+      <c r="I128" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 107 "Uno para todos"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7D3A2D-6EB8-48A5-A9B5-12ED290A1097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C6CA4F-EDBD-43CC-BE5B-75B71CFDFD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="209">
   <si>
     <t>Película</t>
   </si>
@@ -1191,6 +1191,9 @@
   </si>
   <si>
     <t>Dale duro</t>
+  </si>
+  <si>
+    <t>Uno para todos</t>
   </si>
 </sst>
 </file>
@@ -1543,10 +1546,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I128" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I128" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I128">
-    <sortCondition descending="1" ref="C2:C128"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I129" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I129" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I129">
+    <sortCondition descending="1" ref="C2:C129"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4237,10 +4240,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K128"/>
+  <dimension ref="B2:K129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6528,18 +6531,18 @@
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="2" t="s">
-        <v>134</v>
+      <c r="B86" s="9" t="s">
+        <v>208</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.3125</v>
+        <v>6.35</v>
       </c>
       <c r="D86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F86" s="1">
         <v>6</v>
@@ -6548,42 +6551,42 @@
         <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I86" s="3">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E87" s="1">
         <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I87" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
@@ -6593,142 +6596,142 @@
         <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H88" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I88" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F89" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I89" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D90" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E90" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" s="1">
         <v>8</v>
       </c>
       <c r="G90" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H90" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I90" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D91" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E91" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F91" s="1">
         <v>8</v>
       </c>
       <c r="G91" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H91" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I91" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D92" s="1">
         <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G92" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H92" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I92" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>6.05</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D93" s="1">
         <v>7</v>
       </c>
       <c r="E93" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F93" s="1">
         <v>7</v>
@@ -6737,46 +6740,46 @@
         <v>7</v>
       </c>
       <c r="H93" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I93" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
         <v>6.05</v>
       </c>
       <c r="D94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E94" s="1">
         <v>6</v>
       </c>
       <c r="F94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H94" s="3">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="I94" s="3">
-        <v>5.4</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D95" s="1">
         <v>6</v>
@@ -6785,79 +6788,79 @@
         <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G95" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H95" s="3">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="I95" s="3">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>5.8875000000000011</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D96" s="1">
         <v>6</v>
       </c>
       <c r="E96" s="1">
+        <v>6</v>
+      </c>
+      <c r="F96" s="1">
+        <v>8</v>
+      </c>
+      <c r="G96" s="1">
         <v>5</v>
       </c>
-      <c r="F96" s="1">
-        <v>6</v>
-      </c>
-      <c r="G96" s="1">
-        <v>6</v>
-      </c>
       <c r="H96" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I96" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.8125000000000009</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D97" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E97" s="1">
         <v>5</v>
       </c>
       <c r="F97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I97" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D98" s="1">
         <v>7</v>
@@ -6866,25 +6869,25 @@
         <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G98" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H98" s="3">
-        <v>6.8</v>
+        <v>6.2</v>
       </c>
       <c r="I98" s="3">
-        <v>5.3</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D99" s="1">
         <v>7</v>
@@ -6896,37 +6899,37 @@
         <v>4</v>
       </c>
       <c r="G99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I99" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D100" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E100" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
+        <v>4</v>
+      </c>
+      <c r="G100" s="1">
         <v>5</v>
       </c>
-      <c r="G100" s="1">
-        <v>6</v>
-      </c>
       <c r="H100" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I100" s="3">
         <v>6.4</v>
@@ -6934,50 +6937,50 @@
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D101" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E101" s="1">
+        <v>3</v>
+      </c>
+      <c r="F101" s="1">
         <v>5</v>
       </c>
-      <c r="F101" s="1">
-        <v>6</v>
-      </c>
       <c r="G101" s="1">
         <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I101" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D102" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F102" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H102" s="3">
         <v>5.8</v>
@@ -6988,260 +6991,260 @@
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E103" s="1">
         <v>6</v>
       </c>
       <c r="F103" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G103" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H103" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I103" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
         <v>6</v>
       </c>
       <c r="F104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H104" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I104" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>5.3750000000000009</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E105" s="1">
+        <v>6</v>
+      </c>
+      <c r="F105" s="1">
         <v>5</v>
       </c>
-      <c r="F105" s="1">
-        <v>6</v>
-      </c>
       <c r="G105" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I105" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D106" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1">
         <v>6</v>
       </c>
       <c r="G106" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H106" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I106" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D107" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H107" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I107" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D108" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1">
         <v>5</v>
       </c>
       <c r="F108" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G108" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I108" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D109" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E109" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G109" s="1">
         <v>6</v>
       </c>
       <c r="H109" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I109" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E110" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F110" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G110" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I110" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D111" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E111" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F111" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G111" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H111" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I111" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D112" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E112" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1">
         <v>5</v>
@@ -7250,441 +7253,468 @@
         <v>6</v>
       </c>
       <c r="H112" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I112" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D113" s="1">
+        <v>6</v>
+      </c>
+      <c r="E113" s="1">
+        <v>3</v>
+      </c>
+      <c r="F113" s="1">
         <v>5</v>
       </c>
-      <c r="E113" s="1">
-        <v>5</v>
-      </c>
-      <c r="F113" s="1">
-        <v>3</v>
-      </c>
       <c r="G113" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H113" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I113" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D114" s="1">
         <v>5</v>
       </c>
       <c r="E114" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F114" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G114" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H114" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I114" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I114" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D115" s="1">
         <v>5</v>
       </c>
       <c r="E115" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F115" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G115" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H115" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I115" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D116" s="1">
         <v>5</v>
       </c>
       <c r="E116" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F116" s="1">
         <v>5</v>
       </c>
       <c r="G116" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H116" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I116" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D117" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E117" s="1">
         <v>4</v>
       </c>
       <c r="F117" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G117" s="1">
         <v>5</v>
       </c>
       <c r="H117" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I117" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D118" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E118" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F118" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G118" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I118" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B119" s="9" t="s">
-        <v>207</v>
+      <c r="B119" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.3375000000000004</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D119" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E119" s="1">
+        <v>0</v>
+      </c>
+      <c r="F119" s="1">
         <v>2</v>
       </c>
-      <c r="F119" s="1">
-        <v>4</v>
-      </c>
       <c r="G119" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H119" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I119" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D120" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E120" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F120" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G120" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H120" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I120" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D121" s="1">
+        <v>5</v>
+      </c>
+      <c r="E121" s="1">
         <v>3</v>
       </c>
-      <c r="E121" s="1">
-        <v>4</v>
-      </c>
       <c r="F121" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G121" s="1">
         <v>4</v>
       </c>
       <c r="H121" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I121" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D122" s="1">
+        <v>3</v>
+      </c>
+      <c r="E122" s="1">
         <v>4</v>
       </c>
-      <c r="E122" s="1">
-        <v>2</v>
-      </c>
       <c r="F122" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G122" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H122" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I122" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D123" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E123" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F123" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G123" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H123" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I123" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D124" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E124" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F124" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G124" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H124" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I124" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D125" s="1">
+        <v>3</v>
+      </c>
+      <c r="E125" s="1">
+        <v>3</v>
+      </c>
+      <c r="F125" s="1">
+        <v>3</v>
+      </c>
+      <c r="G125" s="1">
         <v>4</v>
       </c>
-      <c r="E125" s="1">
-        <v>1</v>
-      </c>
-      <c r="F125" s="1">
-        <v>2</v>
-      </c>
-      <c r="G125" s="1">
-        <v>2</v>
-      </c>
       <c r="H125" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I125" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D126" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E126" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F126" s="1">
         <v>2</v>
       </c>
       <c r="G126" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H126" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I126" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D127" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E127" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F127" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G127" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H127" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I127" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D128" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F128" s="1">
         <v>0</v>
       </c>
       <c r="G128" s="1">
+        <v>1</v>
+      </c>
+      <c r="H128" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I128" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B129" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C129" s="5">
+        <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D129" s="1">
         <v>0</v>
       </c>
-      <c r="H128" s="3">
+      <c r="E129" s="1">
+        <v>0</v>
+      </c>
+      <c r="F129" s="1">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1">
+        <v>0</v>
+      </c>
+      <c r="H129" s="3">
         <v>7.6</v>
       </c>
-      <c r="I128" s="3">
+      <c r="I129" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 108 "Code 8"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C6CA4F-EDBD-43CC-BE5B-75B71CFDFD10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27CAA75-691C-4061-AF8C-864D73B77259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -567,7 +567,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
   <si>
     <t>Película</t>
   </si>
@@ -1194,6 +1194,9 @@
   </si>
   <si>
     <t>Uno para todos</t>
+  </si>
+  <si>
+    <t>Code 8 (2019)</t>
   </si>
 </sst>
 </file>
@@ -1546,10 +1549,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I129" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I129" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I129">
-    <sortCondition descending="1" ref="C2:C129"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I130" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I130" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I130">
+    <sortCondition descending="1" ref="C2:C130"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4240,10 +4243,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K129"/>
+  <dimension ref="B2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6531,7 +6534,7 @@
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="2" t="s">
         <v>208</v>
       </c>
       <c r="C86" s="5">
@@ -6882,39 +6885,39 @@
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="2" t="s">
-        <v>113</v>
+      <c r="B99" s="9" t="s">
+        <v>209</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="D99" s="1">
         <v>7</v>
       </c>
       <c r="E99" s="1">
+        <v>6</v>
+      </c>
+      <c r="F99" s="1">
         <v>5</v>
       </c>
-      <c r="F99" s="1">
-        <v>4</v>
-      </c>
       <c r="G99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H99" s="3">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="I99" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D100" s="1">
         <v>7</v>
@@ -6926,37 +6929,37 @@
         <v>4</v>
       </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I100" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D101" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E101" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F101" s="1">
+        <v>4</v>
+      </c>
+      <c r="G101" s="1">
         <v>5</v>
       </c>
-      <c r="G101" s="1">
-        <v>6</v>
-      </c>
       <c r="H101" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I101" s="3">
         <v>6.4</v>
@@ -6964,50 +6967,50 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D102" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E102" s="1">
+        <v>3</v>
+      </c>
+      <c r="F102" s="1">
         <v>5</v>
       </c>
-      <c r="F102" s="1">
-        <v>6</v>
-      </c>
       <c r="G102" s="1">
         <v>6</v>
       </c>
       <c r="H102" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I102" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D103" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E103" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F103" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H103" s="3">
         <v>5.8</v>
@@ -7018,260 +7021,260 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D104" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E104" s="1">
         <v>6</v>
       </c>
       <c r="F104" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H104" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I104" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E105" s="1">
         <v>6</v>
       </c>
       <c r="F105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H105" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I105" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>5.3750000000000009</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E106" s="1">
+        <v>6</v>
+      </c>
+      <c r="F106" s="1">
         <v>5</v>
       </c>
-      <c r="F106" s="1">
-        <v>6</v>
-      </c>
       <c r="G106" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I106" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D107" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E107" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F107" s="1">
         <v>6</v>
       </c>
       <c r="G107" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H107" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I107" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D108" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I108" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D109" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1">
         <v>5</v>
       </c>
       <c r="F109" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G109" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I109" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D110" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E110" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F110" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G110" s="1">
         <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I110" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E111" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F111" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G111" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H111" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I111" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D112" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E112" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F112" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G112" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H112" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I112" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D113" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E113" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1">
         <v>5</v>
@@ -7280,441 +7283,468 @@
         <v>6</v>
       </c>
       <c r="H113" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I113" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D114" s="1">
+        <v>6</v>
+      </c>
+      <c r="E114" s="1">
+        <v>3</v>
+      </c>
+      <c r="F114" s="1">
         <v>5</v>
       </c>
-      <c r="E114" s="1">
-        <v>5</v>
-      </c>
-      <c r="F114" s="1">
-        <v>3</v>
-      </c>
       <c r="G114" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H114" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I114" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D115" s="1">
         <v>5</v>
       </c>
       <c r="E115" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F115" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G115" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H115" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I115" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I115" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.5999999999999996</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D116" s="1">
         <v>5</v>
       </c>
       <c r="E116" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F116" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G116" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H116" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I116" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D117" s="1">
         <v>5</v>
       </c>
       <c r="E117" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F117" s="1">
         <v>5</v>
       </c>
       <c r="G117" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H117" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I117" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D118" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E118" s="1">
         <v>4</v>
       </c>
       <c r="F118" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G118" s="1">
         <v>5</v>
       </c>
       <c r="H118" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I118" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D119" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E119" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F119" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G119" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I119" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.3375000000000004</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D120" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E120" s="1">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1">
         <v>2</v>
       </c>
-      <c r="F120" s="1">
-        <v>4</v>
-      </c>
       <c r="G120" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H120" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I120" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D121" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E121" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F121" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G121" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H121" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I121" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D122" s="1">
+        <v>5</v>
+      </c>
+      <c r="E122" s="1">
         <v>3</v>
       </c>
-      <c r="E122" s="1">
-        <v>4</v>
-      </c>
       <c r="F122" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G122" s="1">
         <v>4</v>
       </c>
       <c r="H122" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I122" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3125</v>
       </c>
       <c r="D123" s="1">
+        <v>3</v>
+      </c>
+      <c r="E123" s="1">
         <v>4</v>
       </c>
-      <c r="E123" s="1">
-        <v>2</v>
-      </c>
       <c r="F123" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G123" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H123" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I123" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D124" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E124" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F124" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G124" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H124" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I124" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D125" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E125" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F125" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G125" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H125" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I125" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D126" s="1">
+        <v>3</v>
+      </c>
+      <c r="E126" s="1">
+        <v>3</v>
+      </c>
+      <c r="F126" s="1">
+        <v>3</v>
+      </c>
+      <c r="G126" s="1">
         <v>4</v>
       </c>
-      <c r="E126" s="1">
-        <v>1</v>
-      </c>
-      <c r="F126" s="1">
-        <v>2</v>
-      </c>
-      <c r="G126" s="1">
-        <v>2</v>
-      </c>
       <c r="H126" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I126" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D127" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E127" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F127" s="1">
         <v>2</v>
       </c>
       <c r="G127" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H127" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I127" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D128" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E128" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F128" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G128" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H128" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I128" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C129" s="5">
         <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D129" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F129" s="1">
         <v>0</v>
       </c>
       <c r="G129" s="1">
+        <v>1</v>
+      </c>
+      <c r="H129" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I129" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B130" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C130" s="5">
+        <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D130" s="1">
         <v>0</v>
       </c>
-      <c r="H129" s="3">
+      <c r="E130" s="1">
+        <v>0</v>
+      </c>
+      <c r="F130" s="1">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1">
+        <v>0</v>
+      </c>
+      <c r="H130" s="3">
         <v>7.6</v>
       </c>
-      <c r="I129" s="3">
+      <c r="I130" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 109 "La monja guerrera"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27CAA75-691C-4061-AF8C-864D73B77259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEADEC7-6A35-46FA-B3B8-B8DD74EDBC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -67,6 +67,7 @@
     <author>tc={E34E6F01-0047-4D5E-A9F0-76B7D80CE842}</author>
     <author>tc={66A44D43-B718-4B72-9103-F3288A2AC23B}</author>
     <author>tc={162EA199-65BB-48FF-A9B1-580BDA0F2A25}</author>
+    <author>tc={A8DD2670-DAB9-48F0-9B69-06BCBECDF83A}</author>
     <author>tc={BC097833-5E05-4B57-A72A-B55B23EF385A}</author>
     <author>tc={D69ACFED-A245-418D-8836-7787A10A08B4}</author>
     <author>tc={FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}</author>
@@ -316,7 +317,15 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B35" authorId="28" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+    <comment ref="B35" authorId="28" shapeId="0" xr:uid="{A8DD2670-DAB9-48F0-9B69-06BCBECDF83A}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    2 temporadas</t>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="29" shapeId="0" xr:uid="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -324,7 +333,7 @@
     10 temporadas</t>
       </text>
     </comment>
-    <comment ref="B36" authorId="29" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+    <comment ref="B37" authorId="30" shapeId="0" xr:uid="{D69ACFED-A245-418D-8836-7787A10A08B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -332,7 +341,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B37" authorId="30" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+    <comment ref="B38" authorId="31" shapeId="0" xr:uid="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -340,7 +349,7 @@
     5 temporadas</t>
       </text>
     </comment>
-    <comment ref="B39" authorId="31" shapeId="0" xr:uid="{0372C847-801C-4993-BA73-8301D595FCF1}">
+    <comment ref="B40" authorId="32" shapeId="0" xr:uid="{0372C847-801C-4993-BA73-8301D595FCF1}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -348,7 +357,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B40" authorId="32" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+    <comment ref="B41" authorId="33" shapeId="0" xr:uid="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -356,7 +365,7 @@
     2 temporadas</t>
       </text>
     </comment>
-    <comment ref="B41" authorId="33" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+    <comment ref="B42" authorId="34" shapeId="0" xr:uid="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -364,7 +373,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B43" authorId="34" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+    <comment ref="B44" authorId="35" shapeId="0" xr:uid="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -372,7 +381,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="35" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+    <comment ref="B45" authorId="36" shapeId="0" xr:uid="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -380,7 +389,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B45" authorId="36" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+    <comment ref="B46" authorId="37" shapeId="0" xr:uid="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -388,7 +397,7 @@
     6 temporadas</t>
       </text>
     </comment>
-    <comment ref="B46" authorId="37" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+    <comment ref="B47" authorId="38" shapeId="0" xr:uid="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -396,7 +405,7 @@
     14 temporadas</t>
       </text>
     </comment>
-    <comment ref="B48" authorId="38" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+    <comment ref="B49" authorId="39" shapeId="0" xr:uid="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -404,7 +413,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B49" authorId="39" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+    <comment ref="B50" authorId="40" shapeId="0" xr:uid="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -412,7 +421,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B52" authorId="40" shapeId="0" xr:uid="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
+    <comment ref="B53" authorId="41" shapeId="0" xr:uid="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -420,7 +429,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B53" authorId="41" shapeId="0" xr:uid="{96839C2B-31B6-4DC0-88B7-37E650032258}">
+    <comment ref="B54" authorId="42" shapeId="0" xr:uid="{96839C2B-31B6-4DC0-88B7-37E650032258}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -428,7 +437,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B54" authorId="42" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+    <comment ref="B55" authorId="43" shapeId="0" xr:uid="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -436,7 +445,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B55" authorId="43" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+    <comment ref="B56" authorId="44" shapeId="0" xr:uid="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -444,7 +453,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B56" authorId="44" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+    <comment ref="B57" authorId="45" shapeId="0" xr:uid="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -452,7 +461,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B62" authorId="45" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+    <comment ref="B63" authorId="46" shapeId="0" xr:uid="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -460,7 +469,7 @@
     7 temporadas</t>
       </text>
     </comment>
-    <comment ref="B63" authorId="46" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+    <comment ref="B64" authorId="47" shapeId="0" xr:uid="{25B82680-662E-4149-A9D4-D7D343B29E09}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -468,7 +477,7 @@
     3 temporadas</t>
       </text>
     </comment>
-    <comment ref="B64" authorId="47" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+    <comment ref="B65" authorId="48" shapeId="0" xr:uid="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -476,7 +485,7 @@
     4 temporadas</t>
       </text>
     </comment>
-    <comment ref="B65" authorId="48" shapeId="0" xr:uid="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
+    <comment ref="B66" authorId="49" shapeId="0" xr:uid="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -484,7 +493,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B66" authorId="49" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+    <comment ref="B67" authorId="50" shapeId="0" xr:uid="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -492,7 +501,7 @@
     1 temporada</t>
       </text>
     </comment>
-    <comment ref="B67" authorId="50" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+    <comment ref="B68" authorId="51" shapeId="0" xr:uid="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
       <text>
         <t>[Comentario encadenado]
 Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
@@ -567,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="211">
   <si>
     <t>Película</t>
   </si>
@@ -1197,6 +1206,9 @@
   </si>
   <si>
     <t>Code 8 (2019)</t>
+  </si>
+  <si>
+    <t>La monja guerrera</t>
   </si>
 </sst>
 </file>
@@ -1206,7 +1218,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1242,6 +1254,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1285,7 +1303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1308,9 +1326,6 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1523,10 +1538,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M67" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B2:M67" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M67">
-    <sortCondition descending="1" ref="C2:C67"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}" name="Tabla245" displayName="Tabla245" ref="B2:M68" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B2:M68" xr:uid="{84882D50-2FDD-4492-A7EE-A56F022A40B9}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M68">
+    <sortCondition descending="1" ref="C2:C68"/>
   </sortState>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{72A2CB77-15BB-4AA7-8CE3-1A83E67BCC54}" name="Serie" dataDxfId="21"/>
@@ -1917,73 +1932,76 @@
   <threadedComment ref="B34" dT="2024-07-08T19:06:42.39" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{162EA199-65BB-48FF-A9B1-580BDA0F2A25}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
+  <threadedComment ref="B35" dT="2026-01-04T19:50:03.78" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A8DD2670-DAB9-48F0-9B69-06BCBECDF83A}">
+    <text>2 temporadas</text>
+  </threadedComment>
+  <threadedComment ref="B36" dT="2024-07-08T19:06:30.81" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{BC097833-5E05-4B57-A72A-B55B23EF385A}">
     <text>10 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B36" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
+  <threadedComment ref="B37" dT="2025-04-18T12:26:08.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{D69ACFED-A245-418D-8836-7787A10A08B4}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B37" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
+  <threadedComment ref="B38" dT="2024-07-08T19:08:20.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{FE4CA59D-CA2D-4361-94E4-6EA24C8AD9DE}">
     <text>5 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B39" dT="2025-10-21T19:53:14.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{0372C847-801C-4993-BA73-8301D595FCF1}">
+  <threadedComment ref="B40" dT="2025-10-21T19:53:14.38" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{0372C847-801C-4993-BA73-8301D595FCF1}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B40" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
+  <threadedComment ref="B41" dT="2024-07-08T19:04:29.42" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{64FF07EB-F3D4-47C4-B23E-4905CF85CACC}">
     <text>2 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B41" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
+  <threadedComment ref="B42" dT="2024-12-19T19:39:49.29" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ACBD2AE4-B2D6-490A-B6A8-26BE6D3CC6C9}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
+  <threadedComment ref="B44" dT="2024-07-08T19:08:48.45" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{500EEDC0-7745-4F10-8309-4ED19BDF789B}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B44" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
+  <threadedComment ref="B45" dT="2025-04-09T21:18:34.74" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3E762906-7E78-4A82-82BD-91226BEEE65F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
+  <threadedComment ref="B46" dT="2024-07-08T19:09:26.44" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{A836A830-A167-47D8-ADFF-FC6A88D1B4AF}">
     <text>6 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B46" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
+  <threadedComment ref="B47" dT="2024-07-08T19:07:51.37" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{153818FB-95E4-42BD-AB45-ADAC7CCB6F82}">
     <text>14 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B48" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
+  <threadedComment ref="B49" dT="2024-07-08T19:08:59.55" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3D8C30B1-4F7A-4A97-801E-73E85EF747E6}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B49" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
+  <threadedComment ref="B50" dT="2024-07-08T19:09:15.09" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{008FAA73-DE5D-4913-AE22-80AE836D5D61}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B52" dT="2025-06-14T16:15:11.96" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
+  <threadedComment ref="B53" dT="2025-06-14T16:15:11.96" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{5698F250-EDD4-45DE-B2E5-000AD058A767}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B53" dT="2025-07-02T22:08:33.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{96839C2B-31B6-4DC0-88B7-37E650032258}">
+  <threadedComment ref="B54" dT="2025-07-02T22:08:33.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{96839C2B-31B6-4DC0-88B7-37E650032258}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B54" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
+  <threadedComment ref="B55" dT="2024-07-08T19:09:40.48" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{AC20EAA3-2085-4F9E-9888-5F2AB1B2897A}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B55" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
+  <threadedComment ref="B56" dT="2024-07-08T19:10:11.66" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{6FEDD623-6837-47F8-9B55-96EB3415266F}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B56" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
+  <threadedComment ref="B57" dT="2024-07-08T19:08:34.89" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B9AA30C0-3BCC-4842-ABCD-15892A9A17A4}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B62" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
+  <threadedComment ref="B63" dT="2024-07-08T19:10:27.18" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{ED84D32D-B87E-494D-BC5A-D963B24A65B4}">
     <text>7 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B63" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
+  <threadedComment ref="B64" dT="2024-07-08T18:58:56.17" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{25B82680-662E-4149-A9D4-D7D343B29E09}">
     <text>3 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B64" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
+  <threadedComment ref="B65" dT="2024-10-02T22:28:33.03" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{8D955452-5474-4D7F-9EFB-C317CB8E77C7}">
     <text>4 temporadas</text>
   </threadedComment>
-  <threadedComment ref="B65" dT="2025-10-07T18:49:36.71" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
+  <threadedComment ref="B66" dT="2025-10-07T18:49:36.71" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{3955FC3A-5089-4113-A6FF-7CA6DD36C98F}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B66" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
+  <threadedComment ref="B67" dT="2024-07-09T17:54:39.57" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{C6F778D8-6F01-47AB-B632-8939C5C0B507}">
     <text>1 temporada</text>
   </threadedComment>
-  <threadedComment ref="B67" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
+  <threadedComment ref="B68" dT="2024-07-08T19:10:55.56" personId="{2E232528-F057-4355-8D9E-53D77C4311A2}" id="{B1297543-A2F2-4625-BBB2-C2604CA16AED}">
     <text>4 temporadas</text>
   </threadedComment>
 </ThreadedComments>
@@ -1995,10 +2013,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:O67"/>
+  <dimension ref="B2:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2062,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -2096,7 +2114,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -2129,7 +2147,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2165,7 +2183,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2201,7 +2219,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2235,7 +2253,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2268,7 +2286,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2301,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2334,7 +2352,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2367,7 +2385,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2402,7 +2420,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2437,7 +2455,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2470,7 +2488,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2503,7 +2521,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2538,7 +2556,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2571,7 +2589,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2604,7 +2622,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2637,7 +2655,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2668,7 +2686,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2701,7 +2719,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2734,7 +2752,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2767,7 +2785,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2800,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2833,7 +2851,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2866,7 +2884,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2899,7 +2917,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2932,7 +2950,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2967,7 +2985,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -3000,7 +3018,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
         <v>7.6624999999999996</v>
       </c>
       <c r="D31" s="1">
@@ -3033,7 +3051,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
         <v>7.6000000000000005</v>
       </c>
       <c r="D32" s="1">
@@ -3066,7 +3084,7 @@
         <v>198</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
         <v>7.5625</v>
       </c>
       <c r="D33" s="1">
@@ -3099,7 +3117,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D34" s="1">
@@ -3132,129 +3150,130 @@
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
-        <v>7.5249999999999995</v>
+        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <v>7.5250000000000004</v>
       </c>
       <c r="D35" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E35" s="1">
         <v>8</v>
       </c>
       <c r="F35" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G35" s="1">
         <v>8</v>
       </c>
       <c r="H35" s="3">
-        <v>7.9</v>
+        <v>7</v>
       </c>
       <c r="I35" s="3">
-        <v>6.4</v>
+        <v>5.2</v>
       </c>
       <c r="J35" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K35" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>141</v>
+        <v>105</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
         <v>7.5249999999999995</v>
       </c>
       <c r="D36" s="1">
         <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F36" s="1">
         <v>7</v>
       </c>
       <c r="G36" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H36" s="3">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="I36" s="3">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="J36" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K36" s="1"/>
+      <c r="K36" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
-        <v>7.4874999999999989</v>
+        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <v>7.5249999999999995</v>
       </c>
       <c r="D37" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E37" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F37" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G37" s="1">
         <v>7</v>
       </c>
       <c r="H37" s="3">
-        <v>8.3000000000000007</v>
+        <v>7.8</v>
       </c>
       <c r="I37" s="3">
-        <v>7.3</v>
-      </c>
-      <c r="J37" s="1"/>
+        <v>6.6</v>
+      </c>
+      <c r="J37" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K37" s="1"/>
-      <c r="L37" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
-        <v>7.35</v>
+        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <v>7.4874999999999989</v>
       </c>
       <c r="D38" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F38" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G38" s="1">
         <v>7</v>
       </c>
       <c r="H38" s="3">
-        <v>8.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="I38" s="3">
-        <v>7.8</v>
+        <v>7.3</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -3264,62 +3283,61 @@
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>185</v>
+        <v>50</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
-        <v>7.3</v>
+        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <v>7.35</v>
       </c>
       <c r="D39" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F39" s="1">
         <v>7</v>
       </c>
       <c r="G39" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H39" s="3">
-        <v>7</v>
+        <v>8.5</v>
       </c>
       <c r="I39" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J39" t="e" vm="1">
+        <v>7.8</v>
+      </c>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
-      <c r="M39" s="1"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="2" t="s">
-        <v>80</v>
+        <v>185</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
-        <v>7.2500000000000009</v>
+        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <v>7.3</v>
       </c>
       <c r="D40" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1">
         <v>8</v>
       </c>
       <c r="F40" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G40" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H40" s="3">
-        <v>6.7</v>
+        <v>7</v>
       </c>
       <c r="I40" s="3">
-        <v>4.5999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="J40" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3330,29 +3348,29 @@
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="2" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
-        <v>7.25</v>
+        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <v>7.2500000000000009</v>
       </c>
       <c r="D41" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F41" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G41" s="1">
         <v>7</v>
       </c>
       <c r="H41" s="3">
-        <v>8.4</v>
+        <v>6.7</v>
       </c>
       <c r="I41" s="3">
-        <v>7.2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="J41" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3363,129 +3381,129 @@
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <v>7.25</v>
+      </c>
+      <c r="D42" s="1">
+        <v>8</v>
+      </c>
+      <c r="E42" s="1">
+        <v>5</v>
+      </c>
+      <c r="F42" s="1">
+        <v>7</v>
+      </c>
+      <c r="G42" s="1">
+        <v>7</v>
+      </c>
+      <c r="H42" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="I42" s="3">
         <v>7.2</v>
-      </c>
-      <c r="D42" s="1">
-        <v>8</v>
-      </c>
-      <c r="E42" s="1">
-        <v>8</v>
-      </c>
-      <c r="F42" s="1">
-        <v>7</v>
-      </c>
-      <c r="G42" s="1">
-        <v>5</v>
-      </c>
-      <c r="H42" s="3">
-        <v>8</v>
-      </c>
-      <c r="I42" s="3">
-        <v>6.6</v>
       </c>
       <c r="J42" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K42" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K42" s="1"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
         <v>7.2</v>
       </c>
       <c r="D43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E43" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F43" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G43" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H43" s="3">
-        <v>8.6</v>
+        <v>8</v>
       </c>
       <c r="I43" s="3">
-        <v>7.4</v>
-      </c>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" t="e" vm="5">
+        <v>6.6</v>
+      </c>
+      <c r="J43" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
+      <c r="K43" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B44" s="2" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1875000000000009</v>
+        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <v>7.2</v>
       </c>
       <c r="D44" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E44" s="1">
         <v>7</v>
       </c>
       <c r="F44" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G44" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H44" s="3">
-        <v>6.7</v>
+        <v>8.6</v>
       </c>
       <c r="I44" s="3">
-        <v>6.1</v>
-      </c>
-      <c r="J44" t="e" vm="1">
+        <v>7.4</v>
+      </c>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
-        <v>45</v>
+        <v>140</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1875</v>
+        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <v>7.1875000000000009</v>
       </c>
       <c r="D45" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E45" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F45" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G45" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H45" s="3">
-        <v>9.1</v>
+        <v>6.7</v>
       </c>
       <c r="I45" s="3">
-        <v>8.3000000000000007</v>
+        <v>6.1</v>
       </c>
       <c r="J45" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3496,100 +3514,98 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" s="2" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
-        <v>7.1749999999999998</v>
+        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <v>7.1875</v>
       </c>
       <c r="D46" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
         <v>6</v>
       </c>
       <c r="F46" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G46" s="1">
         <v>7</v>
       </c>
       <c r="H46" s="3">
-        <v>7.5</v>
+        <v>9.1</v>
       </c>
       <c r="I46" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="J46" s="1"/>
-      <c r="K46" t="e" vm="2">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J46" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="L46" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
         <v>7.1749999999999998</v>
       </c>
       <c r="D47" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E47" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F47" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G47" s="1">
         <v>7</v>
       </c>
       <c r="H47" s="3">
-        <v>8.5</v>
+        <v>7.5</v>
       </c>
       <c r="I47" s="3">
-        <v>7.4</v>
+        <v>5.4</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
+      <c r="L47" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9750000000000005</v>
+        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <v>7.1749999999999998</v>
       </c>
       <c r="D48" s="1">
         <v>6</v>
       </c>
       <c r="E48" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G48" s="1">
         <v>7</v>
       </c>
       <c r="H48" s="3">
-        <v>7.7</v>
+        <v>8.5</v>
       </c>
       <c r="I48" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J48" t="e" vm="1">
-        <v>#VALUE!</v>
-      </c>
+        <v>7.4</v>
+      </c>
+      <c r="J48" s="1"/>
       <c r="K48" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -3598,94 +3614,97 @@
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9</v>
+        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <v>6.9750000000000005</v>
       </c>
       <c r="D49" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F49" s="1">
         <v>7</v>
       </c>
       <c r="G49" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H49" s="3">
-        <v>8</v>
+        <v>7.7</v>
       </c>
       <c r="I49" s="3">
-        <v>7.2</v>
+        <v>6.4</v>
       </c>
       <c r="J49" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K49" s="1"/>
+      <c r="K49" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
       <c r="L49" s="1"/>
       <c r="M49" s="1"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B50" s="2" t="s">
-        <v>44</v>
+        <v>76</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8750000000000009</v>
+        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <v>6.9</v>
       </c>
       <c r="D50" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E50" s="1">
         <v>6</v>
       </c>
       <c r="F50" s="1">
+        <v>7</v>
+      </c>
+      <c r="G50" s="1">
         <v>5</v>
       </c>
-      <c r="G50" s="1">
-        <v>7</v>
-      </c>
       <c r="H50" s="3">
-        <v>8.6999999999999993</v>
+        <v>8</v>
       </c>
       <c r="I50" s="3">
-        <v>8.6</v>
-      </c>
-      <c r="J50" s="1"/>
+        <v>7.2</v>
+      </c>
+      <c r="J50" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K50" s="1"/>
-      <c r="L50" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B51" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8</v>
+        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <v>6.8750000000000009</v>
       </c>
       <c r="D51" s="1">
         <v>6</v>
       </c>
       <c r="E51" s="1">
+        <v>6</v>
+      </c>
+      <c r="F51" s="1">
         <v>5</v>
       </c>
-      <c r="F51" s="1">
-        <v>6</v>
-      </c>
       <c r="G51" s="1">
         <v>7</v>
       </c>
       <c r="H51" s="3">
-        <v>8.5</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="I51" s="3">
-        <v>7.4</v>
+        <v>8.6</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -3695,17 +3714,17 @@
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B52" s="2" t="s">
-        <v>148</v>
+        <v>48</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7750000000000004</v>
+        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <v>6.8</v>
       </c>
       <c r="D52" s="1">
         <v>6</v>
       </c>
       <c r="E52" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F52" s="1">
         <v>6</v>
@@ -3714,43 +3733,42 @@
         <v>7</v>
       </c>
       <c r="H52" s="3">
-        <v>7.7</v>
+        <v>8.5</v>
       </c>
       <c r="I52" s="3">
-        <v>6.8</v>
-      </c>
-      <c r="J52" t="e" vm="1">
+        <v>7.4</v>
+      </c>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B53" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
-        <v>6.75</v>
+        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <v>6.7750000000000004</v>
       </c>
       <c r="D53" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F53" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G53" s="1">
         <v>7</v>
       </c>
       <c r="H53" s="3">
-        <v>5.9</v>
+        <v>7.7</v>
       </c>
       <c r="I53" s="3">
-        <v>4.2</v>
+        <v>6.8</v>
       </c>
       <c r="J53" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3761,61 +3779,62 @@
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B54" s="2" t="s">
-        <v>17</v>
+        <v>153</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7250000000000005</v>
+        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <v>6.75</v>
       </c>
       <c r="D54" s="1">
         <v>8</v>
       </c>
       <c r="E54" s="1">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F54" s="1">
         <v>7</v>
       </c>
       <c r="G54" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H54" s="3">
-        <v>7.7</v>
+        <v>5.9</v>
       </c>
       <c r="I54" s="3">
-        <v>6.4</v>
-      </c>
-      <c r="J54" s="1"/>
+        <v>4.2</v>
+      </c>
+      <c r="J54" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K54" s="1"/>
-      <c r="L54" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7</v>
+        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <v>6.7250000000000005</v>
       </c>
       <c r="D55" s="1">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E55" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F55" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G55" s="1">
         <v>6</v>
       </c>
       <c r="H55" s="3">
-        <v>8.6</v>
+        <v>7.7</v>
       </c>
       <c r="I55" s="3">
-        <v>7.4</v>
+        <v>6.4</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -3825,79 +3844,76 @@
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B56" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
-        <v>6.55</v>
+        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <v>6.7</v>
       </c>
       <c r="D56" s="1">
         <v>5</v>
       </c>
       <c r="E56" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F56" s="1">
         <v>6</v>
       </c>
       <c r="G56" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H56" s="3">
-        <v>7</v>
+        <v>8.6</v>
       </c>
       <c r="I56" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="J56" t="e" vm="1">
+        <v>7.4</v>
+      </c>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
-      <c r="M56" s="1"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
-        <v>6.4875000000000007</v>
+        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <v>6.55</v>
       </c>
       <c r="D57" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E57" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F57" s="1">
         <v>6</v>
       </c>
       <c r="G57" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H57" s="3">
-        <v>8.1</v>
+        <v>7</v>
       </c>
       <c r="I57" s="3">
-        <v>7.7</v>
-      </c>
-      <c r="J57" s="1"/>
-      <c r="K57" t="e" vm="2">
+        <v>5.4</v>
+      </c>
+      <c r="J57" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
+      <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" s="1" t="e" vm="3">
-        <v>#VALUE!</v>
-      </c>
+      <c r="M57" s="1"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B58" s="2" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
-        <v>6.4</v>
+        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <v>6.4875000000000007</v>
       </c>
       <c r="D58" s="1">
         <v>6</v>
@@ -3909,46 +3925,48 @@
         <v>6</v>
       </c>
       <c r="G58" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H58" s="3">
         <v>8.1</v>
       </c>
       <c r="I58" s="3">
-        <v>6</v>
-      </c>
-      <c r="J58" t="e" vm="1">
+        <v>7.7</v>
+      </c>
+      <c r="J58" s="1"/>
+      <c r="K58" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
+      <c r="M58" s="1" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B59" s="2" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
-        <v>6.3999999999999995</v>
+        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <v>6.4</v>
       </c>
       <c r="D59" s="1">
         <v>6</v>
       </c>
       <c r="E59" s="1">
+        <v>6</v>
+      </c>
+      <c r="F59" s="1">
+        <v>6</v>
+      </c>
+      <c r="G59" s="1">
         <v>5</v>
       </c>
-      <c r="F59" s="1">
-        <v>6</v>
-      </c>
-      <c r="G59" s="1">
-        <v>6</v>
-      </c>
       <c r="H59" s="3">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="I59" s="3">
-        <v>6.6</v>
+        <v>6</v>
       </c>
       <c r="J59" t="e" vm="1">
         <v>#VALUE!</v>
@@ -3959,66 +3977,66 @@
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B60" s="2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
-        <v>6.2250000000000005</v>
+        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D60" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E60" s="1">
         <v>5</v>
       </c>
       <c r="F60" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G60" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H60" s="3">
-        <v>8.1999999999999993</v>
+        <v>7.8</v>
       </c>
       <c r="I60" s="3">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="J60" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K60" t="e" vm="2">
-        <v>#VALUE!</v>
-      </c>
+      <c r="K60" s="1"/>
       <c r="L60" s="1"/>
       <c r="M60" s="1"/>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B61" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1750000000000007</v>
+        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <v>6.2250000000000005</v>
       </c>
       <c r="D61" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E61" s="1">
         <v>5</v>
       </c>
       <c r="F61" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G61" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H61" s="3">
-        <v>6.6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I61" s="3">
-        <v>6.2</v>
-      </c>
-      <c r="J61" s="1"/>
+        <v>6.4</v>
+      </c>
+      <c r="J61" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K61" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
@@ -4027,62 +4045,62 @@
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B62" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1624999999999996</v>
+        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <v>6.1750000000000007</v>
       </c>
       <c r="D62" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E62" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F62" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G62" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H62" s="3">
-        <v>7.5</v>
+        <v>6.6</v>
       </c>
       <c r="I62" s="3">
-        <v>6.3</v>
-      </c>
-      <c r="J62" t="e" vm="1">
+        <v>6.2</v>
+      </c>
+      <c r="J62" s="1"/>
+      <c r="K62" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-      <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B63" s="2" t="s">
-        <v>89</v>
+        <v>11</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
-        <v>5.9749999999999996</v>
+        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <v>6.1624999999999996</v>
       </c>
       <c r="D63" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E63" s="1">
         <v>7</v>
       </c>
       <c r="F63" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G63" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H63" s="3">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
       <c r="I63" s="3">
-        <v>6.2</v>
+        <v>6.3</v>
       </c>
       <c r="J63" t="e" vm="1">
         <v>#VALUE!</v>
@@ -4093,29 +4111,29 @@
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B64" s="2" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
-        <v>5.7750000000000004</v>
+        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
+        <v>5.9749999999999996</v>
       </c>
       <c r="D64" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E64" s="1">
         <v>7</v>
       </c>
       <c r="F64" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G64" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H64" s="3">
-        <v>6.1</v>
+        <v>7.3</v>
       </c>
       <c r="I64" s="3">
-        <v>5</v>
+        <v>6.2</v>
       </c>
       <c r="J64" t="e" vm="1">
         <v>#VALUE!</v>
@@ -4126,29 +4144,29 @@
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B65" s="2" t="s">
-        <v>180</v>
+        <v>99</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
-        <v>5.7625000000000002</v>
+        <f>AVERAGE(D65,E65,F65,F65,G65,H65,H65,I65)</f>
+        <v>5.7750000000000004</v>
       </c>
       <c r="D65" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F65" s="1">
+        <v>7</v>
+      </c>
+      <c r="G65" s="1">
+        <v>3</v>
+      </c>
+      <c r="H65" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="I65" s="3">
         <v>5</v>
-      </c>
-      <c r="G65" s="1">
-        <v>5</v>
-      </c>
-      <c r="H65" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="I65" s="3">
-        <v>4.0999999999999996</v>
       </c>
       <c r="J65" t="e" vm="1">
         <v>#VALUE!</v>
@@ -4159,68 +4177,101 @@
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B66" s="2" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
-        <v>5.4625000000000004</v>
+        <f>AVERAGE(D66,E66,F66,F66,G66,H66,H66,I66)</f>
+        <v>5.7625000000000002</v>
       </c>
       <c r="D66" s="1">
+        <v>8</v>
+      </c>
+      <c r="E66" s="1">
+        <v>8</v>
+      </c>
+      <c r="F66" s="1">
         <v>5</v>
       </c>
-      <c r="E66" s="1">
-        <v>7</v>
-      </c>
-      <c r="F66" s="1">
-        <v>6</v>
-      </c>
       <c r="G66" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H66" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I66" s="3">
         <v>4.0999999999999996</v>
       </c>
-      <c r="I66" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="J66" s="1"/>
+      <c r="J66" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
       <c r="K66" s="1"/>
-      <c r="L66" t="e" vm="5">
-        <v>#VALUE!</v>
-      </c>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" s="5">
+        <f>AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+        <v>5.4625000000000004</v>
+      </c>
+      <c r="D67" s="1">
+        <v>5</v>
+      </c>
+      <c r="E67" s="1">
+        <v>7</v>
+      </c>
+      <c r="F67" s="1">
+        <v>6</v>
+      </c>
+      <c r="G67" s="1">
+        <v>7</v>
+      </c>
+      <c r="H67" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I67" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="5">
-        <f t="shared" ref="C67" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+      <c r="C68" s="5">
+        <f>AVERAGE(D68,E68,F68,F68,G68,H68,H68,I68)</f>
         <v>4.5874999999999995</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D68" s="1">
         <v>2</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E68" s="1">
         <v>4</v>
       </c>
-      <c r="F67" s="1">
+      <c r="F68" s="1">
         <v>2</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G68" s="1">
         <v>5</v>
       </c>
-      <c r="H67" s="3">
+      <c r="H68" s="3">
         <v>7.7</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I68" s="3">
         <v>6.3</v>
       </c>
-      <c r="J67" t="e" vm="1">
+      <c r="J68" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4245,8 +4296,8 @@
   </sheetPr>
   <dimension ref="B2:K130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4295,7 +4346,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4323,7 +4374,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4351,7 +4402,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4378,7 +4429,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4405,7 +4456,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4432,7 +4483,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4459,7 +4510,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4486,7 +4537,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4513,7 +4564,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4540,7 +4591,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4567,7 +4618,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4594,7 +4645,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4621,7 +4672,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4648,7 +4699,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4675,7 +4726,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4702,7 +4753,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4729,7 +4780,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4756,7 +4807,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4783,7 +4834,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4810,7 +4861,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4837,7 +4888,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4864,7 +4915,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4891,7 +4942,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4918,7 +4969,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4945,7 +4996,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -4972,7 +5023,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7750000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -4999,7 +5050,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7375000000000007</v>
       </c>
       <c r="D29" s="1">
@@ -5026,7 +5077,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.7000000000000011</v>
       </c>
       <c r="D30" s="1">
@@ -5053,7 +5104,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -5080,7 +5131,7 @@
         <v>123</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.5874999999999995</v>
       </c>
       <c r="D32" s="1">
@@ -5107,7 +5158,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5750000000000011</v>
       </c>
       <c r="D33" s="1">
@@ -5134,7 +5185,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5750000000000002</v>
       </c>
       <c r="D34" s="1">
@@ -5161,7 +5212,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5625</v>
       </c>
       <c r="D35" s="1">
@@ -5188,7 +5239,7 @@
         <v>55</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5624999999999991</v>
       </c>
       <c r="D36" s="1">
@@ -5215,7 +5266,7 @@
         <v>201</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.55</v>
       </c>
       <c r="D37" s="1">
@@ -5242,7 +5293,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -5269,7 +5320,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5296,7 +5347,7 @@
         <v>205</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.4875000000000007</v>
       </c>
       <c r="D40" s="1">
@@ -5323,7 +5374,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
@@ -5350,7 +5401,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
@@ -5377,7 +5428,7 @@
         <v>97</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.4375</v>
       </c>
       <c r="D43" s="1">
@@ -5404,7 +5455,7 @@
         <v>100</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.4249999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -5431,7 +5482,7 @@
         <v>131</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.4124999999999996</v>
       </c>
       <c r="D45" s="1">
@@ -5458,7 +5509,7 @@
         <v>175</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.3624999999999989</v>
       </c>
       <c r="D46" s="1">
@@ -5485,7 +5536,7 @@
         <v>52</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.3500000000000005</v>
       </c>
       <c r="D47" s="1">
@@ -5512,7 +5563,7 @@
         <v>165</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>7.3249999999999993</v>
       </c>
       <c r="D48" s="1">
@@ -5539,7 +5590,7 @@
         <v>111</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D49" s="1">
@@ -5566,7 +5617,7 @@
         <v>103</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -5593,7 +5644,7 @@
         <v>181</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>7.2750000000000004</v>
       </c>
       <c r="D51" s="1">
@@ -5620,7 +5671,7 @@
         <v>147</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>7.2374999999999998</v>
       </c>
       <c r="D52" s="1">
@@ -5647,7 +5698,7 @@
         <v>59</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>7.2250000000000005</v>
       </c>
       <c r="D53" s="1">
@@ -5674,7 +5725,7 @@
         <v>65</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>7.2125000000000004</v>
       </c>
       <c r="D54" s="1">
@@ -5701,7 +5752,7 @@
         <v>146</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>7.2124999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -5728,7 +5779,7 @@
         <v>94</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>7.1999999999999993</v>
       </c>
       <c r="D56" s="1">
@@ -5755,7 +5806,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>7.1499999999999995</v>
       </c>
       <c r="D57" s="1">
@@ -5782,7 +5833,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>7.1375000000000011</v>
       </c>
       <c r="D58" s="1">
@@ -5809,7 +5860,7 @@
         <v>40</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>7.1250000000000009</v>
       </c>
       <c r="D59" s="1">
@@ -5836,7 +5887,7 @@
         <v>39</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>7.125</v>
       </c>
       <c r="D60" s="1">
@@ -5863,7 +5914,7 @@
         <v>133</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>7.0875000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -5890,7 +5941,7 @@
         <v>98</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D62" s="1">
@@ -5917,7 +5968,7 @@
         <v>171</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000011</v>
       </c>
       <c r="D63" s="1">
@@ -5944,7 +5995,7 @@
         <v>110</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D64" s="1">
@@ -5971,7 +6022,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>7.0750000000000002</v>
       </c>
       <c r="D65" s="1">
@@ -5998,7 +6049,7 @@
         <v>177</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>7.0749999999999993</v>
       </c>
       <c r="D66" s="1">
@@ -6025,7 +6076,7 @@
         <v>176</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>7.05</v>
       </c>
       <c r="D67" s="1">
@@ -6052,7 +6103,7 @@
         <v>95</v>
       </c>
       <c r="C68" s="5">
-        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
+        <f t="shared" si="2"/>
         <v>6.9375</v>
       </c>
       <c r="D68" s="1">
@@ -6079,7 +6130,7 @@
         <v>164</v>
       </c>
       <c r="C69" s="5">
-        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
+        <f t="shared" si="2"/>
         <v>6.9124999999999996</v>
       </c>
       <c r="D69" s="1">
@@ -6106,7 +6157,7 @@
         <v>157</v>
       </c>
       <c r="C70" s="5">
-        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
+        <f t="shared" si="2"/>
         <v>6.8999999999999995</v>
       </c>
       <c r="D70" s="1">
@@ -6133,7 +6184,7 @@
         <v>88</v>
       </c>
       <c r="C71" s="5">
-        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D71" s="1">
@@ -6160,7 +6211,7 @@
         <v>184</v>
       </c>
       <c r="C72" s="5">
-        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
+        <f t="shared" si="2"/>
         <v>6.8624999999999989</v>
       </c>
       <c r="D72" s="1">
@@ -6187,7 +6238,7 @@
         <v>119</v>
       </c>
       <c r="C73" s="5">
-        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
+        <f t="shared" si="2"/>
         <v>6.85</v>
       </c>
       <c r="D73" s="1">
@@ -6214,7 +6265,7 @@
         <v>196</v>
       </c>
       <c r="C74" s="5">
-        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
+        <f t="shared" si="2"/>
         <v>6.7999999999999989</v>
       </c>
       <c r="D74" s="1">
@@ -6241,7 +6292,7 @@
         <v>57</v>
       </c>
       <c r="C75" s="5">
-        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
+        <f t="shared" si="2"/>
         <v>6.6999999999999993</v>
       </c>
       <c r="D75" s="1">
@@ -6268,7 +6319,7 @@
         <v>87</v>
       </c>
       <c r="C76" s="5">
-        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
+        <f t="shared" si="2"/>
         <v>6.6875</v>
       </c>
       <c r="D76" s="1">
@@ -6295,7 +6346,7 @@
         <v>41</v>
       </c>
       <c r="C77" s="5">
-        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <f t="shared" si="2"/>
         <v>6.6124999999999989</v>
       </c>
       <c r="D77" s="1">
@@ -6322,7 +6373,7 @@
         <v>117</v>
       </c>
       <c r="C78" s="5">
-        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D78" s="1">
@@ -6349,7 +6400,7 @@
         <v>179</v>
       </c>
       <c r="C79" s="5">
-        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
+        <f t="shared" si="2"/>
         <v>6.5874999999999995</v>
       </c>
       <c r="D79" s="1">
@@ -6376,7 +6427,7 @@
         <v>168</v>
       </c>
       <c r="C80" s="5">
-        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <f t="shared" si="2"/>
         <v>6.5499999999999989</v>
       </c>
       <c r="D80" s="1">
@@ -6403,7 +6454,7 @@
         <v>197</v>
       </c>
       <c r="C81" s="5">
-        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <f t="shared" si="2"/>
         <v>6.5375000000000005</v>
       </c>
       <c r="D81" s="1">
@@ -6430,7 +6481,7 @@
         <v>202</v>
       </c>
       <c r="C82" s="5">
-        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <f t="shared" si="2"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D82" s="1">
@@ -6457,7 +6508,7 @@
         <v>183</v>
       </c>
       <c r="C83" s="5">
-        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <f t="shared" si="2"/>
         <v>6.3624999999999998</v>
       </c>
       <c r="D83" s="1">
@@ -6484,7 +6535,7 @@
         <v>200</v>
       </c>
       <c r="C84" s="5">
-        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
+        <f t="shared" si="2"/>
         <v>6.3624999999999998</v>
       </c>
       <c r="D84" s="1">
@@ -6511,7 +6562,7 @@
         <v>188</v>
       </c>
       <c r="C85" s="5">
-        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <f t="shared" si="2"/>
         <v>6.35</v>
       </c>
       <c r="D85" s="1">
@@ -6538,7 +6589,7 @@
         <v>208</v>
       </c>
       <c r="C86" s="5">
-        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
+        <f t="shared" si="2"/>
         <v>6.35</v>
       </c>
       <c r="D86" s="1">
@@ -6565,7 +6616,7 @@
         <v>134</v>
       </c>
       <c r="C87" s="5">
-        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <f t="shared" si="2"/>
         <v>6.3125</v>
       </c>
       <c r="D87" s="1">
@@ -6592,7 +6643,7 @@
         <v>144</v>
       </c>
       <c r="C88" s="5">
-        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D88" s="1">
@@ -6619,7 +6670,7 @@
         <v>64</v>
       </c>
       <c r="C89" s="5">
-        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
+        <f t="shared" si="2"/>
         <v>6.2749999999999995</v>
       </c>
       <c r="D89" s="1">
@@ -6646,7 +6697,7 @@
         <v>75</v>
       </c>
       <c r="C90" s="5">
-        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <f t="shared" si="2"/>
         <v>6.2125000000000004</v>
       </c>
       <c r="D90" s="1">
@@ -6673,7 +6724,7 @@
         <v>19</v>
       </c>
       <c r="C91" s="5">
-        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <f t="shared" si="2"/>
         <v>6.2124999999999995</v>
       </c>
       <c r="D91" s="1">
@@ -6700,7 +6751,7 @@
         <v>101</v>
       </c>
       <c r="C92" s="5">
-        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <f t="shared" si="2"/>
         <v>6.15</v>
       </c>
       <c r="D92" s="1">
@@ -6727,7 +6778,7 @@
         <v>158</v>
       </c>
       <c r="C93" s="5">
-        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <f t="shared" si="2"/>
         <v>6.0874999999999995</v>
       </c>
       <c r="D93" s="1">
@@ -6754,7 +6805,7 @@
         <v>160</v>
       </c>
       <c r="C94" s="5">
-        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
       <c r="D94" s="1">
@@ -6781,7 +6832,7 @@
         <v>206</v>
       </c>
       <c r="C95" s="5">
-        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
+        <f t="shared" si="2"/>
         <v>6.05</v>
       </c>
       <c r="D95" s="1">
@@ -6808,7 +6859,7 @@
         <v>159</v>
       </c>
       <c r="C96" s="5">
-        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <f t="shared" si="2"/>
         <v>5.9499999999999993</v>
       </c>
       <c r="D96" s="1">
@@ -6835,7 +6886,7 @@
         <v>195</v>
       </c>
       <c r="C97" s="5">
-        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <f t="shared" si="2"/>
         <v>5.8875000000000011</v>
       </c>
       <c r="D97" s="1">
@@ -6862,7 +6913,7 @@
         <v>186</v>
       </c>
       <c r="C98" s="5">
-        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <f t="shared" si="2"/>
         <v>5.8125000000000009</v>
       </c>
       <c r="D98" s="1">
@@ -6885,11 +6936,11 @@
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="2" t="s">
         <v>209</v>
       </c>
       <c r="C99" s="5">
-        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
         <v>5.8000000000000007</v>
       </c>
       <c r="D99" s="1">
@@ -6916,7 +6967,7 @@
         <v>113</v>
       </c>
       <c r="C100" s="5">
-        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <f t="shared" si="3"/>
         <v>5.7374999999999989</v>
       </c>
       <c r="D100" s="1">
@@ -6943,7 +6994,7 @@
         <v>187</v>
       </c>
       <c r="C101" s="5">
-        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <f t="shared" si="3"/>
         <v>5.7250000000000005</v>
       </c>
       <c r="D101" s="1">
@@ -6970,7 +7021,7 @@
         <v>26</v>
       </c>
       <c r="C102" s="5">
-        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <f t="shared" si="3"/>
         <v>5.6749999999999998</v>
       </c>
       <c r="D102" s="1">
@@ -6997,7 +7048,7 @@
         <v>149</v>
       </c>
       <c r="C103" s="5">
-        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <f t="shared" si="3"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D103" s="1">
@@ -7024,7 +7075,7 @@
         <v>156</v>
       </c>
       <c r="C104" s="5">
-        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
+        <f t="shared" si="3"/>
         <v>5.5624999999999991</v>
       </c>
       <c r="D104" s="1">
@@ -7051,7 +7102,7 @@
         <v>166</v>
       </c>
       <c r="C105" s="5">
-        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <f t="shared" si="3"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D105" s="1">
@@ -7078,7 +7129,7 @@
         <v>191</v>
       </c>
       <c r="C106" s="5">
-        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
+        <f t="shared" si="3"/>
         <v>5.4874999999999989</v>
       </c>
       <c r="D106" s="1">
@@ -7105,7 +7156,7 @@
         <v>204</v>
       </c>
       <c r="C107" s="5">
-        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <f t="shared" si="3"/>
         <v>5.3750000000000009</v>
       </c>
       <c r="D107" s="1">
@@ -7132,7 +7183,7 @@
         <v>190</v>
       </c>
       <c r="C108" s="5">
-        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
+        <f t="shared" si="3"/>
         <v>5.375</v>
       </c>
       <c r="D108" s="1">
@@ -7159,7 +7210,7 @@
         <v>182</v>
       </c>
       <c r="C109" s="5">
-        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
+        <f t="shared" si="3"/>
         <v>5.2875000000000005</v>
       </c>
       <c r="D109" s="1">
@@ -7186,7 +7237,7 @@
         <v>74</v>
       </c>
       <c r="C110" s="5">
-        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
+        <f t="shared" si="3"/>
         <v>5.1875</v>
       </c>
       <c r="D110" s="1">
@@ -7213,7 +7264,7 @@
         <v>145</v>
       </c>
       <c r="C111" s="5">
-        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
+        <f t="shared" si="3"/>
         <v>5.1124999999999998</v>
       </c>
       <c r="D111" s="1">
@@ -7240,7 +7291,7 @@
         <v>21</v>
       </c>
       <c r="C112" s="5">
-        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
+        <f t="shared" si="3"/>
         <v>5.05</v>
       </c>
       <c r="D112" s="1">
@@ -7267,7 +7318,7 @@
         <v>203</v>
       </c>
       <c r="C113" s="5">
-        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
+        <f t="shared" si="3"/>
         <v>4.9875000000000007</v>
       </c>
       <c r="D113" s="1">
@@ -7294,7 +7345,7 @@
         <v>169</v>
       </c>
       <c r="C114" s="5">
-        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
+        <f t="shared" si="3"/>
         <v>4.9874999999999998</v>
       </c>
       <c r="D114" s="1">
@@ -7321,7 +7372,7 @@
         <v>163</v>
       </c>
       <c r="C115" s="5">
-        <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
+        <f t="shared" si="3"/>
         <v>4.8499999999999996</v>
       </c>
       <c r="D115" s="1">
@@ -7348,7 +7399,7 @@
         <v>162</v>
       </c>
       <c r="C116" s="5">
-        <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
+        <f t="shared" si="3"/>
         <v>4.7875000000000005</v>
       </c>
       <c r="D116" s="1">
@@ -7375,7 +7426,7 @@
         <v>154</v>
       </c>
       <c r="C117" s="5">
-        <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
+        <f t="shared" si="3"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="D117" s="1">
@@ -7402,7 +7453,7 @@
         <v>135</v>
       </c>
       <c r="C118" s="5">
-        <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
+        <f t="shared" si="3"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D118" s="1">
@@ -7429,7 +7480,7 @@
         <v>161</v>
       </c>
       <c r="C119" s="5">
-        <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
+        <f t="shared" si="3"/>
         <v>4.4249999999999998</v>
       </c>
       <c r="D119" s="1">
@@ -7456,7 +7507,7 @@
         <v>114</v>
       </c>
       <c r="C120" s="5">
-        <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
+        <f t="shared" si="3"/>
         <v>4.4124999999999996</v>
       </c>
       <c r="D120" s="1">
@@ -7483,7 +7534,7 @@
         <v>207</v>
       </c>
       <c r="C121" s="5">
-        <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
+        <f t="shared" si="3"/>
         <v>4.3375000000000004</v>
       </c>
       <c r="D121" s="1">
@@ -7510,7 +7561,7 @@
         <v>150</v>
       </c>
       <c r="C122" s="5">
-        <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
+        <f t="shared" si="3"/>
         <v>4.3374999999999995</v>
       </c>
       <c r="D122" s="1">
@@ -7537,7 +7588,7 @@
         <v>173</v>
       </c>
       <c r="C123" s="5">
-        <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
+        <f t="shared" si="3"/>
         <v>4.3125</v>
       </c>
       <c r="D123" s="1">
@@ -7564,7 +7615,7 @@
         <v>167</v>
       </c>
       <c r="C124" s="5">
-        <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
+        <f t="shared" si="3"/>
         <v>4.2749999999999995</v>
       </c>
       <c r="D124" s="1">
@@ -7591,7 +7642,7 @@
         <v>68</v>
       </c>
       <c r="C125" s="5">
-        <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
+        <f t="shared" si="3"/>
         <v>4.1124999999999998</v>
       </c>
       <c r="D125" s="1">
@@ -7618,7 +7669,7 @@
         <v>199</v>
       </c>
       <c r="C126" s="5">
-        <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
+        <f t="shared" si="3"/>
         <v>3.7375000000000003</v>
       </c>
       <c r="D126" s="1">
@@ -7645,7 +7696,7 @@
         <v>189</v>
       </c>
       <c r="C127" s="5">
-        <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
+        <f t="shared" si="3"/>
         <v>3.3250000000000002</v>
       </c>
       <c r="D127" s="1">
@@ -7672,7 +7723,7 @@
         <v>194</v>
       </c>
       <c r="C128" s="5">
-        <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
+        <f t="shared" si="3"/>
         <v>3.2749999999999995</v>
       </c>
       <c r="D128" s="1">
@@ -7699,7 +7750,7 @@
         <v>155</v>
       </c>
       <c r="C129" s="5">
-        <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
+        <f t="shared" si="3"/>
         <v>2.9124999999999996</v>
       </c>
       <c r="D129" s="1">
@@ -7726,7 +7777,7 @@
         <v>174</v>
       </c>
       <c r="C130" s="5">
-        <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
+        <f t="shared" si="3"/>
         <v>2.6375000000000002</v>
       </c>
       <c r="D130" s="1">

</xml_diff>

<commit_message>
V. 110 "El niño que domó el viento"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEADEC7-6A35-46FA-B3B8-B8DD74EDBC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71706AAB-156A-447C-BBC6-692F6574FE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Series" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="212">
   <si>
     <t>Película</t>
   </si>
@@ -1209,6 +1209,9 @@
   </si>
   <si>
     <t>La monja guerrera</t>
+  </si>
+  <si>
+    <t>El niño que domó el viento</t>
   </si>
 </sst>
 </file>
@@ -1218,7 +1221,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1254,12 +1257,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1303,7 +1300,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1326,6 +1323,9 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1564,10 +1564,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I130" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I130" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I130">
-    <sortCondition descending="1" ref="C2:C130"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I131" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I131" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I131">
+    <sortCondition descending="1" ref="C2:C131"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -2015,7 +2015,7 @@
   </sheetPr>
   <dimension ref="B2:O68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
@@ -2080,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="5">
-        <f>AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
+        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,F3,F3,G3,H3,H3,I3)</f>
         <v>9.5250000000000004</v>
       </c>
       <c r="D3" s="1">
@@ -2114,7 +2114,7 @@
         <v>118</v>
       </c>
       <c r="C4" s="5">
-        <f>AVERAGE(D4,E4,F4,F4,G4,H4,H4,I4)</f>
+        <f t="shared" si="0"/>
         <v>8.9749999999999996</v>
       </c>
       <c r="D4" s="1">
@@ -2147,7 +2147,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="5">
-        <f>AVERAGE(D5,E5,F5,F5,G5,H5,H5,I5)</f>
+        <f t="shared" si="0"/>
         <v>8.6062500000000011</v>
       </c>
       <c r="D5" s="1">
@@ -2183,7 +2183,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="5">
-        <f>AVERAGE(D6,E6,F6,F6,G6,H6,H6,I6)</f>
+        <f t="shared" si="0"/>
         <v>8.5874999999999986</v>
       </c>
       <c r="D6" s="1">
@@ -2219,7 +2219,7 @@
         <v>112</v>
       </c>
       <c r="C7" s="5">
-        <f>AVERAGE(D7,E7,F7,F7,G7,H7,H7,I7)</f>
+        <f t="shared" si="0"/>
         <v>8.5750000000000011</v>
       </c>
       <c r="D7" s="1">
@@ -2253,7 +2253,7 @@
         <v>83</v>
       </c>
       <c r="C8" s="5">
-        <f>AVERAGE(D8,E8,F8,F8,G8,H8,H8,I8)</f>
+        <f t="shared" si="0"/>
         <v>8.5125000000000011</v>
       </c>
       <c r="D8" s="1">
@@ -2286,7 +2286,7 @@
         <v>178</v>
       </c>
       <c r="C9" s="5">
-        <f>AVERAGE(D9,E9,F9,F9,G9,H9,H9,I9)</f>
+        <f t="shared" si="0"/>
         <v>8.5124999999999993</v>
       </c>
       <c r="D9" s="1">
@@ -2319,7 +2319,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="5">
-        <f>AVERAGE(D10,E10,F10,F10,G10,H10,H10,I10)</f>
+        <f t="shared" si="0"/>
         <v>8.4875000000000007</v>
       </c>
       <c r="D10" s="1">
@@ -2352,7 +2352,7 @@
         <v>93</v>
       </c>
       <c r="C11" s="5">
-        <f>AVERAGE(D11,E11,F11,F11,G11,H11,H11,I11)</f>
+        <f t="shared" si="0"/>
         <v>8.4</v>
       </c>
       <c r="D11" s="1">
@@ -2385,7 +2385,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="5">
-        <f>AVERAGE(D12,E12,F12,F12,G12,H12,H12,I12)</f>
+        <f t="shared" si="0"/>
         <v>8.3875000000000011</v>
       </c>
       <c r="D12" s="1">
@@ -2420,7 +2420,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="5">
-        <f>AVERAGE(D13,E13,F13,F13,G13,H13,H13,I13)</f>
+        <f t="shared" si="0"/>
         <v>8.3625000000000007</v>
       </c>
       <c r="D13" s="1">
@@ -2455,7 +2455,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="5">
-        <f>AVERAGE(D14,E14,F14,F14,G14,H14,H14,I14)</f>
+        <f t="shared" si="0"/>
         <v>8.3624999999999989</v>
       </c>
       <c r="D14" s="1">
@@ -2488,7 +2488,7 @@
         <v>137</v>
       </c>
       <c r="C15" s="5">
-        <f>AVERAGE(D15,E15,F15,F15,G15,H15,H15,I15)</f>
+        <f t="shared" si="0"/>
         <v>8.3125</v>
       </c>
       <c r="D15" s="1">
@@ -2521,7 +2521,7 @@
         <v>28</v>
       </c>
       <c r="C16" s="5">
-        <f>AVERAGE(D16,E16,F16,F16,G16,H16,H16,I16)</f>
+        <f t="shared" si="0"/>
         <v>8.2875000000000014</v>
       </c>
       <c r="D16" s="1">
@@ -2556,7 +2556,7 @@
         <v>139</v>
       </c>
       <c r="C17" s="5">
-        <f>AVERAGE(D17,E17,F17,F17,G17,H17,H17,I17)</f>
+        <f t="shared" si="0"/>
         <v>8.2874999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -2589,7 +2589,7 @@
         <v>46</v>
       </c>
       <c r="C18" s="5">
-        <f>AVERAGE(D18,E18,F18,F18,G18,H18,H18,I18)</f>
+        <f t="shared" si="0"/>
         <v>8.1375000000000011</v>
       </c>
       <c r="D18" s="1">
@@ -2622,7 +2622,7 @@
         <v>136</v>
       </c>
       <c r="C19" s="5">
-        <f>AVERAGE(D19,E19,F19,F19,G19,H19,H19,I19)</f>
+        <f t="shared" si="0"/>
         <v>8.125</v>
       </c>
       <c r="D19" s="1">
@@ -2655,7 +2655,7 @@
         <v>70</v>
       </c>
       <c r="C20" s="5">
-        <f>AVERAGE(D20,E20,F20,F20,G20,H20,H20,I20)</f>
+        <f t="shared" si="0"/>
         <v>8.1</v>
       </c>
       <c r="D20" s="1">
@@ -2686,7 +2686,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="5">
-        <f>AVERAGE(D21,E21,F21,F21,G21,H21,H21,I21)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D21" s="1">
@@ -2719,7 +2719,7 @@
         <v>33</v>
       </c>
       <c r="C22" s="5">
-        <f>AVERAGE(D22,E22,F22,F22,G22,H22,H22,I22)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D22" s="1">
@@ -2752,7 +2752,7 @@
         <v>120</v>
       </c>
       <c r="C23" s="5">
-        <f>AVERAGE(D23,E23,F23,F23,G23,H23,H23,I23)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D23" s="1">
@@ -2785,7 +2785,7 @@
         <v>34</v>
       </c>
       <c r="C24" s="5">
-        <f>AVERAGE(D24,E24,F24,F24,G24,H24,H24,I24)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="D24" s="1">
@@ -2818,7 +2818,7 @@
         <v>5</v>
       </c>
       <c r="C25" s="5">
-        <f>AVERAGE(D25,E25,F25,F25,G25,H25,H25,I25)</f>
+        <f t="shared" si="0"/>
         <v>7.8750000000000009</v>
       </c>
       <c r="D25" s="1">
@@ -2851,7 +2851,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="5">
-        <f>AVERAGE(D26,E26,F26,F26,G26,H26,H26,I26)</f>
+        <f t="shared" si="0"/>
         <v>7.8125000000000009</v>
       </c>
       <c r="D26" s="1">
@@ -2884,7 +2884,7 @@
         <v>138</v>
       </c>
       <c r="C27" s="5">
-        <f>AVERAGE(D27,E27,F27,F27,G27,H27,H27,I27)</f>
+        <f t="shared" si="0"/>
         <v>7.8125</v>
       </c>
       <c r="D27" s="1">
@@ -2917,7 +2917,7 @@
         <v>82</v>
       </c>
       <c r="C28" s="5">
-        <f>AVERAGE(D28,E28,F28,F28,G28,H28,H28,I28)</f>
+        <f t="shared" si="0"/>
         <v>7.7874999999999996</v>
       </c>
       <c r="D28" s="1">
@@ -2950,7 +2950,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="5">
-        <f>AVERAGE(D29,E29,F29,F29,G29,H29,H29,I29)</f>
+        <f t="shared" si="0"/>
         <v>7.7250000000000005</v>
       </c>
       <c r="D29" s="1">
@@ -2985,7 +2985,7 @@
         <v>142</v>
       </c>
       <c r="C30" s="5">
-        <f>AVERAGE(D30,E30,F30,F30,G30,H30,H30,I30)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D30" s="1">
@@ -3018,7 +3018,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="5">
-        <f>AVERAGE(D31,E31,F31,F31,G31,H31,H31,I31)</f>
+        <f t="shared" si="0"/>
         <v>7.6624999999999996</v>
       </c>
       <c r="D31" s="1">
@@ -3051,7 +3051,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="5">
-        <f>AVERAGE(D32,E32,F32,F32,G32,H32,H32,I32)</f>
+        <f t="shared" si="0"/>
         <v>7.6000000000000005</v>
       </c>
       <c r="D32" s="1">
@@ -3084,7 +3084,7 @@
         <v>198</v>
       </c>
       <c r="C33" s="5">
-        <f>AVERAGE(D33,E33,F33,F33,G33,H33,H33,I33)</f>
+        <f t="shared" si="0"/>
         <v>7.5625</v>
       </c>
       <c r="D33" s="1">
@@ -3117,7 +3117,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="5">
-        <f>AVERAGE(D34,E34,F34,F34,G34,H34,H34,I34)</f>
+        <f t="shared" si="0"/>
         <v>7.5250000000000004</v>
       </c>
       <c r="D34" s="1">
@@ -3153,7 +3153,7 @@
         <v>210</v>
       </c>
       <c r="C35" s="5">
-        <f>AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
+        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,F35,F35,G35,H35,H35,I35)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D35" s="1">
@@ -3186,7 +3186,7 @@
         <v>105</v>
       </c>
       <c r="C36" s="5">
-        <f>AVERAGE(D36,E36,F36,F36,G36,H36,H36,I36)</f>
+        <f t="shared" si="1"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D36" s="1">
@@ -3221,7 +3221,7 @@
         <v>141</v>
       </c>
       <c r="C37" s="5">
-        <f>AVERAGE(D37,E37,F37,F37,G37,H37,H37,I37)</f>
+        <f t="shared" si="1"/>
         <v>7.5249999999999995</v>
       </c>
       <c r="D37" s="1">
@@ -3254,7 +3254,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="5">
-        <f>AVERAGE(D38,E38,F38,F38,G38,H38,H38,I38)</f>
+        <f t="shared" si="1"/>
         <v>7.4874999999999989</v>
       </c>
       <c r="D38" s="1">
@@ -3286,7 +3286,7 @@
         <v>50</v>
       </c>
       <c r="C39" s="5">
-        <f>AVERAGE(D39,E39,F39,F39,G39,H39,H39,I39)</f>
+        <f t="shared" si="1"/>
         <v>7.35</v>
       </c>
       <c r="D39" s="1">
@@ -3318,7 +3318,7 @@
         <v>185</v>
       </c>
       <c r="C40" s="5">
-        <f>AVERAGE(D40,E40,F40,F40,G40,H40,H40,I40)</f>
+        <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
       <c r="D40" s="1">
@@ -3351,7 +3351,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="5">
-        <f>AVERAGE(D41,E41,F41,F41,G41,H41,H41,I41)</f>
+        <f t="shared" si="1"/>
         <v>7.2500000000000009</v>
       </c>
       <c r="D41" s="1">
@@ -3384,7 +3384,7 @@
         <v>115</v>
       </c>
       <c r="C42" s="5">
-        <f>AVERAGE(D42,E42,F42,F42,G42,H42,H42,I42)</f>
+        <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
       <c r="D42" s="1">
@@ -3417,7 +3417,7 @@
         <v>29</v>
       </c>
       <c r="C43" s="5">
-        <f>AVERAGE(D43,E43,F43,F43,G43,H43,H43,I43)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D43" s="1">
@@ -3452,7 +3452,7 @@
         <v>22</v>
       </c>
       <c r="C44" s="5">
-        <f>AVERAGE(D44,E44,F44,F44,G44,H44,H44,I44)</f>
+        <f t="shared" si="1"/>
         <v>7.2</v>
       </c>
       <c r="D44" s="1">
@@ -3484,7 +3484,7 @@
         <v>140</v>
       </c>
       <c r="C45" s="5">
-        <f>AVERAGE(D45,E45,F45,F45,G45,H45,H45,I45)</f>
+        <f t="shared" si="1"/>
         <v>7.1875000000000009</v>
       </c>
       <c r="D45" s="1">
@@ -3517,7 +3517,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="5">
-        <f>AVERAGE(D46,E46,F46,F46,G46,H46,H46,I46)</f>
+        <f t="shared" si="1"/>
         <v>7.1875</v>
       </c>
       <c r="D46" s="1">
@@ -3550,7 +3550,7 @@
         <v>27</v>
       </c>
       <c r="C47" s="5">
-        <f>AVERAGE(D47,E47,F47,F47,G47,H47,H47,I47)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D47" s="1">
@@ -3584,7 +3584,7 @@
         <v>49</v>
       </c>
       <c r="C48" s="5">
-        <f>AVERAGE(D48,E48,F48,F48,G48,H48,H48,I48)</f>
+        <f t="shared" si="1"/>
         <v>7.1749999999999998</v>
       </c>
       <c r="D48" s="1">
@@ -3617,7 +3617,7 @@
         <v>71</v>
       </c>
       <c r="C49" s="5">
-        <f>AVERAGE(D49,E49,F49,F49,G49,H49,H49,I49)</f>
+        <f t="shared" si="1"/>
         <v>6.9750000000000005</v>
       </c>
       <c r="D49" s="1">
@@ -3652,7 +3652,7 @@
         <v>76</v>
       </c>
       <c r="C50" s="5">
-        <f>AVERAGE(D50,E50,F50,F50,G50,H50,H50,I50)</f>
+        <f t="shared" si="1"/>
         <v>6.9</v>
       </c>
       <c r="D50" s="1">
@@ -3685,7 +3685,7 @@
         <v>44</v>
       </c>
       <c r="C51" s="5">
-        <f>AVERAGE(D51,E51,F51,F51,G51,H51,H51,I51)</f>
+        <f t="shared" si="1"/>
         <v>6.8750000000000009</v>
       </c>
       <c r="D51" s="1">
@@ -3717,7 +3717,7 @@
         <v>48</v>
       </c>
       <c r="C52" s="5">
-        <f>AVERAGE(D52,E52,F52,F52,G52,H52,H52,I52)</f>
+        <f t="shared" si="1"/>
         <v>6.8</v>
       </c>
       <c r="D52" s="1">
@@ -3749,7 +3749,7 @@
         <v>148</v>
       </c>
       <c r="C53" s="5">
-        <f>AVERAGE(D53,E53,F53,F53,G53,H53,H53,I53)</f>
+        <f t="shared" si="1"/>
         <v>6.7750000000000004</v>
       </c>
       <c r="D53" s="1">
@@ -3782,7 +3782,7 @@
         <v>153</v>
       </c>
       <c r="C54" s="5">
-        <f>AVERAGE(D54,E54,F54,F54,G54,H54,H54,I54)</f>
+        <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
       <c r="D54" s="1">
@@ -3815,7 +3815,7 @@
         <v>17</v>
       </c>
       <c r="C55" s="5">
-        <f>AVERAGE(D55,E55,F55,F55,G55,H55,H55,I55)</f>
+        <f t="shared" si="1"/>
         <v>6.7250000000000005</v>
       </c>
       <c r="D55" s="1">
@@ -3847,7 +3847,7 @@
         <v>18</v>
       </c>
       <c r="C56" s="5">
-        <f>AVERAGE(D56,E56,F56,F56,G56,H56,H56,I56)</f>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="D56" s="1">
@@ -3879,7 +3879,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="5">
-        <f>AVERAGE(D57,E57,F57,F57,G57,H57,H57,I57)</f>
+        <f t="shared" si="1"/>
         <v>6.55</v>
       </c>
       <c r="D57" s="1">
@@ -3912,7 +3912,7 @@
         <v>106</v>
       </c>
       <c r="C58" s="5">
-        <f>AVERAGE(D58,E58,F58,F58,G58,H58,H58,I58)</f>
+        <f t="shared" si="1"/>
         <v>6.4875000000000007</v>
       </c>
       <c r="D58" s="1">
@@ -3947,7 +3947,7 @@
         <v>30</v>
       </c>
       <c r="C59" s="5">
-        <f>AVERAGE(D59,E59,F59,F59,G59,H59,H59,I59)</f>
+        <f t="shared" si="1"/>
         <v>6.4</v>
       </c>
       <c r="D59" s="1">
@@ -3980,7 +3980,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="5">
-        <f>AVERAGE(D60,E60,F60,F60,G60,H60,H60,I60)</f>
+        <f t="shared" si="1"/>
         <v>6.3999999999999995</v>
       </c>
       <c r="D60" s="1">
@@ -4013,7 +4013,7 @@
         <v>32</v>
       </c>
       <c r="C61" s="5">
-        <f>AVERAGE(D61,E61,F61,F61,G61,H61,H61,I61)</f>
+        <f t="shared" si="1"/>
         <v>6.2250000000000005</v>
       </c>
       <c r="D61" s="1">
@@ -4048,7 +4048,7 @@
         <v>42</v>
       </c>
       <c r="C62" s="5">
-        <f>AVERAGE(D62,E62,F62,F62,G62,H62,H62,I62)</f>
+        <f t="shared" si="1"/>
         <v>6.1750000000000007</v>
       </c>
       <c r="D62" s="1">
@@ -4081,7 +4081,7 @@
         <v>11</v>
       </c>
       <c r="C63" s="5">
-        <f>AVERAGE(D63,E63,F63,F63,G63,H63,H63,I63)</f>
+        <f t="shared" si="1"/>
         <v>6.1624999999999996</v>
       </c>
       <c r="D63" s="1">
@@ -4114,7 +4114,7 @@
         <v>89</v>
       </c>
       <c r="C64" s="5">
-        <f>AVERAGE(D64,E64,F64,F64,G64,H64,H64,I64)</f>
+        <f t="shared" si="1"/>
         <v>5.9749999999999996</v>
       </c>
       <c r="D64" s="1">
@@ -4147,7 +4147,7 @@
         <v>99</v>
       </c>
       <c r="C65" s="5">
-        <f>AVERAGE(D65,E65,F65,F65,G65,H65,H65,I65)</f>
+        <f t="shared" si="1"/>
         <v>5.7750000000000004</v>
       </c>
       <c r="D65" s="1">
@@ -4180,7 +4180,7 @@
         <v>180</v>
       </c>
       <c r="C66" s="5">
-        <f>AVERAGE(D66,E66,F66,F66,G66,H66,H66,I66)</f>
+        <f t="shared" si="1"/>
         <v>5.7625000000000002</v>
       </c>
       <c r="D66" s="1">
@@ -4213,7 +4213,7 @@
         <v>91</v>
       </c>
       <c r="C67" s="5">
-        <f>AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
         <v>5.4625000000000004</v>
       </c>
       <c r="D67" s="1">
@@ -4245,7 +4245,7 @@
         <v>36</v>
       </c>
       <c r="C68" s="5">
-        <f>AVERAGE(D68,E68,F68,F68,G68,H68,H68,I68)</f>
+        <f t="shared" si="2"/>
         <v>4.5874999999999995</v>
       </c>
       <c r="D68" s="1">
@@ -4294,10 +4294,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K130"/>
+  <dimension ref="B2:K131"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4346,7 +4346,7 @@
         <v>107</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" ref="C3:C34" si="0">AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
+        <f>AVERAGE(D3,E3,E3,F3,G3,H3,H3,I3)</f>
         <v>8.9250000000000007</v>
       </c>
       <c r="D3" s="1">
@@ -4374,7 +4374,7 @@
         <v>66</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D4,E4,E4,F4,G4,H4,H4,I4)</f>
         <v>8.8625000000000007</v>
       </c>
       <c r="D4" s="1">
@@ -4402,7 +4402,7 @@
         <v>51</v>
       </c>
       <c r="C5" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D5,E5,E5,F5,G5,H5,H5,I5)</f>
         <v>8.85</v>
       </c>
       <c r="D5" s="1">
@@ -4429,7 +4429,7 @@
         <v>79</v>
       </c>
       <c r="C6" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D6,E6,E6,F6,G6,H6,H6,I6)</f>
         <v>8.8375000000000004</v>
       </c>
       <c r="D6" s="1">
@@ -4456,7 +4456,7 @@
         <v>128</v>
       </c>
       <c r="C7" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D7,E7,E7,F7,G7,H7,H7,I7)</f>
         <v>8.65</v>
       </c>
       <c r="D7" s="1">
@@ -4483,7 +4483,7 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D8,E8,E8,F8,G8,H8,H8,I8)</f>
         <v>8.625</v>
       </c>
       <c r="D8" s="1">
@@ -4510,7 +4510,7 @@
         <v>121</v>
       </c>
       <c r="C9" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D9,E9,E9,F9,G9,H9,H9,I9)</f>
         <v>8.5250000000000004</v>
       </c>
       <c r="D9" s="1">
@@ -4537,7 +4537,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D10,E10,E10,F10,G10,H10,H10,I10)</f>
         <v>8.5</v>
       </c>
       <c r="D10" s="1">
@@ -4564,7 +4564,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D11,E11,E11,F11,G11,H11,H11,I11)</f>
         <v>8.5</v>
       </c>
       <c r="D11" s="1">
@@ -4591,7 +4591,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D12,E12,E12,F12,G12,H12,H12,I12)</f>
         <v>8.5</v>
       </c>
       <c r="D12" s="1">
@@ -4618,7 +4618,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D13,E13,E13,F13,G13,H13,H13,I13)</f>
         <v>8.4375</v>
       </c>
       <c r="D13" s="1">
@@ -4645,7 +4645,7 @@
         <v>96</v>
       </c>
       <c r="C14" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D14,E14,E14,F14,G14,H14,H14,I14)</f>
         <v>8.4124999999999996</v>
       </c>
       <c r="D14" s="1">
@@ -4672,7 +4672,7 @@
         <v>170</v>
       </c>
       <c r="C15" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D15,E15,E15,F15,G15,H15,H15,I15)</f>
         <v>8.3999999999999986</v>
       </c>
       <c r="D15" s="1">
@@ -4699,7 +4699,7 @@
         <v>125</v>
       </c>
       <c r="C16" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D16,E16,E16,F16,G16,H16,H16,I16)</f>
         <v>8.1750000000000007</v>
       </c>
       <c r="D16" s="1">
@@ -4726,7 +4726,7 @@
         <v>81</v>
       </c>
       <c r="C17" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D17,E17,E17,F17,G17,H17,H17,I17)</f>
         <v>8.1624999999999996</v>
       </c>
       <c r="D17" s="1">
@@ -4753,7 +4753,7 @@
         <v>77</v>
       </c>
       <c r="C18" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D18,E18,E18,F18,G18,H18,H18,I18)</f>
         <v>8.15</v>
       </c>
       <c r="D18" s="1">
@@ -4780,7 +4780,7 @@
         <v>54</v>
       </c>
       <c r="C19" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D19,E19,E19,F19,G19,H19,H19,I19)</f>
         <v>8.1</v>
       </c>
       <c r="D19" s="1">
@@ -4807,7 +4807,7 @@
         <v>126</v>
       </c>
       <c r="C20" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D20,E20,E20,F20,G20,H20,H20,I20)</f>
         <v>8.0750000000000011</v>
       </c>
       <c r="D20" s="1">
@@ -4834,7 +4834,7 @@
         <v>58</v>
       </c>
       <c r="C21" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D21,E21,E21,F21,G21,H21,H21,I21)</f>
         <v>8.0625</v>
       </c>
       <c r="D21" s="1">
@@ -4861,7 +4861,7 @@
         <v>23</v>
       </c>
       <c r="C22" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D22,E22,E22,F22,G22,H22,H22,I22)</f>
         <v>7.9249999999999998</v>
       </c>
       <c r="D22" s="1">
@@ -4888,7 +4888,7 @@
         <v>122</v>
       </c>
       <c r="C23" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D23,E23,E23,F23,G23,H23,H23,I23)</f>
         <v>7.9124999999999996</v>
       </c>
       <c r="D23" s="1">
@@ -4915,7 +4915,7 @@
         <v>108</v>
       </c>
       <c r="C24" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D24,E24,E24,F24,G24,H24,H24,I24)</f>
         <v>7.8999999999999995</v>
       </c>
       <c r="D24" s="1">
@@ -4942,7 +4942,7 @@
         <v>78</v>
       </c>
       <c r="C25" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D25,E25,E25,F25,G25,H25,H25,I25)</f>
         <v>7.875</v>
       </c>
       <c r="D25" s="1">
@@ -4969,7 +4969,7 @@
         <v>109</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D26,E26,E26,F26,G26,H26,H26,I26)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D26" s="1">
@@ -4996,7 +4996,7 @@
         <v>61</v>
       </c>
       <c r="C27" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D27,E27,E27,F27,G27,H27,H27,I27)</f>
         <v>7.7875000000000005</v>
       </c>
       <c r="D27" s="1">
@@ -5023,7 +5023,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D28,E28,E28,F28,G28,H28,H28,I28)</f>
         <v>7.7750000000000004</v>
       </c>
       <c r="D28" s="1">
@@ -5050,7 +5050,7 @@
         <v>60</v>
       </c>
       <c r="C29" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D29,E29,E29,F29,G29,H29,H29,I29)</f>
         <v>7.7375000000000007</v>
       </c>
       <c r="D29" s="1">
@@ -5077,7 +5077,7 @@
         <v>38</v>
       </c>
       <c r="C30" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D30,E30,E30,F30,G30,H30,H30,I30)</f>
         <v>7.7000000000000011</v>
       </c>
       <c r="D30" s="1">
@@ -5104,7 +5104,7 @@
         <v>63</v>
       </c>
       <c r="C31" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D31,E31,E31,F31,G31,H31,H31,I31)</f>
         <v>7.6999999999999993</v>
       </c>
       <c r="D31" s="1">
@@ -5131,7 +5131,7 @@
         <v>123</v>
       </c>
       <c r="C32" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D32,E32,E32,F32,G32,H32,H32,I32)</f>
         <v>7.5874999999999995</v>
       </c>
       <c r="D32" s="1">
@@ -5158,7 +5158,7 @@
         <v>37</v>
       </c>
       <c r="C33" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D33,E33,E33,F33,G33,H33,H33,I33)</f>
         <v>7.5750000000000011</v>
       </c>
       <c r="D33" s="1">
@@ -5185,7 +5185,7 @@
         <v>67</v>
       </c>
       <c r="C34" s="5">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D34,E34,E34,F34,G34,H34,H34,I34)</f>
         <v>7.5750000000000002</v>
       </c>
       <c r="D34" s="1">
@@ -5212,7 +5212,7 @@
         <v>62</v>
       </c>
       <c r="C35" s="5">
-        <f t="shared" ref="C35:C66" si="1">AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
+        <f>AVERAGE(D35,E35,E35,F35,G35,H35,H35,I35)</f>
         <v>7.5625</v>
       </c>
       <c r="D35" s="1">
@@ -5239,7 +5239,7 @@
         <v>55</v>
       </c>
       <c r="C36" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D36,E36,E36,F36,G36,H36,H36,I36)</f>
         <v>7.5624999999999991</v>
       </c>
       <c r="D36" s="1">
@@ -5266,7 +5266,7 @@
         <v>201</v>
       </c>
       <c r="C37" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D37,E37,E37,F37,G37,H37,H37,I37)</f>
         <v>7.55</v>
       </c>
       <c r="D37" s="1">
@@ -5293,7 +5293,7 @@
         <v>69</v>
       </c>
       <c r="C38" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D38,E38,E38,F38,G38,H38,H38,I38)</f>
         <v>7.5250000000000004</v>
       </c>
       <c r="D38" s="1">
@@ -5320,7 +5320,7 @@
         <v>132</v>
       </c>
       <c r="C39" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D39,E39,E39,F39,G39,H39,H39,I39)</f>
         <v>7.5125000000000002</v>
       </c>
       <c r="D39" s="1">
@@ -5347,7 +5347,7 @@
         <v>205</v>
       </c>
       <c r="C40" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D40,E40,E40,F40,G40,H40,H40,I40)</f>
         <v>7.4875000000000007</v>
       </c>
       <c r="D40" s="1">
@@ -5374,7 +5374,7 @@
         <v>172</v>
       </c>
       <c r="C41" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D41,E41,E41,F41,G41,H41,H41,I41)</f>
         <v>7.4749999999999996</v>
       </c>
       <c r="D41" s="1">
@@ -5401,7 +5401,7 @@
         <v>130</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D42,E42,E42,F42,G42,H42,H42,I42)</f>
         <v>7.4625000000000004</v>
       </c>
       <c r="D42" s="1">
@@ -5428,7 +5428,7 @@
         <v>97</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D43,E43,E43,F43,G43,H43,H43,I43)</f>
         <v>7.4375</v>
       </c>
       <c r="D43" s="1">
@@ -5455,7 +5455,7 @@
         <v>100</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D44,E44,E44,F44,G44,H44,H44,I44)</f>
         <v>7.4249999999999998</v>
       </c>
       <c r="D44" s="1">
@@ -5482,7 +5482,7 @@
         <v>131</v>
       </c>
       <c r="C45" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D45,E45,E45,F45,G45,H45,H45,I45)</f>
         <v>7.4124999999999996</v>
       </c>
       <c r="D45" s="1">
@@ -5509,7 +5509,7 @@
         <v>175</v>
       </c>
       <c r="C46" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D46,E46,E46,F46,G46,H46,H46,I46)</f>
         <v>7.3624999999999989</v>
       </c>
       <c r="D46" s="1">
@@ -5536,7 +5536,7 @@
         <v>52</v>
       </c>
       <c r="C47" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D47,E47,E47,F47,G47,H47,H47,I47)</f>
         <v>7.3500000000000005</v>
       </c>
       <c r="D47" s="1">
@@ -5563,7 +5563,7 @@
         <v>165</v>
       </c>
       <c r="C48" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D48,E48,E48,F48,G48,H48,H48,I48)</f>
         <v>7.3249999999999993</v>
       </c>
       <c r="D48" s="1">
@@ -5590,7 +5590,7 @@
         <v>111</v>
       </c>
       <c r="C49" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D49,E49,E49,F49,G49,H49,H49,I49)</f>
         <v>7.3</v>
       </c>
       <c r="D49" s="1">
@@ -5617,7 +5617,7 @@
         <v>103</v>
       </c>
       <c r="C50" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D50,E50,E50,F50,G50,H50,H50,I50)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D50" s="1">
@@ -5644,7 +5644,7 @@
         <v>181</v>
       </c>
       <c r="C51" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D51,E51,E51,F51,G51,H51,H51,I51)</f>
         <v>7.2750000000000004</v>
       </c>
       <c r="D51" s="1">
@@ -5671,7 +5671,7 @@
         <v>147</v>
       </c>
       <c r="C52" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D52,E52,E52,F52,G52,H52,H52,I52)</f>
         <v>7.2374999999999998</v>
       </c>
       <c r="D52" s="1">
@@ -5698,7 +5698,7 @@
         <v>59</v>
       </c>
       <c r="C53" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D53,E53,E53,F53,G53,H53,H53,I53)</f>
         <v>7.2250000000000005</v>
       </c>
       <c r="D53" s="1">
@@ -5725,7 +5725,7 @@
         <v>65</v>
       </c>
       <c r="C54" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D54,E54,E54,F54,G54,H54,H54,I54)</f>
         <v>7.2125000000000004</v>
       </c>
       <c r="D54" s="1">
@@ -5752,7 +5752,7 @@
         <v>146</v>
       </c>
       <c r="C55" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D55,E55,E55,F55,G55,H55,H55,I55)</f>
         <v>7.2124999999999995</v>
       </c>
       <c r="D55" s="1">
@@ -5779,7 +5779,7 @@
         <v>94</v>
       </c>
       <c r="C56" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D56,E56,E56,F56,G56,H56,H56,I56)</f>
         <v>7.1999999999999993</v>
       </c>
       <c r="D56" s="1">
@@ -5806,7 +5806,7 @@
         <v>53</v>
       </c>
       <c r="C57" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D57,E57,E57,F57,G57,H57,H57,I57)</f>
         <v>7.1499999999999995</v>
       </c>
       <c r="D57" s="1">
@@ -5833,7 +5833,7 @@
         <v>104</v>
       </c>
       <c r="C58" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D58,E58,E58,F58,G58,H58,H58,I58)</f>
         <v>7.1375000000000011</v>
       </c>
       <c r="D58" s="1">
@@ -5860,7 +5860,7 @@
         <v>40</v>
       </c>
       <c r="C59" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D59,E59,E59,F59,G59,H59,H59,I59)</f>
         <v>7.1250000000000009</v>
       </c>
       <c r="D59" s="1">
@@ -5887,7 +5887,7 @@
         <v>39</v>
       </c>
       <c r="C60" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D60,E60,E60,F60,G60,H60,H60,I60)</f>
         <v>7.125</v>
       </c>
       <c r="D60" s="1">
@@ -5914,7 +5914,7 @@
         <v>133</v>
       </c>
       <c r="C61" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D61,E61,E61,F61,G61,H61,H61,I61)</f>
         <v>7.0875000000000004</v>
       </c>
       <c r="D61" s="1">
@@ -5941,7 +5941,7 @@
         <v>98</v>
       </c>
       <c r="C62" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D62,E62,E62,F62,G62,H62,H62,I62)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D62" s="1">
@@ -5968,7 +5968,7 @@
         <v>171</v>
       </c>
       <c r="C63" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D63,E63,E63,F63,G63,H63,H63,I63)</f>
         <v>7.0750000000000011</v>
       </c>
       <c r="D63" s="1">
@@ -5995,7 +5995,7 @@
         <v>110</v>
       </c>
       <c r="C64" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D64,E64,E64,F64,G64,H64,H64,I64)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D64" s="1">
@@ -6022,7 +6022,7 @@
         <v>143</v>
       </c>
       <c r="C65" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D65,E65,E65,F65,G65,H65,H65,I65)</f>
         <v>7.0750000000000002</v>
       </c>
       <c r="D65" s="1">
@@ -6049,7 +6049,7 @@
         <v>177</v>
       </c>
       <c r="C66" s="5">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D66,E66,E66,F66,G66,H66,H66,I66)</f>
         <v>7.0749999999999993</v>
       </c>
       <c r="D66" s="1">
@@ -6076,7 +6076,7 @@
         <v>176</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
+        <f>AVERAGE(D67,E67,E67,F67,G67,H67,H67,I67)</f>
         <v>7.05</v>
       </c>
       <c r="D67" s="1">
@@ -6103,7 +6103,7 @@
         <v>95</v>
       </c>
       <c r="C68" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D68,E68,E68,F68,G68,H68,H68,I68)</f>
         <v>6.9375</v>
       </c>
       <c r="D68" s="1">
@@ -6130,7 +6130,7 @@
         <v>164</v>
       </c>
       <c r="C69" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D69,E69,E69,F69,G69,H69,H69,I69)</f>
         <v>6.9124999999999996</v>
       </c>
       <c r="D69" s="1">
@@ -6157,7 +6157,7 @@
         <v>157</v>
       </c>
       <c r="C70" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D70,E70,E70,F70,G70,H70,H70,I70)</f>
         <v>6.8999999999999995</v>
       </c>
       <c r="D70" s="1">
@@ -6184,7 +6184,7 @@
         <v>88</v>
       </c>
       <c r="C71" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D71,E71,E71,F71,G71,H71,H71,I71)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D71" s="1">
@@ -6211,7 +6211,7 @@
         <v>184</v>
       </c>
       <c r="C72" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D72,E72,E72,F72,G72,H72,H72,I72)</f>
         <v>6.8624999999999989</v>
       </c>
       <c r="D72" s="1">
@@ -6238,7 +6238,7 @@
         <v>119</v>
       </c>
       <c r="C73" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D73,E73,E73,F73,G73,H73,H73,I73)</f>
         <v>6.85</v>
       </c>
       <c r="D73" s="1">
@@ -6265,7 +6265,7 @@
         <v>196</v>
       </c>
       <c r="C74" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D74,E74,E74,F74,G74,H74,H74,I74)</f>
         <v>6.7999999999999989</v>
       </c>
       <c r="D74" s="1">
@@ -6292,7 +6292,7 @@
         <v>57</v>
       </c>
       <c r="C75" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D75,E75,E75,F75,G75,H75,H75,I75)</f>
         <v>6.6999999999999993</v>
       </c>
       <c r="D75" s="1">
@@ -6319,7 +6319,7 @@
         <v>87</v>
       </c>
       <c r="C76" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D76,E76,E76,F76,G76,H76,H76,I76)</f>
         <v>6.6875</v>
       </c>
       <c r="D76" s="1">
@@ -6342,93 +6342,93 @@
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
-        <v>41</v>
+      <c r="B77" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="C77" s="5">
-        <f t="shared" si="2"/>
-        <v>6.6124999999999989</v>
+        <f>AVERAGE(D77,E77,E77,F77,G77,H77,H77,I77)</f>
+        <v>6.6375000000000002</v>
       </c>
       <c r="D77" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E77" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F77" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H77" s="3">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
       <c r="I77" s="3">
-        <v>5.3</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="2" t="s">
-        <v>117</v>
+        <v>41</v>
       </c>
       <c r="C78" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5874999999999995</v>
+        <f>AVERAGE(D78,E78,E78,F78,G78,H78,H78,I78)</f>
+        <v>6.6124999999999989</v>
       </c>
       <c r="D78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E78" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F78" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G78" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H78" s="3">
         <v>6.3</v>
       </c>
       <c r="I78" s="3">
-        <v>6.1</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" s="2" t="s">
-        <v>179</v>
+        <v>117</v>
       </c>
       <c r="C79" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D79,E79,E79,F79,G79,H79,H79,I79)</f>
         <v>6.5874999999999995</v>
       </c>
       <c r="D79" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E79" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F79" s="1">
         <v>7</v>
       </c>
       <c r="G79" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H79" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I79" s="3">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" s="2" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="C80" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5499999999999989</v>
+        <f>AVERAGE(D80,E80,E80,F80,G80,H80,H80,I80)</f>
+        <v>6.5874999999999995</v>
       </c>
       <c r="D80" s="1">
         <v>8</v>
@@ -6440,79 +6440,79 @@
         <v>7</v>
       </c>
       <c r="G80" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H80" s="3">
-        <v>6.8</v>
+        <v>6.4</v>
       </c>
       <c r="I80" s="3">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C81" s="5">
-        <f t="shared" si="2"/>
-        <v>6.5375000000000005</v>
+        <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D81" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E81" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
       </c>
       <c r="G81" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="I81" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C82" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3999999999999995</v>
+        <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
+        <v>6.5375000000000005</v>
       </c>
       <c r="D82" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E82" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F82" s="1">
         <v>7</v>
       </c>
       <c r="G82" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H82" s="3">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="I82" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C83" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3624999999999998</v>
+        <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D83" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E83" s="1">
         <v>6</v>
@@ -6524,25 +6524,25 @@
         <v>7</v>
       </c>
       <c r="H83" s="3">
-        <v>5.9</v>
+        <v>6.4</v>
       </c>
       <c r="I83" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C84" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D84" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E84" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F84" s="1">
         <v>7</v>
@@ -6551,79 +6551,79 @@
         <v>7</v>
       </c>
       <c r="H84" s="3">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="I84" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C85" s="5">
-        <f t="shared" si="2"/>
-        <v>6.35</v>
+        <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D85" s="1">
         <v>7</v>
       </c>
       <c r="E85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F85" s="1">
         <v>7</v>
       </c>
       <c r="G85" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H85" s="3">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="I85" s="3">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C86" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
         <v>6.35</v>
       </c>
       <c r="D86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G86" s="1">
         <v>6</v>
       </c>
       <c r="H86" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="I86" s="3">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>134</v>
+        <v>208</v>
       </c>
       <c r="C87" s="5">
-        <f t="shared" si="2"/>
-        <v>6.3125</v>
+        <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
+        <v>6.35</v>
       </c>
       <c r="D87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F87" s="1">
         <v>6</v>
@@ -6632,187 +6632,187 @@
         <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I87" s="3">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C88" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2749999999999995</v>
+        <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
+        <v>6.3125</v>
       </c>
       <c r="D88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E88" s="1">
         <v>6</v>
       </c>
       <c r="F88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I88" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C89" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
         <v>6.2749999999999995</v>
       </c>
       <c r="D89" s="1">
         <v>6</v>
       </c>
       <c r="E89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H89" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I89" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C90" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2125000000000004</v>
+        <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D90" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F90" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G90" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H90" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I90" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C91" s="5">
-        <f t="shared" si="2"/>
-        <v>6.2124999999999995</v>
+        <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D91" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E91" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F91" s="1">
         <v>8</v>
       </c>
       <c r="G91" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H91" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I91" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C92" s="5">
-        <f t="shared" si="2"/>
-        <v>6.15</v>
+        <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D92" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E92" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F92" s="1">
         <v>8</v>
       </c>
       <c r="G92" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H92" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I92" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C93" s="5">
-        <f t="shared" si="2"/>
-        <v>6.0874999999999995</v>
+        <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
+        <v>6.15</v>
       </c>
       <c r="D93" s="1">
         <v>7</v>
       </c>
       <c r="E93" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F93" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G93" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H93" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I93" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C94" s="5">
-        <f t="shared" si="2"/>
-        <v>6.05</v>
+        <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D94" s="1">
         <v>7</v>
       </c>
       <c r="E94" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F94" s="1">
         <v>7</v>
@@ -6821,46 +6821,46 @@
         <v>7</v>
       </c>
       <c r="H94" s="3">
-        <v>5.4</v>
+        <v>4.8</v>
       </c>
       <c r="I94" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" s="2" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="C95" s="5">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
         <v>6.05</v>
       </c>
       <c r="D95" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E95" s="1">
         <v>6</v>
       </c>
       <c r="F95" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G95" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H95" s="3">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="I95" s="3">
-        <v>5.4</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" si="2"/>
-        <v>5.9499999999999993</v>
+        <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
+        <v>6.05</v>
       </c>
       <c r="D96" s="1">
         <v>6</v>
@@ -6869,133 +6869,133 @@
         <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G96" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H96" s="3">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="I96" s="3">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C97" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8875000000000011</v>
+        <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D97" s="1">
         <v>6</v>
       </c>
       <c r="E97" s="1">
+        <v>6</v>
+      </c>
+      <c r="F97" s="1">
+        <v>8</v>
+      </c>
+      <c r="G97" s="1">
         <v>5</v>
       </c>
-      <c r="F97" s="1">
-        <v>6</v>
-      </c>
-      <c r="G97" s="1">
-        <v>6</v>
-      </c>
       <c r="H97" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I97" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C98" s="5">
-        <f t="shared" si="2"/>
-        <v>5.8125000000000009</v>
+        <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D98" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E98" s="1">
         <v>5</v>
       </c>
       <c r="F98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I98" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C99" s="5">
-        <f t="shared" ref="C99:C130" si="3">AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.8000000000000007</v>
+        <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D99" s="1">
         <v>7</v>
       </c>
       <c r="E99" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F99" s="1">
         <v>5</v>
       </c>
       <c r="G99" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H99" s="3">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="I99" s="3">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>113</v>
+        <v>209</v>
       </c>
       <c r="C100" s="5">
-        <f t="shared" si="3"/>
-        <v>5.7374999999999989</v>
+        <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
+        <v>5.8000000000000007</v>
       </c>
       <c r="D100" s="1">
         <v>7</v>
       </c>
       <c r="E100" s="1">
+        <v>6</v>
+      </c>
+      <c r="F100" s="1">
         <v>5</v>
       </c>
-      <c r="F100" s="1">
-        <v>4</v>
-      </c>
       <c r="G100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H100" s="3">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="I100" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C101" s="5">
-        <f t="shared" si="3"/>
-        <v>5.7250000000000005</v>
+        <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D101" s="1">
         <v>7</v>
@@ -7007,37 +7007,37 @@
         <v>4</v>
       </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H101" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I101" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C102" s="5">
-        <f t="shared" si="3"/>
-        <v>5.6749999999999998</v>
+        <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D102" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E102" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F102" s="1">
+        <v>4</v>
+      </c>
+      <c r="G102" s="1">
         <v>5</v>
       </c>
-      <c r="G102" s="1">
-        <v>6</v>
-      </c>
       <c r="H102" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I102" s="3">
         <v>6.4</v>
@@ -7045,50 +7045,50 @@
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C103" s="5">
-        <f t="shared" si="3"/>
-        <v>5.5624999999999991</v>
+        <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D103" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E103" s="1">
+        <v>3</v>
+      </c>
+      <c r="F103" s="1">
         <v>5</v>
       </c>
-      <c r="F103" s="1">
-        <v>6</v>
-      </c>
       <c r="G103" s="1">
         <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I103" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C104" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D104" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E104" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G104" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H104" s="3">
         <v>5.8</v>
@@ -7099,260 +7099,260 @@
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C105" s="5">
-        <f t="shared" si="3"/>
-        <v>5.4874999999999989</v>
+        <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D105" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E105" s="1">
         <v>6</v>
       </c>
       <c r="F105" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H105" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I105" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C106" s="5">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E106" s="1">
         <v>6</v>
       </c>
       <c r="F106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H106" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I106" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C107" s="5">
-        <f t="shared" si="3"/>
-        <v>5.3750000000000009</v>
+        <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D107" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E107" s="1">
+        <v>6</v>
+      </c>
+      <c r="F107" s="1">
         <v>5</v>
       </c>
-      <c r="F107" s="1">
-        <v>6</v>
-      </c>
       <c r="G107" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I107" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C108" s="5">
-        <f t="shared" si="3"/>
-        <v>5.375</v>
+        <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D108" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E108" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F108" s="1">
         <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H108" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I108" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C109" s="5">
-        <f t="shared" si="3"/>
-        <v>5.2875000000000005</v>
+        <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
+        <v>5.375</v>
       </c>
       <c r="D109" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G109" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H109" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I109" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C110" s="5">
-        <f t="shared" si="3"/>
-        <v>5.1875</v>
+        <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D110" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E110" s="1">
         <v>5</v>
       </c>
       <c r="F110" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G110" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H110" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I110" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C111" s="5">
-        <f t="shared" si="3"/>
-        <v>5.1124999999999998</v>
+        <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
+        <v>5.1875</v>
       </c>
       <c r="D111" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E111" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F111" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G111" s="1">
         <v>6</v>
       </c>
       <c r="H111" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I111" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C112" s="5">
-        <f t="shared" si="3"/>
-        <v>5.05</v>
+        <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D112" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E112" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F112" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G112" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H112" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I112" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C113" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9875000000000007</v>
+        <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
+        <v>5.05</v>
       </c>
       <c r="D113" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E113" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F113" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G113" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H113" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I113" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C114" s="5">
-        <f t="shared" si="3"/>
-        <v>4.9874999999999998</v>
+        <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D114" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E114" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F114" s="1">
         <v>5</v>
@@ -7361,441 +7361,468 @@
         <v>6</v>
       </c>
       <c r="H114" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I114" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C115" s="5">
-        <f t="shared" si="3"/>
-        <v>4.8499999999999996</v>
+        <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D115" s="1">
+        <v>6</v>
+      </c>
+      <c r="E115" s="1">
+        <v>3</v>
+      </c>
+      <c r="F115" s="1">
         <v>5</v>
       </c>
-      <c r="E115" s="1">
-        <v>5</v>
-      </c>
-      <c r="F115" s="1">
-        <v>3</v>
-      </c>
       <c r="G115" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H115" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I115" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C116" s="5">
-        <f t="shared" si="3"/>
-        <v>4.7875000000000005</v>
+        <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D116" s="1">
         <v>5</v>
       </c>
       <c r="E116" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F116" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G116" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H116" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I116" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I116" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C117" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5999999999999996</v>
+        <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D117" s="1">
         <v>5</v>
       </c>
       <c r="E117" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F117" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G117" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H117" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.8</v>
       </c>
       <c r="I117" s="3">
-        <v>4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C118" s="5">
-        <f t="shared" si="3"/>
-        <v>4.5874999999999995</v>
+        <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D118" s="1">
         <v>5</v>
       </c>
       <c r="E118" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F118" s="1">
         <v>5</v>
       </c>
       <c r="G118" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H118" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I118" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C119" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4249999999999998</v>
+        <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D119" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E119" s="1">
         <v>4</v>
       </c>
       <c r="F119" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G119" s="1">
         <v>5</v>
       </c>
       <c r="H119" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I119" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C120" s="5">
-        <f t="shared" si="3"/>
-        <v>4.4124999999999996</v>
+        <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D120" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E120" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F120" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G120" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I120" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="C121" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3375000000000004</v>
+        <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D121" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E121" s="1">
+        <v>0</v>
+      </c>
+      <c r="F121" s="1">
         <v>2</v>
       </c>
-      <c r="F121" s="1">
-        <v>4</v>
-      </c>
       <c r="G121" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H121" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I121" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C122" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3374999999999995</v>
+        <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D122" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E122" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F122" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G122" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H122" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I122" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C123" s="5">
-        <f t="shared" si="3"/>
-        <v>4.3125</v>
+        <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D123" s="1">
+        <v>5</v>
+      </c>
+      <c r="E123" s="1">
         <v>3</v>
       </c>
-      <c r="E123" s="1">
-        <v>4</v>
-      </c>
       <c r="F123" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G123" s="1">
         <v>4</v>
       </c>
       <c r="H123" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I123" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="C124" s="5">
-        <f t="shared" si="3"/>
-        <v>4.2749999999999995</v>
+        <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
+        <v>4.3125</v>
       </c>
       <c r="D124" s="1">
+        <v>3</v>
+      </c>
+      <c r="E124" s="1">
         <v>4</v>
       </c>
-      <c r="E124" s="1">
-        <v>2</v>
-      </c>
       <c r="F124" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G124" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H124" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
       <c r="I124" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C125" s="5">
-        <f t="shared" si="3"/>
-        <v>4.1124999999999998</v>
+        <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D125" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E125" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F125" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G125" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H125" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I125" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C126" s="5">
-        <f t="shared" si="3"/>
-        <v>3.7375000000000003</v>
+        <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D126" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E126" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F126" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G126" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H126" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I126" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C127" s="5">
-        <f t="shared" si="3"/>
-        <v>3.3250000000000002</v>
+        <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D127" s="1">
+        <v>3</v>
+      </c>
+      <c r="E127" s="1">
+        <v>3</v>
+      </c>
+      <c r="F127" s="1">
+        <v>3</v>
+      </c>
+      <c r="G127" s="1">
         <v>4</v>
       </c>
-      <c r="E127" s="1">
-        <v>1</v>
-      </c>
-      <c r="F127" s="1">
-        <v>2</v>
-      </c>
-      <c r="G127" s="1">
-        <v>2</v>
-      </c>
       <c r="H127" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I127" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C128" s="5">
-        <f t="shared" si="3"/>
-        <v>3.2749999999999995</v>
+        <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D128" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E128" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F128" s="1">
         <v>2</v>
       </c>
       <c r="G128" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H128" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I128" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C129" s="5">
-        <f t="shared" si="3"/>
-        <v>2.9124999999999996</v>
+        <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D129" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E129" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F129" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G129" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H129" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I129" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C130" s="5">
-        <f t="shared" si="3"/>
-        <v>2.6375000000000002</v>
+        <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F130" s="1">
         <v>0</v>
       </c>
       <c r="G130" s="1">
+        <v>1</v>
+      </c>
+      <c r="H130" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I130" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B131" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C131" s="5">
+        <f>AVERAGE(D131,E131,E131,F131,G131,H131,H131,I131)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D131" s="1">
         <v>0</v>
       </c>
-      <c r="H130" s="3">
+      <c r="E131" s="1">
+        <v>0</v>
+      </c>
+      <c r="F131" s="1">
+        <v>0</v>
+      </c>
+      <c r="G131" s="1">
+        <v>0</v>
+      </c>
+      <c r="H131" s="3">
         <v>7.6</v>
       </c>
-      <c r="I130" s="3">
+      <c r="I131" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 111 "EL juego bonito"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71706AAB-156A-447C-BBC6-692F6574FE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4787C48-9A79-496D-A1D2-43C076505AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="213">
   <si>
     <t>Película</t>
   </si>
@@ -1212,6 +1212,9 @@
   </si>
   <si>
     <t>El niño que domó el viento</t>
+  </si>
+  <si>
+    <t>El juego bonito</t>
   </si>
 </sst>
 </file>
@@ -1564,10 +1567,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I131" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I131" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I131">
-    <sortCondition descending="1" ref="C2:C131"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I132" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I132" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I132">
+    <sortCondition descending="1" ref="C2:C132"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4213,7 +4216,7 @@
         <v>91</v>
       </c>
       <c r="C67" s="5">
-        <f t="shared" ref="C67:C98" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
+        <f t="shared" ref="C67:C68" si="2">AVERAGE(D67,E67,F67,F67,G67,H67,H67,I67)</f>
         <v>5.4625000000000004</v>
       </c>
       <c r="D67" s="1">
@@ -4294,10 +4297,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K131"/>
+  <dimension ref="B2:K132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C131" sqref="C131"/>
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6342,7 +6345,7 @@
       </c>
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="2" t="s">
         <v>211</v>
       </c>
       <c r="C77" s="5">
@@ -7638,191 +7641,218 @@
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="2" t="s">
-        <v>167</v>
+      <c r="B125" s="9" t="s">
+        <v>212</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3</v>
       </c>
       <c r="D125" s="1">
         <v>4</v>
       </c>
       <c r="E125" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F125" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G125" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H125" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="I125" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D126" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E126" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F126" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G126" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H126" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I126" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D127" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E127" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F127" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G127" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H127" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I127" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D128" s="1">
+        <v>3</v>
+      </c>
+      <c r="E128" s="1">
+        <v>3</v>
+      </c>
+      <c r="F128" s="1">
+        <v>3</v>
+      </c>
+      <c r="G128" s="1">
         <v>4</v>
       </c>
-      <c r="E128" s="1">
-        <v>1</v>
-      </c>
-      <c r="F128" s="1">
-        <v>2</v>
-      </c>
-      <c r="G128" s="1">
-        <v>2</v>
-      </c>
       <c r="H128" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I128" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C129" s="5">
         <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D129" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E129" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F129" s="1">
         <v>2</v>
       </c>
       <c r="G129" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H129" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I129" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C130" s="5">
         <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D130" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E130" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F130" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G130" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H130" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I130" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C131" s="5">
         <f>AVERAGE(D131,E131,E131,F131,G131,H131,H131,I131)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D131" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F131" s="1">
         <v>0</v>
       </c>
       <c r="G131" s="1">
+        <v>1</v>
+      </c>
+      <c r="H131" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I131" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B132" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C132" s="5">
+        <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D132" s="1">
         <v>0</v>
       </c>
-      <c r="H131" s="3">
+      <c r="E132" s="1">
+        <v>0</v>
+      </c>
+      <c r="F132" s="1">
+        <v>0</v>
+      </c>
+      <c r="G132" s="1">
+        <v>0</v>
+      </c>
+      <c r="H132" s="3">
         <v>7.6</v>
       </c>
-      <c r="I131" s="3">
+      <c r="I132" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 112 "La vieja guardia"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4787C48-9A79-496D-A1D2-43C076505AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067AF27B-9095-4EFB-A778-F4186A20AF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="214">
   <si>
     <t>Película</t>
   </si>
@@ -1215,6 +1215,9 @@
   </si>
   <si>
     <t>El juego bonito</t>
+  </si>
+  <si>
+    <t>La vieja guardia</t>
   </si>
 </sst>
 </file>
@@ -1567,10 +1570,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I132" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I132" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I132">
-    <sortCondition descending="1" ref="C2:C132"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I133" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I133" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I133">
+    <sortCondition descending="1" ref="C2:C133"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4297,10 +4300,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K132"/>
+  <dimension ref="B2:K133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7452,407 +7455,434 @@
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B118" s="2" t="s">
-        <v>154</v>
+      <c r="B118" s="9" t="s">
+        <v>213</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.5999999999999996</v>
+        <v>4.6124999999999998</v>
       </c>
       <c r="D118" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E118" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F118" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G118" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H118" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
       <c r="I118" s="3">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D119" s="1">
         <v>5</v>
       </c>
       <c r="E119" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F119" s="1">
         <v>5</v>
       </c>
       <c r="G119" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H119" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I119" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D120" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E120" s="1">
         <v>4</v>
       </c>
       <c r="F120" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G120" s="1">
         <v>5</v>
       </c>
       <c r="H120" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I120" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D121" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E121" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F121" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G121" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I121" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.3375000000000004</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D122" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E122" s="1">
+        <v>0</v>
+      </c>
+      <c r="F122" s="1">
         <v>2</v>
       </c>
-      <c r="F122" s="1">
-        <v>4</v>
-      </c>
       <c r="G122" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H122" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I122" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D123" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E123" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F123" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G123" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H123" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I123" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D124" s="1">
+        <v>5</v>
+      </c>
+      <c r="E124" s="1">
         <v>3</v>
       </c>
-      <c r="E124" s="1">
-        <v>4</v>
-      </c>
       <c r="F124" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G124" s="1">
         <v>4</v>
       </c>
       <c r="H124" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I124" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B125" s="9" t="s">
-        <v>212</v>
+      <c r="B125" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>4.3</v>
+        <v>4.3125</v>
       </c>
       <c r="D125" s="1">
+        <v>3</v>
+      </c>
+      <c r="E125" s="1">
         <v>4</v>
       </c>
-      <c r="E125" s="1">
-        <v>3</v>
-      </c>
       <c r="F125" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G125" s="1">
         <v>4</v>
       </c>
       <c r="H125" s="3">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="I125" s="3">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3</v>
       </c>
       <c r="D126" s="1">
         <v>4</v>
       </c>
       <c r="E126" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F126" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G126" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H126" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="I126" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D127" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E127" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F127" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G127" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H127" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I127" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D128" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E128" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F128" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G128" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H128" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I128" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C129" s="5">
         <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D129" s="1">
+        <v>3</v>
+      </c>
+      <c r="E129" s="1">
+        <v>3</v>
+      </c>
+      <c r="F129" s="1">
+        <v>3</v>
+      </c>
+      <c r="G129" s="1">
         <v>4</v>
       </c>
-      <c r="E129" s="1">
-        <v>1</v>
-      </c>
-      <c r="F129" s="1">
-        <v>2</v>
-      </c>
-      <c r="G129" s="1">
-        <v>2</v>
-      </c>
       <c r="H129" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I129" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C130" s="5">
         <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D130" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E130" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F130" s="1">
         <v>2</v>
       </c>
       <c r="G130" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H130" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I130" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C131" s="5">
         <f>AVERAGE(D131,E131,E131,F131,G131,H131,H131,I131)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D131" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E131" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F131" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G131" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H131" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I131" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C132" s="5">
         <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D132" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E132" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F132" s="1">
         <v>0</v>
       </c>
       <c r="G132" s="1">
+        <v>1</v>
+      </c>
+      <c r="H132" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I132" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B133" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C133" s="5">
+        <f>AVERAGE(D133,E133,E133,F133,G133,H133,H133,I133)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D133" s="1">
         <v>0</v>
       </c>
-      <c r="H132" s="3">
+      <c r="E133" s="1">
+        <v>0</v>
+      </c>
+      <c r="F133" s="1">
+        <v>0</v>
+      </c>
+      <c r="G133" s="1">
+        <v>0</v>
+      </c>
+      <c r="H133" s="3">
         <v>7.6</v>
       </c>
-      <c r="I132" s="3">
+      <c r="I133" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 113 "La vieja guardia 2"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067AF27B-9095-4EFB-A778-F4186A20AF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50277C5-55AE-4123-93E4-0B8F45CA60EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="215">
   <si>
     <t>Película</t>
   </si>
@@ -1218,6 +1218,9 @@
   </si>
   <si>
     <t>La vieja guardia</t>
+  </si>
+  <si>
+    <t>La vieja guardia 2</t>
   </si>
 </sst>
 </file>
@@ -1570,10 +1573,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I133" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I133" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I133">
-    <sortCondition descending="1" ref="C2:C133"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I134" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I134" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I134">
+    <sortCondition descending="1" ref="C2:C134"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4300,10 +4303,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K133"/>
+  <dimension ref="B2:K134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+      <selection activeCell="C106" sqref="C106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6834,12 +6837,12 @@
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="2" t="s">
-        <v>160</v>
+      <c r="B95" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>6.05</v>
+        <v>6.0500000000000007</v>
       </c>
       <c r="D95" s="1">
         <v>7</v>
@@ -6851,49 +6854,49 @@
         <v>7</v>
       </c>
       <c r="G95" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H95" s="3">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I95" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
         <v>6.05</v>
       </c>
       <c r="D96" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E96" s="1">
         <v>6</v>
       </c>
       <c r="F96" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G96" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H96" s="3">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="I96" s="3">
-        <v>5.4</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D97" s="1">
         <v>6</v>
@@ -6902,133 +6905,133 @@
         <v>6</v>
       </c>
       <c r="F97" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G97" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="I97" s="3">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.8875000000000011</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D98" s="1">
         <v>6</v>
       </c>
       <c r="E98" s="1">
+        <v>6</v>
+      </c>
+      <c r="F98" s="1">
+        <v>8</v>
+      </c>
+      <c r="G98" s="1">
         <v>5</v>
       </c>
-      <c r="F98" s="1">
-        <v>6</v>
-      </c>
-      <c r="G98" s="1">
-        <v>6</v>
-      </c>
       <c r="H98" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I98" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.8125000000000009</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D99" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E99" s="1">
         <v>5</v>
       </c>
       <c r="F99" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G99" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H99" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I99" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.8000000000000007</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D100" s="1">
         <v>7</v>
       </c>
       <c r="E100" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F100" s="1">
         <v>5</v>
       </c>
       <c r="G100" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H100" s="3">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="I100" s="3">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>113</v>
+        <v>209</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="D101" s="1">
         <v>7</v>
       </c>
       <c r="E101" s="1">
+        <v>6</v>
+      </c>
+      <c r="F101" s="1">
         <v>5</v>
       </c>
-      <c r="F101" s="1">
-        <v>4</v>
-      </c>
       <c r="G101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H101" s="3">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="I101" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D102" s="1">
         <v>7</v>
@@ -7040,37 +7043,37 @@
         <v>4</v>
       </c>
       <c r="G102" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H102" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I102" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D103" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E103" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F103" s="1">
+        <v>4</v>
+      </c>
+      <c r="G103" s="1">
         <v>5</v>
       </c>
-      <c r="G103" s="1">
-        <v>6</v>
-      </c>
       <c r="H103" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I103" s="3">
         <v>6.4</v>
@@ -7078,50 +7081,50 @@
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D104" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E104" s="1">
+        <v>3</v>
+      </c>
+      <c r="F104" s="1">
         <v>5</v>
       </c>
-      <c r="F104" s="1">
-        <v>6</v>
-      </c>
       <c r="G104" s="1">
         <v>6</v>
       </c>
       <c r="H104" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I104" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D105" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E105" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F105" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G105" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H105" s="3">
         <v>5.8</v>
@@ -7132,260 +7135,260 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D106" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E106" s="1">
         <v>6</v>
       </c>
       <c r="F106" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H106" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I106" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E107" s="1">
         <v>6</v>
       </c>
       <c r="F107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G107" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H107" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I107" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
-        <v>5.3750000000000009</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D108" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E108" s="1">
+        <v>6</v>
+      </c>
+      <c r="F108" s="1">
         <v>5</v>
       </c>
-      <c r="F108" s="1">
-        <v>6</v>
-      </c>
       <c r="G108" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H108" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I108" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D109" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E109" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F109" s="1">
         <v>6</v>
       </c>
       <c r="G109" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H109" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I109" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D110" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G110" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H110" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I110" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D111" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E111" s="1">
         <v>5</v>
       </c>
       <c r="F111" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G111" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H111" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I111" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D112" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E112" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F112" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G112" s="1">
         <v>6</v>
       </c>
       <c r="H112" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I112" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D113" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E113" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F113" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G113" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H113" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I113" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D114" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E114" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F114" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G114" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H114" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I114" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D115" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E115" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F115" s="1">
         <v>5</v>
@@ -7394,495 +7397,522 @@
         <v>6</v>
       </c>
       <c r="H115" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I115" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D116" s="1">
+        <v>6</v>
+      </c>
+      <c r="E116" s="1">
+        <v>3</v>
+      </c>
+      <c r="F116" s="1">
         <v>5</v>
       </c>
-      <c r="E116" s="1">
-        <v>5</v>
-      </c>
-      <c r="F116" s="1">
-        <v>3</v>
-      </c>
       <c r="G116" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H116" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I116" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D117" s="1">
         <v>5</v>
       </c>
       <c r="E117" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F117" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G117" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H117" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I117" s="3">
         <v>4.8</v>
       </c>
-      <c r="I117" s="3">
-        <v>3.7</v>
-      </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B118" s="9" t="s">
-        <v>213</v>
+      <c r="B118" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.6124999999999998</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D118" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E118" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F118" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G118" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H118" s="3">
-        <v>6.7</v>
+        <v>4.8</v>
       </c>
       <c r="I118" s="3">
-        <v>5.5</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.5999999999999996</v>
+        <v>4.6124999999999998</v>
       </c>
       <c r="D119" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E119" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F119" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G119" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H119" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
       <c r="I119" s="3">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D120" s="1">
         <v>5</v>
       </c>
       <c r="E120" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F120" s="1">
         <v>5</v>
       </c>
       <c r="G120" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H120" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I120" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D121" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E121" s="1">
         <v>4</v>
       </c>
       <c r="F121" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G121" s="1">
         <v>5</v>
       </c>
       <c r="H121" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I121" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D122" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E122" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F122" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G122" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I122" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>4.3375000000000004</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D123" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E123" s="1">
+        <v>0</v>
+      </c>
+      <c r="F123" s="1">
         <v>2</v>
       </c>
-      <c r="F123" s="1">
-        <v>4</v>
-      </c>
       <c r="G123" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H123" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I123" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D124" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E124" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F124" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G124" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H124" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I124" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D125" s="1">
+        <v>5</v>
+      </c>
+      <c r="E125" s="1">
         <v>3</v>
       </c>
-      <c r="E125" s="1">
-        <v>4</v>
-      </c>
       <c r="F125" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G125" s="1">
         <v>4</v>
       </c>
       <c r="H125" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I125" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>4.3</v>
+        <v>4.3125</v>
       </c>
       <c r="D126" s="1">
+        <v>3</v>
+      </c>
+      <c r="E126" s="1">
         <v>4</v>
       </c>
-      <c r="E126" s="1">
-        <v>3</v>
-      </c>
       <c r="F126" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G126" s="1">
         <v>4</v>
       </c>
       <c r="H126" s="3">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="I126" s="3">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3</v>
       </c>
       <c r="D127" s="1">
         <v>4</v>
       </c>
       <c r="E127" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F127" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G127" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H127" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="I127" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D128" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E128" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F128" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G128" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H128" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I128" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C129" s="5">
         <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D129" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E129" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F129" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G129" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H129" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I129" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C130" s="5">
         <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D130" s="1">
+        <v>3</v>
+      </c>
+      <c r="E130" s="1">
+        <v>3</v>
+      </c>
+      <c r="F130" s="1">
+        <v>3</v>
+      </c>
+      <c r="G130" s="1">
         <v>4</v>
       </c>
-      <c r="E130" s="1">
-        <v>1</v>
-      </c>
-      <c r="F130" s="1">
-        <v>2</v>
-      </c>
-      <c r="G130" s="1">
-        <v>2</v>
-      </c>
       <c r="H130" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I130" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C131" s="5">
         <f>AVERAGE(D131,E131,E131,F131,G131,H131,H131,I131)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D131" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E131" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F131" s="1">
         <v>2</v>
       </c>
       <c r="G131" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H131" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I131" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C132" s="5">
         <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D132" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E132" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F132" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G132" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H132" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I132" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C133" s="5">
         <f>AVERAGE(D133,E133,E133,F133,G133,H133,H133,I133)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F133" s="1">
         <v>0</v>
       </c>
       <c r="G133" s="1">
+        <v>1</v>
+      </c>
+      <c r="H133" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I133" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B134" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C134" s="5">
+        <f>AVERAGE(D134,E134,E134,F134,G134,H134,H134,I134)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D134" s="1">
         <v>0</v>
       </c>
-      <c r="H133" s="3">
+      <c r="E134" s="1">
+        <v>0</v>
+      </c>
+      <c r="F134" s="1">
+        <v>0</v>
+      </c>
+      <c r="G134" s="1">
+        <v>0</v>
+      </c>
+      <c r="H134" s="3">
         <v>7.6</v>
       </c>
-      <c r="I133" s="3">
+      <c r="I134" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 114 "El hombre invisible"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50277C5-55AE-4123-93E4-0B8F45CA60EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A2CF7C-5702-406B-8859-964741FAF662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="216">
   <si>
     <t>Película</t>
   </si>
@@ -1221,6 +1221,9 @@
   </si>
   <si>
     <t>La vieja guardia 2</t>
+  </si>
+  <si>
+    <t>El agente invisible</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1576,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I134" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I134" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I134">
-    <sortCondition descending="1" ref="C2:C134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I135" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I135" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I135">
+    <sortCondition descending="1" ref="C2:C135"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4303,10 +4306,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K134"/>
+  <dimension ref="B2:K135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,18 +6462,18 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="2" t="s">
-        <v>168</v>
+      <c r="B81" s="9" t="s">
+        <v>215</v>
       </c>
       <c r="C81" s="5">
         <f>AVERAGE(D81,E81,E81,F81,G81,H81,H81,I81)</f>
-        <v>6.5499999999999989</v>
+        <v>6.5750000000000002</v>
       </c>
       <c r="D81" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E81" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F81" s="1">
         <v>7</v>
@@ -6479,76 +6482,76 @@
         <v>6</v>
       </c>
       <c r="H81" s="3">
-        <v>6.8</v>
+        <v>6.5</v>
       </c>
       <c r="I81" s="3">
-        <v>5.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="C82" s="5">
         <f>AVERAGE(D82,E82,E82,F82,G82,H82,H82,I82)</f>
-        <v>6.5375000000000005</v>
+        <v>6.5499999999999989</v>
       </c>
       <c r="D82" s="1">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E82" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F82" s="1">
         <v>7</v>
       </c>
       <c r="G82" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H82" s="3">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="I82" s="3">
-        <v>6.1</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="C83" s="5">
         <f>AVERAGE(D83,E83,E83,F83,G83,H83,H83,I83)</f>
-        <v>6.3999999999999995</v>
+        <v>6.5375000000000005</v>
       </c>
       <c r="D83" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E83" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F83" s="1">
         <v>7</v>
       </c>
       <c r="G83" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H83" s="3">
-        <v>6.4</v>
+        <v>7.1</v>
       </c>
       <c r="I83" s="3">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" s="2" t="s">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="C84" s="5">
         <f>AVERAGE(D84,E84,E84,F84,G84,H84,H84,I84)</f>
-        <v>6.3624999999999998</v>
+        <v>6.3999999999999995</v>
       </c>
       <c r="D84" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E84" s="1">
         <v>6</v>
@@ -6560,25 +6563,25 @@
         <v>7</v>
       </c>
       <c r="H84" s="3">
-        <v>5.9</v>
+        <v>6.4</v>
       </c>
       <c r="I84" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" s="2" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="C85" s="5">
         <f>AVERAGE(D85,E85,E85,F85,G85,H85,H85,I85)</f>
         <v>6.3624999999999998</v>
       </c>
       <c r="D85" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E85" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F85" s="1">
         <v>7</v>
@@ -6587,79 +6590,79 @@
         <v>7</v>
       </c>
       <c r="H85" s="3">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="I85" s="3">
-        <v>4.9000000000000004</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" s="2" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C86" s="5">
         <f>AVERAGE(D86,E86,E86,F86,G86,H86,H86,I86)</f>
-        <v>6.35</v>
+        <v>6.3624999999999998</v>
       </c>
       <c r="D86" s="1">
         <v>7</v>
       </c>
       <c r="E86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F86" s="1">
         <v>7</v>
       </c>
       <c r="G86" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H86" s="3">
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
       <c r="I86" s="3">
-        <v>5.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" s="2" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="C87" s="5">
         <f>AVERAGE(D87,E87,E87,F87,G87,H87,H87,I87)</f>
         <v>6.35</v>
       </c>
       <c r="D87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E87" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F87" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G87" s="1">
         <v>6</v>
       </c>
       <c r="H87" s="3">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="I87" s="3">
-        <v>6.2</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" s="2" t="s">
-        <v>134</v>
+        <v>208</v>
       </c>
       <c r="C88" s="5">
         <f>AVERAGE(D88,E88,E88,F88,G88,H88,H88,I88)</f>
-        <v>6.3125</v>
+        <v>6.35</v>
       </c>
       <c r="D88" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E88" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88" s="1">
         <v>6</v>
@@ -6668,42 +6671,42 @@
         <v>6</v>
       </c>
       <c r="H88" s="3">
-        <v>6.9</v>
+        <v>6.3</v>
       </c>
       <c r="I88" s="3">
-        <v>5.7</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C89" s="5">
         <f>AVERAGE(D89,E89,E89,F89,G89,H89,H89,I89)</f>
-        <v>6.2749999999999995</v>
+        <v>6.3125</v>
       </c>
       <c r="D89" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E89" s="1">
         <v>6</v>
       </c>
       <c r="F89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G89" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H89" s="3">
-        <v>6.3</v>
+        <v>6.9</v>
       </c>
       <c r="I89" s="3">
-        <v>5.6</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" s="2" t="s">
-        <v>64</v>
+        <v>144</v>
       </c>
       <c r="C90" s="5">
         <f>AVERAGE(D90,E90,E90,F90,G90,H90,H90,I90)</f>
@@ -6713,163 +6716,163 @@
         <v>6</v>
       </c>
       <c r="E90" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G90" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H90" s="3">
-        <v>6.4</v>
+        <v>6.3</v>
       </c>
       <c r="I90" s="3">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" s="2" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C91" s="5">
         <f>AVERAGE(D91,E91,E91,F91,G91,H91,H91,I91)</f>
-        <v>6.2125000000000004</v>
+        <v>6.2749999999999995</v>
       </c>
       <c r="D91" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E91" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G91" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H91" s="3">
-        <v>5.0999999999999996</v>
+        <v>6.4</v>
       </c>
       <c r="I91" s="3">
-        <v>4.5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" s="2" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="C92" s="5">
         <f>AVERAGE(D92,E92,E92,F92,G92,H92,H92,I92)</f>
-        <v>6.2124999999999995</v>
+        <v>6.2125000000000004</v>
       </c>
       <c r="D92" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E92" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F92" s="1">
         <v>8</v>
       </c>
       <c r="G92" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H92" s="3">
-        <v>4.3</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I92" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" s="2" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="C93" s="5">
         <f>AVERAGE(D93,E93,E93,F93,G93,H93,H93,I93)</f>
-        <v>6.15</v>
+        <v>6.2124999999999995</v>
       </c>
       <c r="D93" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E93" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F93" s="1">
         <v>8</v>
       </c>
       <c r="G93" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H93" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="I93" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" s="2" t="s">
-        <v>158</v>
+        <v>101</v>
       </c>
       <c r="C94" s="5">
         <f>AVERAGE(D94,E94,E94,F94,G94,H94,H94,I94)</f>
-        <v>6.0874999999999995</v>
+        <v>6.15</v>
       </c>
       <c r="D94" s="1">
         <v>7</v>
       </c>
       <c r="E94" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F94" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G94" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H94" s="3">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="I94" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B95" s="9" t="s">
-        <v>214</v>
+      <c r="B95" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="C95" s="5">
         <f>AVERAGE(D95,E95,E95,F95,G95,H95,H95,I95)</f>
-        <v>6.0500000000000007</v>
+        <v>6.0874999999999995</v>
       </c>
       <c r="D95" s="1">
         <v>7</v>
       </c>
       <c r="E95" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F95" s="1">
         <v>7</v>
       </c>
       <c r="G95" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H95" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="I95" s="3">
-        <v>4.2</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" s="2" t="s">
-        <v>160</v>
+        <v>214</v>
       </c>
       <c r="C96" s="5">
         <f>AVERAGE(D96,E96,E96,F96,G96,H96,H96,I96)</f>
-        <v>6.05</v>
+        <v>6.0500000000000007</v>
       </c>
       <c r="D96" s="1">
         <v>7</v>
@@ -6881,49 +6884,49 @@
         <v>7</v>
       </c>
       <c r="G96" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H96" s="3">
-        <v>5.4</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I96" s="3">
-        <v>4.5999999999999996</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" s="2" t="s">
-        <v>206</v>
+        <v>160</v>
       </c>
       <c r="C97" s="5">
         <f>AVERAGE(D97,E97,E97,F97,G97,H97,H97,I97)</f>
         <v>6.05</v>
       </c>
       <c r="D97" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E97" s="1">
         <v>6</v>
       </c>
       <c r="F97" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G97" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H97" s="3">
-        <v>6.5</v>
+        <v>5.4</v>
       </c>
       <c r="I97" s="3">
-        <v>5.4</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" s="2" t="s">
-        <v>159</v>
+        <v>206</v>
       </c>
       <c r="C98" s="5">
         <f>AVERAGE(D98,E98,E98,F98,G98,H98,H98,I98)</f>
-        <v>5.9499999999999993</v>
+        <v>6.05</v>
       </c>
       <c r="D98" s="1">
         <v>6</v>
@@ -6932,133 +6935,133 @@
         <v>6</v>
       </c>
       <c r="F98" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G98" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H98" s="3">
-        <v>5.8</v>
+        <v>6.5</v>
       </c>
       <c r="I98" s="3">
-        <v>5</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" s="2" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="C99" s="5">
         <f>AVERAGE(D99,E99,E99,F99,G99,H99,H99,I99)</f>
-        <v>5.8875000000000011</v>
+        <v>5.9499999999999993</v>
       </c>
       <c r="D99" s="1">
         <v>6</v>
       </c>
       <c r="E99" s="1">
+        <v>6</v>
+      </c>
+      <c r="F99" s="1">
+        <v>8</v>
+      </c>
+      <c r="G99" s="1">
         <v>5</v>
       </c>
-      <c r="F99" s="1">
-        <v>6</v>
-      </c>
-      <c r="G99" s="1">
-        <v>6</v>
-      </c>
       <c r="H99" s="3">
-        <v>6.7</v>
+        <v>5.8</v>
       </c>
       <c r="I99" s="3">
-        <v>5.7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C100" s="5">
         <f>AVERAGE(D100,E100,E100,F100,G100,H100,H100,I100)</f>
-        <v>5.8125000000000009</v>
+        <v>5.8875000000000011</v>
       </c>
       <c r="D100" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E100" s="1">
         <v>5</v>
       </c>
       <c r="F100" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G100" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H100" s="3">
-        <v>6.2</v>
+        <v>6.7</v>
       </c>
       <c r="I100" s="3">
-        <v>5.0999999999999996</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" s="2" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="C101" s="5">
         <f>AVERAGE(D101,E101,E101,F101,G101,H101,H101,I101)</f>
-        <v>5.8000000000000007</v>
+        <v>5.8125000000000009</v>
       </c>
       <c r="D101" s="1">
         <v>7</v>
       </c>
       <c r="E101" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F101" s="1">
         <v>5</v>
       </c>
       <c r="G101" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H101" s="3">
-        <v>6.1</v>
+        <v>6.2</v>
       </c>
       <c r="I101" s="3">
-        <v>5.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" s="2" t="s">
-        <v>113</v>
+        <v>209</v>
       </c>
       <c r="C102" s="5">
         <f>AVERAGE(D102,E102,E102,F102,G102,H102,H102,I102)</f>
-        <v>5.7374999999999989</v>
+        <v>5.8000000000000007</v>
       </c>
       <c r="D102" s="1">
         <v>7</v>
       </c>
       <c r="E102" s="1">
+        <v>6</v>
+      </c>
+      <c r="F102" s="1">
         <v>5</v>
       </c>
-      <c r="F102" s="1">
-        <v>4</v>
-      </c>
       <c r="G102" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H102" s="3">
-        <v>6.8</v>
+        <v>6.1</v>
       </c>
       <c r="I102" s="3">
-        <v>5.3</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" s="2" t="s">
-        <v>187</v>
+        <v>113</v>
       </c>
       <c r="C103" s="5">
         <f>AVERAGE(D103,E103,E103,F103,G103,H103,H103,I103)</f>
-        <v>5.7250000000000005</v>
+        <v>5.7374999999999989</v>
       </c>
       <c r="D103" s="1">
         <v>7</v>
@@ -7070,37 +7073,37 @@
         <v>4</v>
       </c>
       <c r="G103" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H103" s="3">
-        <v>6.7</v>
+        <v>6.8</v>
       </c>
       <c r="I103" s="3">
-        <v>6.4</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" s="2" t="s">
-        <v>26</v>
+        <v>187</v>
       </c>
       <c r="C104" s="5">
         <f>AVERAGE(D104,E104,E104,F104,G104,H104,H104,I104)</f>
-        <v>5.6749999999999998</v>
+        <v>5.7250000000000005</v>
       </c>
       <c r="D104" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E104" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F104" s="1">
+        <v>4</v>
+      </c>
+      <c r="G104" s="1">
         <v>5</v>
       </c>
-      <c r="G104" s="1">
-        <v>6</v>
-      </c>
       <c r="H104" s="3">
-        <v>7</v>
+        <v>6.7</v>
       </c>
       <c r="I104" s="3">
         <v>6.4</v>
@@ -7108,50 +7111,50 @@
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" s="2" t="s">
-        <v>149</v>
+        <v>26</v>
       </c>
       <c r="C105" s="5">
         <f>AVERAGE(D105,E105,E105,F105,G105,H105,H105,I105)</f>
-        <v>5.5624999999999991</v>
+        <v>5.6749999999999998</v>
       </c>
       <c r="D105" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E105" s="1">
+        <v>3</v>
+      </c>
+      <c r="F105" s="1">
         <v>5</v>
       </c>
-      <c r="F105" s="1">
-        <v>6</v>
-      </c>
       <c r="G105" s="1">
         <v>6</v>
       </c>
       <c r="H105" s="3">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="I105" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C106" s="5">
         <f>AVERAGE(D106,E106,E106,F106,G106,H106,H106,I106)</f>
         <v>5.5624999999999991</v>
       </c>
       <c r="D106" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E106" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F106" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G106" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H106" s="3">
         <v>5.8</v>
@@ -7162,260 +7165,260 @@
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C107" s="5">
         <f>AVERAGE(D107,E107,E107,F107,G107,H107,H107,I107)</f>
-        <v>5.4874999999999989</v>
+        <v>5.5624999999999991</v>
       </c>
       <c r="D107" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E107" s="1">
         <v>6</v>
       </c>
       <c r="F107" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G107" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H107" s="3">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
       <c r="I107" s="3">
-        <v>4.3</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" s="2" t="s">
-        <v>191</v>
+        <v>166</v>
       </c>
       <c r="C108" s="5">
         <f>AVERAGE(D108,E108,E108,F108,G108,H108,H108,I108)</f>
         <v>5.4874999999999989</v>
       </c>
       <c r="D108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E108" s="1">
         <v>6</v>
       </c>
       <c r="F108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G108" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I108" s="3">
-        <v>5.3</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" s="2" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="C109" s="5">
         <f>AVERAGE(D109,E109,E109,F109,G109,H109,H109,I109)</f>
-        <v>5.3750000000000009</v>
+        <v>5.4874999999999989</v>
       </c>
       <c r="D109" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E109" s="1">
+        <v>6</v>
+      </c>
+      <c r="F109" s="1">
         <v>5</v>
       </c>
-      <c r="F109" s="1">
-        <v>6</v>
-      </c>
       <c r="G109" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H109" s="3">
-        <v>4.7</v>
+        <v>5.8</v>
       </c>
       <c r="I109" s="3">
-        <v>4.5999999999999996</v>
+        <v>5.3</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" s="2" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="C110" s="5">
         <f>AVERAGE(D110,E110,E110,F110,G110,H110,H110,I110)</f>
-        <v>5.375</v>
+        <v>5.3750000000000009</v>
       </c>
       <c r="D110" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E110" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F110" s="1">
         <v>6</v>
       </c>
       <c r="G110" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H110" s="3">
-        <v>5.6</v>
+        <v>4.7</v>
       </c>
       <c r="I110" s="3">
-        <v>4.8</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" s="2" t="s">
-        <v>182</v>
+        <v>190</v>
       </c>
       <c r="C111" s="5">
         <f>AVERAGE(D111,E111,E111,F111,G111,H111,H111,I111)</f>
-        <v>5.2875000000000005</v>
+        <v>5.375</v>
       </c>
       <c r="D111" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G111" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H111" s="3">
-        <v>6.1</v>
+        <v>5.6</v>
       </c>
       <c r="I111" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" s="2" t="s">
-        <v>74</v>
+        <v>182</v>
       </c>
       <c r="C112" s="5">
         <f>AVERAGE(D112,E112,E112,F112,G112,H112,H112,I112)</f>
-        <v>5.1875</v>
+        <v>5.2875000000000005</v>
       </c>
       <c r="D112" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E112" s="1">
         <v>5</v>
       </c>
       <c r="F112" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G112" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H112" s="3">
-        <v>4.5</v>
+        <v>6.1</v>
       </c>
       <c r="I112" s="3">
-        <v>3.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" s="2" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="C113" s="5">
         <f>AVERAGE(D113,E113,E113,F113,G113,H113,H113,I113)</f>
-        <v>5.1124999999999998</v>
+        <v>5.1875</v>
       </c>
       <c r="D113" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E113" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F113" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G113" s="1">
         <v>6</v>
       </c>
       <c r="H113" s="3">
-        <v>5.9</v>
+        <v>4.5</v>
       </c>
       <c r="I113" s="3">
-        <v>5.0999999999999996</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" s="2" t="s">
-        <v>21</v>
+        <v>145</v>
       </c>
       <c r="C114" s="5">
         <f>AVERAGE(D114,E114,E114,F114,G114,H114,H114,I114)</f>
-        <v>5.05</v>
+        <v>5.1124999999999998</v>
       </c>
       <c r="D114" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E114" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F114" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G114" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H114" s="3">
-        <v>6.8</v>
+        <v>5.9</v>
       </c>
       <c r="I114" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" s="2" t="s">
-        <v>203</v>
+        <v>21</v>
       </c>
       <c r="C115" s="5">
         <f>AVERAGE(D115,E115,E115,F115,G115,H115,H115,I115)</f>
-        <v>4.9875000000000007</v>
+        <v>5.05</v>
       </c>
       <c r="D115" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E115" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F115" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G115" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H115" s="3">
-        <v>4.0999999999999996</v>
+        <v>6.8</v>
       </c>
       <c r="I115" s="3">
-        <v>3.7</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="C116" s="5">
         <f>AVERAGE(D116,E116,E116,F116,G116,H116,H116,I116)</f>
-        <v>4.9874999999999998</v>
+        <v>4.9875000000000007</v>
       </c>
       <c r="D116" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E116" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F116" s="1">
         <v>5</v>
@@ -7424,495 +7427,522 @@
         <v>6</v>
       </c>
       <c r="H116" s="3">
-        <v>6</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="I116" s="3">
-        <v>4.9000000000000004</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="C117" s="5">
         <f>AVERAGE(D117,E117,E117,F117,G117,H117,H117,I117)</f>
-        <v>4.8499999999999996</v>
+        <v>4.9874999999999998</v>
       </c>
       <c r="D117" s="1">
+        <v>6</v>
+      </c>
+      <c r="E117" s="1">
+        <v>3</v>
+      </c>
+      <c r="F117" s="1">
         <v>5</v>
       </c>
-      <c r="E117" s="1">
-        <v>5</v>
-      </c>
-      <c r="F117" s="1">
-        <v>3</v>
-      </c>
       <c r="G117" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H117" s="3">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="I117" s="3">
-        <v>4.8</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C118" s="5">
         <f>AVERAGE(D118,E118,E118,F118,G118,H118,H118,I118)</f>
-        <v>4.7875000000000005</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D118" s="1">
         <v>5</v>
       </c>
       <c r="E118" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F118" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G118" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H118" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I118" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I118" s="3">
-        <v>3.7</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
-        <v>213</v>
+        <v>162</v>
       </c>
       <c r="C119" s="5">
         <f>AVERAGE(D119,E119,E119,F119,G119,H119,H119,I119)</f>
-        <v>4.6124999999999998</v>
+        <v>4.7875000000000005</v>
       </c>
       <c r="D119" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E119" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F119" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G119" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H119" s="3">
-        <v>6.7</v>
+        <v>4.8</v>
       </c>
       <c r="I119" s="3">
-        <v>5.5</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="C120" s="5">
         <f>AVERAGE(D120,E120,E120,F120,G120,H120,H120,I120)</f>
-        <v>4.5999999999999996</v>
+        <v>4.6124999999999998</v>
       </c>
       <c r="D120" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E120" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F120" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G120" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H120" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.7</v>
       </c>
       <c r="I120" s="3">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="C121" s="5">
         <f>AVERAGE(D121,E121,E121,F121,G121,H121,H121,I121)</f>
-        <v>4.5874999999999995</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D121" s="1">
         <v>5</v>
       </c>
       <c r="E121" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F121" s="1">
         <v>5</v>
       </c>
       <c r="G121" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H121" s="3">
         <v>4.9000000000000004</v>
       </c>
       <c r="I121" s="3">
-        <v>3.9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="C122" s="5">
         <f>AVERAGE(D122,E122,E122,F122,G122,H122,H122,I122)</f>
-        <v>4.4249999999999998</v>
+        <v>4.5874999999999995</v>
       </c>
       <c r="D122" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E122" s="1">
         <v>4</v>
       </c>
       <c r="F122" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G122" s="1">
         <v>5</v>
       </c>
       <c r="H122" s="3">
-        <v>5.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I122" s="3">
-        <v>4.4000000000000004</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="C123" s="5">
         <f>AVERAGE(D123,E123,E123,F123,G123,H123,H123,I123)</f>
-        <v>4.4124999999999996</v>
+        <v>4.4249999999999998</v>
       </c>
       <c r="D123" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E123" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F123" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G123" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H123" s="3">
-        <v>8.1999999999999993</v>
+        <v>5.5</v>
       </c>
       <c r="I123" s="3">
-        <v>7.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
-        <v>207</v>
+        <v>114</v>
       </c>
       <c r="C124" s="5">
         <f>AVERAGE(D124,E124,E124,F124,G124,H124,H124,I124)</f>
-        <v>4.3375000000000004</v>
+        <v>4.4124999999999996</v>
       </c>
       <c r="D124" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E124" s="1">
+        <v>0</v>
+      </c>
+      <c r="F124" s="1">
         <v>2</v>
       </c>
-      <c r="F124" s="1">
-        <v>4</v>
-      </c>
       <c r="G124" s="1">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H124" s="3">
-        <v>6</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="I124" s="3">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
-        <v>150</v>
+        <v>207</v>
       </c>
       <c r="C125" s="5">
         <f>AVERAGE(D125,E125,E125,F125,G125,H125,H125,I125)</f>
-        <v>4.3374999999999995</v>
+        <v>4.3375000000000004</v>
       </c>
       <c r="D125" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E125" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F125" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G125" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H125" s="3">
-        <v>5.9</v>
+        <v>6</v>
       </c>
       <c r="I125" s="3">
-        <v>4.9000000000000004</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
-        <v>173</v>
+        <v>150</v>
       </c>
       <c r="C126" s="5">
         <f>AVERAGE(D126,E126,E126,F126,G126,H126,H126,I126)</f>
-        <v>4.3125</v>
+        <v>4.3374999999999995</v>
       </c>
       <c r="D126" s="1">
+        <v>5</v>
+      </c>
+      <c r="E126" s="1">
         <v>3</v>
       </c>
-      <c r="E126" s="1">
-        <v>4</v>
-      </c>
       <c r="F126" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G126" s="1">
         <v>4</v>
       </c>
       <c r="H126" s="3">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
       <c r="I126" s="3">
-        <v>4.7</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="C127" s="5">
         <f>AVERAGE(D127,E127,E127,F127,G127,H127,H127,I127)</f>
-        <v>4.3</v>
+        <v>4.3125</v>
       </c>
       <c r="D127" s="1">
+        <v>3</v>
+      </c>
+      <c r="E127" s="1">
         <v>4</v>
       </c>
-      <c r="E127" s="1">
-        <v>3</v>
-      </c>
       <c r="F127" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G127" s="1">
         <v>4</v>
       </c>
       <c r="H127" s="3">
-        <v>6.3</v>
+        <v>5.4</v>
       </c>
       <c r="I127" s="3">
-        <v>4.8</v>
+        <v>4.7</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
-        <v>167</v>
+        <v>212</v>
       </c>
       <c r="C128" s="5">
         <f>AVERAGE(D128,E128,E128,F128,G128,H128,H128,I128)</f>
-        <v>4.2749999999999995</v>
+        <v>4.3</v>
       </c>
       <c r="D128" s="1">
         <v>4</v>
       </c>
       <c r="E128" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F128" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G128" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H128" s="3">
-        <v>4.9000000000000004</v>
+        <v>6.3</v>
       </c>
       <c r="I128" s="3">
-        <v>4.4000000000000004</v>
+        <v>4.8</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="C129" s="5">
         <f>AVERAGE(D129,E129,E129,F129,G129,H129,H129,I129)</f>
-        <v>4.1124999999999998</v>
+        <v>4.2749999999999995</v>
       </c>
       <c r="D129" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E129" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F129" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G129" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H129" s="3">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I129" s="3">
-        <v>3.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
-        <v>199</v>
+        <v>68</v>
       </c>
       <c r="C130" s="5">
         <f>AVERAGE(D130,E130,E130,F130,G130,H130,H130,I130)</f>
-        <v>3.7375000000000003</v>
+        <v>4.1124999999999998</v>
       </c>
       <c r="D130" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E130" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F130" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G130" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H130" s="3">
-        <v>4.8</v>
+        <v>4.5</v>
       </c>
       <c r="I130" s="3">
-        <v>4.3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
       <c r="C131" s="5">
         <f>AVERAGE(D131,E131,E131,F131,G131,H131,H131,I131)</f>
-        <v>3.3250000000000002</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D131" s="1">
+        <v>3</v>
+      </c>
+      <c r="E131" s="1">
+        <v>3</v>
+      </c>
+      <c r="F131" s="1">
+        <v>3</v>
+      </c>
+      <c r="G131" s="1">
         <v>4</v>
       </c>
-      <c r="E131" s="1">
-        <v>1</v>
-      </c>
-      <c r="F131" s="1">
-        <v>2</v>
-      </c>
-      <c r="G131" s="1">
-        <v>2</v>
-      </c>
       <c r="H131" s="3">
-        <v>5.8</v>
+        <v>4.8</v>
       </c>
       <c r="I131" s="3">
-        <v>5</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C132" s="5">
         <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D132" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E132" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F132" s="1">
         <v>2</v>
       </c>
       <c r="G132" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H132" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I132" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C133" s="5">
         <f>AVERAGE(D133,E133,E133,F133,G133,H133,H133,I133)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D133" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F133" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G133" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H133" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I133" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C134" s="5">
         <f>AVERAGE(D134,E134,E134,F134,G134,H134,H134,I134)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D134" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E134" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F134" s="1">
         <v>0</v>
       </c>
       <c r="G134" s="1">
+        <v>1</v>
+      </c>
+      <c r="H134" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I134" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B135" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C135" s="5">
+        <f>AVERAGE(D135,E135,E135,F135,G135,H135,H135,I135)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D135" s="1">
         <v>0</v>
       </c>
-      <c r="H134" s="3">
+      <c r="E135" s="1">
+        <v>0</v>
+      </c>
+      <c r="F135" s="1">
+        <v>0</v>
+      </c>
+      <c r="G135" s="1">
+        <v>0</v>
+      </c>
+      <c r="H135" s="3">
         <v>7.6</v>
       </c>
-      <c r="I134" s="3">
+      <c r="I135" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 115 "Tiempo para mi"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A2CF7C-5702-406B-8859-964741FAF662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC0707-06FC-4D9F-B53B-EEEDA333AA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="217">
   <si>
     <t>Película</t>
   </si>
@@ -1224,6 +1224,9 @@
   </si>
   <si>
     <t>El agente invisible</t>
+  </si>
+  <si>
+    <t>Tiempo para mi</t>
   </si>
 </sst>
 </file>
@@ -1576,10 +1579,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I135" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I135" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I135">
-    <sortCondition descending="1" ref="C2:C135"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I136" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I136" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I136">
+    <sortCondition descending="1" ref="C2:C136"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4306,10 +4309,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K135"/>
+  <dimension ref="B2:K136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C136" sqref="C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6462,7 +6465,7 @@
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="2" t="s">
         <v>215</v>
       </c>
       <c r="C81" s="5">
@@ -7839,110 +7842,137 @@
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
-        <v>189</v>
+      <c r="B132" s="9" t="s">
+        <v>216</v>
       </c>
       <c r="C132" s="5">
         <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
-        <v>3.3250000000000002</v>
+        <v>3.5375000000000005</v>
       </c>
       <c r="D132" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E132" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F132" s="1">
         <v>2</v>
       </c>
       <c r="G132" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H132" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I132" s="3">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C133" s="5">
         <f>AVERAGE(D133,E133,E133,F133,G133,H133,H133,I133)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D133" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E133" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F133" s="1">
         <v>2</v>
       </c>
       <c r="G133" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H133" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I133" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C134" s="5">
         <f>AVERAGE(D134,E134,E134,F134,G134,H134,H134,I134)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D134" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E134" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F134" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G134" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H134" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I134" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C135" s="5">
         <f>AVERAGE(D135,E135,E135,F135,G135,H135,H135,I135)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" s="1">
         <v>0</v>
       </c>
       <c r="G135" s="1">
+        <v>1</v>
+      </c>
+      <c r="H135" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I135" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B136" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C136" s="5">
+        <f>AVERAGE(D136,E136,E136,F136,G136,H136,H136,I136)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D136" s="1">
         <v>0</v>
       </c>
-      <c r="H135" s="3">
+      <c r="E136" s="1">
+        <v>0</v>
+      </c>
+      <c r="F136" s="1">
+        <v>0</v>
+      </c>
+      <c r="G136" s="1">
+        <v>0</v>
+      </c>
+      <c r="H136" s="3">
         <v>7.6</v>
       </c>
-      <c r="I135" s="3">
+      <c r="I136" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
V. 117 "Blue Beetle"
</commit_message>
<xml_diff>
--- a/Calificacion.xlsx
+++ b/Calificacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE127FE-A09A-4A5A-B570-FB6CE79E4AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB1D494-7649-41CC-ACC8-E35F622E27C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -576,7 +576,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="219">
   <si>
     <t>Película</t>
   </si>
@@ -1230,6 +1230,9 @@
   </si>
   <si>
     <t>Damsel</t>
+  </si>
+  <si>
+    <t>Blue Beetle</t>
   </si>
 </sst>
 </file>
@@ -1582,10 +1585,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I137" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B2:I137" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I137">
-    <sortCondition descending="1" ref="C2:C137"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}" name="Tabla24" displayName="Tabla24" ref="B2:I138" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B2:I138" xr:uid="{BCA867C2-0242-44D1-BB58-FF0B1A23C5D8}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:I138">
+    <sortCondition descending="1" ref="C2:C138"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{349FB812-864A-4C0A-99F7-6285DFA6525F}" name="Película" dataDxfId="7"/>
@@ -4312,10 +4315,10 @@
     <tabColor theme="9"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:K137"/>
+  <dimension ref="B2:K138"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A112" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+      <selection activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5253,7 +5256,7 @@
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="2" t="s">
         <v>217</v>
       </c>
       <c r="C36" s="5">
@@ -7845,12 +7848,12 @@
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B132" s="2" t="s">
-        <v>199</v>
+      <c r="B132" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="C132" s="5">
         <f>AVERAGE(D132,E132,E132,F132,G132,H132,H132,I132)</f>
-        <v>3.7375000000000003</v>
+        <v>3.9499999999999997</v>
       </c>
       <c r="D132" s="1">
         <v>3</v>
@@ -7859,150 +7862,177 @@
         <v>3</v>
       </c>
       <c r="F132" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G132" s="1">
         <v>4</v>
       </c>
       <c r="H132" s="3">
+        <v>5.9</v>
+      </c>
+      <c r="I132" s="3">
         <v>4.8</v>
-      </c>
-      <c r="I132" s="3">
-        <v>4.3</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="C133" s="5">
         <f>AVERAGE(D133,E133,E133,F133,G133,H133,H133,I133)</f>
-        <v>3.5375000000000005</v>
+        <v>3.7375000000000003</v>
       </c>
       <c r="D133" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E133" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F133" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G133" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H133" s="3">
-        <v>5.0999999999999996</v>
+        <v>4.8</v>
       </c>
       <c r="I133" s="3">
-        <v>4.0999999999999996</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
-        <v>189</v>
+        <v>216</v>
       </c>
       <c r="C134" s="5">
         <f>AVERAGE(D134,E134,E134,F134,G134,H134,H134,I134)</f>
-        <v>3.3250000000000002</v>
+        <v>3.5375000000000005</v>
       </c>
       <c r="D134" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E134" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F134" s="1">
         <v>2</v>
       </c>
       <c r="G134" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H134" s="3">
-        <v>5.8</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="I134" s="3">
-        <v>5</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C135" s="5">
         <f>AVERAGE(D135,E135,E135,F135,G135,H135,H135,I135)</f>
-        <v>3.2749999999999995</v>
+        <v>3.3250000000000002</v>
       </c>
       <c r="D135" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E135" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F135" s="1">
         <v>2</v>
       </c>
       <c r="G135" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H135" s="3">
-        <v>5.4</v>
+        <v>5.8</v>
       </c>
       <c r="I135" s="3">
-        <v>4.4000000000000004</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="C136" s="5">
         <f>AVERAGE(D136,E136,E136,F136,G136,H136,H136,I136)</f>
-        <v>2.9124999999999996</v>
+        <v>3.2749999999999995</v>
       </c>
       <c r="D136" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E136" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F136" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G136" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H136" s="3">
-        <v>6.7</v>
+        <v>5.4</v>
       </c>
       <c r="I136" s="3">
-        <v>5.9</v>
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
-        <v>174</v>
+        <v>155</v>
       </c>
       <c r="C137" s="5">
         <f>AVERAGE(D137,E137,E137,F137,G137,H137,H137,I137)</f>
-        <v>2.6375000000000002</v>
+        <v>2.9124999999999996</v>
       </c>
       <c r="D137" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F137" s="1">
         <v>0</v>
       </c>
       <c r="G137" s="1">
+        <v>1</v>
+      </c>
+      <c r="H137" s="3">
+        <v>6.7</v>
+      </c>
+      <c r="I137" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B138" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C138" s="5">
+        <f>AVERAGE(D138,E138,E138,F138,G138,H138,H138,I138)</f>
+        <v>2.6375000000000002</v>
+      </c>
+      <c r="D138" s="1">
         <v>0</v>
       </c>
-      <c r="H137" s="3">
+      <c r="E138" s="1">
+        <v>0</v>
+      </c>
+      <c r="F138" s="1">
+        <v>0</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+      <c r="H138" s="3">
         <v>7.6</v>
       </c>
-      <c r="I137" s="3">
+      <c r="I138" s="3">
         <v>5.9</v>
       </c>
     </row>

</xml_diff>